<commit_message>
Working on the ability to dump individual files, as well as fixing a major bug, on file 72
</commit_message>
<xml_diff>
--- a/Covid_19_Dataset_and_References/References/10.xlsx
+++ b/Covid_19_Dataset_and_References/References/10.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="234">
   <si>
     <t>Doi</t>
   </si>
@@ -1024,6 +1024,216 @@
   </si>
   <si>
     <t>PMC7287415</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Background
+Skilled nursing facilities (SNFs) are high-risk settings for SARS-CoV-2 transmission.
+ Infection rates among employees are infrequently described.
+Objective
+id="Par2"&gt;To describe SARS-CoV-2 rates among SNF employees and residents during a non-outbreak time period, we measured cross-sectional SARS-CoV-2 prevalence across multiple sites in the Seattle area.
+Design
+id="Par3"&gt;SARS-CoV-2 testing was performed for SNF employees and residents using quantitative real-time reverse transcription polymerase chain reaction.
+ A subset of employees completed a sociodemographic and symptom questionnaire.
+Participants
+id="Par4"&gt;Between March 29 and May 13, 2020, we tested 1583 employees and 1208 residents at 16 SNFs for SARS-CoV-2.
+Main Measure
+id="Par5"&gt;SARS-CoV-2 testing results and symptom report among employees and residents.
+Key Results
+id="Par6"&gt;Eleven of the 16 SNFs had one or more resident or employee test positive.
+ Overall, 46 (2.9%) employees had positive or inconclusive testing for SARS-CoV-2, and among those who completed surveys, most were asymptomatic and involved in direct patient care.
+ The majority of employees tested were female (934, 73%), and most employees were Asian (392, 30%), Black (360, 28%), or white (360, 28%).
+ Among the 1208 residents tested, 110 (9.1%) had positive or inconclusive results.
+ There was no association between the presence of positive residents and positive employees within a SNF (p = 0.62, McNemar’s test).
+Conclusions
+id="Par7"&gt;In the largest study of SNFs to date, SARS-CoV-2 infections were detected among both employees and residents.
+ Employees testing positive were often asymptomatic and involved in direct patient care.
+ Surveillance testing is needed for SNF employees and residents during the pandemic response.
+Electronic supplementary material
+The online version of this article (10.1007/s11606-020-06165-7) contains supplementary material, which is available to authorized users.
+</t>
+  </si>
+  <si>
+    <t>[Ana A.%Weil%anaweil@uw.edu%1,  Kira L.%Newman%NULL%2,  Kira L.%Newman%NULL%0,  Thuan D.%Ong%NULL%1,  Giana H.%Davidson%NULL%1,  Jennifer%Logue%NULL%1,  Elisabeth%Brandstetter%NULL%1,  Ariana%Magedson%NULL%1,  Dylan%McDonald%NULL%1,  Denise J.%McCulloch%NULL%1,  Santiago%Neme%NULL%1,  James%Lewis%NULL%0,  Jeff S.%Duchin%NULL%1,  Weizhi%Zhong%NULL%1,  Lea M.%Starita%NULL%1,  Trevor%Bedford%NULL%1,  Alison C.%Roxby%NULL%1,  Helen Y.%Chu%helenchu@uw.edu%2]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Background
+Skilled nursing facilities (SNFs) are high-risk settings for SARS-CoV-2 transmission.
+ Infection rates among employees are infrequently described.
+Objective
+To describe SARS-CoV-2 rates among SNF employees and residents during a non-outbreak time period, we measured cross-sectional SARS-CoV-2 prevalence across multiple sites in the Seattle area.
+Design
+id="Par3"&gt;SARS-CoV-2 testing was performed for SNF employees and residents using quantitative real-time reverse transcription polymerase chain reaction.
+ A subset of employees completed a sociodemographic and symptom questionnaire.
+Participants
+id="Par4"&gt;Between March 29 and May 13, 2020, we tested 1583 employees and 1208 residents at 16 SNFs for SARS-CoV-2.
+Main Measure
+id="Par5"&gt;SARS-CoV-2 testing results and symptom report among employees and residents.
+Key Results
+id="Par6"&gt;Eleven of the 16 SNFs had one or more resident or employee test positive.
+ Overall, 46 (2.9%) employees had positive or inconclusive testing for SARS-CoV-2, and among those who completed surveys, most were asymptomatic and involved in direct patient care.
+ The majority of employees tested were female (934, 73%), and most employees were Asian (392, 30%), Black (360, 28%), or white (360, 28%).
+ Among the 1208 residents tested, 110 (9.1%) had positive or inconclusive results.
+ There was no association between the presence of positive residents and positive employees within a SNF (p = 0.62, McNemar’s test).
+Conclusions
+id="Par7"&gt;In the largest study of SNFs to date, SARS-CoV-2 infections were detected among both employees and residents.
+ Employees testing positive were often asymptomatic and involved in direct patient care.
+ Surveillance testing is needed for SNF employees and residents during the pandemic response.
+Electronic supplementary material
+The online version of this article (10.1007/s11606-020-06165-7) contains supplementary material, which is available to authorized users.
+</t>
+  </si>
+  <si>
+    <t>[Ana A.%Weil%anaweil@uw.edu%1,   Kira L.%Newman%NULL%4,   Kira L.%Newman%NULL%0,   Thuan D.%Ong%NULL%1,   Giana H.%Davidson%NULL%1,   Jennifer%Logue%NULL%1,   Elisabeth%Brandstetter%NULL%2,   Ariana%Magedson%NULL%1,   Dylan%McDonald%NULL%1,   Denise J.%McCulloch%NULL%1,   Santiago%Neme%NULL%4,   James%Lewis%NULL%1,   Jeff S.%Duchin%NULL%1,   Weizhi%Zhong%NULL%1,   Lea M.%Starita%NULL%2,   Trevor%Bedford%NULL%3,   Alison C.%Roxby%NULL%1,   Helen Y.%Chu%helenchu@uw.edu%2]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Background
+Skilled nursing facilities (SNFs) are high-risk settings for SARS-CoV-2 transmission.
+ Infection rates among employees are infrequently described.
+Objective
+To describe SARS-CoV-2 rates among SNF employees and residents during a non-outbreak time period, we measured cross-sectional SARS-CoV-2 prevalence across multiple sites in the Seattle area.
+Design
+SARS-CoV-2 testing was performed for SNF employees and residents using quantitative real-time reverse transcription polymerase chain reaction.
+ A subset of employees completed a sociodemographic and symptom questionnaire.
+Participants
+id="Par4"&gt;Between March 29 and May 13, 2020, we tested 1583 employees and 1208 residents at 16 SNFs for SARS-CoV-2.
+Main Measure
+id="Par5"&gt;SARS-CoV-2 testing results and symptom report among employees and residents.
+Key Results
+id="Par6"&gt;Eleven of the 16 SNFs had one or more resident or employee test positive.
+ Overall, 46 (2.9%) employees had positive or inconclusive testing for SARS-CoV-2, and among those who completed surveys, most were asymptomatic and involved in direct patient care.
+ The majority of employees tested were female (934, 73%), and most employees were Asian (392, 30%), Black (360, 28%), or white (360, 28%).
+ Among the 1208 residents tested, 110 (9.1%) had positive or inconclusive results.
+ There was no association between the presence of positive residents and positive employees within a SNF (p = 0.62, McNemar’s test).
+Conclusions
+id="Par7"&gt;In the largest study of SNFs to date, SARS-CoV-2 infections were detected among both employees and residents.
+ Employees testing positive were often asymptomatic and involved in direct patient care.
+ Surveillance testing is needed for SNF employees and residents during the pandemic response.
+Electronic supplementary material
+The online version of this article (10.1007/s11606-020-06165-7) contains supplementary material, which is available to authorized users.
+</t>
+  </si>
+  <si>
+    <t>[Ana A.%Weil%anaweil@uw.edu%1,    Kira L.%Newman%NULL%2,    Kira L.%Newman%NULL%0,    Thuan D.%Ong%NULL%1,    Giana H.%Davidson%NULL%1,    Jennifer%Logue%NULL%1,    Elisabeth%Brandstetter%NULL%1,    Ariana%Magedson%NULL%1,    Dylan%McDonald%NULL%1,    Denise J.%McCulloch%NULL%1,    Santiago%Neme%NULL%1,    James%Lewis%NULL%1,    Jeff S.%Duchin%NULL%1,    Weizhi%Zhong%NULL%1,    Lea M.%Starita%NULL%1,    Trevor%Bedford%NULL%1,    Alison C.%Roxby%NULL%1,    Helen Y.%Chu%helenchu@uw.edu%1]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Background
+Skilled nursing facilities (SNFs) are high-risk settings for SARS-CoV-2 transmission.
+ Infection rates among employees are infrequently described.
+Objective
+To describe SARS-CoV-2 rates among SNF employees and residents during a non-outbreak time period, we measured cross-sectional SARS-CoV-2 prevalence across multiple sites in the Seattle area.
+Design
+SARS-CoV-2 testing was performed for SNF employees and residents using quantitative real-time reverse transcription polymerase chain reaction.
+ A subset of employees completed a sociodemographic and symptom questionnaire.
+Participants
+Between March 29 and May 13, 2020, we tested 1583 employees and 1208 residents at 16 SNFs for SARS-CoV-2.
+Main Measure
+id="Par5"&gt;SARS-CoV-2 testing results and symptom report among employees and residents.
+Key Results
+id="Par6"&gt;Eleven of the 16 SNFs had one or more resident or employee test positive.
+ Overall, 46 (2.9%) employees had positive or inconclusive testing for SARS-CoV-2, and among those who completed surveys, most were asymptomatic and involved in direct patient care.
+ The majority of employees tested were female (934, 73%), and most employees were Asian (392, 30%), Black (360, 28%), or white (360, 28%).
+ Among the 1208 residents tested, 110 (9.1%) had positive or inconclusive results.
+ There was no association between the presence of positive residents and positive employees within a SNF (p = 0.62, McNemar’s test).
+Conclusions
+id="Par7"&gt;In the largest study of SNFs to date, SARS-CoV-2 infections were detected among both employees and residents.
+ Employees testing positive were often asymptomatic and involved in direct patient care.
+ Surveillance testing is needed for SNF employees and residents during the pandemic response.
+Electronic supplementary material
+The online version of this article (10.1007/s11606-020-06165-7) contains supplementary material, which is available to authorized users.
+</t>
+  </si>
+  <si>
+    <t>[Ana A.%Weil%anaweil@uw.edu%1,     Kira L.%Newman%NULL%2,     Kira L.%Newman%NULL%0,     Thuan D.%Ong%NULL%1,     Giana H.%Davidson%NULL%1,     Jennifer%Logue%NULL%1,     Elisabeth%Brandstetter%NULL%1,     Ariana%Magedson%NULL%1,     Dylan%McDonald%NULL%1,     Denise J.%McCulloch%NULL%1,     Santiago%Neme%NULL%2,     James%Lewis%NULL%1,     Jeff S.%Duchin%NULL%1,     Weizhi%Zhong%NULL%1,     Lea M.%Starita%NULL%1,     Trevor%Bedford%NULL%1,     Alison C.%Roxby%NULL%1,     Helen Y.%Chu%helenchu@uw.edu%1]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Background
+Skilled nursing facilities (SNFs) are high-risk settings for SARS-CoV-2 transmission.
+ Infection rates among employees are infrequently described.
+Objective
+To describe SARS-CoV-2 rates among SNF employees and residents during a non-outbreak time period, we measured cross-sectional SARS-CoV-2 prevalence across multiple sites in the Seattle area.
+Design
+SARS-CoV-2 testing was performed for SNF employees and residents using quantitative real-time reverse transcription polymerase chain reaction.
+ A subset of employees completed a sociodemographic and symptom questionnaire.
+Participants
+Between March 29 and May 13, 2020, we tested 1583 employees and 1208 residents at 16 SNFs for SARS-CoV-2.
+Main Measure
+SARS-CoV-2 testing results and symptom report among employees and residents.
+Key Results
+id="Par6"&gt;Eleven of the 16 SNFs had one or more resident or employee test positive.
+ Overall, 46 (2.9%) employees had positive or inconclusive testing for SARS-CoV-2, and among those who completed surveys, most were asymptomatic and involved in direct patient care.
+ The majority of employees tested were female (934, 73%), and most employees were Asian (392, 30%), Black (360, 28%), or white (360, 28%).
+ Among the 1208 residents tested, 110 (9.1%) had positive or inconclusive results.
+ There was no association between the presence of positive residents and positive employees within a SNF (p = 0.62, McNemar’s test).
+Conclusions
+id="Par7"&gt;In the largest study of SNFs to date, SARS-CoV-2 infections were detected among both employees and residents.
+ Employees testing positive were often asymptomatic and involved in direct patient care.
+ Surveillance testing is needed for SNF employees and residents during the pandemic response.
+Electronic supplementary material
+The online version of this article (10.1007/s11606-020-06165-7) contains supplementary material, which is available to authorized users.
+</t>
+  </si>
+  <si>
+    <t>[Ana A.%Weil%anaweil@uw.edu%1,      Kira L.%Newman%NULL%2,      Kira L.%Newman%NULL%0,      Thuan D.%Ong%NULL%1,      Giana H.%Davidson%NULL%1,      Jennifer%Logue%NULL%1,      Elisabeth%Brandstetter%NULL%1,      Ariana%Magedson%NULL%1,      Dylan%McDonald%NULL%1,      Denise J.%McCulloch%NULL%1,      Santiago%Neme%NULL%1,      James%Lewis%NULL%1,      Jeff S.%Duchin%NULL%1,      Weizhi%Zhong%NULL%1,      Lea M.%Starita%NULL%1,      Trevor%Bedford%NULL%1,      Alison C.%Roxby%NULL%1,      Helen Y.%Chu%helenchu@uw.edu%1]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Background
+Skilled nursing facilities (SNFs) are high-risk settings for SARS-CoV-2 transmission.
+ Infection rates among employees are infrequently described.
+Objective
+To describe SARS-CoV-2 rates among SNF employees and residents during a non-outbreak time period, we measured cross-sectional SARS-CoV-2 prevalence across multiple sites in the Seattle area.
+Design
+SARS-CoV-2 testing was performed for SNF employees and residents using quantitative real-time reverse transcription polymerase chain reaction.
+ A subset of employees completed a sociodemographic and symptom questionnaire.
+Participants
+Between March 29 and May 13, 2020, we tested 1583 employees and 1208 residents at 16 SNFs for SARS-CoV-2.
+Main Measure
+SARS-CoV-2 testing results and symptom report among employees and residents.
+Key Results
+Eleven of the 16 SNFs had one or more resident or employee test positive.
+ Overall, 46 (2.9%) employees had positive or inconclusive testing for SARS-CoV-2, and among those who completed surveys, most were asymptomatic and involved in direct patient care.
+ The majority of employees tested were female (934, 73%), and most employees were Asian (392, 30%), Black (360, 28%), or white (360, 28%).
+ Among the 1208 residents tested, 110 (9.1%) had positive or inconclusive results.
+ There was no association between the presence of positive residents and positive employees within a SNF (p = 0.62, McNemar’s test).
+Conclusions
+id="Par7"&gt;In the largest study of SNFs to date, SARS-CoV-2 infections were detected among both employees and residents.
+ Employees testing positive were often asymptomatic and involved in direct patient care.
+ Surveillance testing is needed for SNF employees and residents during the pandemic response.
+Electronic supplementary material
+The online version of this article (10.1007/s11606-020-06165-7) contains supplementary material, which is available to authorized users.
+</t>
+  </si>
+  <si>
+    <t>[Ana A.%Weil%anaweil@uw.edu%1,       Kira L.%Newman%NULL%2,       Kira L.%Newman%NULL%0,       Thuan D.%Ong%NULL%1,       Giana H.%Davidson%NULL%1,       Jennifer%Logue%NULL%1,       Elisabeth%Brandstetter%NULL%1,       Ariana%Magedson%NULL%1,       Dylan%McDonald%NULL%1,       Denise J.%McCulloch%NULL%1,       Santiago%Neme%NULL%1,       James%Lewis%NULL%1,       Jeff S.%Duchin%NULL%1,       Weizhi%Zhong%NULL%1,       Lea M.%Starita%NULL%1,       Trevor%Bedford%NULL%1,       Alison C.%Roxby%NULL%1,       Helen Y.%Chu%helenchu@uw.edu%0]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Background
+Skilled nursing facilities (SNFs) are high-risk settings for SARS-CoV-2 transmission.
+ Infection rates among employees are infrequently described.
+Objective
+To describe SARS-CoV-2 rates among SNF employees and residents during a non-outbreak time period, we measured cross-sectional SARS-CoV-2 prevalence across multiple sites in the Seattle area.
+Design
+SARS-CoV-2 testing was performed for SNF employees and residents using quantitative real-time reverse transcription polymerase chain reaction.
+ A subset of employees completed a sociodemographic and symptom questionnaire.
+Participants
+Between March 29 and May 13, 2020, we tested 1583 employees and 1208 residents at 16 SNFs for SARS-CoV-2.
+Main Measure
+SARS-CoV-2 testing results and symptom report among employees and residents.
+Key Results
+Eleven of the 16 SNFs had one or more resident or employee test positive.
+ Overall, 46 (2.9%) employees had positive or inconclusive testing for SARS-CoV-2, and among those who completed surveys, most were asymptomatic and involved in direct patient care.
+ The majority of employees tested were female (934, 73%), and most employees were Asian (392, 30%), Black (360, 28%), or white (360, 28%).
+ Among the 1208 residents tested, 110 (9.1%) had positive or inconclusive results.
+ There was no association between the presence of positive residents and positive employees within a SNF (p = 0.62, McNemar’s test).
+Conclusions
+In the largest study of SNFs to date, SARS-CoV-2 infections were detected among both employees and residents.
+ Employees testing positive were often asymptomatic and involved in direct patient care.
+ Surveillance testing is needed for SNF employees and residents during the pandemic response.
+Electronic supplementary material
+The online version of this article (10.1007/s11606-020-06165-7) contains supplementary material, which is available to authorized users.
+</t>
+  </si>
+  <si>
+    <t>[Ana A.%Weil%anaweil@uw.edu%1,        Kira L.%Newman%NULL%2,        Kira L.%Newman%NULL%0,        Thuan D.%Ong%NULL%1,        Giana H.%Davidson%NULL%1,        Jennifer%Logue%NULL%1,        Elisabeth%Brandstetter%NULL%1,        Ariana%Magedson%NULL%1,        Dylan%McDonald%NULL%1,        Denise J.%McCulloch%NULL%1,        Santiago%Neme%NULL%1,        James%Lewis%NULL%1,        Jeff S.%Duchin%NULL%1,        Weizhi%Zhong%NULL%1,        Lea M.%Starita%NULL%1,        Trevor%Bedford%NULL%1,        Alison C.%Roxby%NULL%1,        Helen Y.%Chu%helenchu@uw.edu%1]</t>
   </si>
 </sst>
 </file>
@@ -2304,10 +2514,10 @@
         <v>190</v>
       </c>
       <c r="D38" t="s">
-        <v>191</v>
+        <v>232</v>
       </c>
       <c r="E38" t="s">
-        <v>192</v>
+        <v>233</v>
       </c>
       <c r="F38" t="s">
         <v>193</v>

</xml_diff>

<commit_message>
Revert "Working on the ability to dump individual files, as well as fixing a major bug, on file 72"
This reverts commit 6dc3ea4dc8dc75539df8f49d3309a795f7c5e9bc.
</commit_message>
<xml_diff>
--- a/Covid_19_Dataset_and_References/References/10.xlsx
+++ b/Covid_19_Dataset_and_References/References/10.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="220">
   <si>
     <t>Doi</t>
   </si>
@@ -1024,216 +1024,6 @@
   </si>
   <si>
     <t>PMC7287415</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Background
-Skilled nursing facilities (SNFs) are high-risk settings for SARS-CoV-2 transmission.
- Infection rates among employees are infrequently described.
-Objective
-id="Par2"&gt;To describe SARS-CoV-2 rates among SNF employees and residents during a non-outbreak time period, we measured cross-sectional SARS-CoV-2 prevalence across multiple sites in the Seattle area.
-Design
-id="Par3"&gt;SARS-CoV-2 testing was performed for SNF employees and residents using quantitative real-time reverse transcription polymerase chain reaction.
- A subset of employees completed a sociodemographic and symptom questionnaire.
-Participants
-id="Par4"&gt;Between March 29 and May 13, 2020, we tested 1583 employees and 1208 residents at 16 SNFs for SARS-CoV-2.
-Main Measure
-id="Par5"&gt;SARS-CoV-2 testing results and symptom report among employees and residents.
-Key Results
-id="Par6"&gt;Eleven of the 16 SNFs had one or more resident or employee test positive.
- Overall, 46 (2.9%) employees had positive or inconclusive testing for SARS-CoV-2, and among those who completed surveys, most were asymptomatic and involved in direct patient care.
- The majority of employees tested were female (934, 73%), and most employees were Asian (392, 30%), Black (360, 28%), or white (360, 28%).
- Among the 1208 residents tested, 110 (9.1%) had positive or inconclusive results.
- There was no association between the presence of positive residents and positive employees within a SNF (p = 0.62, McNemar’s test).
-Conclusions
-id="Par7"&gt;In the largest study of SNFs to date, SARS-CoV-2 infections were detected among both employees and residents.
- Employees testing positive were often asymptomatic and involved in direct patient care.
- Surveillance testing is needed for SNF employees and residents during the pandemic response.
-Electronic supplementary material
-The online version of this article (10.1007/s11606-020-06165-7) contains supplementary material, which is available to authorized users.
-</t>
-  </si>
-  <si>
-    <t>[Ana A.%Weil%anaweil@uw.edu%1,  Kira L.%Newman%NULL%2,  Kira L.%Newman%NULL%0,  Thuan D.%Ong%NULL%1,  Giana H.%Davidson%NULL%1,  Jennifer%Logue%NULL%1,  Elisabeth%Brandstetter%NULL%1,  Ariana%Magedson%NULL%1,  Dylan%McDonald%NULL%1,  Denise J.%McCulloch%NULL%1,  Santiago%Neme%NULL%1,  James%Lewis%NULL%0,  Jeff S.%Duchin%NULL%1,  Weizhi%Zhong%NULL%1,  Lea M.%Starita%NULL%1,  Trevor%Bedford%NULL%1,  Alison C.%Roxby%NULL%1,  Helen Y.%Chu%helenchu@uw.edu%2]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Background
-Skilled nursing facilities (SNFs) are high-risk settings for SARS-CoV-2 transmission.
- Infection rates among employees are infrequently described.
-Objective
-To describe SARS-CoV-2 rates among SNF employees and residents during a non-outbreak time period, we measured cross-sectional SARS-CoV-2 prevalence across multiple sites in the Seattle area.
-Design
-id="Par3"&gt;SARS-CoV-2 testing was performed for SNF employees and residents using quantitative real-time reverse transcription polymerase chain reaction.
- A subset of employees completed a sociodemographic and symptom questionnaire.
-Participants
-id="Par4"&gt;Between March 29 and May 13, 2020, we tested 1583 employees and 1208 residents at 16 SNFs for SARS-CoV-2.
-Main Measure
-id="Par5"&gt;SARS-CoV-2 testing results and symptom report among employees and residents.
-Key Results
-id="Par6"&gt;Eleven of the 16 SNFs had one or more resident or employee test positive.
- Overall, 46 (2.9%) employees had positive or inconclusive testing for SARS-CoV-2, and among those who completed surveys, most were asymptomatic and involved in direct patient care.
- The majority of employees tested were female (934, 73%), and most employees were Asian (392, 30%), Black (360, 28%), or white (360, 28%).
- Among the 1208 residents tested, 110 (9.1%) had positive or inconclusive results.
- There was no association between the presence of positive residents and positive employees within a SNF (p = 0.62, McNemar’s test).
-Conclusions
-id="Par7"&gt;In the largest study of SNFs to date, SARS-CoV-2 infections were detected among both employees and residents.
- Employees testing positive were often asymptomatic and involved in direct patient care.
- Surveillance testing is needed for SNF employees and residents during the pandemic response.
-Electronic supplementary material
-The online version of this article (10.1007/s11606-020-06165-7) contains supplementary material, which is available to authorized users.
-</t>
-  </si>
-  <si>
-    <t>[Ana A.%Weil%anaweil@uw.edu%1,   Kira L.%Newman%NULL%4,   Kira L.%Newman%NULL%0,   Thuan D.%Ong%NULL%1,   Giana H.%Davidson%NULL%1,   Jennifer%Logue%NULL%1,   Elisabeth%Brandstetter%NULL%2,   Ariana%Magedson%NULL%1,   Dylan%McDonald%NULL%1,   Denise J.%McCulloch%NULL%1,   Santiago%Neme%NULL%4,   James%Lewis%NULL%1,   Jeff S.%Duchin%NULL%1,   Weizhi%Zhong%NULL%1,   Lea M.%Starita%NULL%2,   Trevor%Bedford%NULL%3,   Alison C.%Roxby%NULL%1,   Helen Y.%Chu%helenchu@uw.edu%2]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Background
-Skilled nursing facilities (SNFs) are high-risk settings for SARS-CoV-2 transmission.
- Infection rates among employees are infrequently described.
-Objective
-To describe SARS-CoV-2 rates among SNF employees and residents during a non-outbreak time period, we measured cross-sectional SARS-CoV-2 prevalence across multiple sites in the Seattle area.
-Design
-SARS-CoV-2 testing was performed for SNF employees and residents using quantitative real-time reverse transcription polymerase chain reaction.
- A subset of employees completed a sociodemographic and symptom questionnaire.
-Participants
-id="Par4"&gt;Between March 29 and May 13, 2020, we tested 1583 employees and 1208 residents at 16 SNFs for SARS-CoV-2.
-Main Measure
-id="Par5"&gt;SARS-CoV-2 testing results and symptom report among employees and residents.
-Key Results
-id="Par6"&gt;Eleven of the 16 SNFs had one or more resident or employee test positive.
- Overall, 46 (2.9%) employees had positive or inconclusive testing for SARS-CoV-2, and among those who completed surveys, most were asymptomatic and involved in direct patient care.
- The majority of employees tested were female (934, 73%), and most employees were Asian (392, 30%), Black (360, 28%), or white (360, 28%).
- Among the 1208 residents tested, 110 (9.1%) had positive or inconclusive results.
- There was no association between the presence of positive residents and positive employees within a SNF (p = 0.62, McNemar’s test).
-Conclusions
-id="Par7"&gt;In the largest study of SNFs to date, SARS-CoV-2 infections were detected among both employees and residents.
- Employees testing positive were often asymptomatic and involved in direct patient care.
- Surveillance testing is needed for SNF employees and residents during the pandemic response.
-Electronic supplementary material
-The online version of this article (10.1007/s11606-020-06165-7) contains supplementary material, which is available to authorized users.
-</t>
-  </si>
-  <si>
-    <t>[Ana A.%Weil%anaweil@uw.edu%1,    Kira L.%Newman%NULL%2,    Kira L.%Newman%NULL%0,    Thuan D.%Ong%NULL%1,    Giana H.%Davidson%NULL%1,    Jennifer%Logue%NULL%1,    Elisabeth%Brandstetter%NULL%1,    Ariana%Magedson%NULL%1,    Dylan%McDonald%NULL%1,    Denise J.%McCulloch%NULL%1,    Santiago%Neme%NULL%1,    James%Lewis%NULL%1,    Jeff S.%Duchin%NULL%1,    Weizhi%Zhong%NULL%1,    Lea M.%Starita%NULL%1,    Trevor%Bedford%NULL%1,    Alison C.%Roxby%NULL%1,    Helen Y.%Chu%helenchu@uw.edu%1]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Background
-Skilled nursing facilities (SNFs) are high-risk settings for SARS-CoV-2 transmission.
- Infection rates among employees are infrequently described.
-Objective
-To describe SARS-CoV-2 rates among SNF employees and residents during a non-outbreak time period, we measured cross-sectional SARS-CoV-2 prevalence across multiple sites in the Seattle area.
-Design
-SARS-CoV-2 testing was performed for SNF employees and residents using quantitative real-time reverse transcription polymerase chain reaction.
- A subset of employees completed a sociodemographic and symptom questionnaire.
-Participants
-Between March 29 and May 13, 2020, we tested 1583 employees and 1208 residents at 16 SNFs for SARS-CoV-2.
-Main Measure
-id="Par5"&gt;SARS-CoV-2 testing results and symptom report among employees and residents.
-Key Results
-id="Par6"&gt;Eleven of the 16 SNFs had one or more resident or employee test positive.
- Overall, 46 (2.9%) employees had positive or inconclusive testing for SARS-CoV-2, and among those who completed surveys, most were asymptomatic and involved in direct patient care.
- The majority of employees tested were female (934, 73%), and most employees were Asian (392, 30%), Black (360, 28%), or white (360, 28%).
- Among the 1208 residents tested, 110 (9.1%) had positive or inconclusive results.
- There was no association between the presence of positive residents and positive employees within a SNF (p = 0.62, McNemar’s test).
-Conclusions
-id="Par7"&gt;In the largest study of SNFs to date, SARS-CoV-2 infections were detected among both employees and residents.
- Employees testing positive were often asymptomatic and involved in direct patient care.
- Surveillance testing is needed for SNF employees and residents during the pandemic response.
-Electronic supplementary material
-The online version of this article (10.1007/s11606-020-06165-7) contains supplementary material, which is available to authorized users.
-</t>
-  </si>
-  <si>
-    <t>[Ana A.%Weil%anaweil@uw.edu%1,     Kira L.%Newman%NULL%2,     Kira L.%Newman%NULL%0,     Thuan D.%Ong%NULL%1,     Giana H.%Davidson%NULL%1,     Jennifer%Logue%NULL%1,     Elisabeth%Brandstetter%NULL%1,     Ariana%Magedson%NULL%1,     Dylan%McDonald%NULL%1,     Denise J.%McCulloch%NULL%1,     Santiago%Neme%NULL%2,     James%Lewis%NULL%1,     Jeff S.%Duchin%NULL%1,     Weizhi%Zhong%NULL%1,     Lea M.%Starita%NULL%1,     Trevor%Bedford%NULL%1,     Alison C.%Roxby%NULL%1,     Helen Y.%Chu%helenchu@uw.edu%1]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Background
-Skilled nursing facilities (SNFs) are high-risk settings for SARS-CoV-2 transmission.
- Infection rates among employees are infrequently described.
-Objective
-To describe SARS-CoV-2 rates among SNF employees and residents during a non-outbreak time period, we measured cross-sectional SARS-CoV-2 prevalence across multiple sites in the Seattle area.
-Design
-SARS-CoV-2 testing was performed for SNF employees and residents using quantitative real-time reverse transcription polymerase chain reaction.
- A subset of employees completed a sociodemographic and symptom questionnaire.
-Participants
-Between March 29 and May 13, 2020, we tested 1583 employees and 1208 residents at 16 SNFs for SARS-CoV-2.
-Main Measure
-SARS-CoV-2 testing results and symptom report among employees and residents.
-Key Results
-id="Par6"&gt;Eleven of the 16 SNFs had one or more resident or employee test positive.
- Overall, 46 (2.9%) employees had positive or inconclusive testing for SARS-CoV-2, and among those who completed surveys, most were asymptomatic and involved in direct patient care.
- The majority of employees tested were female (934, 73%), and most employees were Asian (392, 30%), Black (360, 28%), or white (360, 28%).
- Among the 1208 residents tested, 110 (9.1%) had positive or inconclusive results.
- There was no association between the presence of positive residents and positive employees within a SNF (p = 0.62, McNemar’s test).
-Conclusions
-id="Par7"&gt;In the largest study of SNFs to date, SARS-CoV-2 infections were detected among both employees and residents.
- Employees testing positive were often asymptomatic and involved in direct patient care.
- Surveillance testing is needed for SNF employees and residents during the pandemic response.
-Electronic supplementary material
-The online version of this article (10.1007/s11606-020-06165-7) contains supplementary material, which is available to authorized users.
-</t>
-  </si>
-  <si>
-    <t>[Ana A.%Weil%anaweil@uw.edu%1,      Kira L.%Newman%NULL%2,      Kira L.%Newman%NULL%0,      Thuan D.%Ong%NULL%1,      Giana H.%Davidson%NULL%1,      Jennifer%Logue%NULL%1,      Elisabeth%Brandstetter%NULL%1,      Ariana%Magedson%NULL%1,      Dylan%McDonald%NULL%1,      Denise J.%McCulloch%NULL%1,      Santiago%Neme%NULL%1,      James%Lewis%NULL%1,      Jeff S.%Duchin%NULL%1,      Weizhi%Zhong%NULL%1,      Lea M.%Starita%NULL%1,      Trevor%Bedford%NULL%1,      Alison C.%Roxby%NULL%1,      Helen Y.%Chu%helenchu@uw.edu%1]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Background
-Skilled nursing facilities (SNFs) are high-risk settings for SARS-CoV-2 transmission.
- Infection rates among employees are infrequently described.
-Objective
-To describe SARS-CoV-2 rates among SNF employees and residents during a non-outbreak time period, we measured cross-sectional SARS-CoV-2 prevalence across multiple sites in the Seattle area.
-Design
-SARS-CoV-2 testing was performed for SNF employees and residents using quantitative real-time reverse transcription polymerase chain reaction.
- A subset of employees completed a sociodemographic and symptom questionnaire.
-Participants
-Between March 29 and May 13, 2020, we tested 1583 employees and 1208 residents at 16 SNFs for SARS-CoV-2.
-Main Measure
-SARS-CoV-2 testing results and symptom report among employees and residents.
-Key Results
-Eleven of the 16 SNFs had one or more resident or employee test positive.
- Overall, 46 (2.9%) employees had positive or inconclusive testing for SARS-CoV-2, and among those who completed surveys, most were asymptomatic and involved in direct patient care.
- The majority of employees tested were female (934, 73%), and most employees were Asian (392, 30%), Black (360, 28%), or white (360, 28%).
- Among the 1208 residents tested, 110 (9.1%) had positive or inconclusive results.
- There was no association between the presence of positive residents and positive employees within a SNF (p = 0.62, McNemar’s test).
-Conclusions
-id="Par7"&gt;In the largest study of SNFs to date, SARS-CoV-2 infections were detected among both employees and residents.
- Employees testing positive were often asymptomatic and involved in direct patient care.
- Surveillance testing is needed for SNF employees and residents during the pandemic response.
-Electronic supplementary material
-The online version of this article (10.1007/s11606-020-06165-7) contains supplementary material, which is available to authorized users.
-</t>
-  </si>
-  <si>
-    <t>[Ana A.%Weil%anaweil@uw.edu%1,       Kira L.%Newman%NULL%2,       Kira L.%Newman%NULL%0,       Thuan D.%Ong%NULL%1,       Giana H.%Davidson%NULL%1,       Jennifer%Logue%NULL%1,       Elisabeth%Brandstetter%NULL%1,       Ariana%Magedson%NULL%1,       Dylan%McDonald%NULL%1,       Denise J.%McCulloch%NULL%1,       Santiago%Neme%NULL%1,       James%Lewis%NULL%1,       Jeff S.%Duchin%NULL%1,       Weizhi%Zhong%NULL%1,       Lea M.%Starita%NULL%1,       Trevor%Bedford%NULL%1,       Alison C.%Roxby%NULL%1,       Helen Y.%Chu%helenchu@uw.edu%0]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Background
-Skilled nursing facilities (SNFs) are high-risk settings for SARS-CoV-2 transmission.
- Infection rates among employees are infrequently described.
-Objective
-To describe SARS-CoV-2 rates among SNF employees and residents during a non-outbreak time period, we measured cross-sectional SARS-CoV-2 prevalence across multiple sites in the Seattle area.
-Design
-SARS-CoV-2 testing was performed for SNF employees and residents using quantitative real-time reverse transcription polymerase chain reaction.
- A subset of employees completed a sociodemographic and symptom questionnaire.
-Participants
-Between March 29 and May 13, 2020, we tested 1583 employees and 1208 residents at 16 SNFs for SARS-CoV-2.
-Main Measure
-SARS-CoV-2 testing results and symptom report among employees and residents.
-Key Results
-Eleven of the 16 SNFs had one or more resident or employee test positive.
- Overall, 46 (2.9%) employees had positive or inconclusive testing for SARS-CoV-2, and among those who completed surveys, most were asymptomatic and involved in direct patient care.
- The majority of employees tested were female (934, 73%), and most employees were Asian (392, 30%), Black (360, 28%), or white (360, 28%).
- Among the 1208 residents tested, 110 (9.1%) had positive or inconclusive results.
- There was no association between the presence of positive residents and positive employees within a SNF (p = 0.62, McNemar’s test).
-Conclusions
-In the largest study of SNFs to date, SARS-CoV-2 infections were detected among both employees and residents.
- Employees testing positive were often asymptomatic and involved in direct patient care.
- Surveillance testing is needed for SNF employees and residents during the pandemic response.
-Electronic supplementary material
-The online version of this article (10.1007/s11606-020-06165-7) contains supplementary material, which is available to authorized users.
-</t>
-  </si>
-  <si>
-    <t>[Ana A.%Weil%anaweil@uw.edu%1,        Kira L.%Newman%NULL%2,        Kira L.%Newman%NULL%0,        Thuan D.%Ong%NULL%1,        Giana H.%Davidson%NULL%1,        Jennifer%Logue%NULL%1,        Elisabeth%Brandstetter%NULL%1,        Ariana%Magedson%NULL%1,        Dylan%McDonald%NULL%1,        Denise J.%McCulloch%NULL%1,        Santiago%Neme%NULL%1,        James%Lewis%NULL%1,        Jeff S.%Duchin%NULL%1,        Weizhi%Zhong%NULL%1,        Lea M.%Starita%NULL%1,        Trevor%Bedford%NULL%1,        Alison C.%Roxby%NULL%1,        Helen Y.%Chu%helenchu@uw.edu%1]</t>
   </si>
 </sst>
 </file>
@@ -2514,10 +2304,10 @@
         <v>190</v>
       </c>
       <c r="D38" t="s">
-        <v>232</v>
+        <v>191</v>
       </c>
       <c r="E38" t="s">
-        <v>233</v>
+        <v>192</v>
       </c>
       <c r="F38" t="s">
         <v>193</v>

</xml_diff>

<commit_message>
Going through the dataset, updating
</commit_message>
<xml_diff>
--- a/Covid_19_Dataset_and_References/References/10.xlsx
+++ b/Covid_19_Dataset_and_References/References/10.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1036" uniqueCount="262">
   <si>
     <t>Doi</t>
   </si>
@@ -1024,6 +1024,132 @@
   </si>
   <si>
     <t>PMC7287415</t>
+  </si>
+  <si>
+    <t>Other found locations</t>
+  </si>
+  <si>
+    <t>[Daniel J%Escobar%Daniel.escobar@pennmedicine.upenn.edu%1,  Maria%Lanzi%NULL%1,  Pouné%Saberi%NULL%1,  Ruby%Love%NULL%1,  Darren R%Linkin%NULL%1,  John J%Kelly%NULL%1,  Darshana%Jhala%NULL%1,  Valerianna%Amorosa%NULL%1,  Mary%Hofmann%NULL%1,  Jeffrey B%Doyon%NULL%1]</t>
+  </si>
+  <si>
+    <t>_PMC</t>
+  </si>
+  <si>
+    <t>[James L.%Rudolph%NULL%1,  Christopher W.%Halladay%NULL%1,  Malisa%Barber%NULL%1,  Kevin W.%McConeghy%NULL%1,  Vince%Mor%NULL%1,  Aman%Nanda%NULL%1,  Stefan%Gravenstein%NULL%1]</t>
+  </si>
+  <si>
+    <t>_PMC_elsevier</t>
+  </si>
+  <si>
+    <t>[Paula%Eckardt%NULL%1,  Rachel%Guran%NULL%1,  Jon%Hennemyre%NULL%1,  Roshan%Arikupurathu%NULL%1,  Julie%Poveda%NULL%1,  Nancimae%Miller%NULL%1,  Randy%Katz%NULL%1,  Judith%Frum%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Carson%Telford%NULL%1,  Udodirim%Onwubiko%NULL%1,  David%Holland%NULL%1,  Kim%Turner%NULL%2,  Juliana%Prieto%NULL%2,  Sasha%Smith%NULL%2,  Jane%Yoon%NULL%1,  Wecheeta%Brown%NULL%1,  Allison%Chamberlain%NULL%1,  Neel%Gandhi%NULL%1,  Shamimul%Khan%NULL%1,  Steve%Williams%NULL%1,  Fazle%Khan%NULL%1,  Sarita%Shah%NULL%2,   C. T.%Telford%null%1,   U.% Onwubiko%null%1,   D.% Holland%null%1,   K.% Turner%null%1,   J.% Prieto%null%1,   S.% Smith%null%1,   J.% Yoon%null%1,   W.% Brown%null%1,   A.% Chamberlain%null%1,   N.% Gandhi%null%1,   S.% Khan%null%1,   S.% Williams%null%1,   F.% Khan%null%1,   S. % Shah%null%1,  C. T.%Telford%null%1,  U.% Onwubiko%null%1,  D.% Holland%null%1,  K.% Turner%null%1,  J.% Prieto%null%1,  S.% Smith%null%1,  J.% Yoon%null%1,  W.% Brown%null%1,  A.% Chamberlain%null%1,  N.% Gandhi%null%1,  S.% Khan%null%1,  S.% Williams%null%1,  F.% Khan%null%1,  S. % Shah%null%1]</t>
+  </si>
+  <si>
+    <t>medrxiv/biorxiv doi</t>
+  </si>
+  <si>
+    <t>[Sandra M.%Shi%NULL%1,  Innokentiy%Bakaev%NULL%1,  Helen%Chen%NULL%1,  Thomas G.%Travison%NULL%1,  Sarah D.%Berry%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Temet M.%McMichael%NULL%0,  Dustin W.%Currie%NULL%0,  Shauna%Clark%NULL%0,  Sargis%Pogosjans%NULL%0,  Meagan%Kay%NULL%0,  Noah G.%Schwartz%NULL%0,  James%Lewis%NULL%0,  Atar%Baer%NULL%0,  Vance%Kawakami%NULL%0,  Margaret D.%Lukoff%NULL%0,  Jessica%Ferro%NULL%0,  Claire%Brostrom-Smith%NULL%0,  Thomas D.%Rea%NULL%1,  Michael R.%Sayre%NULL%1,  Francis X.%Riedo%NULL%0,  Denny%Russell%NULL%0,  Brian%Hiatt%NULL%0,  Patricia%Montgomery%NULL%0,  Agam K.%Rao%NULL%0,  Eric J.%Chow%NULL%0,  Farrell%Tobolowsky%NULL%0,  Michael J.%Hughes%NULL%1,  Ana C.%Bardossy%NULL%0,  Lisa P.%Oakley%NULL%0,  Jesica R.%Jacobs%NULL%0,  Nimalie D.%Stone%NULL%1,  Sujan C.%Reddy%NULL%0,  John A.%Jernigan%NULL%0,  Margaret A.%Honein%NULL%0,  Thomas A.%Clark%NULL%0,  Jeffrey S.%Duchin%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Nathan M.%Stall%nathan.stall@sinaihealth.ca%1,  Carolyn%Farquharson%NULL%2,  Carolyn%Farquharson%NULL%0,  Chris%Fan‐Lun%NULL%1,  Lesley%Wiesenfeld%NULL%1,  Carla A.%Loftus%NULL%1,  Dylan%Kain%NULL%1,  Jennie%Johnstone%NULL%1,  Liz%McCreight%NULL%1,  Russell D.%Goldman%NULL%1,  Ramona%Mahtani%NULL%1]</t>
+  </si>
+  <si>
+    <t>[ Nathan M.%Stall%null%2,   Aaron%Jones%null%1,   Kevin A.%Brown%null%1,   Paula A.%Rochon%null%1,   Andrew P.%Costa%null%1,  Nathan M.%Stall%null%0,  Aaron%Jones%null%1,  Kevin A.%Brown%null%1,  Paula A.%Rochon%null%1,  Andrew P.%Costa%null%1]</t>
+  </si>
+  <si>
+    <t>[Hubert%Blain%NULL%1,  Yves%Rolland%NULL%1,  Edouard%Tuaillon%NULL%1,  Nadia%Giacosa%NULL%1,  Mylène%Albrand%NULL%1,  Audrey%Jaussent%NULL%1,  Athanase%Benetos%NULL%1,  Stéphanie%Miot%NULL%1,  Jean%Bousquet%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Guillaume%Sacco%NULL%1,  Gonzague%Foucault%NULL%1,  Olivier%Briere%NULL%1,  Cédric%Annweiler%NULL%1]</t>
+  </si>
+  <si>
+    <t>[R.%Guery%NULL%1,  C.%Delaye%NULL%1,  N.%Brule%NULL%1,  V.%Nael%NULL%1,  L.%Castain%NULL%1,  F.%Raffi%NULL%1,  L.%De Decker%NULL%1]</t>
+  </si>
+  <si>
+    <t>[A.%Klein%anke.klein@uke.de%1,  C.%Edler%NULL%1,  A.%Fitzek%NULL%1,  D.%Fröb%NULL%1,  A.%Heinemann%NULL%1,  K.%Meißner%NULL%1,  H.%Mushumba%NULL%1,  K.%Püschel%NULL%1,  A. S.%Schröder%NULL%1,  J. P.%Sperhake%NULL%1,  F.%Ishorst-Witte%NULL%1,  M.%Aepfelbacher%NULL%1,  F.%Heinrich%NULL%1]</t>
+  </si>
+  <si>
+    <t>_PMC_Springer</t>
+  </si>
+  <si>
+    <t>[Sean P%Kennelly%Sean.Kennelly@tuh.ie%1,  Adam H%Dyer%dyera@tcd.ie%1,  Claire%Noonan%claire.noonan@tuh.ie%2,  Claire%Noonan%claire.noonan@tuh.ie%0,  Ruth%Martin%ruth.martin1@hse.ie%1,  Siobhan M%Kennelly%siobhan.kennelly1@hse.ie%1,  Alan%Martin%alanmartin@beaumont.ie%1,  Desmond%O’Neill%NULL%1,  Aoife%Fallon%aoife.fallon1@hotmail.com%1]</t>
+  </si>
+  <si>
+    <t>[Antonio%Nouvenne%NULL%1,  Andrea%Ticinesi%NULL%1,  Alberto%Parise%NULL%1,  Beatrice%Prati%NULL%1,  Marcello%Esposito%NULL%1,  Valentina%Cocchi%NULL%1,  Emanuele%Crisafulli%NULL%1,  Annalisa%Volpi%NULL%1,  Sandra%Rossi%NULL%1,  Elena Giovanna%Bignami%NULL%1,  Marco%Baciarello%NULL%1,  Ettore%Brianti%NULL%1,  Massimo%Fabi%NULL%1,  Tiziana%Meschi%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Nicola%Veronese%NULL%1,  Luca Gino%Sbrogiò%NULL%1,  Roberto%Valle%NULL%1,  Laura%Marin%NULL%1,  Elena%Boscolo Fiore%NULL%1,  Andrea%Tiozzo%NULL%1]</t>
+  </si>
+  <si>
+    <t>[ J. H.%van den Besselaar%null%1,   R. S.% Sikkema%null%1,   F. M. H. P. A.% Koene%null%1,   L. W.% van Buul%null%1,   B. B.% Oude Munnink%null%1,   I.% Frenay%null%1,   R.% te Witt%null%1,   M. P. G.% Koopmans%null%1,   C. M. P. M.% Hertogh%null%1,   B. M. % Buurman%null%1]</t>
+  </si>
+  <si>
+    <t>_MedBiorxiv</t>
+  </si>
+  <si>
+    <t>[Laura W.%van Buul%NULL%1,  Judith H.%van den Besselaar%NULL%2,  Judith H.%van den Besselaar%NULL%0,  Fleur M. H. P. H.%Koene%NULL%1,  Bianca M.%Buurman%NULL%1,  Cees M. P. M.%Hertogh%NULL%1,  Martin%Smalbrugge%NULL%1,  Jeanine J. S.%Rutten%NULL%1,  Elke M.%den Boogert%NULL%1,  Michel D.%Wissing%NULL%1,  Ariene%Rietveld%NULL%1,  Mariska W. W.%van Elsakker%NULL%1,  Marga M. G.%Nonneman%NULL%1,  Florien%van Eeden%NULL%1,  Saskia%van de Merwe%NULL%1,  Sophie L.%Niemansburg%NULL%1,  Ewout%Fanoy%NULL%1,  Hinke S.%Bootsma%NULL%1,  Nicoline%van der Hagen%NULL%1,  Mariska%Petrignani%NULL%1,  Jessica Edwards%van Muijen%NULL%1,  Karolien E. M.%Biesheuvel%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Shin Young%Park%NULL%1,  Gawon%Choi%NULL%2,  Gawon%Choi%NULL%0,  Hyeyoung%Lee%NULL%2,  Hyeyoung%Lee%NULL%0,  Na-young%Kim%NULL%2,  Na-young%Kim%NULL%0,  Seon-young%Lee%NULL%2,  Seon-young%Lee%NULL%0,  Kyungnam%Kim%NULL%2,  Kyungnam%Kim%NULL%0,  Soyoung%Shin%NULL%2,  Soyoung%Shin%NULL%0,  Eunsu%Jang%NULL%2,  Eunsu%Jang%NULL%0,  YoungSin%Moon%NULL%2,  YoungSin%Moon%NULL%0,  KwangHwan%Oh%NULL%2,  KwangHwan%Oh%NULL%0,  JaeRin%Choi%NULL%2,  JaeRin%Choi%NULL%0,  Sangeun%Lee%NULL%2,  Sangeun%Lee%NULL%0,  Young-Man%Kim%NULL%2,  Young-Man%Kim%NULL%0,  Jieun%Kim%NULL%2,  Jieun%Kim%NULL%0,  Seonju%Yi%NULL%2,  Seonju%Yi%NULL%0,  Jin%Gwack%NULL%2,  Jin%Gwack%NULL%0,  Ok%Park%NULL%2,  Ok%Park%NULL%0,  Young Joon%Park%NULL%2,  Young Joon%Park%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Rok%Song%NULL%1,  Hee-Sook%Kim%NULL%2,  Hee-Sook%Kim%NULL%0,  Seok-Ju%Yoo%NULL%2,  Seok-Ju%Yoo%NULL%0,  Kwan%Lee%NULL%2,  Kwan%Lee%NULL%0,  Ji-Hyuk%Park%NULL%2,  Ji-Hyuk%Park%NULL%0,  Joon Ho%Jang%NULL%2,  Joon Ho%Jang%NULL%0,  Gyoung-Sook%Ahn%NULL%2,  Gyoung-Sook%Ahn%NULL%0,  Jun-Nyun%Kim%NULL%2,  Jun-Nyun%Kim%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Blanca%Borras-Bermejo%NULL%1,  Xavier%Martínez-Gómez%NULL%1,  María Gutierrez%San Miguel%NULL%1,  Juliana%Esperalba%NULL%1,  Andrés%Antón%NULL%1,  Elisabet%Martin%NULL%1,  Marta%Selvi%NULL%1,  María José%Abadías%NULL%1,  Antonio%Román%NULL%1,  Tomàs%Pumarola%NULL%1,  Magda%Campins%NULL%1,  Benito%Almirante%NULL%1]</t>
+  </si>
+  <si>
+    <t>[M.%Bernabeu-Wittel%NULL%1,  J.E.%Ternero-Vega%NULL%1,  P.%Díaz-Jiménez%NULL%1,  C.%Conde-Guzmán%NULL%1,  M.D.%Nieto-Martín%NULL%1,  L.%Moreno-Gaviño%NULL%1,  J.%Delgado-Cuesta%NULL%1,  M.%Rincón-Gómez%NULL%1,  L.%Giménez-Miranda%NULL%1,  M.D.%Navarro-Amuedo%NULL%1,  M.M.%Muñoz-García%NULL%1,  S.%Calzón-Fernández%NULL%1,  M.%Ollero-Baturone%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Shamez N%Ladhani%shamez.ladhani@phe.gov.uk%1,  J.Yimmy%Chow%NULL%1,  Roshni%Janarthanan%NULL%1,  Jonathan%Fok%NULL%1,  Emma%Crawley-Boevey%NULL%1,  Amoolya%Vusirikala%NULL%1,  Elena%Fernandez%NULL%1,  Marina Sanchez%Perez%NULL%1,  Suzanne%Tang%NULL%1,  Kate%Dun-Campbell%NULL%1,  Edward Wynne-%Evans%NULL%1,  Anita%Bell%NULL%1,  Bharat%Patel%NULL%1,  Zahin%Amin-Chowdhury%NULL%1,  Felicity%Aiano%NULL%1,  Karthik%Paranthaman%NULL%1,  Thomas%Ma%NULL%1,  Maria%Saavedra-Campos%NULL%1,  Richard%Myers%NULL%1,  Joanna%Ellis%NULL%2,  Angie%Lackenby%NULL%1,  Robin%Gopal%NULL%1,  Monika%Patel%NULL%1,  Colin%Brown%NULL%1,  Meera%Chand%NULL%1,  Kevin%Brown%NULL%1,  Mary E%Ramsay%NULL%1,  Susan%Hopkins%NULL%2,  Nandini%Shetty%NULL%1,  Maria%Zambon%NULL%2]</t>
+  </si>
+  <si>
+    <t>[N.S.N.%Graham%NULL%1,  C.%Junghans%NULL%1,  R.%Downes%NULL%1,  C.%Sendall%NULL%1,  H.%Lai%NULL%1,  A.%McKirdy%NULL%1,  P.%Elliott%NULL%1,  R.%Howard%NULL%1,  D.%Wingfield%NULL%1,  M.%Priestman%NULL%1,  M.%Ciechonska%NULL%1,  L.%Cameron%NULL%1,  M.%Storch%NULL%1,  M.A.%Crone%NULL%1,  P.S.%Freemont%NULL%1,  P.%Randell%NULL%1,  R.%McLaren%NULL%1,  N.%Lang%NULL%1,  S.%Ladhani%NULL%1,  F.%Sanderson%NULL%1,  D.J.%Sharp%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Agnes%Marossy%agnesmarossy@nhs.net%1,  Stefan%Rakowicz%NULL%1,  Angela%Bhan%NULL%1,  Sarah%Noon%NULL%1,  Amanda%Rees%NULL%1,  Manjinder%Virk%NULL%1,  Ayazali%Nazafi%NULL%1,  Evie%Hay%NULL%1,  Louise%de Thomasson%NULL%1,  Christina%Windle%NULL%1,  Mark%Zuckerman%Mark.Zuckerman@nhs.net%1]</t>
+  </si>
+  <si>
+    <t>[Laura%Shallcross%NULL%1,  Danielle%Burke%NULL%1,  Owen%Abbott%NULL%1,  Alasdair%Donaldson%NULL%1,  Gemma%Hallatt%NULL%1,  Andrew%Hayward%NULL%1,  Susan%Hopkins%NULL%0,  Maria%Krutikov%NULL%1,  Katie%Sharp%NULL%1,  Leone%Wardman%NULL%1,  Sapphira%Thorne%NULL%1]</t>
+  </si>
+  <si>
+    <t>[ E.%Smith%null%1,   C. F.% Aldus%null%1,   J.% Brainard%null%1,   S.% Dunham%null%1,   P. R.% Hunter%null%1,   N.% Steel%null%1,   P. % Everden%null%1]</t>
+  </si>
+  <si>
+    <t>[Mahesh C%Patel%mp3@uic.edu%1,  Lelia H%Chaisson%NULL%1,  Scott%Borgetti%NULL%1,  Deborah%Burdsall%NULL%1,  Rashmi K%Chugh%NULL%1,  Christopher R%Hoff%NULL%1,  Elizabeth B%Murphy%NULL%1,  Emily A%Murskyj%NULL%1,  Shannon%Wilson%NULL%1,  Joe%Ramos%NULL%1,  Lynn%Akker%NULL%1,  Debra%Bryars%NULL%1,  Evonda%Thomas-Smith%NULL%1,  Susan C%Bleasdale%NULL%1,  Ngozi O%Ezike%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Helena%Temkin‐Greener%helena_temkin-greener@urmc.rochester.edu%1,  Wenhan%Guo%NULL%2,  Wenhan%Guo%NULL%0,  Yunjiao%Mao%NULL%1,  Xueya%Cai%NULL%1,  Yue%Li%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Ana A.%Weil%anaweil@uw.edu%1,  Kira L.%Newman%NULL%4,  Kira L.%Newman%NULL%0,  Thuan D.%Ong%NULL%1,  Giana H.%Davidson%NULL%1,  Jennifer%Logue%NULL%1,  Elisabeth%Brandstetter%NULL%2,  Ariana%Magedson%NULL%1,  Dylan%McDonald%NULL%1,  Denise J.%McCulloch%NULL%1,  Santiago%Neme%NULL%1,  James%Lewis%NULL%0,  Jeff S.%Duchin%NULL%1,  Weizhi%Zhong%NULL%1,  Lea M.%Starita%NULL%2,  Trevor%Bedford%NULL%3,  Alison C.%Roxby%NULL%1,  Helen Y.%Chu%helenchu@uw.edu%3]</t>
+  </si>
+  <si>
+    <t>[Guillermo V.%Sanchez%NULL%1,  Caitlin%Biedron%NULL%1,  Lauren R.%Fink%NULL%1,  Kelly M.%Hatfield%NULL%1,  Jordan Micah F.%Polistico%NULL%1,  Monica P.%Meyer%NULL%1,  Rebecca S.%Noe%NULL%1,  Casey E.%Copen%NULL%1,  Amanda K.%Lyons%NULL%1,  Gonzalo%Gonzalez%NULL%1,  Keith%Kiama%NULL%1,  Mark%Lebednick%NULL%1,  Bonnie K.%Czander%NULL%1,  Amen%Agbonze%NULL%1,  Aimee R.%Surma%NULL%1,  Avnish%Sandhu%NULL%1,  Valerie H.%Mika%NULL%1,  Tyler%Prentiss%NULL%1,  John%Zervos%NULL%1,  Donia A.%Dalal%NULL%1,  Amber M.%Vasquez%NULL%1,  Sujan C.%Reddy%NULL%0,  John%Jernigan%NULL%1,  Paul E.%Kilgore%NULL%1,  Marcus J.%Zervos%NULL%1,  Teena%Chopra%NULL%1,  Carla P.%Bezold%NULL%1,  Najibah K.%Rehman%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Janice K%Louie%Janice.louie@sfdph.org%1,  Hyman M%Scott%NULL%1,  Amie%DuBois%NULL%1,  Natalya%Sturtz%NULL%1,  Wendy%Lu%NULL%1,  Juliet%Stoltey%NULL%2,  Godfred%Masinde%NULL%1,  Stephanie%Cohen%NULL%3,  Darpun%Sachdev%NULL%1,  Susan%Philip%NULL%1,  Naveena%Bobba%NULL%2,  Tomas%Aragon%NULL%1,  NULL%NULL%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Scott A%Goldberg%sagoldberg@bwh.harvard.edu%1,  Jochen%Lennerz%NULL%1,  Michael%Klompas%NULL%1,  Eden%Mark%NULL%1,  Virginia M%Pierce%NULL%1,  Ryan W%Thompson%NULL%1,  Charles T%Pu%NULL%1,  Lauren L%Ritterhouse%NULL%1,  Anand%Dighe%NULL%1,  Eric S%Rosenberg%NULL%1,  David C%Grabowski%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Amy V.%Dora%NULL%1,  Alexander%Winnett%NULL%3,  Lauren P.%Jatt%NULL%1,  Kusha%Davar%NULL%1,  Mika%Watanabe%NULL%1,  Linda%Sohn%NULL%1,  Hannah S.%Kern%NULL%1,  Christopher J.%Graber%NULL%3,  Matthew B.%Goetz%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Benjamin F.%Bigelow%NULL%1,  Olive%Tang%NULL%1,  Gregory R.%Toci%NULL%1,  Norberth%Stracker%NULL%1,  Fatima%Sheikh%NULL%1,  Kara M.%Jacobs Slifka%NULL%1,  Shannon A.%Novosad%NULL%1,  John A.%Jernigan%NULL%0,  Sujan C.%Reddy%NULL%0,  Morgan J.%Katz%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Matt%Feaster%NULL%1,  Ying-Ying%Goh%NULL%1]</t>
+  </si>
+  <si>
+    <t>[William R.%Mills%NULL%1,  Janet M.%Buccola%NULL%1,  Susan%Sender%NULL%1,  Joseph%Lichtefeld%NULL%1,  Nicholas%Romano%NULL%1,  Karen%Reynolds%NULL%1,  Melissa%Price%NULL%1,  Jennifer%Phipps%NULL%1,  Leigh%White%NULL%1,  Shauen%Howard%NULL%1]</t>
   </si>
 </sst>
 </file>
@@ -1356,6 +1482,9 @@
       <c r="H1" t="s">
         <v>58</v>
       </c>
+      <c r="I1" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
@@ -1371,7 +1500,7 @@
         <v>60</v>
       </c>
       <c r="E2" t="s">
-        <v>61</v>
+        <v>221</v>
       </c>
       <c r="F2" t="s">
         <v>62</v>
@@ -1381,6 +1510,9 @@
       </c>
       <c r="H2" t="s">
         <v>64</v>
+      </c>
+      <c r="I2" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="3">
@@ -1397,7 +1529,7 @@
         <v>66</v>
       </c>
       <c r="E3" t="s">
-        <v>67</v>
+        <v>223</v>
       </c>
       <c r="F3" t="s">
         <v>68</v>
@@ -1407,6 +1539,9 @@
       </c>
       <c r="H3" t="s">
         <v>64</v>
+      </c>
+      <c r="I3" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="4">
@@ -1423,7 +1558,7 @@
         <v>70</v>
       </c>
       <c r="E4" t="s">
-        <v>71</v>
+        <v>225</v>
       </c>
       <c r="F4" t="s">
         <v>72</v>
@@ -1433,6 +1568,9 @@
       </c>
       <c r="H4" t="s">
         <v>64</v>
+      </c>
+      <c r="I4" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="5">
@@ -1460,6 +1598,9 @@
       <c r="H5" t="s">
         <v>64</v>
       </c>
+      <c r="I5" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="5" t="s">
@@ -1475,16 +1616,19 @@
         <v>74</v>
       </c>
       <c r="E6" t="s">
-        <v>75</v>
+        <v>226</v>
       </c>
       <c r="F6" t="s">
         <v>6</v>
       </c>
       <c r="G6" t="s">
-        <v>76</v>
+        <v>227</v>
       </c>
       <c r="H6" t="s">
         <v>77</v>
+      </c>
+      <c r="I6" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="7">
@@ -1501,7 +1645,7 @@
         <v>79</v>
       </c>
       <c r="E7" t="s">
-        <v>80</v>
+        <v>228</v>
       </c>
       <c r="F7" t="s">
         <v>81</v>
@@ -1511,6 +1655,9 @@
       </c>
       <c r="H7" t="s">
         <v>64</v>
+      </c>
+      <c r="I7" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="8">
@@ -1527,7 +1674,7 @@
         <v>83</v>
       </c>
       <c r="E8" t="s">
-        <v>84</v>
+        <v>229</v>
       </c>
       <c r="F8" t="s">
         <v>85</v>
@@ -1537,6 +1684,9 @@
       </c>
       <c r="H8" t="s">
         <v>64</v>
+      </c>
+      <c r="I8" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="9">
@@ -1564,6 +1714,9 @@
       <c r="H9" t="s">
         <v>64</v>
       </c>
+      <c r="I9" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
@@ -1579,7 +1732,7 @@
         <v>87</v>
       </c>
       <c r="E10" t="s">
-        <v>88</v>
+        <v>230</v>
       </c>
       <c r="F10" t="s">
         <v>89</v>
@@ -1589,6 +1742,9 @@
       </c>
       <c r="H10" t="s">
         <v>90</v>
+      </c>
+      <c r="I10" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="11">
@@ -1605,7 +1761,7 @@
         <v>92</v>
       </c>
       <c r="E11" t="s">
-        <v>93</v>
+        <v>231</v>
       </c>
       <c r="F11" t="s">
         <v>94</v>
@@ -1615,6 +1771,9 @@
       </c>
       <c r="H11" t="s">
         <v>96</v>
+      </c>
+      <c r="I11" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="12">
@@ -1631,7 +1790,7 @@
         <v>98</v>
       </c>
       <c r="E12" t="s">
-        <v>99</v>
+        <v>232</v>
       </c>
       <c r="F12" t="s">
         <v>100</v>
@@ -1641,6 +1800,9 @@
       </c>
       <c r="H12" t="s">
         <v>64</v>
+      </c>
+      <c r="I12" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="13">
@@ -1668,6 +1830,9 @@
       <c r="H13" t="s">
         <v>64</v>
       </c>
+      <c r="I13" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="9" t="s">
@@ -1683,7 +1848,7 @@
         <v>102</v>
       </c>
       <c r="E14" t="s">
-        <v>103</v>
+        <v>233</v>
       </c>
       <c r="F14" t="s">
         <v>104</v>
@@ -1693,6 +1858,9 @@
       </c>
       <c r="H14" t="s">
         <v>105</v>
+      </c>
+      <c r="I14" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="15">
@@ -1709,7 +1877,7 @@
         <v>107</v>
       </c>
       <c r="E15" t="s">
-        <v>108</v>
+        <v>234</v>
       </c>
       <c r="F15" t="s">
         <v>109</v>
@@ -1719,6 +1887,9 @@
       </c>
       <c r="H15" t="s">
         <v>110</v>
+      </c>
+      <c r="I15" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="16">
@@ -1735,7 +1906,7 @@
         <v>112</v>
       </c>
       <c r="E16" t="s">
-        <v>113</v>
+        <v>235</v>
       </c>
       <c r="F16" t="s">
         <v>114</v>
@@ -1745,6 +1916,9 @@
       </c>
       <c r="H16" t="s">
         <v>64</v>
+      </c>
+      <c r="I16" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="17">
@@ -1772,6 +1946,9 @@
       <c r="H17" t="s">
         <v>64</v>
       </c>
+      <c r="I17" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
@@ -1798,6 +1975,9 @@
       <c r="H18" t="s">
         <v>64</v>
       </c>
+      <c r="I18" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
@@ -1824,6 +2004,9 @@
       <c r="H19" t="s">
         <v>64</v>
       </c>
+      <c r="I19" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
@@ -1839,7 +2022,7 @@
         <v>119</v>
       </c>
       <c r="E20" t="s">
-        <v>120</v>
+        <v>237</v>
       </c>
       <c r="F20" t="s">
         <v>121</v>
@@ -1849,6 +2032,9 @@
       </c>
       <c r="H20" t="s">
         <v>122</v>
+      </c>
+      <c r="I20" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="21">
@@ -1865,7 +2051,7 @@
         <v>124</v>
       </c>
       <c r="E21" t="s">
-        <v>125</v>
+        <v>238</v>
       </c>
       <c r="F21" t="s">
         <v>126</v>
@@ -1875,6 +2061,9 @@
       </c>
       <c r="H21" t="s">
         <v>64</v>
+      </c>
+      <c r="I21" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="22">
@@ -1891,7 +2080,7 @@
         <v>128</v>
       </c>
       <c r="E22" t="s">
-        <v>129</v>
+        <v>239</v>
       </c>
       <c r="F22" t="s">
         <v>130</v>
@@ -1901,6 +2090,9 @@
       </c>
       <c r="H22" t="s">
         <v>64</v>
+      </c>
+      <c r="I22" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="23">
@@ -1928,6 +2120,9 @@
       <c r="H23" t="s">
         <v>64</v>
       </c>
+      <c r="I23" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
@@ -1943,16 +2138,19 @@
         <v>132</v>
       </c>
       <c r="E24" t="s">
-        <v>133</v>
+        <v>240</v>
       </c>
       <c r="F24" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="G24" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="H24" t="s">
         <v>134</v>
+      </c>
+      <c r="I24" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="25">
@@ -1969,7 +2167,7 @@
         <v>136</v>
       </c>
       <c r="E25" t="s">
-        <v>137</v>
+        <v>242</v>
       </c>
       <c r="F25" t="s">
         <v>138</v>
@@ -1979,6 +2177,9 @@
       </c>
       <c r="H25" t="s">
         <v>139</v>
+      </c>
+      <c r="I25" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="26">
@@ -2006,6 +2207,9 @@
       <c r="H26" t="s">
         <v>64</v>
       </c>
+      <c r="I26" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
@@ -2021,7 +2225,7 @@
         <v>141</v>
       </c>
       <c r="E27" t="s">
-        <v>142</v>
+        <v>243</v>
       </c>
       <c r="F27" t="s">
         <v>143</v>
@@ -2031,6 +2235,9 @@
       </c>
       <c r="H27" t="s">
         <v>144</v>
+      </c>
+      <c r="I27" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="28">
@@ -2047,7 +2254,7 @@
         <v>146</v>
       </c>
       <c r="E28" t="s">
-        <v>147</v>
+        <v>244</v>
       </c>
       <c r="F28" t="s">
         <v>148</v>
@@ -2057,6 +2264,9 @@
       </c>
       <c r="H28" t="s">
         <v>149</v>
+      </c>
+      <c r="I28" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="29">
@@ -2073,7 +2283,7 @@
         <v>151</v>
       </c>
       <c r="E29" t="s">
-        <v>152</v>
+        <v>245</v>
       </c>
       <c r="F29" t="s">
         <v>153</v>
@@ -2083,6 +2293,9 @@
       </c>
       <c r="H29" t="s">
         <v>64</v>
+      </c>
+      <c r="I29" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="30">
@@ -2099,7 +2312,7 @@
         <v>107</v>
       </c>
       <c r="E30" t="s">
-        <v>155</v>
+        <v>246</v>
       </c>
       <c r="F30" t="s">
         <v>156</v>
@@ -2109,6 +2322,9 @@
       </c>
       <c r="H30" t="s">
         <v>157</v>
+      </c>
+      <c r="I30" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="31">
@@ -2125,7 +2341,7 @@
         <v>159</v>
       </c>
       <c r="E31" t="s">
-        <v>160</v>
+        <v>247</v>
       </c>
       <c r="F31" t="s">
         <v>161</v>
@@ -2135,6 +2351,9 @@
       </c>
       <c r="H31" t="s">
         <v>162</v>
+      </c>
+      <c r="I31" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="32">
@@ -2151,7 +2370,7 @@
         <v>164</v>
       </c>
       <c r="E32" t="s">
-        <v>165</v>
+        <v>248</v>
       </c>
       <c r="F32" t="s">
         <v>166</v>
@@ -2161,6 +2380,9 @@
       </c>
       <c r="H32" t="s">
         <v>167</v>
+      </c>
+      <c r="I32" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="33">
@@ -2177,7 +2399,7 @@
         <v>169</v>
       </c>
       <c r="E33" t="s">
-        <v>170</v>
+        <v>249</v>
       </c>
       <c r="F33" t="s">
         <v>171</v>
@@ -2187,6 +2409,9 @@
       </c>
       <c r="H33" t="s">
         <v>64</v>
+      </c>
+      <c r="I33" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="34">
@@ -2203,7 +2428,7 @@
         <v>173</v>
       </c>
       <c r="E34" t="s">
-        <v>174</v>
+        <v>250</v>
       </c>
       <c r="F34" t="s">
         <v>175</v>
@@ -2213,6 +2438,9 @@
       </c>
       <c r="H34" t="s">
         <v>64</v>
+      </c>
+      <c r="I34" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="35">
@@ -2229,16 +2457,19 @@
         <v>177</v>
       </c>
       <c r="E35" t="s">
-        <v>178</v>
+        <v>251</v>
       </c>
       <c r="F35" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="G35" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="H35" t="s">
         <v>179</v>
+      </c>
+      <c r="I35" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="36">
@@ -2255,7 +2486,7 @@
         <v>181</v>
       </c>
       <c r="E36" t="s">
-        <v>182</v>
+        <v>252</v>
       </c>
       <c r="F36" t="s">
         <v>183</v>
@@ -2265,6 +2496,9 @@
       </c>
       <c r="H36" t="s">
         <v>184</v>
+      </c>
+      <c r="I36" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="37">
@@ -2281,7 +2515,7 @@
         <v>186</v>
       </c>
       <c r="E37" t="s">
-        <v>187</v>
+        <v>253</v>
       </c>
       <c r="F37" t="s">
         <v>188</v>
@@ -2291,6 +2525,9 @@
       </c>
       <c r="H37" t="s">
         <v>189</v>
+      </c>
+      <c r="I37" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="38">
@@ -2307,7 +2544,7 @@
         <v>191</v>
       </c>
       <c r="E38" t="s">
-        <v>192</v>
+        <v>254</v>
       </c>
       <c r="F38" t="s">
         <v>193</v>
@@ -2317,6 +2554,9 @@
       </c>
       <c r="H38" t="s">
         <v>194</v>
+      </c>
+      <c r="I38" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="39">
@@ -2333,7 +2573,7 @@
         <v>107</v>
       </c>
       <c r="E39" t="s">
-        <v>196</v>
+        <v>255</v>
       </c>
       <c r="F39" t="s">
         <v>197</v>
@@ -2343,6 +2583,9 @@
       </c>
       <c r="H39" t="s">
         <v>64</v>
+      </c>
+      <c r="I39" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="40">
@@ -2359,7 +2602,7 @@
         <v>199</v>
       </c>
       <c r="E40" t="s">
-        <v>200</v>
+        <v>256</v>
       </c>
       <c r="F40" t="s">
         <v>201</v>
@@ -2369,6 +2612,9 @@
       </c>
       <c r="H40" t="s">
         <v>64</v>
+      </c>
+      <c r="I40" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="41">
@@ -2385,7 +2631,7 @@
         <v>203</v>
       </c>
       <c r="E41" t="s">
-        <v>204</v>
+        <v>257</v>
       </c>
       <c r="F41" t="s">
         <v>205</v>
@@ -2395,6 +2641,9 @@
       </c>
       <c r="H41" t="s">
         <v>64</v>
+      </c>
+      <c r="I41" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="42">
@@ -2411,7 +2660,7 @@
         <v>107</v>
       </c>
       <c r="E42" t="s">
-        <v>207</v>
+        <v>258</v>
       </c>
       <c r="F42" t="s">
         <v>208</v>
@@ -2421,6 +2670,9 @@
       </c>
       <c r="H42" t="s">
         <v>64</v>
+      </c>
+      <c r="I42" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="43">
@@ -2437,7 +2689,7 @@
         <v>107</v>
       </c>
       <c r="E43" t="s">
-        <v>210</v>
+        <v>259</v>
       </c>
       <c r="F43" t="s">
         <v>211</v>
@@ -2447,6 +2699,9 @@
       </c>
       <c r="H43" t="s">
         <v>64</v>
+      </c>
+      <c r="I43" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="44">
@@ -2463,7 +2718,7 @@
         <v>213</v>
       </c>
       <c r="E44" t="s">
-        <v>214</v>
+        <v>260</v>
       </c>
       <c r="F44" t="s">
         <v>215</v>
@@ -2473,6 +2728,9 @@
       </c>
       <c r="H44" t="s">
         <v>64</v>
+      </c>
+      <c r="I44" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="45">
@@ -2489,7 +2747,7 @@
         <v>217</v>
       </c>
       <c r="E45" t="s">
-        <v>218</v>
+        <v>261</v>
       </c>
       <c r="F45" t="s">
         <v>219</v>
@@ -2499,6 +2757,9 @@
       </c>
       <c r="H45" t="s">
         <v>64</v>
+      </c>
+      <c r="I45" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="46">
@@ -2526,6 +2787,9 @@
       <c r="H46" t="s">
         <v>64</v>
       </c>
+      <c r="I46" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="2" t="s">
@@ -2551,6 +2815,9 @@
       </c>
       <c r="H47" t="s">
         <v>64</v>
+      </c>
+      <c r="I47" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added and updated with crossref
</commit_message>
<xml_diff>
--- a/Covid_19_Dataset_and_References/References/10.xlsx
+++ b/Covid_19_Dataset_and_References/References/10.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2352" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3010" uniqueCount="510">
   <si>
     <t>Doi</t>
   </si>
@@ -1638,6 +1638,279 @@
   </si>
   <si>
     <t>[William R.%Mills%NULL%1,      Janet M.%Buccola%NULL%1,      Susan%Sender%NULL%1,      Joseph%Lichtefeld%NULL%1,      Nicholas%Romano%NULL%1,      Karen%Reynolds%NULL%1,      Melissa%Price%NULL%1,      Jennifer%Phipps%NULL%1,      Leigh%White%NULL%1,      Shauen%Howard%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Daniel J%Escobar%Daniel.escobar@pennmedicine.upenn.edu%1,       Maria%Lanzi%NULL%1,       Pouné%Saberi%NULL%1,       Ruby%Love%NULL%1,       Darren R%Linkin%NULL%1,       John J%Kelly%NULL%1,       Darshana%Jhala%NULL%1,       Valerianna%Amorosa%NULL%1,       Mary%Hofmann%NULL%1,       Jeffrey B%Doyon%NULL%1]</t>
+  </si>
+  <si>
+    <t>[James L.%Rudolph%NULL%1,       Christopher W.%Halladay%NULL%1,       Malisa%Barber%NULL%1,       Kevin W.%McConeghy%NULL%1,       Vince%Mor%NULL%1,       Aman%Nanda%NULL%1,       Stefan%Gravenstein%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Paula%Eckardt%NULL%1,       Rachel%Guran%NULL%1,       Jon%Hennemyre%NULL%1,       Roshan%Arikupurathu%NULL%1,       Julie%Poveda%NULL%1,       Nancimae%Miller%NULL%1,       Randy%Katz%NULL%1,       Judith%Frum%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Carson%Telford%NULL%1,       Udodirim%Onwubiko%NULL%1,       David%Holland%NULL%1,       Kim%Turner%NULL%1,       Juliana%Prieto%NULL%1,       Sasha%Smith%NULL%1,       Jane%Yoon%NULL%1,       Wecheeta%Brown%NULL%1,       Allison%Chamberlain%NULL%1,       Neel%Gandhi%NULL%1,       Shamimul%Khan%NULL%1,       Steve%Williams%NULL%1,       Fazle%Khan%NULL%1,       Sarita%Shah%NULL%1,        C. T.%Telford%null%1,        U.% Onwubiko%null%1,        D.% Holland%null%1,        K.% Turner%null%1,        J.% Prieto%null%1,        S.% Smith%null%1,        J.% Yoon%null%1,        W.% Brown%null%1,        A.% Chamberlain%null%1,        N.% Gandhi%null%1,        S.% Khan%null%1,        S.% Williams%null%1,        F.% Khan%null%1,        S. % Shah%null%1,       C. T.%Telford%null%1,       U.% Onwubiko%null%1,       D.% Holland%null%1,       K.% Turner%null%1,       J.% Prieto%null%1,       S.% Smith%null%1,       J.% Yoon%null%1,       W.% Brown%null%1,       A.% Chamberlain%null%1,       N.% Gandhi%null%1,       S.% Khan%null%1,       S.% Williams%null%1,       F.% Khan%null%1,       S. % Shah%null%1]</t>
+  </si>
+  <si>
+    <t>[Sandra M.%Shi%NULL%1,       Innokentiy%Bakaev%NULL%1,       Helen%Chen%NULL%1,       Thomas G.%Travison%NULL%1,       Sarah D.%Berry%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Temet M.%McMichael%NULL%0,       Dustin W.%Currie%NULL%0,       Shauna%Clark%NULL%0,       Sargis%Pogosjans%NULL%0,       Meagan%Kay%NULL%0,       Noah G.%Schwartz%NULL%0,       James%Lewis%NULL%0,       Atar%Baer%NULL%0,       Vance%Kawakami%NULL%0,       Margaret D.%Lukoff%NULL%0,       Jessica%Ferro%NULL%0,       Claire%Brostrom-Smith%NULL%0,       Thomas D.%Rea%NULL%1,       Michael R.%Sayre%NULL%1,       Francis X.%Riedo%NULL%0,       Denny%Russell%NULL%0,       Brian%Hiatt%NULL%0,       Patricia%Montgomery%NULL%0,       Agam K.%Rao%NULL%0,       Eric J.%Chow%NULL%0,       Farrell%Tobolowsky%NULL%0,       Michael J.%Hughes%NULL%1,       Ana C.%Bardossy%NULL%0,       Lisa P.%Oakley%NULL%0,       Jesica R.%Jacobs%NULL%0,       Nimalie D.%Stone%NULL%1,       Sujan C.%Reddy%NULL%0,       John A.%Jernigan%NULL%0,       Margaret A.%Honein%NULL%0,       Thomas A.%Clark%NULL%0,       Jeffrey S.%Duchin%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Nathan M.%Stall%nathan.stall@sinaihealth.ca%1,       Carolyn%Farquharson%NULL%2,       Carolyn%Farquharson%NULL%0,       Chris%Fan‐Lun%NULL%1,       Lesley%Wiesenfeld%NULL%1,       Carla A.%Loftus%NULL%1,       Dylan%Kain%NULL%1,       Jennie%Johnstone%NULL%1,       Liz%McCreight%NULL%1,       Russell D.%Goldman%NULL%1,       Ramona%Mahtani%NULL%1]</t>
+  </si>
+  <si>
+    <t>[ Nathan M.%Stall%null%1,        Aaron%Jones%null%1,        Kevin A.%Brown%null%1,        Paula A.%Rochon%null%1,        Andrew P.%Costa%null%1,       Nathan M.%Stall%null%1,       Aaron%Jones%null%1,       Kevin A.%Brown%null%1,       Paula A.%Rochon%null%1,       Andrew P.%Costa%null%1]</t>
+  </si>
+  <si>
+    <t>[Hubert%Blain%NULL%1,       Yves%Rolland%NULL%1,       Edouard%Tuaillon%NULL%1,       Nadia%Giacosa%NULL%1,       Mylène%Albrand%NULL%1,       Audrey%Jaussent%NULL%1,       Athanase%Benetos%NULL%1,       Stéphanie%Miot%NULL%1,       Jean%Bousquet%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Guillaume%Sacco%NULL%1,       Gonzague%Foucault%NULL%1,       Olivier%Briere%NULL%1,       Cédric%Annweiler%NULL%1]</t>
+  </si>
+  <si>
+    <t>[R.%Guery%NULL%1,       C.%Delaye%NULL%1,       N.%Brule%NULL%1,       V.%Nael%NULL%1,       L.%Castain%NULL%1,       F.%Raffi%NULL%1,       L.%De Decker%NULL%1]</t>
+  </si>
+  <si>
+    <t>[A.%Klein%anke.klein@uke.de%1,       C.%Edler%NULL%1,       A.%Fitzek%NULL%1,       D.%Fröb%NULL%1,       A.%Heinemann%NULL%1,       K.%Meißner%NULL%1,       H.%Mushumba%NULL%1,       K.%Püschel%NULL%1,       A. S.%Schröder%NULL%1,       J. P.%Sperhake%NULL%1,       F.%Ishorst-Witte%NULL%1,       M.%Aepfelbacher%NULL%1,       F.%Heinrich%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Buntinx%Frank%coreGivesNoEmail%1,     Claes%Peter%coreGivesNoEmail%1,     Gulikers%Marjo%coreGivesNoEmail%1,     Jan%De Lepeleire%coreGivesNoEmail%1,     Van%der Elst Michael%coreGivesNoEmail%1,     Van%Elslande Jan%coreGivesNoEmail%1,     Van%Ranst Marc%coreGivesNoEmail%1,     Verbakel%Jan%coreGivesNoEmail%1,     Vernneersch%Pieter%coreGivesNoEmail%1]</t>
+  </si>
+  <si>
+    <t>"Clinical and Epidemiological Features of 34 Nursing Home Elderly with Coronavirus Disease 2019 (COVID-19) in Wuhan, China: An Observational Cohort Study"</t>
+  </si>
+  <si>
+    <t>[Liangcong%Hu%xref no email%2, Wanyuan%Zhen%xref no email%1, Xudong%Xie%xref no email%2, Ze%Lin%xref no email%2, Tiantian%Wang%xref no email%1, Jing%Liu%xref no email%0, Hang%Xue%xref no email%2, Adriana C.%Panayi%xref no email%2, Ke%Xu%xref no email%1, Zexi%Ling%xref no email%1, Xugui%Li%xref no email%1, Bobin%Mi%xref no email%2, Wu%Zhou%xref no email%2, Guohui%Liu%xref no email%2]</t>
+  </si>
+  <si>
+    <t>CROSSREF</t>
+  </si>
+  <si>
+    <t>2022-03-31</t>
+  </si>
+  <si>
+    <t>[Sean P%Kennelly%Sean.Kennelly@tuh.ie%1,       Adam H%Dyer%dyera@tcd.ie%1,       Claire%Noonan%claire.noonan@tuh.ie%2,       Claire%Noonan%claire.noonan@tuh.ie%0,       Ruth%Martin%ruth.martin1@hse.ie%1,       Siobhan M%Kennelly%siobhan.kennelly1@hse.ie%1,       Alan%Martin%alanmartin@beaumont.ie%1,       Desmond%O’Neill%NULL%1,       Aoife%Fallon%aoife.fallon1@hotmail.com%1]</t>
+  </si>
+  <si>
+    <t>[Antonio%Nouvenne%NULL%1,       Andrea%Ticinesi%NULL%1,       Alberto%Parise%NULL%1,       Beatrice%Prati%NULL%1,       Marcello%Esposito%NULL%1,       Valentina%Cocchi%NULL%1,       Emanuele%Crisafulli%NULL%1,       Annalisa%Volpi%NULL%1,       Sandra%Rossi%NULL%1,       Elena Giovanna%Bignami%NULL%1,       Marco%Baciarello%NULL%1,       Ettore%Brianti%NULL%1,       Massimo%Fabi%NULL%1,       Tiziana%Meschi%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Nicola%Veronese%NULL%1,       Luca Gino%Sbrogiò%NULL%1,       Roberto%Valle%NULL%1,       Laura%Marin%NULL%1,       Elena%Boscolo Fiore%NULL%1,       Andrea%Tiozzo%NULL%1]</t>
+  </si>
+  <si>
+    <t>[ J. H.%van den Besselaar%null%1,        R. S.% Sikkema%null%1,        F. M. H. P. A.% Koene%null%1,        L. W.% van Buul%null%1,        B. B.% Oude Munnink%null%1,        I.% Frenay%null%1,        R.% te Witt%null%1,        M. P. G.% Koopmans%null%1,        C. M. P. M.% Hertogh%null%1,        B. M. % Buurman%null%1]</t>
+  </si>
+  <si>
+    <t>[Laura W.%van Buul%NULL%1,       Judith H.%van den Besselaar%NULL%2,       Judith H.%van den Besselaar%NULL%0,       Fleur M. H. P. H.%Koene%NULL%1,       Bianca M.%Buurman%NULL%1,       Cees M. P. M.%Hertogh%NULL%1,       Martin%Smalbrugge%NULL%1,       Jeanine J. S.%Rutten%NULL%1,       Elke M.%den Boogert%NULL%1,       Michel D.%Wissing%NULL%1,       Ariene%Rietveld%NULL%1,       Mariska W. W.%van Elsakker%NULL%1,       Marga M. G.%Nonneman%NULL%1,       Florien%van Eeden%NULL%1,       Saskia%van de Merwe%NULL%1,       Sophie L.%Niemansburg%NULL%1,       Ewout%Fanoy%NULL%1,       Hinke S.%Bootsma%NULL%1,       Nicoline%van der Hagen%NULL%1,       Mariska%Petrignani%NULL%1,       Jessica Edwards%van Muijen%NULL%1,       Karolien E. M.%Biesheuvel%NULL%1]</t>
+  </si>
+  <si>
+    <t>[B\u00e5rd%Reiakvam Kittang%coreGivesNoEmail%1,     Karina%Koller L\u00f8land%coreGivesNoEmail%1,     Kjell%Kr\u00fcger%coreGivesNoEmail%1,     Kristian%Jansen%coreGivesNoEmail%1,     Sabine%Piepenstock Solheim%coreGivesNoEmail%1,     Sebastian%von Hofacker%coreGivesNoEmail%1]</t>
+  </si>
+  <si>
+    <t>[Shin Young%Park%NULL%1,       Gawon%Choi%NULL%2,       Gawon%Choi%NULL%0,       Hyeyoung%Lee%NULL%2,       Hyeyoung%Lee%NULL%0,       Na-young%Kim%NULL%2,       Na-young%Kim%NULL%0,       Seon-young%Lee%NULL%2,       Seon-young%Lee%NULL%0,       Kyungnam%Kim%NULL%2,       Kyungnam%Kim%NULL%0,       Soyoung%Shin%NULL%2,       Soyoung%Shin%NULL%0,       Eunsu%Jang%NULL%2,       Eunsu%Jang%NULL%0,       YoungSin%Moon%NULL%2,       YoungSin%Moon%NULL%0,       KwangHwan%Oh%NULL%2,       KwangHwan%Oh%NULL%0,       JaeRin%Choi%NULL%2,       JaeRin%Choi%NULL%0,       Sangeun%Lee%NULL%2,       Sangeun%Lee%NULL%0,       Young-Man%Kim%NULL%2,       Young-Man%Kim%NULL%0,       Jieun%Kim%NULL%2,       Jieun%Kim%NULL%0,       Seonju%Yi%NULL%2,       Seonju%Yi%NULL%0,       Jin%Gwack%NULL%2,       Jin%Gwack%NULL%0,       Ok%Park%NULL%2,       Ok%Park%NULL%0,       Young Joon%Park%NULL%2,       Young Joon%Park%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Rok%Song%NULL%1,       Hee-Sook%Kim%NULL%2,       Hee-Sook%Kim%NULL%0,       Seok-Ju%Yoo%NULL%2,       Seok-Ju%Yoo%NULL%0,       Kwan%Lee%NULL%2,       Kwan%Lee%NULL%0,       Ji-Hyuk%Park%NULL%2,       Ji-Hyuk%Park%NULL%0,       Joon Ho%Jang%NULL%2,       Joon Ho%Jang%NULL%0,       Gyoung-Sook%Ahn%NULL%2,       Gyoung-Sook%Ahn%NULL%0,       Jun-Nyun%Kim%NULL%2,       Jun-Nyun%Kim%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Blanca%Borras-Bermejo%NULL%1,       Xavier%Martínez-Gómez%NULL%1,       María Gutierrez%San Miguel%NULL%1,       Juliana%Esperalba%NULL%1,       Andrés%Antón%NULL%1,       Elisabet%Martin%NULL%1,       Marta%Selvi%NULL%1,       María José%Abadías%NULL%1,       Antonio%Román%NULL%1,       Tomàs%Pumarola%NULL%1,       Magda%Campins%NULL%1,       Benito%Almirante%NULL%1]</t>
+  </si>
+  <si>
+    <t>[M.%Bernabeu-Wittel%NULL%1,       J.E.%Ternero-Vega%NULL%1,       P.%Díaz-Jiménez%NULL%1,       C.%Conde-Guzmán%NULL%1,       M.D.%Nieto-Martín%NULL%1,       L.%Moreno-Gaviño%NULL%1,       J.%Delgado-Cuesta%NULL%1,       M.%Rincón-Gómez%NULL%1,       L.%Giménez-Miranda%NULL%1,       M.D.%Navarro-Amuedo%NULL%1,       M.M.%Muñoz-García%NULL%1,       S.%Calzón-Fernández%NULL%1,       M.%Ollero-Baturone%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Shamez N%Ladhani%shamez.ladhani@phe.gov.uk%1,       J.Yimmy%Chow%NULL%1,       Roshni%Janarthanan%NULL%1,       Jonathan%Fok%NULL%1,       Emma%Crawley-Boevey%NULL%1,       Amoolya%Vusirikala%NULL%1,       Elena%Fernandez%NULL%1,       Marina Sanchez%Perez%NULL%1,       Suzanne%Tang%NULL%1,       Kate%Dun-Campbell%NULL%1,       Edward Wynne-%Evans%NULL%1,       Anita%Bell%NULL%1,       Bharat%Patel%NULL%1,       Zahin%Amin-Chowdhury%NULL%1,       Felicity%Aiano%NULL%1,       Karthik%Paranthaman%NULL%1,       Thomas%Ma%NULL%1,       Maria%Saavedra-Campos%NULL%1,       Richard%Myers%NULL%1,       Joanna%Ellis%NULL%2,       Angie%Lackenby%NULL%1,       Robin%Gopal%NULL%1,       Monika%Patel%NULL%1,       Colin%Brown%NULL%1,       Meera%Chand%NULL%1,       Kevin%Brown%NULL%1,       Mary E%Ramsay%NULL%1,       Susan%Hopkins%NULL%2,       Nandini%Shetty%NULL%1,       Maria%Zambon%NULL%2]</t>
+  </si>
+  <si>
+    <t>[N.S.N.%Graham%NULL%1,       C.%Junghans%NULL%1,       R.%Downes%NULL%1,       C.%Sendall%NULL%1,       H.%Lai%NULL%1,       A.%McKirdy%NULL%1,       P.%Elliott%NULL%1,       R.%Howard%NULL%1,       D.%Wingfield%NULL%1,       M.%Priestman%NULL%1,       M.%Ciechonska%NULL%1,       L.%Cameron%NULL%1,       M.%Storch%NULL%1,       M.A.%Crone%NULL%1,       P.S.%Freemont%NULL%1,       P.%Randell%NULL%1,       R.%McLaren%NULL%1,       N.%Lang%NULL%1,       S.%Ladhani%NULL%1,       F.%Sanderson%NULL%1,       D.J.%Sharp%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Agnes%Marossy%agnesmarossy@nhs.net%1,       Stefan%Rakowicz%NULL%1,       Angela%Bhan%NULL%1,       Sarah%Noon%NULL%1,       Amanda%Rees%NULL%1,       Manjinder%Virk%NULL%1,       Ayazali%Nazafi%NULL%1,       Evie%Hay%NULL%1,       Louise%de Thomasson%NULL%1,       Christina%Windle%NULL%1,       Mark%Zuckerman%Mark.Zuckerman@nhs.net%1]</t>
+  </si>
+  <si>
+    <t>[Laura%Shallcross%NULL%1,       Danielle%Burke%NULL%1,       Owen%Abbott%NULL%1,       Alasdair%Donaldson%NULL%1,       Gemma%Hallatt%NULL%1,       Andrew%Hayward%NULL%1,       Susan%Hopkins%NULL%0,       Maria%Krutikov%NULL%1,       Katie%Sharp%NULL%1,       Leone%Wardman%NULL%1,       Sapphira%Thorne%NULL%1]</t>
+  </si>
+  <si>
+    <t>[ E.%Smith%null%1,        C. F.% Aldus%null%1,        J.% Brainard%null%1,        S.% Dunham%null%1,        P. R.% Hunter%null%1,        N.% Steel%null%1,        P. % Everden%null%1]</t>
+  </si>
+  <si>
+    <t>[Mahesh C%Patel%mp3@uic.edu%1,       Lelia H%Chaisson%NULL%1,       Scott%Borgetti%NULL%1,       Deborah%Burdsall%NULL%1,       Rashmi K%Chugh%NULL%1,       Christopher R%Hoff%NULL%1,       Elizabeth B%Murphy%NULL%1,       Emily A%Murskyj%NULL%1,       Shannon%Wilson%NULL%1,       Joe%Ramos%NULL%1,       Lynn%Akker%NULL%1,       Debra%Bryars%NULL%1,       Evonda%Thomas-Smith%NULL%1,       Susan C%Bleasdale%NULL%1,       Ngozi O%Ezike%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Helena%Temkin‐Greener%helena_temkin-greener@urmc.rochester.edu%1,       Wenhan%Guo%NULL%2,       Wenhan%Guo%NULL%0,       Yunjiao%Mao%NULL%1,       Xueya%Cai%NULL%1,       Yue%Li%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Ana A.%Weil%anaweil@uw.edu%1,       Kira L.%Newman%NULL%2,       Kira L.%Newman%NULL%0,       Thuan D.%Ong%NULL%1,       Giana H.%Davidson%NULL%1,       Jennifer%Logue%NULL%1,       Elisabeth%Brandstetter%NULL%1,       Ariana%Magedson%NULL%1,       Dylan%McDonald%NULL%1,       Denise J.%McCulloch%NULL%1,       Santiago%Neme%NULL%1,       James%Lewis%NULL%0,       Jeff S.%Duchin%NULL%1,       Weizhi%Zhong%NULL%1,       Lea M.%Starita%NULL%1,       Trevor%Bedford%NULL%1,       Alison C.%Roxby%NULL%1,       Helen Y.%Chu%helenchu@uw.edu%2]</t>
+  </si>
+  <si>
+    <t>[Guillermo V.%Sanchez%NULL%1,       Caitlin%Biedron%NULL%1,       Lauren R.%Fink%NULL%1,       Kelly M.%Hatfield%NULL%1,       Jordan Micah F.%Polistico%NULL%1,       Monica P.%Meyer%NULL%1,       Rebecca S.%Noe%NULL%1,       Casey E.%Copen%NULL%1,       Amanda K.%Lyons%NULL%1,       Gonzalo%Gonzalez%NULL%1,       Keith%Kiama%NULL%1,       Mark%Lebednick%NULL%1,       Bonnie K.%Czander%NULL%1,       Amen%Agbonze%NULL%1,       Aimee R.%Surma%NULL%1,       Avnish%Sandhu%NULL%1,       Valerie H.%Mika%NULL%1,       Tyler%Prentiss%NULL%1,       John%Zervos%NULL%1,       Donia A.%Dalal%NULL%1,       Amber M.%Vasquez%NULL%1,       Sujan C.%Reddy%NULL%0,       John%Jernigan%NULL%1,       Paul E.%Kilgore%NULL%1,       Marcus J.%Zervos%NULL%1,       Teena%Chopra%NULL%1,       Carla P.%Bezold%NULL%1,       Najibah K.%Rehman%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Janice K%Louie%Janice.louie@sfdph.org%1,       Hyman M%Scott%NULL%1,       Amie%DuBois%NULL%1,       Natalya%Sturtz%NULL%1,       Wendy%Lu%NULL%1,       Juliet%Stoltey%NULL%1,       Godfred%Masinde%NULL%1,       Stephanie%Cohen%NULL%1,       Darpun%Sachdev%NULL%1,       Susan%Philip%NULL%1,       Naveena%Bobba%NULL%1,       Tomas%Aragon%NULL%1,       NULL%NULL%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Scott A%Goldberg%sagoldberg@bwh.harvard.edu%1,       Jochen%Lennerz%NULL%1,       Michael%Klompas%NULL%1,       Eden%Mark%NULL%1,       Virginia M%Pierce%NULL%1,       Ryan W%Thompson%NULL%1,       Charles T%Pu%NULL%1,       Lauren L%Ritterhouse%NULL%1,       Anand%Dighe%NULL%1,       Eric S%Rosenberg%NULL%1,       David C%Grabowski%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Amy V.%Dora%NULL%1,       Alexander%Winnett%NULL%1,       Lauren P.%Jatt%NULL%1,       Kusha%Davar%NULL%1,       Mika%Watanabe%NULL%1,       Linda%Sohn%NULL%1,       Hannah S.%Kern%NULL%1,       Christopher J.%Graber%NULL%1,       Matthew B.%Goetz%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Benjamin F.%Bigelow%NULL%1,       Olive%Tang%NULL%1,       Gregory R.%Toci%NULL%1,       Norberth%Stracker%NULL%1,       Fatima%Sheikh%NULL%1,       Kara M.%Jacobs Slifka%NULL%1,       Shannon A.%Novosad%NULL%1,       John A.%Jernigan%NULL%0,       Sujan C.%Reddy%NULL%0,       Morgan J.%Katz%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Matt%Feaster%NULL%1,       Ying-Ying%Goh%NULL%1]</t>
+  </si>
+  <si>
+    <t>[William R.%Mills%NULL%1,       Janet M.%Buccola%NULL%1,       Susan%Sender%NULL%1,       Joseph%Lichtefeld%NULL%1,       Nicholas%Romano%NULL%1,       Karen%Reynolds%NULL%1,       Melissa%Price%NULL%1,       Jennifer%Phipps%NULL%1,       Leigh%White%NULL%1,       Shauen%Howard%NULL%1]</t>
+  </si>
+  <si>
+    <t>"Rapid Telehealth-Centered Response to COVID-19 Outbreaks in Postacute and Long-Term Care Facilities"</t>
+  </si>
+  <si>
+    <t>[Drew A.%Harris%xref no email%1, Laurie%Archbald-Pannone%xref no email%1, Jasveen%Kaur%xref no email%1, David%Cattell-Gordon%xref no email%1, Karen S.%Rheuban%xref no email%1, Rachel L.%Ombres%xref no email%1, Kimberly%Albero%xref no email%1, Rebecca%Steele%xref no email%1, Taison D.%Bell%xref no email%1, Justin B.%Mutter%xref no email%1]</t>
+  </si>
+  <si>
+    <t>2023-05-17</t>
+  </si>
+  <si>
+    <t>"Responding to a COVID-19 Outbreak at a Long-Term Care Facility"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">" This article describes an outbreak of COVID-19 in a long-term care facility (LTCF) in West Virginia that was the epicenter of the state\u2019s pandemic.
+ Beginning with the index case, we describe the sequential order of procedures undertaken by the facility including testing, infection control, treatment, and communication with facility residents, staff, and family members.
+ We also describe the lessons learned during the process and provide recommendations for handling an outbreak at other LTCFs.
+ </t>
+  </si>
+  <si>
+    <t>[Carl D.%Shrader%xref no email%1, Shauna%Assadzandi%xref no email%1, Courtney S.%Pilkerton%xref no email%1, Amie M.%Ashcraft%xref no email%1]</t>
+  </si>
+  <si>
+    <t>2023-03-03</t>
+  </si>
+  <si>
+    <t>[Daniel J%Escobar%Daniel.escobar@pennmedicine.upenn.edu%1,        Maria%Lanzi%NULL%1,        Pouné%Saberi%NULL%1,        Ruby%Love%NULL%1,        Darren R%Linkin%NULL%1,        John J%Kelly%NULL%1,        Darshana%Jhala%NULL%1,        Valerianna%Amorosa%NULL%1,        Mary%Hofmann%NULL%1,        Jeffrey B%Doyon%NULL%1]</t>
+  </si>
+  <si>
+    <t>[James L.%Rudolph%NULL%1,        Christopher W.%Halladay%NULL%1,        Malisa%Barber%NULL%1,        Kevin W.%McConeghy%NULL%1,        Vince%Mor%NULL%1,        Aman%Nanda%NULL%1,        Stefan%Gravenstein%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Paula%Eckardt%NULL%1,        Rachel%Guran%NULL%1,        Jon%Hennemyre%NULL%1,        Roshan%Arikupurathu%NULL%1,        Julie%Poveda%NULL%1,        Nancimae%Miller%NULL%1,        Randy%Katz%NULL%1,        Judith%Frum%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Carson%Telford%NULL%1,        Udodirim%Onwubiko%NULL%1,        David%Holland%NULL%1,        Kim%Turner%NULL%1,        Juliana%Prieto%NULL%1,        Sasha%Smith%NULL%1,        Jane%Yoon%NULL%1,        Wecheeta%Brown%NULL%1,        Allison%Chamberlain%NULL%1,        Neel%Gandhi%NULL%1,        Shamimul%Khan%NULL%1,        Steve%Williams%NULL%1,        Fazle%Khan%NULL%1,        Sarita%Shah%NULL%1,         C. T.%Telford%null%1,         U.% Onwubiko%null%1,         D.% Holland%null%1,         K.% Turner%null%1,         J.% Prieto%null%1,         S.% Smith%null%1,         J.% Yoon%null%1,         W.% Brown%null%1,         A.% Chamberlain%null%1,         N.% Gandhi%null%1,         S.% Khan%null%1,         S.% Williams%null%1,         F.% Khan%null%1,         S. % Shah%null%1,        C. T.%Telford%null%1,        U.% Onwubiko%null%1,        D.% Holland%null%1,        K.% Turner%null%1,        J.% Prieto%null%1,        S.% Smith%null%1,        J.% Yoon%null%1,        W.% Brown%null%1,        A.% Chamberlain%null%1,        N.% Gandhi%null%1,        S.% Khan%null%1,        S.% Williams%null%1,        F.% Khan%null%1,        S. % Shah%null%1]</t>
+  </si>
+  <si>
+    <t>[Sandra M.%Shi%NULL%1,        Innokentiy%Bakaev%NULL%1,        Helen%Chen%NULL%1,        Thomas G.%Travison%NULL%1,        Sarah D.%Berry%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Temet M.%McMichael%NULL%0,        Dustin W.%Currie%NULL%0,        Shauna%Clark%NULL%0,        Sargis%Pogosjans%NULL%0,        Meagan%Kay%NULL%0,        Noah G.%Schwartz%NULL%0,        James%Lewis%NULL%0,        Atar%Baer%NULL%0,        Vance%Kawakami%NULL%0,        Margaret D.%Lukoff%NULL%0,        Jessica%Ferro%NULL%0,        Claire%Brostrom-Smith%NULL%0,        Thomas D.%Rea%NULL%1,        Michael R.%Sayre%NULL%1,        Francis X.%Riedo%NULL%0,        Denny%Russell%NULL%0,        Brian%Hiatt%NULL%0,        Patricia%Montgomery%NULL%0,        Agam K.%Rao%NULL%0,        Eric J.%Chow%NULL%0,        Farrell%Tobolowsky%NULL%0,        Michael J.%Hughes%NULL%1,        Ana C.%Bardossy%NULL%0,        Lisa P.%Oakley%NULL%0,        Jesica R.%Jacobs%NULL%0,        Nimalie D.%Stone%NULL%1,        Sujan C.%Reddy%NULL%0,        John A.%Jernigan%NULL%0,        Margaret A.%Honein%NULL%0,        Thomas A.%Clark%NULL%0,        Jeffrey S.%Duchin%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Nathan M.%Stall%nathan.stall@sinaihealth.ca%1,        Carolyn%Farquharson%NULL%2,        Carolyn%Farquharson%NULL%0,        Chris%Fan‐Lun%NULL%1,        Lesley%Wiesenfeld%NULL%1,        Carla A.%Loftus%NULL%1,        Dylan%Kain%NULL%1,        Jennie%Johnstone%NULL%1,        Liz%McCreight%NULL%1,        Russell D.%Goldman%NULL%1,        Ramona%Mahtani%NULL%1]</t>
+  </si>
+  <si>
+    <t>[ Nathan M.%Stall%null%1,         Aaron%Jones%null%1,         Kevin A.%Brown%null%1,         Paula A.%Rochon%null%1,         Andrew P.%Costa%null%1,        Nathan M.%Stall%null%1,        Aaron%Jones%null%1,        Kevin A.%Brown%null%1,        Paula A.%Rochon%null%1,        Andrew P.%Costa%null%1]</t>
+  </si>
+  <si>
+    <t>[Hubert%Blain%NULL%1,        Yves%Rolland%NULL%1,        Edouard%Tuaillon%NULL%1,        Nadia%Giacosa%NULL%1,        Mylène%Albrand%NULL%1,        Audrey%Jaussent%NULL%1,        Athanase%Benetos%NULL%1,        Stéphanie%Miot%NULL%1,        Jean%Bousquet%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Guillaume%Sacco%NULL%1,        Gonzague%Foucault%NULL%1,        Olivier%Briere%NULL%1,        Cédric%Annweiler%NULL%1]</t>
+  </si>
+  <si>
+    <t>[R.%Guery%NULL%1,        C.%Delaye%NULL%1,        N.%Brule%NULL%1,        V.%Nael%NULL%1,        L.%Castain%NULL%1,        F.%Raffi%NULL%1,        L.%De Decker%NULL%1]</t>
+  </si>
+  <si>
+    <t>[A.%Klein%anke.klein@uke.de%1,        C.%Edler%NULL%1,        A.%Fitzek%NULL%1,        D.%Fröb%NULL%1,        A.%Heinemann%NULL%1,        K.%Meißner%NULL%1,        H.%Mushumba%NULL%1,        K.%Püschel%NULL%1,        A. S.%Schröder%NULL%1,        J. P.%Sperhake%NULL%1,        F.%Ishorst-Witte%NULL%1,        M.%Aepfelbacher%NULL%1,        F.%Heinrich%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Buntinx%Frank%coreGivesNoEmail%1,      Claes%Peter%coreGivesNoEmail%1,      Gulikers%Marjo%coreGivesNoEmail%1,      Jan%De Lepeleire%coreGivesNoEmail%1,      Van%der Elst Michael%coreGivesNoEmail%1,      Van%Elslande Jan%coreGivesNoEmail%1,      Van%Ranst Marc%coreGivesNoEmail%1,      Verbakel%Jan%coreGivesNoEmail%1,      Vernneersch%Pieter%coreGivesNoEmail%1]</t>
+  </si>
+  <si>
+    <t>[Liangcong%Hu%xref no email%1,  Wanyuan%Zhen%xref no email%1,  Xudong%Xie%xref no email%2,  Ze%Lin%xref no email%2,  Tiantian%Wang%xref no email%1,  Jing%Liu%xref no email%5,  Hang%Xue%xref no email%2,  Adriana C.%Panayi%xref no email%2,  Ke%Xu%xref no email%1,  Zexi%Ling%xref no email%1,  Xugui%Li%xref no email%1,  Bobin%Mi%xref no email%1,  Wu%Zhou%xref no email%2,  Guohui%Liu%xref no email%2]</t>
+  </si>
+  <si>
+    <t>[Sean P%Kennelly%Sean.Kennelly@tuh.ie%1,        Adam H%Dyer%dyera@tcd.ie%1,        Claire%Noonan%claire.noonan@tuh.ie%2,        Claire%Noonan%claire.noonan@tuh.ie%0,        Ruth%Martin%ruth.martin1@hse.ie%1,        Siobhan M%Kennelly%siobhan.kennelly1@hse.ie%1,        Alan%Martin%alanmartin@beaumont.ie%1,        Desmond%O’Neill%NULL%1,        Aoife%Fallon%aoife.fallon1@hotmail.com%1]</t>
+  </si>
+  <si>
+    <t>[Antonio%Nouvenne%NULL%1,        Andrea%Ticinesi%NULL%1,        Alberto%Parise%NULL%1,        Beatrice%Prati%NULL%1,        Marcello%Esposito%NULL%1,        Valentina%Cocchi%NULL%1,        Emanuele%Crisafulli%NULL%1,        Annalisa%Volpi%NULL%1,        Sandra%Rossi%NULL%1,        Elena Giovanna%Bignami%NULL%1,        Marco%Baciarello%NULL%1,        Ettore%Brianti%NULL%1,        Massimo%Fabi%NULL%1,        Tiziana%Meschi%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Nicola%Veronese%NULL%1,        Luca Gino%Sbrogiò%NULL%1,        Roberto%Valle%NULL%1,        Laura%Marin%NULL%1,        Elena%Boscolo Fiore%NULL%1,        Andrea%Tiozzo%NULL%1]</t>
+  </si>
+  <si>
+    <t>[ J. H.%van den Besselaar%null%1,         R. S.% Sikkema%null%1,         F. M. H. P. A.% Koene%null%1,         L. W.% van Buul%null%1,         B. B.% Oude Munnink%null%1,         I.% Frenay%null%1,         R.% te Witt%null%1,         M. P. G.% Koopmans%null%1,         C. M. P. M.% Hertogh%null%1,         B. M. % Buurman%null%1]</t>
+  </si>
+  <si>
+    <t>[Laura W.%van Buul%NULL%1,        Judith H.%van den Besselaar%NULL%2,        Judith H.%van den Besselaar%NULL%0,        Fleur M. H. P. H.%Koene%NULL%1,        Bianca M.%Buurman%NULL%1,        Cees M. P. M.%Hertogh%NULL%1,        Martin%Smalbrugge%NULL%1,        Jeanine J. S.%Rutten%NULL%1,        Elke M.%den Boogert%NULL%1,        Michel D.%Wissing%NULL%1,        Ariene%Rietveld%NULL%1,        Mariska W. W.%van Elsakker%NULL%1,        Marga M. G.%Nonneman%NULL%1,        Florien%van Eeden%NULL%1,        Saskia%van de Merwe%NULL%1,        Sophie L.%Niemansburg%NULL%1,        Ewout%Fanoy%NULL%1,        Hinke S.%Bootsma%NULL%1,        Nicoline%van der Hagen%NULL%1,        Mariska%Petrignani%NULL%1,        Jessica Edwards%van Muijen%NULL%1,        Karolien E. M.%Biesheuvel%NULL%1]</t>
+  </si>
+  <si>
+    <t>[B\u00e5rd%Reiakvam Kittang%coreGivesNoEmail%1,      Karina%Koller L\u00f8land%coreGivesNoEmail%1,      Kjell%Kr\u00fcger%coreGivesNoEmail%1,      Kristian%Jansen%coreGivesNoEmail%1,      Sabine%Piepenstock Solheim%coreGivesNoEmail%1,      Sebastian%von Hofacker%coreGivesNoEmail%1]</t>
+  </si>
+  <si>
+    <t>[Shin Young%Park%NULL%1,        Gawon%Choi%NULL%2,        Gawon%Choi%NULL%0,        Hyeyoung%Lee%NULL%2,        Hyeyoung%Lee%NULL%0,        Na-young%Kim%NULL%2,        Na-young%Kim%NULL%0,        Seon-young%Lee%NULL%2,        Seon-young%Lee%NULL%0,        Kyungnam%Kim%NULL%2,        Kyungnam%Kim%NULL%0,        Soyoung%Shin%NULL%2,        Soyoung%Shin%NULL%0,        Eunsu%Jang%NULL%2,        Eunsu%Jang%NULL%0,        YoungSin%Moon%NULL%2,        YoungSin%Moon%NULL%0,        KwangHwan%Oh%NULL%2,        KwangHwan%Oh%NULL%0,        JaeRin%Choi%NULL%2,        JaeRin%Choi%NULL%0,        Sangeun%Lee%NULL%2,        Sangeun%Lee%NULL%0,        Young-Man%Kim%NULL%2,        Young-Man%Kim%NULL%0,        Jieun%Kim%NULL%2,        Jieun%Kim%NULL%0,        Seonju%Yi%NULL%2,        Seonju%Yi%NULL%0,        Jin%Gwack%NULL%2,        Jin%Gwack%NULL%0,        Ok%Park%NULL%2,        Ok%Park%NULL%0,        Young Joon%Park%NULL%2,        Young Joon%Park%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Rok%Song%NULL%1,        Hee-Sook%Kim%NULL%2,        Hee-Sook%Kim%NULL%0,        Seok-Ju%Yoo%NULL%2,        Seok-Ju%Yoo%NULL%0,        Kwan%Lee%NULL%2,        Kwan%Lee%NULL%0,        Ji-Hyuk%Park%NULL%2,        Ji-Hyuk%Park%NULL%0,        Joon Ho%Jang%NULL%2,        Joon Ho%Jang%NULL%0,        Gyoung-Sook%Ahn%NULL%2,        Gyoung-Sook%Ahn%NULL%0,        Jun-Nyun%Kim%NULL%2,        Jun-Nyun%Kim%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Blanca%Borras-Bermejo%NULL%1,        Xavier%Martínez-Gómez%NULL%1,        María Gutierrez%San Miguel%NULL%1,        Juliana%Esperalba%NULL%1,        Andrés%Antón%NULL%1,        Elisabet%Martin%NULL%1,        Marta%Selvi%NULL%1,        María José%Abadías%NULL%1,        Antonio%Román%NULL%1,        Tomàs%Pumarola%NULL%1,        Magda%Campins%NULL%1,        Benito%Almirante%NULL%1]</t>
+  </si>
+  <si>
+    <t>[M.%Bernabeu-Wittel%NULL%1,        J.E.%Ternero-Vega%NULL%1,        P.%Díaz-Jiménez%NULL%1,        C.%Conde-Guzmán%NULL%1,        M.D.%Nieto-Martín%NULL%1,        L.%Moreno-Gaviño%NULL%1,        J.%Delgado-Cuesta%NULL%1,        M.%Rincón-Gómez%NULL%1,        L.%Giménez-Miranda%NULL%1,        M.D.%Navarro-Amuedo%NULL%1,        M.M.%Muñoz-García%NULL%1,        S.%Calzón-Fernández%NULL%1,        M.%Ollero-Baturone%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Shamez N%Ladhani%shamez.ladhani@phe.gov.uk%1,        J.Yimmy%Chow%NULL%1,        Roshni%Janarthanan%NULL%1,        Jonathan%Fok%NULL%1,        Emma%Crawley-Boevey%NULL%1,        Amoolya%Vusirikala%NULL%1,        Elena%Fernandez%NULL%1,        Marina Sanchez%Perez%NULL%1,        Suzanne%Tang%NULL%1,        Kate%Dun-Campbell%NULL%1,        Edward Wynne-%Evans%NULL%1,        Anita%Bell%NULL%1,        Bharat%Patel%NULL%1,        Zahin%Amin-Chowdhury%NULL%1,        Felicity%Aiano%NULL%1,        Karthik%Paranthaman%NULL%1,        Thomas%Ma%NULL%1,        Maria%Saavedra-Campos%NULL%1,        Richard%Myers%NULL%1,        Joanna%Ellis%NULL%2,        Angie%Lackenby%NULL%1,        Robin%Gopal%NULL%1,        Monika%Patel%NULL%1,        Colin%Brown%NULL%1,        Meera%Chand%NULL%1,        Kevin%Brown%NULL%1,        Mary E%Ramsay%NULL%1,        Susan%Hopkins%NULL%2,        Nandini%Shetty%NULL%1,        Maria%Zambon%NULL%2]</t>
+  </si>
+  <si>
+    <t>[N.S.N.%Graham%NULL%1,        C.%Junghans%NULL%1,        R.%Downes%NULL%1,        C.%Sendall%NULL%1,        H.%Lai%NULL%1,        A.%McKirdy%NULL%1,        P.%Elliott%NULL%1,        R.%Howard%NULL%1,        D.%Wingfield%NULL%1,        M.%Priestman%NULL%1,        M.%Ciechonska%NULL%1,        L.%Cameron%NULL%1,        M.%Storch%NULL%1,        M.A.%Crone%NULL%1,        P.S.%Freemont%NULL%1,        P.%Randell%NULL%1,        R.%McLaren%NULL%1,        N.%Lang%NULL%1,        S.%Ladhani%NULL%1,        F.%Sanderson%NULL%1,        D.J.%Sharp%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Agnes%Marossy%agnesmarossy@nhs.net%1,        Stefan%Rakowicz%NULL%1,        Angela%Bhan%NULL%1,        Sarah%Noon%NULL%1,        Amanda%Rees%NULL%1,        Manjinder%Virk%NULL%1,        Ayazali%Nazafi%NULL%1,        Evie%Hay%NULL%1,        Louise%de Thomasson%NULL%1,        Christina%Windle%NULL%1,        Mark%Zuckerman%Mark.Zuckerman@nhs.net%1]</t>
+  </si>
+  <si>
+    <t>[Laura%Shallcross%NULL%1,        Danielle%Burke%NULL%1,        Owen%Abbott%NULL%1,        Alasdair%Donaldson%NULL%1,        Gemma%Hallatt%NULL%1,        Andrew%Hayward%NULL%1,        Susan%Hopkins%NULL%0,        Maria%Krutikov%NULL%1,        Katie%Sharp%NULL%1,        Leone%Wardman%NULL%1,        Sapphira%Thorne%NULL%1]</t>
+  </si>
+  <si>
+    <t>[ E.%Smith%null%1,         C. F.% Aldus%null%1,         J.% Brainard%null%1,         S.% Dunham%null%1,         P. R.% Hunter%null%1,         N.% Steel%null%1,         P. % Everden%null%1]</t>
+  </si>
+  <si>
+    <t>[Mahesh C%Patel%mp3@uic.edu%1,        Lelia H%Chaisson%NULL%1,        Scott%Borgetti%NULL%1,        Deborah%Burdsall%NULL%1,        Rashmi K%Chugh%NULL%1,        Christopher R%Hoff%NULL%1,        Elizabeth B%Murphy%NULL%1,        Emily A%Murskyj%NULL%1,        Shannon%Wilson%NULL%1,        Joe%Ramos%NULL%1,        Lynn%Akker%NULL%1,        Debra%Bryars%NULL%1,        Evonda%Thomas-Smith%NULL%1,        Susan C%Bleasdale%NULL%1,        Ngozi O%Ezike%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Helena%Temkin‐Greener%helena_temkin-greener@urmc.rochester.edu%1,        Wenhan%Guo%NULL%2,        Wenhan%Guo%NULL%0,        Yunjiao%Mao%NULL%1,        Xueya%Cai%NULL%1,        Yue%Li%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Ana A.%Weil%anaweil@uw.edu%1,        Kira L.%Newman%NULL%2,        Kira L.%Newman%NULL%0,        Thuan D.%Ong%NULL%1,        Giana H.%Davidson%NULL%1,        Jennifer%Logue%NULL%1,        Elisabeth%Brandstetter%NULL%1,        Ariana%Magedson%NULL%1,        Dylan%McDonald%NULL%1,        Denise J.%McCulloch%NULL%1,        Santiago%Neme%NULL%1,        James%Lewis%NULL%0,        Jeff S.%Duchin%NULL%1,        Weizhi%Zhong%NULL%1,        Lea M.%Starita%NULL%1,        Trevor%Bedford%NULL%1,        Alison C.%Roxby%NULL%1,        Helen Y.%Chu%helenchu@uw.edu%2]</t>
+  </si>
+  <si>
+    <t>[Guillermo V.%Sanchez%NULL%1,        Caitlin%Biedron%NULL%1,        Lauren R.%Fink%NULL%1,        Kelly M.%Hatfield%NULL%1,        Jordan Micah F.%Polistico%NULL%1,        Monica P.%Meyer%NULL%1,        Rebecca S.%Noe%NULL%1,        Casey E.%Copen%NULL%1,        Amanda K.%Lyons%NULL%1,        Gonzalo%Gonzalez%NULL%1,        Keith%Kiama%NULL%1,        Mark%Lebednick%NULL%1,        Bonnie K.%Czander%NULL%1,        Amen%Agbonze%NULL%1,        Aimee R.%Surma%NULL%1,        Avnish%Sandhu%NULL%1,        Valerie H.%Mika%NULL%1,        Tyler%Prentiss%NULL%1,        John%Zervos%NULL%1,        Donia A.%Dalal%NULL%1,        Amber M.%Vasquez%NULL%1,        Sujan C.%Reddy%NULL%0,        John%Jernigan%NULL%1,        Paul E.%Kilgore%NULL%1,        Marcus J.%Zervos%NULL%1,        Teena%Chopra%NULL%1,        Carla P.%Bezold%NULL%1,        Najibah K.%Rehman%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Janice K%Louie%Janice.louie@sfdph.org%1,        Hyman M%Scott%NULL%1,        Amie%DuBois%NULL%1,        Natalya%Sturtz%NULL%1,        Wendy%Lu%NULL%1,        Juliet%Stoltey%NULL%1,        Godfred%Masinde%NULL%1,        Stephanie%Cohen%NULL%1,        Darpun%Sachdev%NULL%1,        Susan%Philip%NULL%1,        Naveena%Bobba%NULL%1,        Tomas%Aragon%NULL%1,        NULL%NULL%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Scott A%Goldberg%sagoldberg@bwh.harvard.edu%1,        Jochen%Lennerz%NULL%1,        Michael%Klompas%NULL%1,        Eden%Mark%NULL%1,        Virginia M%Pierce%NULL%1,        Ryan W%Thompson%NULL%1,        Charles T%Pu%NULL%1,        Lauren L%Ritterhouse%NULL%1,        Anand%Dighe%NULL%1,        Eric S%Rosenberg%NULL%1,        David C%Grabowski%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Amy V.%Dora%NULL%1,        Alexander%Winnett%NULL%1,        Lauren P.%Jatt%NULL%1,        Kusha%Davar%NULL%1,        Mika%Watanabe%NULL%1,        Linda%Sohn%NULL%1,        Hannah S.%Kern%NULL%1,        Christopher J.%Graber%NULL%1,        Matthew B.%Goetz%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Benjamin F.%Bigelow%NULL%1,        Olive%Tang%NULL%1,        Gregory R.%Toci%NULL%1,        Norberth%Stracker%NULL%1,        Fatima%Sheikh%NULL%1,        Kara M.%Jacobs Slifka%NULL%1,        Shannon A.%Novosad%NULL%1,        John A.%Jernigan%NULL%0,        Sujan C.%Reddy%NULL%0,        Morgan J.%Katz%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Matt%Feaster%NULL%1,        Ying-Ying%Goh%NULL%1]</t>
+  </si>
+  <si>
+    <t>[William R.%Mills%NULL%1,        Janet M.%Buccola%NULL%1,        Susan%Sender%NULL%1,        Joseph%Lichtefeld%NULL%1,        Nicholas%Romano%NULL%1,        Karen%Reynolds%NULL%1,        Melissa%Price%NULL%1,        Jennifer%Phipps%NULL%1,        Leigh%White%NULL%1,        Shauen%Howard%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Drew A.%Harris%xref no email%1,  Laurie%Archbald-Pannone%xref no email%1,  Jasveen%Kaur%xref no email%1,  David%Cattell-Gordon%xref no email%1,  Karen S.%Rheuban%xref no email%1,  Rachel L.%Ombres%xref no email%1,  Kimberly%Albero%xref no email%1,  Rebecca%Steele%xref no email%1,  Taison D.%Bell%xref no email%1,  Justin B.%Mutter%xref no email%1]</t>
+  </si>
+  <si>
+    <t>[Carl D.%Shrader%xref no email%1,  Shauna%Assadzandi%xref no email%1,  Courtney S.%Pilkerton%xref no email%1,  Amie M.%Ashcraft%xref no email%1]</t>
   </si>
 </sst>
 </file>
@@ -1988,7 +2261,7 @@
         <v>60</v>
       </c>
       <c r="E2" t="s">
-        <v>382</v>
+        <v>469</v>
       </c>
       <c r="F2" t="s">
         <v>62</v>
@@ -2017,7 +2290,7 @@
         <v>66</v>
       </c>
       <c r="E3" t="s">
-        <v>383</v>
+        <v>470</v>
       </c>
       <c r="F3" t="s">
         <v>68</v>
@@ -2046,7 +2319,7 @@
         <v>70</v>
       </c>
       <c r="E4" t="s">
-        <v>384</v>
+        <v>471</v>
       </c>
       <c r="F4" t="s">
         <v>72</v>
@@ -2104,7 +2377,7 @@
         <v>74</v>
       </c>
       <c r="E6" t="s">
-        <v>385</v>
+        <v>472</v>
       </c>
       <c r="F6" t="s">
         <v>6</v>
@@ -2133,7 +2406,7 @@
         <v>79</v>
       </c>
       <c r="E7" t="s">
-        <v>386</v>
+        <v>473</v>
       </c>
       <c r="F7" t="s">
         <v>81</v>
@@ -2162,7 +2435,7 @@
         <v>83</v>
       </c>
       <c r="E8" t="s">
-        <v>387</v>
+        <v>474</v>
       </c>
       <c r="F8" t="s">
         <v>85</v>
@@ -2220,7 +2493,7 @@
         <v>87</v>
       </c>
       <c r="E10" t="s">
-        <v>388</v>
+        <v>475</v>
       </c>
       <c r="F10" t="s">
         <v>89</v>
@@ -2249,7 +2522,7 @@
         <v>92</v>
       </c>
       <c r="E11" t="s">
-        <v>389</v>
+        <v>476</v>
       </c>
       <c r="F11" t="s">
         <v>94</v>
@@ -2278,7 +2551,7 @@
         <v>98</v>
       </c>
       <c r="E12" t="s">
-        <v>390</v>
+        <v>477</v>
       </c>
       <c r="F12" t="s">
         <v>100</v>
@@ -2336,7 +2609,7 @@
         <v>102</v>
       </c>
       <c r="E14" t="s">
-        <v>391</v>
+        <v>478</v>
       </c>
       <c r="F14" t="s">
         <v>104</v>
@@ -2365,7 +2638,7 @@
         <v>107</v>
       </c>
       <c r="E15" t="s">
-        <v>392</v>
+        <v>479</v>
       </c>
       <c r="F15" t="s">
         <v>109</v>
@@ -2394,7 +2667,7 @@
         <v>112</v>
       </c>
       <c r="E16" t="s">
-        <v>393</v>
+        <v>480</v>
       </c>
       <c r="F16" t="s">
         <v>114</v>
@@ -2423,7 +2696,7 @@
         <v>277</v>
       </c>
       <c r="E17" t="s">
-        <v>394</v>
+        <v>481</v>
       </c>
       <c r="F17" t="s">
         <v>17</v>
@@ -2475,22 +2748,22 @@
         <v>43922.0</v>
       </c>
       <c r="C19" t="s">
-        <v>51</v>
+        <v>433</v>
       </c>
       <c r="D19" t="s">
         <v>52</v>
       </c>
       <c r="E19" t="s">
-        <v>55</v>
+        <v>482</v>
       </c>
       <c r="F19" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="G19" t="s">
-        <v>57</v>
+        <v>435</v>
       </c>
       <c r="H19" t="s">
-        <v>64</v>
+        <v>436</v>
       </c>
       <c r="I19" t="s">
         <v>107</v>
@@ -2510,7 +2783,7 @@
         <v>119</v>
       </c>
       <c r="E20" t="s">
-        <v>395</v>
+        <v>483</v>
       </c>
       <c r="F20" t="s">
         <v>121</v>
@@ -2539,7 +2812,7 @@
         <v>124</v>
       </c>
       <c r="E21" t="s">
-        <v>396</v>
+        <v>484</v>
       </c>
       <c r="F21" t="s">
         <v>126</v>
@@ -2568,7 +2841,7 @@
         <v>128</v>
       </c>
       <c r="E22" t="s">
-        <v>397</v>
+        <v>485</v>
       </c>
       <c r="F22" t="s">
         <v>130</v>
@@ -2626,7 +2899,7 @@
         <v>132</v>
       </c>
       <c r="E24" t="s">
-        <v>398</v>
+        <v>486</v>
       </c>
       <c r="F24" t="s">
         <v>56</v>
@@ -2655,7 +2928,7 @@
         <v>136</v>
       </c>
       <c r="E25" t="s">
-        <v>399</v>
+        <v>487</v>
       </c>
       <c r="F25" t="s">
         <v>138</v>
@@ -2684,7 +2957,7 @@
         <v>52</v>
       </c>
       <c r="E26" t="s">
-        <v>400</v>
+        <v>488</v>
       </c>
       <c r="F26" t="s">
         <v>26</v>
@@ -2713,7 +2986,7 @@
         <v>141</v>
       </c>
       <c r="E27" t="s">
-        <v>401</v>
+        <v>489</v>
       </c>
       <c r="F27" t="s">
         <v>143</v>
@@ -2742,7 +3015,7 @@
         <v>146</v>
       </c>
       <c r="E28" t="s">
-        <v>402</v>
+        <v>490</v>
       </c>
       <c r="F28" t="s">
         <v>148</v>
@@ -2771,7 +3044,7 @@
         <v>151</v>
       </c>
       <c r="E29" t="s">
-        <v>403</v>
+        <v>491</v>
       </c>
       <c r="F29" t="s">
         <v>153</v>
@@ -2800,7 +3073,7 @@
         <v>107</v>
       </c>
       <c r="E30" t="s">
-        <v>404</v>
+        <v>492</v>
       </c>
       <c r="F30" t="s">
         <v>156</v>
@@ -2829,7 +3102,7 @@
         <v>159</v>
       </c>
       <c r="E31" t="s">
-        <v>405</v>
+        <v>493</v>
       </c>
       <c r="F31" t="s">
         <v>161</v>
@@ -2858,7 +3131,7 @@
         <v>164</v>
       </c>
       <c r="E32" t="s">
-        <v>406</v>
+        <v>494</v>
       </c>
       <c r="F32" t="s">
         <v>166</v>
@@ -2887,7 +3160,7 @@
         <v>169</v>
       </c>
       <c r="E33" t="s">
-        <v>407</v>
+        <v>495</v>
       </c>
       <c r="F33" t="s">
         <v>171</v>
@@ -2916,7 +3189,7 @@
         <v>173</v>
       </c>
       <c r="E34" t="s">
-        <v>408</v>
+        <v>496</v>
       </c>
       <c r="F34" t="s">
         <v>175</v>
@@ -2945,7 +3218,7 @@
         <v>177</v>
       </c>
       <c r="E35" t="s">
-        <v>409</v>
+        <v>497</v>
       </c>
       <c r="F35" t="s">
         <v>56</v>
@@ -2974,7 +3247,7 @@
         <v>181</v>
       </c>
       <c r="E36" t="s">
-        <v>410</v>
+        <v>498</v>
       </c>
       <c r="F36" t="s">
         <v>183</v>
@@ -3003,7 +3276,7 @@
         <v>186</v>
       </c>
       <c r="E37" t="s">
-        <v>411</v>
+        <v>499</v>
       </c>
       <c r="F37" t="s">
         <v>188</v>
@@ -3032,7 +3305,7 @@
         <v>191</v>
       </c>
       <c r="E38" t="s">
-        <v>412</v>
+        <v>500</v>
       </c>
       <c r="F38" t="s">
         <v>193</v>
@@ -3061,7 +3334,7 @@
         <v>107</v>
       </c>
       <c r="E39" t="s">
-        <v>413</v>
+        <v>501</v>
       </c>
       <c r="F39" t="s">
         <v>197</v>
@@ -3090,7 +3363,7 @@
         <v>199</v>
       </c>
       <c r="E40" t="s">
-        <v>414</v>
+        <v>502</v>
       </c>
       <c r="F40" t="s">
         <v>201</v>
@@ -3119,7 +3392,7 @@
         <v>203</v>
       </c>
       <c r="E41" t="s">
-        <v>415</v>
+        <v>503</v>
       </c>
       <c r="F41" t="s">
         <v>205</v>
@@ -3148,7 +3421,7 @@
         <v>107</v>
       </c>
       <c r="E42" t="s">
-        <v>416</v>
+        <v>504</v>
       </c>
       <c r="F42" t="s">
         <v>208</v>
@@ -3177,7 +3450,7 @@
         <v>107</v>
       </c>
       <c r="E43" t="s">
-        <v>417</v>
+        <v>505</v>
       </c>
       <c r="F43" t="s">
         <v>211</v>
@@ -3206,7 +3479,7 @@
         <v>213</v>
       </c>
       <c r="E44" t="s">
-        <v>418</v>
+        <v>506</v>
       </c>
       <c r="F44" t="s">
         <v>215</v>
@@ -3235,7 +3508,7 @@
         <v>217</v>
       </c>
       <c r="E45" t="s">
-        <v>419</v>
+        <v>507</v>
       </c>
       <c r="F45" t="s">
         <v>219</v>
@@ -3258,22 +3531,22 @@
         <v>44197.0</v>
       </c>
       <c r="C46" t="s">
-        <v>51</v>
+        <v>462</v>
       </c>
       <c r="D46" t="s">
         <v>52</v>
       </c>
       <c r="E46" t="s">
-        <v>55</v>
+        <v>508</v>
       </c>
       <c r="F46" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="G46" t="s">
-        <v>57</v>
+        <v>435</v>
       </c>
       <c r="H46" t="s">
-        <v>64</v>
+        <v>464</v>
       </c>
       <c r="I46" t="s">
         <v>107</v>
@@ -3287,22 +3560,22 @@
         <v>44197.0</v>
       </c>
       <c r="C47" t="s">
-        <v>51</v>
+        <v>465</v>
       </c>
       <c r="D47" t="s">
-        <v>52</v>
+        <v>466</v>
       </c>
       <c r="E47" t="s">
-        <v>55</v>
+        <v>509</v>
       </c>
       <c r="F47" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="G47" t="s">
-        <v>57</v>
+        <v>435</v>
       </c>
       <c r="H47" t="s">
-        <v>64</v>
+        <v>468</v>
       </c>
       <c r="I47" t="s">
         <v>107</v>

</xml_diff>

<commit_message>
Fixed a bug where the springer api wouldn't properly fill in the abstract in some situations
</commit_message>
<xml_diff>
--- a/Covid_19_Dataset_and_References/References/10.xlsx
+++ b/Covid_19_Dataset_and_References/References/10.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3010" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3668" uniqueCount="592">
   <si>
     <t>Doi</t>
   </si>
@@ -1911,6 +1911,252 @@
   </si>
   <si>
     <t>[Carl D.%Shrader%xref no email%1,  Shauna%Assadzandi%xref no email%1,  Courtney S.%Pilkerton%xref no email%1,  Amie M.%Ashcraft%xref no email%1]</t>
+  </si>
+  <si>
+    <t>[Daniel J%Escobar%Daniel.escobar@pennmedicine.upenn.edu%1,         Maria%Lanzi%NULL%1,         Pouné%Saberi%NULL%1,         Ruby%Love%NULL%1,         Darren R%Linkin%NULL%1,         John J%Kelly%NULL%1,         Darshana%Jhala%NULL%1,         Valerianna%Amorosa%NULL%1,         Mary%Hofmann%NULL%1,         Jeffrey B%Doyon%NULL%1]</t>
+  </si>
+  <si>
+    <t>[James L.%Rudolph%NULL%1,         Christopher W.%Halladay%NULL%1,         Malisa%Barber%NULL%1,         Kevin W.%McConeghy%NULL%1,         Vince%Mor%NULL%1,         Aman%Nanda%NULL%1,         Stefan%Gravenstein%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Paula%Eckardt%NULL%1,         Rachel%Guran%NULL%1,         Jon%Hennemyre%NULL%1,         Roshan%Arikupurathu%NULL%1,         Julie%Poveda%NULL%1,         Nancimae%Miller%NULL%1,         Randy%Katz%NULL%1,         Judith%Frum%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Carson%Telford%NULL%1,         Udodirim%Onwubiko%NULL%1,         David%Holland%NULL%1,         Kim%Turner%NULL%1,         Juliana%Prieto%NULL%1,         Sasha%Smith%NULL%1,         Jane%Yoon%NULL%1,         Wecheeta%Brown%NULL%1,         Allison%Chamberlain%NULL%1,         Neel%Gandhi%NULL%1,         Shamimul%Khan%NULL%1,         Steve%Williams%NULL%1,         Fazle%Khan%NULL%1,         Sarita%Shah%NULL%1,          C. T.%Telford%null%1,          U.% Onwubiko%null%1,          D.% Holland%null%1,          K.% Turner%null%1,          J.% Prieto%null%1,          S.% Smith%null%1,          J.% Yoon%null%1,          W.% Brown%null%1,          A.% Chamberlain%null%1,          N.% Gandhi%null%1,          S.% Khan%null%1,          S.% Williams%null%1,          F.% Khan%null%1,          S. % Shah%null%1,         C. T.%Telford%null%1,         U.% Onwubiko%null%1,         D.% Holland%null%1,         K.% Turner%null%1,         J.% Prieto%null%1,         S.% Smith%null%1,         J.% Yoon%null%1,         W.% Brown%null%1,         A.% Chamberlain%null%1,         N.% Gandhi%null%1,         S.% Khan%null%1,         S.% Williams%null%1,         F.% Khan%null%1,         S. % Shah%null%1]</t>
+  </si>
+  <si>
+    <t>[Sandra M.%Shi%NULL%1,         Innokentiy%Bakaev%NULL%1,         Helen%Chen%NULL%1,         Thomas G.%Travison%NULL%1,         Sarah D.%Berry%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Temet M.%McMichael%NULL%0,         Dustin W.%Currie%NULL%0,         Shauna%Clark%NULL%0,         Sargis%Pogosjans%NULL%0,         Meagan%Kay%NULL%0,         Noah G.%Schwartz%NULL%0,         James%Lewis%NULL%0,         Atar%Baer%NULL%0,         Vance%Kawakami%NULL%0,         Margaret D.%Lukoff%NULL%0,         Jessica%Ferro%NULL%0,         Claire%Brostrom-Smith%NULL%0,         Thomas D.%Rea%NULL%1,         Michael R.%Sayre%NULL%1,         Francis X.%Riedo%NULL%0,         Denny%Russell%NULL%0,         Brian%Hiatt%NULL%0,         Patricia%Montgomery%NULL%0,         Agam K.%Rao%NULL%0,         Eric J.%Chow%NULL%0,         Farrell%Tobolowsky%NULL%0,         Michael J.%Hughes%NULL%1,         Ana C.%Bardossy%NULL%0,         Lisa P.%Oakley%NULL%0,         Jesica R.%Jacobs%NULL%0,         Nimalie D.%Stone%NULL%1,         Sujan C.%Reddy%NULL%0,         John A.%Jernigan%NULL%0,         Margaret A.%Honein%NULL%0,         Thomas A.%Clark%NULL%0,         Jeffrey S.%Duchin%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Nathan M.%Stall%nathan.stall@sinaihealth.ca%1,         Carolyn%Farquharson%NULL%2,         Carolyn%Farquharson%NULL%0,         Chris%Fan‐Lun%NULL%1,         Lesley%Wiesenfeld%NULL%1,         Carla A.%Loftus%NULL%1,         Dylan%Kain%NULL%1,         Jennie%Johnstone%NULL%1,         Liz%McCreight%NULL%1,         Russell D.%Goldman%NULL%1,         Ramona%Mahtani%NULL%1]</t>
+  </si>
+  <si>
+    <t>[ Nathan M.%Stall%null%1,          Aaron%Jones%null%1,          Kevin A.%Brown%null%1,          Paula A.%Rochon%null%1,          Andrew P.%Costa%null%1,         Nathan M.%Stall%null%1,         Aaron%Jones%null%1,         Kevin A.%Brown%null%1,         Paula A.%Rochon%null%1,         Andrew P.%Costa%null%1]</t>
+  </si>
+  <si>
+    <t>[Hubert%Blain%NULL%1,         Yves%Rolland%NULL%1,         Edouard%Tuaillon%NULL%1,         Nadia%Giacosa%NULL%1,         Mylène%Albrand%NULL%1,         Audrey%Jaussent%NULL%1,         Athanase%Benetos%NULL%1,         Stéphanie%Miot%NULL%1,         Jean%Bousquet%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Guillaume%Sacco%NULL%1,         Gonzague%Foucault%NULL%1,         Olivier%Briere%NULL%1,         Cédric%Annweiler%NULL%1]</t>
+  </si>
+  <si>
+    <t>[R.%Guery%NULL%1,         C.%Delaye%NULL%1,         N.%Brule%NULL%1,         V.%Nael%NULL%1,         L.%Castain%NULL%1,         F.%Raffi%NULL%1,         L.%De Decker%NULL%1]</t>
+  </si>
+  <si>
+    <t>[A.%Klein%anke.klein@uke.de%1,         C.%Edler%NULL%1,         A.%Fitzek%NULL%1,         D.%Fröb%NULL%1,         A.%Heinemann%NULL%1,         K.%Meißner%NULL%1,         H.%Mushumba%NULL%1,         K.%Püschel%NULL%1,         A. S.%Schröder%NULL%1,         J. P.%Sperhake%NULL%1,         F.%Ishorst-Witte%NULL%1,         M.%Aepfelbacher%NULL%1,         F.%Heinrich%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Buntinx%Frank%coreGivesNoEmail%1,       Claes%Peter%coreGivesNoEmail%1,       Gulikers%Marjo%coreGivesNoEmail%1,       Jan%De Lepeleire%coreGivesNoEmail%1,       Van%der Elst Michael%coreGivesNoEmail%1,       Van%Elslande Jan%coreGivesNoEmail%1,       Van%Ranst Marc%coreGivesNoEmail%1,       Verbakel%Jan%coreGivesNoEmail%1,       Vernneersch%Pieter%coreGivesNoEmail%1]</t>
+  </si>
+  <si>
+    <t>[Liangcong%Hu%xref no email%1,   Wanyuan%Zhen%xref no email%1,   Xudong%Xie%xref no email%2,   Ze%Lin%xref no email%2,   Tiantian%Wang%xref no email%1,   Jing%Liu%xref no email%5,   Hang%Xue%xref no email%2,   Adriana C.%Panayi%xref no email%2,   Ke%Xu%xref no email%1,   Zexi%Ling%xref no email%1,   Xugui%Li%xref no email%1,   Bobin%Mi%xref no email%1,   Wu%Zhou%xref no email%2,   Guohui%Liu%xref no email%2]</t>
+  </si>
+  <si>
+    <t>[Sean P%Kennelly%Sean.Kennelly@tuh.ie%1,         Adam H%Dyer%dyera@tcd.ie%1,         Claire%Noonan%claire.noonan@tuh.ie%2,         Claire%Noonan%claire.noonan@tuh.ie%0,         Ruth%Martin%ruth.martin1@hse.ie%1,         Siobhan M%Kennelly%siobhan.kennelly1@hse.ie%1,         Alan%Martin%alanmartin@beaumont.ie%1,         Desmond%O’Neill%NULL%1,         Aoife%Fallon%aoife.fallon1@hotmail.com%1]</t>
+  </si>
+  <si>
+    <t>[Antonio%Nouvenne%NULL%1,         Andrea%Ticinesi%NULL%1,         Alberto%Parise%NULL%1,         Beatrice%Prati%NULL%1,         Marcello%Esposito%NULL%1,         Valentina%Cocchi%NULL%1,         Emanuele%Crisafulli%NULL%1,         Annalisa%Volpi%NULL%1,         Sandra%Rossi%NULL%1,         Elena Giovanna%Bignami%NULL%1,         Marco%Baciarello%NULL%1,         Ettore%Brianti%NULL%1,         Massimo%Fabi%NULL%1,         Tiziana%Meschi%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Nicola%Veronese%NULL%1,         Luca Gino%Sbrogiò%NULL%1,         Roberto%Valle%NULL%1,         Laura%Marin%NULL%1,         Elena%Boscolo Fiore%NULL%1,         Andrea%Tiozzo%NULL%1]</t>
+  </si>
+  <si>
+    <t>[ J. H.%van den Besselaar%null%1,          R. S.% Sikkema%null%1,          F. M. H. P. A.% Koene%null%1,          L. W.% van Buul%null%1,          B. B.% Oude Munnink%null%1,          I.% Frenay%null%1,          R.% te Witt%null%1,          M. P. G.% Koopmans%null%1,          C. M. P. M.% Hertogh%null%1,          B. M. % Buurman%null%1]</t>
+  </si>
+  <si>
+    <t>[Laura W.%van Buul%NULL%1,         Judith H.%van den Besselaar%NULL%2,         Judith H.%van den Besselaar%NULL%0,         Fleur M. H. P. H.%Koene%NULL%1,         Bianca M.%Buurman%NULL%1,         Cees M. P. M.%Hertogh%NULL%1,         Martin%Smalbrugge%NULL%1,         Jeanine J. S.%Rutten%NULL%1,         Elke M.%den Boogert%NULL%1,         Michel D.%Wissing%NULL%1,         Ariene%Rietveld%NULL%1,         Mariska W. W.%van Elsakker%NULL%1,         Marga M. G.%Nonneman%NULL%1,         Florien%van Eeden%NULL%1,         Saskia%van de Merwe%NULL%1,         Sophie L.%Niemansburg%NULL%1,         Ewout%Fanoy%NULL%1,         Hinke S.%Bootsma%NULL%1,         Nicoline%van der Hagen%NULL%1,         Mariska%Petrignani%NULL%1,         Jessica Edwards%van Muijen%NULL%1,         Karolien E. M.%Biesheuvel%NULL%1]</t>
+  </si>
+  <si>
+    <t>[B\u00e5rd%Reiakvam Kittang%coreGivesNoEmail%1,       Karina%Koller L\u00f8land%coreGivesNoEmail%1,       Kjell%Kr\u00fcger%coreGivesNoEmail%1,       Kristian%Jansen%coreGivesNoEmail%1,       Sabine%Piepenstock Solheim%coreGivesNoEmail%1,       Sebastian%von Hofacker%coreGivesNoEmail%1]</t>
+  </si>
+  <si>
+    <t>[Shin Young%Park%NULL%1,         Gawon%Choi%NULL%2,         Gawon%Choi%NULL%0,         Hyeyoung%Lee%NULL%2,         Hyeyoung%Lee%NULL%0,         Na-young%Kim%NULL%2,         Na-young%Kim%NULL%0,         Seon-young%Lee%NULL%2,         Seon-young%Lee%NULL%0,         Kyungnam%Kim%NULL%2,         Kyungnam%Kim%NULL%0,         Soyoung%Shin%NULL%2,         Soyoung%Shin%NULL%0,         Eunsu%Jang%NULL%2,         Eunsu%Jang%NULL%0,         YoungSin%Moon%NULL%2,         YoungSin%Moon%NULL%0,         KwangHwan%Oh%NULL%2,         KwangHwan%Oh%NULL%0,         JaeRin%Choi%NULL%2,         JaeRin%Choi%NULL%0,         Sangeun%Lee%NULL%2,         Sangeun%Lee%NULL%0,         Young-Man%Kim%NULL%2,         Young-Man%Kim%NULL%0,         Jieun%Kim%NULL%2,         Jieun%Kim%NULL%0,         Seonju%Yi%NULL%2,         Seonju%Yi%NULL%0,         Jin%Gwack%NULL%2,         Jin%Gwack%NULL%0,         Ok%Park%NULL%2,         Ok%Park%NULL%0,         Young Joon%Park%NULL%2,         Young Joon%Park%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Rok%Song%NULL%1,         Hee-Sook%Kim%NULL%2,         Hee-Sook%Kim%NULL%0,         Seok-Ju%Yoo%NULL%2,         Seok-Ju%Yoo%NULL%0,         Kwan%Lee%NULL%2,         Kwan%Lee%NULL%0,         Ji-Hyuk%Park%NULL%2,         Ji-Hyuk%Park%NULL%0,         Joon Ho%Jang%NULL%2,         Joon Ho%Jang%NULL%0,         Gyoung-Sook%Ahn%NULL%2,         Gyoung-Sook%Ahn%NULL%0,         Jun-Nyun%Kim%NULL%2,         Jun-Nyun%Kim%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Blanca%Borras-Bermejo%NULL%1,         Xavier%Martínez-Gómez%NULL%1,         María Gutierrez%San Miguel%NULL%1,         Juliana%Esperalba%NULL%1,         Andrés%Antón%NULL%1,         Elisabet%Martin%NULL%1,         Marta%Selvi%NULL%1,         María José%Abadías%NULL%1,         Antonio%Román%NULL%1,         Tomàs%Pumarola%NULL%1,         Magda%Campins%NULL%1,         Benito%Almirante%NULL%1]</t>
+  </si>
+  <si>
+    <t>[M.%Bernabeu-Wittel%NULL%1,         J.E.%Ternero-Vega%NULL%1,         P.%Díaz-Jiménez%NULL%1,         C.%Conde-Guzmán%NULL%1,         M.D.%Nieto-Martín%NULL%1,         L.%Moreno-Gaviño%NULL%1,         J.%Delgado-Cuesta%NULL%1,         M.%Rincón-Gómez%NULL%1,         L.%Giménez-Miranda%NULL%1,         M.D.%Navarro-Amuedo%NULL%1,         M.M.%Muñoz-García%NULL%1,         S.%Calzón-Fernández%NULL%1,         M.%Ollero-Baturone%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Shamez N%Ladhani%shamez.ladhani@phe.gov.uk%1,         J.Yimmy%Chow%NULL%1,         Roshni%Janarthanan%NULL%1,         Jonathan%Fok%NULL%1,         Emma%Crawley-Boevey%NULL%1,         Amoolya%Vusirikala%NULL%1,         Elena%Fernandez%NULL%1,         Marina Sanchez%Perez%NULL%1,         Suzanne%Tang%NULL%1,         Kate%Dun-Campbell%NULL%1,         Edward Wynne-%Evans%NULL%1,         Anita%Bell%NULL%1,         Bharat%Patel%NULL%1,         Zahin%Amin-Chowdhury%NULL%1,         Felicity%Aiano%NULL%1,         Karthik%Paranthaman%NULL%1,         Thomas%Ma%NULL%1,         Maria%Saavedra-Campos%NULL%1,         Richard%Myers%NULL%1,         Joanna%Ellis%NULL%2,         Angie%Lackenby%NULL%1,         Robin%Gopal%NULL%1,         Monika%Patel%NULL%1,         Colin%Brown%NULL%1,         Meera%Chand%NULL%1,         Kevin%Brown%NULL%1,         Mary E%Ramsay%NULL%1,         Susan%Hopkins%NULL%2,         Nandini%Shetty%NULL%1,         Maria%Zambon%NULL%2]</t>
+  </si>
+  <si>
+    <t>[N.S.N.%Graham%NULL%1,         C.%Junghans%NULL%1,         R.%Downes%NULL%1,         C.%Sendall%NULL%1,         H.%Lai%NULL%1,         A.%McKirdy%NULL%1,         P.%Elliott%NULL%1,         R.%Howard%NULL%1,         D.%Wingfield%NULL%1,         M.%Priestman%NULL%1,         M.%Ciechonska%NULL%1,         L.%Cameron%NULL%1,         M.%Storch%NULL%1,         M.A.%Crone%NULL%1,         P.S.%Freemont%NULL%1,         P.%Randell%NULL%1,         R.%McLaren%NULL%1,         N.%Lang%NULL%1,         S.%Ladhani%NULL%1,         F.%Sanderson%NULL%1,         D.J.%Sharp%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Agnes%Marossy%agnesmarossy@nhs.net%1,         Stefan%Rakowicz%NULL%1,         Angela%Bhan%NULL%1,         Sarah%Noon%NULL%1,         Amanda%Rees%NULL%1,         Manjinder%Virk%NULL%1,         Ayazali%Nazafi%NULL%1,         Evie%Hay%NULL%1,         Louise%de Thomasson%NULL%1,         Christina%Windle%NULL%1,         Mark%Zuckerman%Mark.Zuckerman@nhs.net%1]</t>
+  </si>
+  <si>
+    <t>[Laura%Shallcross%NULL%1,         Danielle%Burke%NULL%1,         Owen%Abbott%NULL%1,         Alasdair%Donaldson%NULL%1,         Gemma%Hallatt%NULL%1,         Andrew%Hayward%NULL%1,         Susan%Hopkins%NULL%0,         Maria%Krutikov%NULL%1,         Katie%Sharp%NULL%1,         Leone%Wardman%NULL%1,         Sapphira%Thorne%NULL%1]</t>
+  </si>
+  <si>
+    <t>[ E.%Smith%null%1,          C. F.% Aldus%null%1,          J.% Brainard%null%1,          S.% Dunham%null%1,          P. R.% Hunter%null%1,          N.% Steel%null%1,          P. % Everden%null%1]</t>
+  </si>
+  <si>
+    <t>[Mahesh C%Patel%mp3@uic.edu%1,         Lelia H%Chaisson%NULL%1,         Scott%Borgetti%NULL%1,         Deborah%Burdsall%NULL%1,         Rashmi K%Chugh%NULL%1,         Christopher R%Hoff%NULL%1,         Elizabeth B%Murphy%NULL%1,         Emily A%Murskyj%NULL%1,         Shannon%Wilson%NULL%1,         Joe%Ramos%NULL%1,         Lynn%Akker%NULL%1,         Debra%Bryars%NULL%1,         Evonda%Thomas-Smith%NULL%1,         Susan C%Bleasdale%NULL%1,         Ngozi O%Ezike%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Helena%Temkin‐Greener%helena_temkin-greener@urmc.rochester.edu%1,         Wenhan%Guo%NULL%2,         Wenhan%Guo%NULL%0,         Yunjiao%Mao%NULL%1,         Xueya%Cai%NULL%1,         Yue%Li%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Ana A.%Weil%anaweil@uw.edu%1,         Kira L.%Newman%NULL%2,         Kira L.%Newman%NULL%0,         Thuan D.%Ong%NULL%1,         Giana H.%Davidson%NULL%1,         Jennifer%Logue%NULL%1,         Elisabeth%Brandstetter%NULL%1,         Ariana%Magedson%NULL%1,         Dylan%McDonald%NULL%1,         Denise J.%McCulloch%NULL%1,         Santiago%Neme%NULL%1,         James%Lewis%NULL%0,         Jeff S.%Duchin%NULL%1,         Weizhi%Zhong%NULL%1,         Lea M.%Starita%NULL%1,         Trevor%Bedford%NULL%1,         Alison C.%Roxby%NULL%1,         Helen Y.%Chu%helenchu@uw.edu%2]</t>
+  </si>
+  <si>
+    <t>[Guillermo V.%Sanchez%NULL%1,         Caitlin%Biedron%NULL%1,         Lauren R.%Fink%NULL%1,         Kelly M.%Hatfield%NULL%1,         Jordan Micah F.%Polistico%NULL%1,         Monica P.%Meyer%NULL%1,         Rebecca S.%Noe%NULL%1,         Casey E.%Copen%NULL%1,         Amanda K.%Lyons%NULL%1,         Gonzalo%Gonzalez%NULL%1,         Keith%Kiama%NULL%1,         Mark%Lebednick%NULL%1,         Bonnie K.%Czander%NULL%1,         Amen%Agbonze%NULL%1,         Aimee R.%Surma%NULL%1,         Avnish%Sandhu%NULL%1,         Valerie H.%Mika%NULL%1,         Tyler%Prentiss%NULL%1,         John%Zervos%NULL%1,         Donia A.%Dalal%NULL%1,         Amber M.%Vasquez%NULL%1,         Sujan C.%Reddy%NULL%0,         John%Jernigan%NULL%1,         Paul E.%Kilgore%NULL%1,         Marcus J.%Zervos%NULL%1,         Teena%Chopra%NULL%1,         Carla P.%Bezold%NULL%1,         Najibah K.%Rehman%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Janice K%Louie%Janice.louie@sfdph.org%1,         Hyman M%Scott%NULL%1,         Amie%DuBois%NULL%1,         Natalya%Sturtz%NULL%1,         Wendy%Lu%NULL%1,         Juliet%Stoltey%NULL%1,         Godfred%Masinde%NULL%1,         Stephanie%Cohen%NULL%1,         Darpun%Sachdev%NULL%1,         Susan%Philip%NULL%1,         Naveena%Bobba%NULL%1,         Tomas%Aragon%NULL%1,         NULL%NULL%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Scott A%Goldberg%sagoldberg@bwh.harvard.edu%1,         Jochen%Lennerz%NULL%1,         Michael%Klompas%NULL%1,         Eden%Mark%NULL%1,         Virginia M%Pierce%NULL%1,         Ryan W%Thompson%NULL%1,         Charles T%Pu%NULL%1,         Lauren L%Ritterhouse%NULL%1,         Anand%Dighe%NULL%1,         Eric S%Rosenberg%NULL%1,         David C%Grabowski%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Amy V.%Dora%NULL%1,         Alexander%Winnett%NULL%1,         Lauren P.%Jatt%NULL%1,         Kusha%Davar%NULL%1,         Mika%Watanabe%NULL%1,         Linda%Sohn%NULL%1,         Hannah S.%Kern%NULL%1,         Christopher J.%Graber%NULL%1,         Matthew B.%Goetz%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Benjamin F.%Bigelow%NULL%1,         Olive%Tang%NULL%1,         Gregory R.%Toci%NULL%1,         Norberth%Stracker%NULL%1,         Fatima%Sheikh%NULL%1,         Kara M.%Jacobs Slifka%NULL%1,         Shannon A.%Novosad%NULL%1,         John A.%Jernigan%NULL%0,         Sujan C.%Reddy%NULL%0,         Morgan J.%Katz%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Matt%Feaster%NULL%1,         Ying-Ying%Goh%NULL%1]</t>
+  </si>
+  <si>
+    <t>[William R.%Mills%NULL%1,         Janet M.%Buccola%NULL%1,         Susan%Sender%NULL%1,         Joseph%Lichtefeld%NULL%1,         Nicholas%Romano%NULL%1,         Karen%Reynolds%NULL%1,         Melissa%Price%NULL%1,         Jennifer%Phipps%NULL%1,         Leigh%White%NULL%1,         Shauen%Howard%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Drew A.%Harris%xref no email%1,   Laurie%Archbald-Pannone%xref no email%1,   Jasveen%Kaur%xref no email%1,   David%Cattell-Gordon%xref no email%1,   Karen S.%Rheuban%xref no email%1,   Rachel L.%Ombres%xref no email%1,   Kimberly%Albero%xref no email%1,   Rebecca%Steele%xref no email%1,   Taison D.%Bell%xref no email%1,   Justin B.%Mutter%xref no email%1]</t>
+  </si>
+  <si>
+    <t>[Carl D.%Shrader%xref no email%1,   Shauna%Assadzandi%xref no email%1,   Courtney S.%Pilkerton%xref no email%1,   Amie M.%Ashcraft%xref no email%1]</t>
+  </si>
+  <si>
+    <t>[Daniel J%Escobar%Daniel.escobar@pennmedicine.upenn.edu%1,          Maria%Lanzi%NULL%1,          Pouné%Saberi%NULL%1,          Ruby%Love%NULL%1,          Darren R%Linkin%NULL%1,          John J%Kelly%NULL%1,          Darshana%Jhala%NULL%1,          Valerianna%Amorosa%NULL%1,          Mary%Hofmann%NULL%1,          Jeffrey B%Doyon%NULL%1]</t>
+  </si>
+  <si>
+    <t>[James L.%Rudolph%NULL%1,          Christopher W.%Halladay%NULL%1,          Malisa%Barber%NULL%1,          Kevin W.%McConeghy%NULL%1,          Vince%Mor%NULL%1,          Aman%Nanda%NULL%1,          Stefan%Gravenstein%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Paula%Eckardt%NULL%1,          Rachel%Guran%NULL%1,          Jon%Hennemyre%NULL%1,          Roshan%Arikupurathu%NULL%1,          Julie%Poveda%NULL%1,          Nancimae%Miller%NULL%1,          Randy%Katz%NULL%1,          Judith%Frum%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Carson%Telford%NULL%1,          Udodirim%Onwubiko%NULL%1,          David%Holland%NULL%1,          Kim%Turner%NULL%1,          Juliana%Prieto%NULL%1,          Sasha%Smith%NULL%1,          Jane%Yoon%NULL%1,          Wecheeta%Brown%NULL%1,          Allison%Chamberlain%NULL%1,          Neel%Gandhi%NULL%1,          Shamimul%Khan%NULL%1,          Steve%Williams%NULL%1,          Fazle%Khan%NULL%1,          Sarita%Shah%NULL%1,           C. T.%Telford%null%1,           U.% Onwubiko%null%1,           D.% Holland%null%1,           K.% Turner%null%1,           J.% Prieto%null%1,           S.% Smith%null%1,           J.% Yoon%null%1,           W.% Brown%null%1,           A.% Chamberlain%null%1,           N.% Gandhi%null%1,           S.% Khan%null%1,           S.% Williams%null%1,           F.% Khan%null%1,           S. % Shah%null%1,          C. T.%Telford%null%1,          U.% Onwubiko%null%1,          D.% Holland%null%1,          K.% Turner%null%1,          J.% Prieto%null%1,          S.% Smith%null%1,          J.% Yoon%null%1,          W.% Brown%null%1,          A.% Chamberlain%null%1,          N.% Gandhi%null%1,          S.% Khan%null%1,          S.% Williams%null%1,          F.% Khan%null%1,          S. % Shah%null%1]</t>
+  </si>
+  <si>
+    <t>[Sandra M.%Shi%NULL%1,          Innokentiy%Bakaev%NULL%1,          Helen%Chen%NULL%1,          Thomas G.%Travison%NULL%1,          Sarah D.%Berry%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Temet M.%McMichael%NULL%0,          Dustin W.%Currie%NULL%0,          Shauna%Clark%NULL%0,          Sargis%Pogosjans%NULL%0,          Meagan%Kay%NULL%0,          Noah G.%Schwartz%NULL%0,          James%Lewis%NULL%0,          Atar%Baer%NULL%0,          Vance%Kawakami%NULL%0,          Margaret D.%Lukoff%NULL%0,          Jessica%Ferro%NULL%0,          Claire%Brostrom-Smith%NULL%0,          Thomas D.%Rea%NULL%1,          Michael R.%Sayre%NULL%1,          Francis X.%Riedo%NULL%0,          Denny%Russell%NULL%0,          Brian%Hiatt%NULL%0,          Patricia%Montgomery%NULL%0,          Agam K.%Rao%NULL%0,          Eric J.%Chow%NULL%0,          Farrell%Tobolowsky%NULL%0,          Michael J.%Hughes%NULL%1,          Ana C.%Bardossy%NULL%0,          Lisa P.%Oakley%NULL%0,          Jesica R.%Jacobs%NULL%0,          Nimalie D.%Stone%NULL%1,          Sujan C.%Reddy%NULL%0,          John A.%Jernigan%NULL%0,          Margaret A.%Honein%NULL%0,          Thomas A.%Clark%NULL%0,          Jeffrey S.%Duchin%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Nathan M.%Stall%nathan.stall@sinaihealth.ca%1,          Carolyn%Farquharson%NULL%2,          Carolyn%Farquharson%NULL%0,          Chris%Fan‐Lun%NULL%1,          Lesley%Wiesenfeld%NULL%1,          Carla A.%Loftus%NULL%1,          Dylan%Kain%NULL%1,          Jennie%Johnstone%NULL%1,          Liz%McCreight%NULL%1,          Russell D.%Goldman%NULL%1,          Ramona%Mahtani%NULL%1]</t>
+  </si>
+  <si>
+    <t>[ Nathan M.%Stall%null%1,           Aaron%Jones%null%1,           Kevin A.%Brown%null%1,           Paula A.%Rochon%null%1,           Andrew P.%Costa%null%1,          Nathan M.%Stall%null%1,          Aaron%Jones%null%1,          Kevin A.%Brown%null%1,          Paula A.%Rochon%null%1,          Andrew P.%Costa%null%1]</t>
+  </si>
+  <si>
+    <t>[Hubert%Blain%NULL%1,          Yves%Rolland%NULL%1,          Edouard%Tuaillon%NULL%1,          Nadia%Giacosa%NULL%1,          Mylène%Albrand%NULL%1,          Audrey%Jaussent%NULL%1,          Athanase%Benetos%NULL%1,          Stéphanie%Miot%NULL%1,          Jean%Bousquet%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Guillaume%Sacco%NULL%1,          Gonzague%Foucault%NULL%1,          Olivier%Briere%NULL%1,          Cédric%Annweiler%NULL%1]</t>
+  </si>
+  <si>
+    <t>[R.%Guery%NULL%1,          C.%Delaye%NULL%1,          N.%Brule%NULL%1,          V.%Nael%NULL%1,          L.%Castain%NULL%1,          F.%Raffi%NULL%1,          L.%De Decker%NULL%1]</t>
+  </si>
+  <si>
+    <t>[A.%Klein%anke.klein@uke.de%1,          C.%Edler%NULL%1,          A.%Fitzek%NULL%1,          D.%Fröb%NULL%1,          A.%Heinemann%NULL%1,          K.%Meißner%NULL%1,          H.%Mushumba%NULL%1,          K.%Püschel%NULL%1,          A. S.%Schröder%NULL%1,          J. P.%Sperhake%NULL%1,          F.%Ishorst-Witte%NULL%1,          M.%Aepfelbacher%NULL%1,          F.%Heinrich%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Buntinx%Frank%coreGivesNoEmail%1,        Claes%Peter%coreGivesNoEmail%1,        Gulikers%Marjo%coreGivesNoEmail%1,        Jan%De Lepeleire%coreGivesNoEmail%1,        Van%der Elst Michael%coreGivesNoEmail%1,        Van%Elslande Jan%coreGivesNoEmail%1,        Van%Ranst Marc%coreGivesNoEmail%1,        Verbakel%Jan%coreGivesNoEmail%1,        Vernneersch%Pieter%coreGivesNoEmail%1]</t>
+  </si>
+  <si>
+    <t>[Liangcong%Hu%xref no email%1,    Wanyuan%Zhen%xref no email%1,    Xudong%Xie%xref no email%2,    Ze%Lin%xref no email%2,    Tiantian%Wang%xref no email%1,    Jing%Liu%xref no email%5,    Hang%Xue%xref no email%2,    Adriana C.%Panayi%xref no email%2,    Ke%Xu%xref no email%1,    Zexi%Ling%xref no email%1,    Xugui%Li%xref no email%1,    Bobin%Mi%xref no email%1,    Wu%Zhou%xref no email%2,    Guohui%Liu%xref no email%2]</t>
+  </si>
+  <si>
+    <t>[Sean P%Kennelly%Sean.Kennelly@tuh.ie%1,          Adam H%Dyer%dyera@tcd.ie%1,          Claire%Noonan%claire.noonan@tuh.ie%2,          Claire%Noonan%claire.noonan@tuh.ie%0,          Ruth%Martin%ruth.martin1@hse.ie%1,          Siobhan M%Kennelly%siobhan.kennelly1@hse.ie%1,          Alan%Martin%alanmartin@beaumont.ie%1,          Desmond%O’Neill%NULL%1,          Aoife%Fallon%aoife.fallon1@hotmail.com%1]</t>
+  </si>
+  <si>
+    <t>[Antonio%Nouvenne%NULL%1,          Andrea%Ticinesi%NULL%1,          Alberto%Parise%NULL%1,          Beatrice%Prati%NULL%1,          Marcello%Esposito%NULL%1,          Valentina%Cocchi%NULL%1,          Emanuele%Crisafulli%NULL%1,          Annalisa%Volpi%NULL%1,          Sandra%Rossi%NULL%1,          Elena Giovanna%Bignami%NULL%1,          Marco%Baciarello%NULL%1,          Ettore%Brianti%NULL%1,          Massimo%Fabi%NULL%1,          Tiziana%Meschi%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Nicola%Veronese%NULL%1,          Luca Gino%Sbrogiò%NULL%1,          Roberto%Valle%NULL%1,          Laura%Marin%NULL%1,          Elena%Boscolo Fiore%NULL%1,          Andrea%Tiozzo%NULL%1]</t>
+  </si>
+  <si>
+    <t>[ J. H.%van den Besselaar%null%1,           R. S.% Sikkema%null%1,           F. M. H. P. A.% Koene%null%1,           L. W.% van Buul%null%1,           B. B.% Oude Munnink%null%1,           I.% Frenay%null%1,           R.% te Witt%null%1,           M. P. G.% Koopmans%null%1,           C. M. P. M.% Hertogh%null%1,           B. M. % Buurman%null%1]</t>
+  </si>
+  <si>
+    <t>[Laura W.%van Buul%NULL%1,          Judith H.%van den Besselaar%NULL%2,          Judith H.%van den Besselaar%NULL%0,          Fleur M. H. P. H.%Koene%NULL%1,          Bianca M.%Buurman%NULL%1,          Cees M. P. M.%Hertogh%NULL%1,          Martin%Smalbrugge%NULL%1,          Jeanine J. S.%Rutten%NULL%1,          Elke M.%den Boogert%NULL%1,          Michel D.%Wissing%NULL%1,          Ariene%Rietveld%NULL%1,          Mariska W. W.%van Elsakker%NULL%1,          Marga M. G.%Nonneman%NULL%1,          Florien%van Eeden%NULL%1,          Saskia%van de Merwe%NULL%1,          Sophie L.%Niemansburg%NULL%1,          Ewout%Fanoy%NULL%1,          Hinke S.%Bootsma%NULL%1,          Nicoline%van der Hagen%NULL%1,          Mariska%Petrignani%NULL%1,          Jessica Edwards%van Muijen%NULL%1,          Karolien E. M.%Biesheuvel%NULL%1]</t>
+  </si>
+  <si>
+    <t>[B\u00e5rd%Reiakvam Kittang%coreGivesNoEmail%1,        Karina%Koller L\u00f8land%coreGivesNoEmail%1,        Kjell%Kr\u00fcger%coreGivesNoEmail%1,        Kristian%Jansen%coreGivesNoEmail%1,        Sabine%Piepenstock Solheim%coreGivesNoEmail%1,        Sebastian%von Hofacker%coreGivesNoEmail%1]</t>
+  </si>
+  <si>
+    <t>[Shin Young%Park%NULL%1,          Gawon%Choi%NULL%2,          Gawon%Choi%NULL%0,          Hyeyoung%Lee%NULL%2,          Hyeyoung%Lee%NULL%0,          Na-young%Kim%NULL%2,          Na-young%Kim%NULL%0,          Seon-young%Lee%NULL%2,          Seon-young%Lee%NULL%0,          Kyungnam%Kim%NULL%2,          Kyungnam%Kim%NULL%0,          Soyoung%Shin%NULL%2,          Soyoung%Shin%NULL%0,          Eunsu%Jang%NULL%2,          Eunsu%Jang%NULL%0,          YoungSin%Moon%NULL%2,          YoungSin%Moon%NULL%0,          KwangHwan%Oh%NULL%2,          KwangHwan%Oh%NULL%0,          JaeRin%Choi%NULL%2,          JaeRin%Choi%NULL%0,          Sangeun%Lee%NULL%2,          Sangeun%Lee%NULL%0,          Young-Man%Kim%NULL%2,          Young-Man%Kim%NULL%0,          Jieun%Kim%NULL%2,          Jieun%Kim%NULL%0,          Seonju%Yi%NULL%2,          Seonju%Yi%NULL%0,          Jin%Gwack%NULL%2,          Jin%Gwack%NULL%0,          Ok%Park%NULL%2,          Ok%Park%NULL%0,          Young Joon%Park%NULL%2,          Young Joon%Park%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Rok%Song%NULL%1,          Hee-Sook%Kim%NULL%2,          Hee-Sook%Kim%NULL%0,          Seok-Ju%Yoo%NULL%2,          Seok-Ju%Yoo%NULL%0,          Kwan%Lee%NULL%2,          Kwan%Lee%NULL%0,          Ji-Hyuk%Park%NULL%2,          Ji-Hyuk%Park%NULL%0,          Joon Ho%Jang%NULL%2,          Joon Ho%Jang%NULL%0,          Gyoung-Sook%Ahn%NULL%2,          Gyoung-Sook%Ahn%NULL%0,          Jun-Nyun%Kim%NULL%2,          Jun-Nyun%Kim%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Blanca%Borras-Bermejo%NULL%1,          Xavier%Martínez-Gómez%NULL%1,          María Gutierrez%San Miguel%NULL%1,          Juliana%Esperalba%NULL%1,          Andrés%Antón%NULL%1,          Elisabet%Martin%NULL%1,          Marta%Selvi%NULL%1,          María José%Abadías%NULL%1,          Antonio%Román%NULL%1,          Tomàs%Pumarola%NULL%1,          Magda%Campins%NULL%1,          Benito%Almirante%NULL%1]</t>
+  </si>
+  <si>
+    <t>[M.%Bernabeu-Wittel%NULL%1,          J.E.%Ternero-Vega%NULL%1,          P.%Díaz-Jiménez%NULL%1,          C.%Conde-Guzmán%NULL%1,          M.D.%Nieto-Martín%NULL%1,          L.%Moreno-Gaviño%NULL%1,          J.%Delgado-Cuesta%NULL%1,          M.%Rincón-Gómez%NULL%1,          L.%Giménez-Miranda%NULL%1,          M.D.%Navarro-Amuedo%NULL%1,          M.M.%Muñoz-García%NULL%1,          S.%Calzón-Fernández%NULL%1,          M.%Ollero-Baturone%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Shamez N%Ladhani%shamez.ladhani@phe.gov.uk%1,          J.Yimmy%Chow%NULL%1,          Roshni%Janarthanan%NULL%1,          Jonathan%Fok%NULL%1,          Emma%Crawley-Boevey%NULL%1,          Amoolya%Vusirikala%NULL%1,          Elena%Fernandez%NULL%1,          Marina Sanchez%Perez%NULL%1,          Suzanne%Tang%NULL%1,          Kate%Dun-Campbell%NULL%1,          Edward Wynne-%Evans%NULL%1,          Anita%Bell%NULL%1,          Bharat%Patel%NULL%1,          Zahin%Amin-Chowdhury%NULL%1,          Felicity%Aiano%NULL%1,          Karthik%Paranthaman%NULL%1,          Thomas%Ma%NULL%1,          Maria%Saavedra-Campos%NULL%1,          Richard%Myers%NULL%1,          Joanna%Ellis%NULL%2,          Angie%Lackenby%NULL%1,          Robin%Gopal%NULL%1,          Monika%Patel%NULL%1,          Colin%Brown%NULL%1,          Meera%Chand%NULL%1,          Kevin%Brown%NULL%1,          Mary E%Ramsay%NULL%1,          Susan%Hopkins%NULL%2,          Nandini%Shetty%NULL%1,          Maria%Zambon%NULL%2]</t>
+  </si>
+  <si>
+    <t>[N.S.N.%Graham%NULL%1,          C.%Junghans%NULL%1,          R.%Downes%NULL%1,          C.%Sendall%NULL%1,          H.%Lai%NULL%1,          A.%McKirdy%NULL%1,          P.%Elliott%NULL%1,          R.%Howard%NULL%1,          D.%Wingfield%NULL%1,          M.%Priestman%NULL%1,          M.%Ciechonska%NULL%1,          L.%Cameron%NULL%1,          M.%Storch%NULL%1,          M.A.%Crone%NULL%1,          P.S.%Freemont%NULL%1,          P.%Randell%NULL%1,          R.%McLaren%NULL%1,          N.%Lang%NULL%1,          S.%Ladhani%NULL%1,          F.%Sanderson%NULL%1,          D.J.%Sharp%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Agnes%Marossy%agnesmarossy@nhs.net%1,          Stefan%Rakowicz%NULL%1,          Angela%Bhan%NULL%1,          Sarah%Noon%NULL%1,          Amanda%Rees%NULL%1,          Manjinder%Virk%NULL%1,          Ayazali%Nazafi%NULL%1,          Evie%Hay%NULL%1,          Louise%de Thomasson%NULL%1,          Christina%Windle%NULL%1,          Mark%Zuckerman%Mark.Zuckerman@nhs.net%1]</t>
+  </si>
+  <si>
+    <t>[Laura%Shallcross%NULL%1,          Danielle%Burke%NULL%1,          Owen%Abbott%NULL%1,          Alasdair%Donaldson%NULL%1,          Gemma%Hallatt%NULL%1,          Andrew%Hayward%NULL%1,          Susan%Hopkins%NULL%0,          Maria%Krutikov%NULL%1,          Katie%Sharp%NULL%1,          Leone%Wardman%NULL%1,          Sapphira%Thorne%NULL%1]</t>
+  </si>
+  <si>
+    <t>[ E.%Smith%null%1,           C. F.% Aldus%null%1,           J.% Brainard%null%1,           S.% Dunham%null%1,           P. R.% Hunter%null%1,           N.% Steel%null%1,           P. % Everden%null%1]</t>
+  </si>
+  <si>
+    <t>[Mahesh C%Patel%mp3@uic.edu%1,          Lelia H%Chaisson%NULL%1,          Scott%Borgetti%NULL%1,          Deborah%Burdsall%NULL%1,          Rashmi K%Chugh%NULL%1,          Christopher R%Hoff%NULL%1,          Elizabeth B%Murphy%NULL%1,          Emily A%Murskyj%NULL%1,          Shannon%Wilson%NULL%1,          Joe%Ramos%NULL%1,          Lynn%Akker%NULL%1,          Debra%Bryars%NULL%1,          Evonda%Thomas-Smith%NULL%1,          Susan C%Bleasdale%NULL%1,          Ngozi O%Ezike%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Helena%Temkin‐Greener%helena_temkin-greener@urmc.rochester.edu%1,          Wenhan%Guo%NULL%2,          Wenhan%Guo%NULL%0,          Yunjiao%Mao%NULL%1,          Xueya%Cai%NULL%1,          Yue%Li%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Ana A.%Weil%anaweil@uw.edu%1,          Kira L.%Newman%NULL%2,          Kira L.%Newman%NULL%0,          Thuan D.%Ong%NULL%1,          Giana H.%Davidson%NULL%1,          Jennifer%Logue%NULL%1,          Elisabeth%Brandstetter%NULL%1,          Ariana%Magedson%NULL%1,          Dylan%McDonald%NULL%1,          Denise J.%McCulloch%NULL%1,          Santiago%Neme%NULL%1,          James%Lewis%NULL%0,          Jeff S.%Duchin%NULL%1,          Weizhi%Zhong%NULL%1,          Lea M.%Starita%NULL%1,          Trevor%Bedford%NULL%1,          Alison C.%Roxby%NULL%1,          Helen Y.%Chu%helenchu@uw.edu%2]</t>
+  </si>
+  <si>
+    <t>[Guillermo V.%Sanchez%NULL%1,          Caitlin%Biedron%NULL%1,          Lauren R.%Fink%NULL%1,          Kelly M.%Hatfield%NULL%1,          Jordan Micah F.%Polistico%NULL%1,          Monica P.%Meyer%NULL%1,          Rebecca S.%Noe%NULL%1,          Casey E.%Copen%NULL%1,          Amanda K.%Lyons%NULL%1,          Gonzalo%Gonzalez%NULL%1,          Keith%Kiama%NULL%1,          Mark%Lebednick%NULL%1,          Bonnie K.%Czander%NULL%1,          Amen%Agbonze%NULL%1,          Aimee R.%Surma%NULL%1,          Avnish%Sandhu%NULL%1,          Valerie H.%Mika%NULL%1,          Tyler%Prentiss%NULL%1,          John%Zervos%NULL%1,          Donia A.%Dalal%NULL%1,          Amber M.%Vasquez%NULL%1,          Sujan C.%Reddy%NULL%0,          John%Jernigan%NULL%1,          Paul E.%Kilgore%NULL%1,          Marcus J.%Zervos%NULL%1,          Teena%Chopra%NULL%1,          Carla P.%Bezold%NULL%1,          Najibah K.%Rehman%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Janice K%Louie%Janice.louie@sfdph.org%1,          Hyman M%Scott%NULL%1,          Amie%DuBois%NULL%1,          Natalya%Sturtz%NULL%1,          Wendy%Lu%NULL%1,          Juliet%Stoltey%NULL%1,          Godfred%Masinde%NULL%1,          Stephanie%Cohen%NULL%1,          Darpun%Sachdev%NULL%1,          Susan%Philip%NULL%1,          Naveena%Bobba%NULL%1,          Tomas%Aragon%NULL%1,          NULL%NULL%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Scott A%Goldberg%sagoldberg@bwh.harvard.edu%1,          Jochen%Lennerz%NULL%1,          Michael%Klompas%NULL%1,          Eden%Mark%NULL%1,          Virginia M%Pierce%NULL%1,          Ryan W%Thompson%NULL%1,          Charles T%Pu%NULL%1,          Lauren L%Ritterhouse%NULL%1,          Anand%Dighe%NULL%1,          Eric S%Rosenberg%NULL%1,          David C%Grabowski%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Amy V.%Dora%NULL%1,          Alexander%Winnett%NULL%1,          Lauren P.%Jatt%NULL%1,          Kusha%Davar%NULL%1,          Mika%Watanabe%NULL%1,          Linda%Sohn%NULL%1,          Hannah S.%Kern%NULL%1,          Christopher J.%Graber%NULL%1,          Matthew B.%Goetz%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Benjamin F.%Bigelow%NULL%1,          Olive%Tang%NULL%1,          Gregory R.%Toci%NULL%1,          Norberth%Stracker%NULL%1,          Fatima%Sheikh%NULL%1,          Kara M.%Jacobs Slifka%NULL%1,          Shannon A.%Novosad%NULL%1,          John A.%Jernigan%NULL%0,          Sujan C.%Reddy%NULL%0,          Morgan J.%Katz%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Matt%Feaster%NULL%1,          Ying-Ying%Goh%NULL%1]</t>
+  </si>
+  <si>
+    <t>[William R.%Mills%NULL%1,          Janet M.%Buccola%NULL%1,          Susan%Sender%NULL%1,          Joseph%Lichtefeld%NULL%1,          Nicholas%Romano%NULL%1,          Karen%Reynolds%NULL%1,          Melissa%Price%NULL%1,          Jennifer%Phipps%NULL%1,          Leigh%White%NULL%1,          Shauen%Howard%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Drew A.%Harris%xref no email%1,    Laurie%Archbald-Pannone%xref no email%1,    Jasveen%Kaur%xref no email%1,    David%Cattell-Gordon%xref no email%1,    Karen S.%Rheuban%xref no email%1,    Rachel L.%Ombres%xref no email%1,    Kimberly%Albero%xref no email%1,    Rebecca%Steele%xref no email%1,    Taison D.%Bell%xref no email%1,    Justin B.%Mutter%xref no email%1]</t>
+  </si>
+  <si>
+    <t>[Carl D.%Shrader%xref no email%1,    Shauna%Assadzandi%xref no email%1,    Courtney S.%Pilkerton%xref no email%1,    Amie M.%Ashcraft%xref no email%1]</t>
   </si>
 </sst>
 </file>
@@ -2261,7 +2507,7 @@
         <v>60</v>
       </c>
       <c r="E2" t="s">
-        <v>469</v>
+        <v>551</v>
       </c>
       <c r="F2" t="s">
         <v>62</v>
@@ -2290,7 +2536,7 @@
         <v>66</v>
       </c>
       <c r="E3" t="s">
-        <v>470</v>
+        <v>552</v>
       </c>
       <c r="F3" t="s">
         <v>68</v>
@@ -2319,7 +2565,7 @@
         <v>70</v>
       </c>
       <c r="E4" t="s">
-        <v>471</v>
+        <v>553</v>
       </c>
       <c r="F4" t="s">
         <v>72</v>
@@ -2377,7 +2623,7 @@
         <v>74</v>
       </c>
       <c r="E6" t="s">
-        <v>472</v>
+        <v>554</v>
       </c>
       <c r="F6" t="s">
         <v>6</v>
@@ -2406,7 +2652,7 @@
         <v>79</v>
       </c>
       <c r="E7" t="s">
-        <v>473</v>
+        <v>555</v>
       </c>
       <c r="F7" t="s">
         <v>81</v>
@@ -2435,7 +2681,7 @@
         <v>83</v>
       </c>
       <c r="E8" t="s">
-        <v>474</v>
+        <v>556</v>
       </c>
       <c r="F8" t="s">
         <v>85</v>
@@ -2493,7 +2739,7 @@
         <v>87</v>
       </c>
       <c r="E10" t="s">
-        <v>475</v>
+        <v>557</v>
       </c>
       <c r="F10" t="s">
         <v>89</v>
@@ -2522,7 +2768,7 @@
         <v>92</v>
       </c>
       <c r="E11" t="s">
-        <v>476</v>
+        <v>558</v>
       </c>
       <c r="F11" t="s">
         <v>94</v>
@@ -2551,7 +2797,7 @@
         <v>98</v>
       </c>
       <c r="E12" t="s">
-        <v>477</v>
+        <v>559</v>
       </c>
       <c r="F12" t="s">
         <v>100</v>
@@ -2609,7 +2855,7 @@
         <v>102</v>
       </c>
       <c r="E14" t="s">
-        <v>478</v>
+        <v>560</v>
       </c>
       <c r="F14" t="s">
         <v>104</v>
@@ -2638,7 +2884,7 @@
         <v>107</v>
       </c>
       <c r="E15" t="s">
-        <v>479</v>
+        <v>561</v>
       </c>
       <c r="F15" t="s">
         <v>109</v>
@@ -2667,7 +2913,7 @@
         <v>112</v>
       </c>
       <c r="E16" t="s">
-        <v>480</v>
+        <v>562</v>
       </c>
       <c r="F16" t="s">
         <v>114</v>
@@ -2696,7 +2942,7 @@
         <v>277</v>
       </c>
       <c r="E17" t="s">
-        <v>481</v>
+        <v>563</v>
       </c>
       <c r="F17" t="s">
         <v>17</v>
@@ -2754,7 +3000,7 @@
         <v>52</v>
       </c>
       <c r="E19" t="s">
-        <v>482</v>
+        <v>564</v>
       </c>
       <c r="F19" t="s">
         <v>19</v>
@@ -2783,7 +3029,7 @@
         <v>119</v>
       </c>
       <c r="E20" t="s">
-        <v>483</v>
+        <v>565</v>
       </c>
       <c r="F20" t="s">
         <v>121</v>
@@ -2812,7 +3058,7 @@
         <v>124</v>
       </c>
       <c r="E21" t="s">
-        <v>484</v>
+        <v>566</v>
       </c>
       <c r="F21" t="s">
         <v>126</v>
@@ -2841,7 +3087,7 @@
         <v>128</v>
       </c>
       <c r="E22" t="s">
-        <v>485</v>
+        <v>567</v>
       </c>
       <c r="F22" t="s">
         <v>130</v>
@@ -2899,7 +3145,7 @@
         <v>132</v>
       </c>
       <c r="E24" t="s">
-        <v>486</v>
+        <v>568</v>
       </c>
       <c r="F24" t="s">
         <v>56</v>
@@ -2928,7 +3174,7 @@
         <v>136</v>
       </c>
       <c r="E25" t="s">
-        <v>487</v>
+        <v>569</v>
       </c>
       <c r="F25" t="s">
         <v>138</v>
@@ -2957,7 +3203,7 @@
         <v>52</v>
       </c>
       <c r="E26" t="s">
-        <v>488</v>
+        <v>570</v>
       </c>
       <c r="F26" t="s">
         <v>26</v>
@@ -2986,7 +3232,7 @@
         <v>141</v>
       </c>
       <c r="E27" t="s">
-        <v>489</v>
+        <v>571</v>
       </c>
       <c r="F27" t="s">
         <v>143</v>
@@ -3015,7 +3261,7 @@
         <v>146</v>
       </c>
       <c r="E28" t="s">
-        <v>490</v>
+        <v>572</v>
       </c>
       <c r="F28" t="s">
         <v>148</v>
@@ -3044,7 +3290,7 @@
         <v>151</v>
       </c>
       <c r="E29" t="s">
-        <v>491</v>
+        <v>573</v>
       </c>
       <c r="F29" t="s">
         <v>153</v>
@@ -3073,7 +3319,7 @@
         <v>107</v>
       </c>
       <c r="E30" t="s">
-        <v>492</v>
+        <v>574</v>
       </c>
       <c r="F30" t="s">
         <v>156</v>
@@ -3102,7 +3348,7 @@
         <v>159</v>
       </c>
       <c r="E31" t="s">
-        <v>493</v>
+        <v>575</v>
       </c>
       <c r="F31" t="s">
         <v>161</v>
@@ -3131,7 +3377,7 @@
         <v>164</v>
       </c>
       <c r="E32" t="s">
-        <v>494</v>
+        <v>576</v>
       </c>
       <c r="F32" t="s">
         <v>166</v>
@@ -3160,7 +3406,7 @@
         <v>169</v>
       </c>
       <c r="E33" t="s">
-        <v>495</v>
+        <v>577</v>
       </c>
       <c r="F33" t="s">
         <v>171</v>
@@ -3189,7 +3435,7 @@
         <v>173</v>
       </c>
       <c r="E34" t="s">
-        <v>496</v>
+        <v>578</v>
       </c>
       <c r="F34" t="s">
         <v>175</v>
@@ -3218,7 +3464,7 @@
         <v>177</v>
       </c>
       <c r="E35" t="s">
-        <v>497</v>
+        <v>579</v>
       </c>
       <c r="F35" t="s">
         <v>56</v>
@@ -3247,7 +3493,7 @@
         <v>181</v>
       </c>
       <c r="E36" t="s">
-        <v>498</v>
+        <v>580</v>
       </c>
       <c r="F36" t="s">
         <v>183</v>
@@ -3276,7 +3522,7 @@
         <v>186</v>
       </c>
       <c r="E37" t="s">
-        <v>499</v>
+        <v>581</v>
       </c>
       <c r="F37" t="s">
         <v>188</v>
@@ -3305,7 +3551,7 @@
         <v>191</v>
       </c>
       <c r="E38" t="s">
-        <v>500</v>
+        <v>582</v>
       </c>
       <c r="F38" t="s">
         <v>193</v>
@@ -3334,7 +3580,7 @@
         <v>107</v>
       </c>
       <c r="E39" t="s">
-        <v>501</v>
+        <v>583</v>
       </c>
       <c r="F39" t="s">
         <v>197</v>
@@ -3363,7 +3609,7 @@
         <v>199</v>
       </c>
       <c r="E40" t="s">
-        <v>502</v>
+        <v>584</v>
       </c>
       <c r="F40" t="s">
         <v>201</v>
@@ -3392,7 +3638,7 @@
         <v>203</v>
       </c>
       <c r="E41" t="s">
-        <v>503</v>
+        <v>585</v>
       </c>
       <c r="F41" t="s">
         <v>205</v>
@@ -3421,7 +3667,7 @@
         <v>107</v>
       </c>
       <c r="E42" t="s">
-        <v>504</v>
+        <v>586</v>
       </c>
       <c r="F42" t="s">
         <v>208</v>
@@ -3450,7 +3696,7 @@
         <v>107</v>
       </c>
       <c r="E43" t="s">
-        <v>505</v>
+        <v>587</v>
       </c>
       <c r="F43" t="s">
         <v>211</v>
@@ -3479,7 +3725,7 @@
         <v>213</v>
       </c>
       <c r="E44" t="s">
-        <v>506</v>
+        <v>588</v>
       </c>
       <c r="F44" t="s">
         <v>215</v>
@@ -3508,7 +3754,7 @@
         <v>217</v>
       </c>
       <c r="E45" t="s">
-        <v>507</v>
+        <v>589</v>
       </c>
       <c r="F45" t="s">
         <v>219</v>
@@ -3537,7 +3783,7 @@
         <v>52</v>
       </c>
       <c r="E46" t="s">
-        <v>508</v>
+        <v>590</v>
       </c>
       <c r="F46" t="s">
         <v>46</v>
@@ -3566,7 +3812,7 @@
         <v>466</v>
       </c>
       <c r="E47" t="s">
-        <v>509</v>
+        <v>591</v>
       </c>
       <c r="F47" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
Cleaning more data. Fixed an issue where some files were displaying incorrect info.
</commit_message>
<xml_diff>
--- a/Covid_19_Dataset_and_References/References/10.xlsx
+++ b/Covid_19_Dataset_and_References/References/10.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1036" uniqueCount="326">
   <si>
     <t>Doi</t>
   </si>
@@ -1243,6 +1243,129 @@
   </si>
   <si>
     <t>[Carl D.%Shrader%xref no email%1,       Shauna%Assadzandi%xref no email%1,       Courtney S.%Pilkerton%xref no email%1,       Amie M.%Ashcraft%xref no email%1]</t>
+  </si>
+  <si>
+    <t>[Daniel J%Escobar%Daniel.escobar@pennmedicine.upenn.edu%1,              Maria%Lanzi%NULL%1,              Pouné%Saberi%NULL%1,              Ruby%Love%NULL%1,              Darren R%Linkin%NULL%1,              John J%Kelly%NULL%1,              Darshana%Jhala%NULL%1,              Valerianna%Amorosa%NULL%1,              Mary%Hofmann%NULL%1,              Jeffrey B%Doyon%NULL%1]</t>
+  </si>
+  <si>
+    <t>[James L.%Rudolph%NULL%1,              Christopher W.%Halladay%NULL%1,              Malisa%Barber%NULL%1,              Kevin W.%McConeghy%NULL%1,              Vince%Mor%NULL%1,              Aman%Nanda%NULL%1,              Stefan%Gravenstein%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Paula%Eckardt%NULL%1,              Rachel%Guran%NULL%1,              Jon%Hennemyre%NULL%1,              Roshan%Arikupurathu%NULL%1,              Julie%Poveda%NULL%1,              Nancimae%Miller%NULL%1,              Randy%Katz%NULL%1,              Judith%Frum%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Carson%Telford%NULL%1,              Udodirim%Onwubiko%NULL%1,              David%Holland%NULL%1,              Kim%Turner%NULL%1,              Juliana%Prieto%NULL%1,              Sasha%Smith%NULL%1,              Jane%Yoon%NULL%1,              Wecheeta%Brown%NULL%1,              Allison%Chamberlain%NULL%1,              Neel%Gandhi%NULL%1,              Shamimul%Khan%NULL%1,              Steve%Williams%NULL%1,              Fazle%Khan%NULL%1,              Sarita%Shah%NULL%1,               C. T.%Telford%null%1,               U.% Onwubiko%null%1,               D.% Holland%null%1,               K.% Turner%null%1,               J.% Prieto%null%1,               S.% Smith%null%1,               J.% Yoon%null%1,               W.% Brown%null%1,               A.% Chamberlain%null%1,               N.% Gandhi%null%1,               S.% Khan%null%1,               S.% Williams%null%1,               F.% Khan%null%1,               S. % Shah%null%1,              C. T.%Telford%null%1,              U.% Onwubiko%null%1,              D.% Holland%null%1,              K.% Turner%null%1,              J.% Prieto%null%1,              S.% Smith%null%1,              J.% Yoon%null%1,              W.% Brown%null%1,              A.% Chamberlain%null%1,              N.% Gandhi%null%1,              S.% Khan%null%1,              S.% Williams%null%1,              F.% Khan%null%1,              S. % Shah%null%1]</t>
+  </si>
+  <si>
+    <t>[Sandra M.%Shi%NULL%1,              Innokentiy%Bakaev%NULL%1,              Helen%Chen%NULL%1,              Thomas G.%Travison%NULL%1,              Sarah D.%Berry%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Temet M.%McMichael%NULL%0,              Dustin W.%Currie%NULL%0,              Shauna%Clark%NULL%0,              Sargis%Pogosjans%NULL%0,              Meagan%Kay%NULL%0,              Noah G.%Schwartz%NULL%0,              James%Lewis%NULL%0,              Atar%Baer%NULL%0,              Vance%Kawakami%NULL%0,              Margaret D.%Lukoff%NULL%0,              Jessica%Ferro%NULL%0,              Claire%Brostrom-Smith%NULL%0,              Thomas D.%Rea%NULL%1,              Michael R.%Sayre%NULL%1,              Francis X.%Riedo%NULL%0,              Denny%Russell%NULL%0,              Brian%Hiatt%NULL%0,              Patricia%Montgomery%NULL%0,              Agam K.%Rao%NULL%0,              Eric J.%Chow%NULL%0,              Farrell%Tobolowsky%NULL%0,              Michael J.%Hughes%NULL%1,              Ana C.%Bardossy%NULL%0,              Lisa P.%Oakley%NULL%0,              Jesica R.%Jacobs%NULL%0,              Nimalie D.%Stone%NULL%1,              Sujan C.%Reddy%NULL%0,              John A.%Jernigan%NULL%0,              Margaret A.%Honein%NULL%0,              Thomas A.%Clark%NULL%0,              Jeffrey S.%Duchin%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Nathan M.%Stall%nathan.stall@sinaihealth.ca%1,              Carolyn%Farquharson%NULL%2,              Carolyn%Farquharson%NULL%0,              Chris%Fan‐Lun%NULL%1,              Lesley%Wiesenfeld%NULL%1,              Carla A.%Loftus%NULL%1,              Dylan%Kain%NULL%1,              Jennie%Johnstone%NULL%1,              Liz%McCreight%NULL%1,              Russell D.%Goldman%NULL%1,              Ramona%Mahtani%NULL%1]</t>
+  </si>
+  <si>
+    <t>[ Nathan M.%Stall%null%1,               Aaron%Jones%null%1,               Kevin A.%Brown%null%1,               Paula A.%Rochon%null%1,               Andrew P.%Costa%null%1,              Nathan M.%Stall%null%1,              Aaron%Jones%null%1,              Kevin A.%Brown%null%1,              Paula A.%Rochon%null%1,              Andrew P.%Costa%null%1]</t>
+  </si>
+  <si>
+    <t>[Hubert%Blain%NULL%1,              Yves%Rolland%NULL%1,              Edouard%Tuaillon%NULL%1,              Nadia%Giacosa%NULL%1,              Mylène%Albrand%NULL%1,              Audrey%Jaussent%NULL%1,              Athanase%Benetos%NULL%1,              Stéphanie%Miot%NULL%1,              Jean%Bousquet%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Guillaume%Sacco%NULL%1,              Gonzague%Foucault%NULL%1,              Olivier%Briere%NULL%1,              Cédric%Annweiler%NULL%1]</t>
+  </si>
+  <si>
+    <t>[R.%Guery%NULL%1,              C.%Delaye%NULL%1,              N.%Brule%NULL%1,              V.%Nael%NULL%1,              L.%Castain%NULL%1,              F.%Raffi%NULL%1,              L.%De Decker%NULL%1]</t>
+  </si>
+  <si>
+    <t>[A.%Klein%anke.klein@uke.de%1,              C.%Edler%NULL%1,              A.%Fitzek%NULL%1,              D.%Fröb%NULL%1,              A.%Heinemann%NULL%1,              K.%Meißner%NULL%1,              H.%Mushumba%NULL%1,              K.%Püschel%NULL%1,              A. S.%Schröder%NULL%1,              J. P.%Sperhake%NULL%1,              F.%Ishorst-Witte%NULL%1,              M.%Aepfelbacher%NULL%1,              F.%Heinrich%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Buntinx%Frank%coreGivesNoEmail%1,            Claes%Peter%coreGivesNoEmail%1,            Gulikers%Marjo%coreGivesNoEmail%1,            Jan%De Lepeleire%coreGivesNoEmail%1,            Van%der Elst Michael%coreGivesNoEmail%1,            Van%Elslande Jan%coreGivesNoEmail%1,            Van%Ranst Marc%coreGivesNoEmail%1,            Verbakel%Jan%coreGivesNoEmail%1,            Vernneersch%Pieter%coreGivesNoEmail%1]</t>
+  </si>
+  <si>
+    <t>[Liangcong%Hu%xref no email%1,        Wanyuan%Zhen%xref no email%1,        Xudong%Xie%xref no email%2,        Ze%Lin%xref no email%2,        Tiantian%Wang%xref no email%1,        Jing%Liu%xref no email%5,        Hang%Xue%xref no email%2,        Adriana C.%Panayi%xref no email%2,        Ke%Xu%xref no email%1,        Zexi%Ling%xref no email%1,        Xugui%Li%xref no email%1,        Bobin%Mi%xref no email%1,        Wu%Zhou%xref no email%2,        Guohui%Liu%xref no email%2]</t>
+  </si>
+  <si>
+    <t>[Sean P%Kennelly%Sean.Kennelly@tuh.ie%1,              Adam H%Dyer%dyera@tcd.ie%1,              Claire%Noonan%claire.noonan@tuh.ie%2,              Claire%Noonan%claire.noonan@tuh.ie%0,              Ruth%Martin%ruth.martin1@hse.ie%1,              Siobhan M%Kennelly%siobhan.kennelly1@hse.ie%1,              Alan%Martin%alanmartin@beaumont.ie%1,              Desmond%O’Neill%NULL%1,              Aoife%Fallon%aoife.fallon1@hotmail.com%1]</t>
+  </si>
+  <si>
+    <t>[Antonio%Nouvenne%NULL%1,              Andrea%Ticinesi%NULL%1,              Alberto%Parise%NULL%1,              Beatrice%Prati%NULL%1,              Marcello%Esposito%NULL%1,              Valentina%Cocchi%NULL%1,              Emanuele%Crisafulli%NULL%1,              Annalisa%Volpi%NULL%1,              Sandra%Rossi%NULL%1,              Elena Giovanna%Bignami%NULL%1,              Marco%Baciarello%NULL%1,              Ettore%Brianti%NULL%1,              Massimo%Fabi%NULL%1,              Tiziana%Meschi%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Nicola%Veronese%NULL%1,              Luca Gino%Sbrogiò%NULL%1,              Roberto%Valle%NULL%1,              Laura%Marin%NULL%1,              Elena%Boscolo Fiore%NULL%1,              Andrea%Tiozzo%NULL%1]</t>
+  </si>
+  <si>
+    <t>[ J. H.%van den Besselaar%null%1,               R. S.% Sikkema%null%1,               F. M. H. P. A.% Koene%null%1,               L. W.% van Buul%null%1,               B. B.% Oude Munnink%null%1,               I.% Frenay%null%1,               R.% te Witt%null%1,               M. P. G.% Koopmans%null%1,               C. M. P. M.% Hertogh%null%1,               B. M. % Buurman%null%1]</t>
+  </si>
+  <si>
+    <t>[Laura W.%van Buul%NULL%1,              Judith H.%van den Besselaar%NULL%2,              Judith H.%van den Besselaar%NULL%0,              Fleur M. H. P. H.%Koene%NULL%1,              Bianca M.%Buurman%NULL%1,              Cees M. P. M.%Hertogh%NULL%1,              Martin%Smalbrugge%NULL%1,              Jeanine J. S.%Rutten%NULL%1,              Elke M.%den Boogert%NULL%1,              Michel D.%Wissing%NULL%1,              Ariene%Rietveld%NULL%1,              Mariska W. W.%van Elsakker%NULL%1,              Marga M. G.%Nonneman%NULL%1,              Florien%van Eeden%NULL%1,              Saskia%van de Merwe%NULL%1,              Sophie L.%Niemansburg%NULL%1,              Ewout%Fanoy%NULL%1,              Hinke S.%Bootsma%NULL%1,              Nicoline%van der Hagen%NULL%1,              Mariska%Petrignani%NULL%1,              Jessica Edwards%van Muijen%NULL%1,              Karolien E. M.%Biesheuvel%NULL%1]</t>
+  </si>
+  <si>
+    <t>[B\u00e5rd%Reiakvam Kittang%coreGivesNoEmail%1,            Karina%Koller L\u00f8land%coreGivesNoEmail%1,            Kjell%Kr\u00fcger%coreGivesNoEmail%1,            Kristian%Jansen%coreGivesNoEmail%1,            Sabine%Piepenstock Solheim%coreGivesNoEmail%1,            Sebastian%von Hofacker%coreGivesNoEmail%1]</t>
+  </si>
+  <si>
+    <t>[Shin Young%Park%NULL%1,              Gawon%Choi%NULL%2,              Gawon%Choi%NULL%0,              Hyeyoung%Lee%NULL%2,              Hyeyoung%Lee%NULL%0,              Na-young%Kim%NULL%2,              Na-young%Kim%NULL%0,              Seon-young%Lee%NULL%2,              Seon-young%Lee%NULL%0,              Kyungnam%Kim%NULL%2,              Kyungnam%Kim%NULL%0,              Soyoung%Shin%NULL%2,              Soyoung%Shin%NULL%0,              Eunsu%Jang%NULL%2,              Eunsu%Jang%NULL%0,              YoungSin%Moon%NULL%2,              YoungSin%Moon%NULL%0,              KwangHwan%Oh%NULL%2,              KwangHwan%Oh%NULL%0,              JaeRin%Choi%NULL%2,              JaeRin%Choi%NULL%0,              Sangeun%Lee%NULL%2,              Sangeun%Lee%NULL%0,              Young-Man%Kim%NULL%2,              Young-Man%Kim%NULL%0,              Jieun%Kim%NULL%2,              Jieun%Kim%NULL%0,              Seonju%Yi%NULL%2,              Seonju%Yi%NULL%0,              Jin%Gwack%NULL%2,              Jin%Gwack%NULL%0,              Ok%Park%NULL%2,              Ok%Park%NULL%0,              Young Joon%Park%NULL%2,              Young Joon%Park%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Rok%Song%NULL%1,              Hee-Sook%Kim%NULL%2,              Hee-Sook%Kim%NULL%0,              Seok-Ju%Yoo%NULL%2,              Seok-Ju%Yoo%NULL%0,              Kwan%Lee%NULL%2,              Kwan%Lee%NULL%0,              Ji-Hyuk%Park%NULL%2,              Ji-Hyuk%Park%NULL%0,              Joon Ho%Jang%NULL%2,              Joon Ho%Jang%NULL%0,              Gyoung-Sook%Ahn%NULL%2,              Gyoung-Sook%Ahn%NULL%0,              Jun-Nyun%Kim%NULL%2,              Jun-Nyun%Kim%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Blanca%Borras-Bermejo%NULL%1,              Xavier%Martínez-Gómez%NULL%1,              María Gutierrez%San Miguel%NULL%1,              Juliana%Esperalba%NULL%1,              Andrés%Antón%NULL%1,              Elisabet%Martin%NULL%1,              Marta%Selvi%NULL%1,              María José%Abadías%NULL%1,              Antonio%Román%NULL%1,              Tomàs%Pumarola%NULL%1,              Magda%Campins%NULL%1,              Benito%Almirante%NULL%1]</t>
+  </si>
+  <si>
+    <t>[M.%Bernabeu-Wittel%NULL%1,              J.E.%Ternero-Vega%NULL%1,              P.%Díaz-Jiménez%NULL%1,              C.%Conde-Guzmán%NULL%1,              M.D.%Nieto-Martín%NULL%1,              L.%Moreno-Gaviño%NULL%1,              J.%Delgado-Cuesta%NULL%1,              M.%Rincón-Gómez%NULL%1,              L.%Giménez-Miranda%NULL%1,              M.D.%Navarro-Amuedo%NULL%1,              M.M.%Muñoz-García%NULL%1,              S.%Calzón-Fernández%NULL%1,              M.%Ollero-Baturone%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Shamez N%Ladhani%shamez.ladhani@phe.gov.uk%1,              J.Yimmy%Chow%NULL%1,              Roshni%Janarthanan%NULL%1,              Jonathan%Fok%NULL%1,              Emma%Crawley-Boevey%NULL%1,              Amoolya%Vusirikala%NULL%1,              Elena%Fernandez%NULL%1,              Marina Sanchez%Perez%NULL%1,              Suzanne%Tang%NULL%1,              Kate%Dun-Campbell%NULL%1,              Edward Wynne-%Evans%NULL%1,              Anita%Bell%NULL%1,              Bharat%Patel%NULL%1,              Zahin%Amin-Chowdhury%NULL%1,              Felicity%Aiano%NULL%1,              Karthik%Paranthaman%NULL%1,              Thomas%Ma%NULL%1,              Maria%Saavedra-Campos%NULL%1,              Richard%Myers%NULL%1,              Joanna%Ellis%NULL%2,              Angie%Lackenby%NULL%1,              Robin%Gopal%NULL%1,              Monika%Patel%NULL%1,              Colin%Brown%NULL%1,              Meera%Chand%NULL%1,              Kevin%Brown%NULL%1,              Mary E%Ramsay%NULL%1,              Susan%Hopkins%NULL%2,              Nandini%Shetty%NULL%1,              Maria%Zambon%NULL%2]</t>
+  </si>
+  <si>
+    <t>[N.S.N.%Graham%NULL%1,              C.%Junghans%NULL%1,              R.%Downes%NULL%1,              C.%Sendall%NULL%1,              H.%Lai%NULL%1,              A.%McKirdy%NULL%1,              P.%Elliott%NULL%1,              R.%Howard%NULL%1,              D.%Wingfield%NULL%1,              M.%Priestman%NULL%1,              M.%Ciechonska%NULL%1,              L.%Cameron%NULL%1,              M.%Storch%NULL%1,              M.A.%Crone%NULL%1,              P.S.%Freemont%NULL%1,              P.%Randell%NULL%1,              R.%McLaren%NULL%1,              N.%Lang%NULL%1,              S.%Ladhani%NULL%1,              F.%Sanderson%NULL%1,              D.J.%Sharp%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Agnes%Marossy%agnesmarossy@nhs.net%1,              Stefan%Rakowicz%NULL%1,              Angela%Bhan%NULL%1,              Sarah%Noon%NULL%1,              Amanda%Rees%NULL%1,              Manjinder%Virk%NULL%1,              Ayazali%Nazafi%NULL%1,              Evie%Hay%NULL%1,              Louise%de Thomasson%NULL%1,              Christina%Windle%NULL%1,              Mark%Zuckerman%Mark.Zuckerman@nhs.net%1]</t>
+  </si>
+  <si>
+    <t>[Laura%Shallcross%NULL%1,              Danielle%Burke%NULL%1,              Owen%Abbott%NULL%1,              Alasdair%Donaldson%NULL%1,              Gemma%Hallatt%NULL%1,              Andrew%Hayward%NULL%1,              Susan%Hopkins%NULL%0,              Maria%Krutikov%NULL%1,              Katie%Sharp%NULL%1,              Leone%Wardman%NULL%1,              Sapphira%Thorne%NULL%1]</t>
+  </si>
+  <si>
+    <t>[ E.%Smith%null%1,               C. F.% Aldus%null%1,               J.% Brainard%null%1,               S.% Dunham%null%1,               P. R.% Hunter%null%1,               N.% Steel%null%1,               P. % Everden%null%1]</t>
+  </si>
+  <si>
+    <t>[Mahesh C%Patel%mp3@uic.edu%1,              Lelia H%Chaisson%NULL%1,              Scott%Borgetti%NULL%1,              Deborah%Burdsall%NULL%1,              Rashmi K%Chugh%NULL%1,              Christopher R%Hoff%NULL%1,              Elizabeth B%Murphy%NULL%1,              Emily A%Murskyj%NULL%1,              Shannon%Wilson%NULL%1,              Joe%Ramos%NULL%1,              Lynn%Akker%NULL%1,              Debra%Bryars%NULL%1,              Evonda%Thomas-Smith%NULL%1,              Susan C%Bleasdale%NULL%1,              Ngozi O%Ezike%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Helena%Temkin‐Greener%helena_temkin-greener@urmc.rochester.edu%1,              Wenhan%Guo%NULL%2,              Wenhan%Guo%NULL%0,              Yunjiao%Mao%NULL%1,              Xueya%Cai%NULL%1,              Yue%Li%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Ana A.%Weil%anaweil@uw.edu%1,              Kira L.%Newman%NULL%2,              Kira L.%Newman%NULL%0,              Thuan D.%Ong%NULL%1,              Giana H.%Davidson%NULL%1,              Jennifer%Logue%NULL%1,              Elisabeth%Brandstetter%NULL%1,              Ariana%Magedson%NULL%1,              Dylan%McDonald%NULL%1,              Denise J.%McCulloch%NULL%1,              Santiago%Neme%NULL%1,              James%Lewis%NULL%0,              Jeff S.%Duchin%NULL%1,              Weizhi%Zhong%NULL%1,              Lea M.%Starita%NULL%1,              Trevor%Bedford%NULL%1,              Alison C.%Roxby%NULL%1,              Helen Y.%Chu%helenchu@uw.edu%2]</t>
+  </si>
+  <si>
+    <t>[Guillermo V.%Sanchez%NULL%1,              Caitlin%Biedron%NULL%1,              Lauren R.%Fink%NULL%1,              Kelly M.%Hatfield%NULL%1,              Jordan Micah F.%Polistico%NULL%1,              Monica P.%Meyer%NULL%1,              Rebecca S.%Noe%NULL%1,              Casey E.%Copen%NULL%1,              Amanda K.%Lyons%NULL%1,              Gonzalo%Gonzalez%NULL%1,              Keith%Kiama%NULL%1,              Mark%Lebednick%NULL%1,              Bonnie K.%Czander%NULL%1,              Amen%Agbonze%NULL%1,              Aimee R.%Surma%NULL%1,              Avnish%Sandhu%NULL%1,              Valerie H.%Mika%NULL%1,              Tyler%Prentiss%NULL%1,              John%Zervos%NULL%1,              Donia A.%Dalal%NULL%1,              Amber M.%Vasquez%NULL%1,              Sujan C.%Reddy%NULL%0,              John%Jernigan%NULL%1,              Paul E.%Kilgore%NULL%1,              Marcus J.%Zervos%NULL%1,              Teena%Chopra%NULL%1,              Carla P.%Bezold%NULL%1,              Najibah K.%Rehman%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Janice K%Louie%Janice.louie@sfdph.org%1,              Hyman M%Scott%NULL%1,              Amie%DuBois%NULL%1,              Natalya%Sturtz%NULL%1,              Wendy%Lu%NULL%1,              Juliet%Stoltey%NULL%1,              Godfred%Masinde%NULL%1,              Stephanie%Cohen%NULL%1,              Darpun%Sachdev%NULL%1,              Susan%Philip%NULL%1,              Naveena%Bobba%NULL%1,              Tomas%Aragon%NULL%1,              NULL%NULL%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Scott A%Goldberg%sagoldberg@bwh.harvard.edu%1,              Jochen%Lennerz%NULL%1,              Michael%Klompas%NULL%1,              Eden%Mark%NULL%1,              Virginia M%Pierce%NULL%1,              Ryan W%Thompson%NULL%1,              Charles T%Pu%NULL%1,              Lauren L%Ritterhouse%NULL%1,              Anand%Dighe%NULL%1,              Eric S%Rosenberg%NULL%1,              David C%Grabowski%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Amy V.%Dora%NULL%1,              Alexander%Winnett%NULL%1,              Lauren P.%Jatt%NULL%1,              Kusha%Davar%NULL%1,              Mika%Watanabe%NULL%1,              Linda%Sohn%NULL%1,              Hannah S.%Kern%NULL%1,              Christopher J.%Graber%NULL%1,              Matthew B.%Goetz%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Benjamin F.%Bigelow%NULL%1,              Olive%Tang%NULL%1,              Gregory R.%Toci%NULL%1,              Norberth%Stracker%NULL%1,              Fatima%Sheikh%NULL%1,              Kara M.%Jacobs Slifka%NULL%1,              Shannon A.%Novosad%NULL%1,              John A.%Jernigan%NULL%0,              Sujan C.%Reddy%NULL%0,              Morgan J.%Katz%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Matt%Feaster%NULL%1,              Ying-Ying%Goh%NULL%1]</t>
+  </si>
+  <si>
+    <t>[William R.%Mills%NULL%1,              Janet M.%Buccola%NULL%1,              Susan%Sender%NULL%1,              Joseph%Lichtefeld%NULL%1,              Nicholas%Romano%NULL%1,              Karen%Reynolds%NULL%1,              Melissa%Price%NULL%1,              Jennifer%Phipps%NULL%1,              Leigh%White%NULL%1,              Shauen%Howard%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Drew A.%Harris%xref no email%1,        Laurie%Archbald-Pannone%xref no email%1,        Jasveen%Kaur%xref no email%1,        David%Cattell-Gordon%xref no email%1,        Karen S.%Rheuban%xref no email%1,        Rachel L.%Ombres%xref no email%1,        Kimberly%Albero%xref no email%1,        Rebecca%Steele%xref no email%1,        Taison D.%Bell%xref no email%1,        Justin B.%Mutter%xref no email%1]</t>
+  </si>
+  <si>
+    <t>[Carl D.%Shrader%xref no email%1,        Shauna%Assadzandi%xref no email%1,        Courtney S.%Pilkerton%xref no email%1,        Amie M.%Ashcraft%xref no email%1]</t>
   </si>
 </sst>
 </file>
@@ -1584,7 +1707,7 @@
         <v>59</v>
       </c>
       <c r="E2" t="s">
-        <v>244</v>
+        <v>285</v>
       </c>
       <c r="F2" t="s">
         <v>60</v>
@@ -1613,7 +1736,7 @@
         <v>64</v>
       </c>
       <c r="E3" t="s">
-        <v>245</v>
+        <v>286</v>
       </c>
       <c r="F3" t="s">
         <v>65</v>
@@ -1642,7 +1765,7 @@
         <v>67</v>
       </c>
       <c r="E4" t="s">
-        <v>246</v>
+        <v>287</v>
       </c>
       <c r="F4" t="s">
         <v>68</v>
@@ -1700,7 +1823,7 @@
         <v>70</v>
       </c>
       <c r="E6" t="s">
-        <v>247</v>
+        <v>288</v>
       </c>
       <c r="F6" t="s">
         <v>6</v>
@@ -1729,7 +1852,7 @@
         <v>73</v>
       </c>
       <c r="E7" t="s">
-        <v>248</v>
+        <v>289</v>
       </c>
       <c r="F7" t="s">
         <v>74</v>
@@ -1758,7 +1881,7 @@
         <v>76</v>
       </c>
       <c r="E8" t="s">
-        <v>249</v>
+        <v>290</v>
       </c>
       <c r="F8" t="s">
         <v>77</v>
@@ -1816,7 +1939,7 @@
         <v>79</v>
       </c>
       <c r="E10" t="s">
-        <v>250</v>
+        <v>291</v>
       </c>
       <c r="F10" t="s">
         <v>80</v>
@@ -1845,7 +1968,7 @@
         <v>83</v>
       </c>
       <c r="E11" t="s">
-        <v>251</v>
+        <v>292</v>
       </c>
       <c r="F11" t="s">
         <v>84</v>
@@ -1874,7 +1997,7 @@
         <v>88</v>
       </c>
       <c r="E12" t="s">
-        <v>252</v>
+        <v>293</v>
       </c>
       <c r="F12" t="s">
         <v>89</v>
@@ -1932,7 +2055,7 @@
         <v>91</v>
       </c>
       <c r="E14" t="s">
-        <v>253</v>
+        <v>294</v>
       </c>
       <c r="F14" t="s">
         <v>92</v>
@@ -1961,7 +2084,7 @@
         <v>95</v>
       </c>
       <c r="E15" t="s">
-        <v>254</v>
+        <v>295</v>
       </c>
       <c r="F15" t="s">
         <v>96</v>
@@ -1990,7 +2113,7 @@
         <v>99</v>
       </c>
       <c r="E16" t="s">
-        <v>255</v>
+        <v>296</v>
       </c>
       <c r="F16" t="s">
         <v>100</v>
@@ -2019,7 +2142,7 @@
         <v>190</v>
       </c>
       <c r="E17" t="s">
-        <v>256</v>
+        <v>297</v>
       </c>
       <c r="F17" t="s">
         <v>16</v>
@@ -2077,7 +2200,7 @@
         <v>51</v>
       </c>
       <c r="E19" t="s">
-        <v>257</v>
+        <v>298</v>
       </c>
       <c r="F19" t="s">
         <v>18</v>
@@ -2106,7 +2229,7 @@
         <v>105</v>
       </c>
       <c r="E20" t="s">
-        <v>258</v>
+        <v>299</v>
       </c>
       <c r="F20" t="s">
         <v>106</v>
@@ -2135,7 +2258,7 @@
         <v>109</v>
       </c>
       <c r="E21" t="s">
-        <v>259</v>
+        <v>300</v>
       </c>
       <c r="F21" t="s">
         <v>110</v>
@@ -2164,7 +2287,7 @@
         <v>112</v>
       </c>
       <c r="E22" t="s">
-        <v>260</v>
+        <v>301</v>
       </c>
       <c r="F22" t="s">
         <v>113</v>
@@ -2222,7 +2345,7 @@
         <v>115</v>
       </c>
       <c r="E24" t="s">
-        <v>261</v>
+        <v>302</v>
       </c>
       <c r="F24" t="s">
         <v>23</v>
@@ -2251,7 +2374,7 @@
         <v>118</v>
       </c>
       <c r="E25" t="s">
-        <v>262</v>
+        <v>303</v>
       </c>
       <c r="F25" t="s">
         <v>119</v>
@@ -2280,7 +2403,7 @@
         <v>51</v>
       </c>
       <c r="E26" t="s">
-        <v>263</v>
+        <v>304</v>
       </c>
       <c r="F26" t="s">
         <v>25</v>
@@ -2309,7 +2432,7 @@
         <v>122</v>
       </c>
       <c r="E27" t="s">
-        <v>264</v>
+        <v>305</v>
       </c>
       <c r="F27" t="s">
         <v>123</v>
@@ -2338,7 +2461,7 @@
         <v>126</v>
       </c>
       <c r="E28" t="s">
-        <v>265</v>
+        <v>306</v>
       </c>
       <c r="F28" t="s">
         <v>127</v>
@@ -2367,7 +2490,7 @@
         <v>130</v>
       </c>
       <c r="E29" t="s">
-        <v>266</v>
+        <v>307</v>
       </c>
       <c r="F29" t="s">
         <v>131</v>
@@ -2396,7 +2519,7 @@
         <v>95</v>
       </c>
       <c r="E30" t="s">
-        <v>267</v>
+        <v>308</v>
       </c>
       <c r="F30" t="s">
         <v>133</v>
@@ -2425,7 +2548,7 @@
         <v>136</v>
       </c>
       <c r="E31" t="s">
-        <v>268</v>
+        <v>309</v>
       </c>
       <c r="F31" t="s">
         <v>137</v>
@@ -2454,7 +2577,7 @@
         <v>140</v>
       </c>
       <c r="E32" t="s">
-        <v>269</v>
+        <v>310</v>
       </c>
       <c r="F32" t="s">
         <v>141</v>
@@ -2483,7 +2606,7 @@
         <v>144</v>
       </c>
       <c r="E33" t="s">
-        <v>270</v>
+        <v>311</v>
       </c>
       <c r="F33" t="s">
         <v>145</v>
@@ -2512,7 +2635,7 @@
         <v>147</v>
       </c>
       <c r="E34" t="s">
-        <v>271</v>
+        <v>312</v>
       </c>
       <c r="F34" t="s">
         <v>148</v>
@@ -2541,7 +2664,7 @@
         <v>150</v>
       </c>
       <c r="E35" t="s">
-        <v>272</v>
+        <v>313</v>
       </c>
       <c r="F35" t="s">
         <v>34</v>
@@ -2570,7 +2693,7 @@
         <v>153</v>
       </c>
       <c r="E36" t="s">
-        <v>273</v>
+        <v>314</v>
       </c>
       <c r="F36" t="s">
         <v>154</v>
@@ -2599,7 +2722,7 @@
         <v>157</v>
       </c>
       <c r="E37" t="s">
-        <v>274</v>
+        <v>315</v>
       </c>
       <c r="F37" t="s">
         <v>158</v>
@@ -2628,7 +2751,7 @@
         <v>201</v>
       </c>
       <c r="E38" t="s">
-        <v>275</v>
+        <v>316</v>
       </c>
       <c r="F38" t="s">
         <v>161</v>
@@ -2657,7 +2780,7 @@
         <v>95</v>
       </c>
       <c r="E39" t="s">
-        <v>276</v>
+        <v>317</v>
       </c>
       <c r="F39" t="s">
         <v>164</v>
@@ -2686,7 +2809,7 @@
         <v>166</v>
       </c>
       <c r="E40" t="s">
-        <v>277</v>
+        <v>318</v>
       </c>
       <c r="F40" t="s">
         <v>167</v>
@@ -2715,7 +2838,7 @@
         <v>169</v>
       </c>
       <c r="E41" t="s">
-        <v>278</v>
+        <v>319</v>
       </c>
       <c r="F41" t="s">
         <v>170</v>
@@ -2744,7 +2867,7 @@
         <v>95</v>
       </c>
       <c r="E42" t="s">
-        <v>279</v>
+        <v>320</v>
       </c>
       <c r="F42" t="s">
         <v>172</v>
@@ -2773,7 +2896,7 @@
         <v>95</v>
       </c>
       <c r="E43" t="s">
-        <v>280</v>
+        <v>321</v>
       </c>
       <c r="F43" t="s">
         <v>174</v>
@@ -2802,7 +2925,7 @@
         <v>176</v>
       </c>
       <c r="E44" t="s">
-        <v>281</v>
+        <v>322</v>
       </c>
       <c r="F44" t="s">
         <v>177</v>
@@ -2831,7 +2954,7 @@
         <v>179</v>
       </c>
       <c r="E45" t="s">
-        <v>282</v>
+        <v>323</v>
       </c>
       <c r="F45" t="s">
         <v>180</v>
@@ -2860,7 +2983,7 @@
         <v>51</v>
       </c>
       <c r="E46" t="s">
-        <v>283</v>
+        <v>324</v>
       </c>
       <c r="F46" t="s">
         <v>45</v>
@@ -2889,7 +3012,7 @@
         <v>199</v>
       </c>
       <c r="E47" t="s">
-        <v>284</v>
+        <v>325</v>
       </c>
       <c r="F47" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
cleaned more data, fixed a problem where some SLRs contained incorrect data.
</commit_message>
<xml_diff>
--- a/Covid_19_Dataset_and_References/References/10.xlsx
+++ b/Covid_19_Dataset_and_References/References/10.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1036" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1694" uniqueCount="408">
   <si>
     <t>Doi</t>
   </si>
@@ -1366,6 +1366,252 @@
   </si>
   <si>
     <t>[Carl D.%Shrader%xref no email%1,        Shauna%Assadzandi%xref no email%1,        Courtney S.%Pilkerton%xref no email%1,        Amie M.%Ashcraft%xref no email%1]</t>
+  </si>
+  <si>
+    <t>[Daniel J%Escobar%Daniel.escobar@pennmedicine.upenn.edu%1,               Maria%Lanzi%NULL%1,               Pouné%Saberi%NULL%1,               Ruby%Love%NULL%1,               Darren R%Linkin%NULL%1,               John J%Kelly%NULL%1,               Darshana%Jhala%NULL%1,               Valerianna%Amorosa%NULL%1,               Mary%Hofmann%NULL%1,               Jeffrey B%Doyon%NULL%1]</t>
+  </si>
+  <si>
+    <t>[James L.%Rudolph%NULL%1,               Christopher W.%Halladay%NULL%1,               Malisa%Barber%NULL%1,               Kevin W.%McConeghy%NULL%1,               Vince%Mor%NULL%1,               Aman%Nanda%NULL%1,               Stefan%Gravenstein%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Paula%Eckardt%NULL%1,               Rachel%Guran%NULL%1,               Jon%Hennemyre%NULL%1,               Roshan%Arikupurathu%NULL%1,               Julie%Poveda%NULL%1,               Nancimae%Miller%NULL%1,               Randy%Katz%NULL%1,               Judith%Frum%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Carson%Telford%NULL%1,               Udodirim%Onwubiko%NULL%1,               David%Holland%NULL%1,               Kim%Turner%NULL%1,               Juliana%Prieto%NULL%1,               Sasha%Smith%NULL%1,               Jane%Yoon%NULL%1,               Wecheeta%Brown%NULL%1,               Allison%Chamberlain%NULL%1,               Neel%Gandhi%NULL%1,               Shamimul%Khan%NULL%1,               Steve%Williams%NULL%1,               Fazle%Khan%NULL%1,               Sarita%Shah%NULL%1,                C. T.%Telford%null%1,                U.% Onwubiko%null%1,                D.% Holland%null%1,                K.% Turner%null%1,                J.% Prieto%null%1,                S.% Smith%null%1,                J.% Yoon%null%1,                W.% Brown%null%1,                A.% Chamberlain%null%1,                N.% Gandhi%null%1,                S.% Khan%null%1,                S.% Williams%null%1,                F.% Khan%null%1,                S. % Shah%null%1,               C. T.%Telford%null%1,               U.% Onwubiko%null%1,               D.% Holland%null%1,               K.% Turner%null%1,               J.% Prieto%null%1,               S.% Smith%null%1,               J.% Yoon%null%1,               W.% Brown%null%1,               A.% Chamberlain%null%1,               N.% Gandhi%null%1,               S.% Khan%null%1,               S.% Williams%null%1,               F.% Khan%null%1,               S. % Shah%null%1]</t>
+  </si>
+  <si>
+    <t>[Sandra M.%Shi%NULL%1,               Innokentiy%Bakaev%NULL%1,               Helen%Chen%NULL%1,               Thomas G.%Travison%NULL%1,               Sarah D.%Berry%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Temet M.%McMichael%NULL%0,               Dustin W.%Currie%NULL%0,               Shauna%Clark%NULL%0,               Sargis%Pogosjans%NULL%0,               Meagan%Kay%NULL%0,               Noah G.%Schwartz%NULL%0,               James%Lewis%NULL%0,               Atar%Baer%NULL%0,               Vance%Kawakami%NULL%0,               Margaret D.%Lukoff%NULL%0,               Jessica%Ferro%NULL%0,               Claire%Brostrom-Smith%NULL%0,               Thomas D.%Rea%NULL%1,               Michael R.%Sayre%NULL%1,               Francis X.%Riedo%NULL%0,               Denny%Russell%NULL%0,               Brian%Hiatt%NULL%0,               Patricia%Montgomery%NULL%0,               Agam K.%Rao%NULL%0,               Eric J.%Chow%NULL%0,               Farrell%Tobolowsky%NULL%0,               Michael J.%Hughes%NULL%1,               Ana C.%Bardossy%NULL%0,               Lisa P.%Oakley%NULL%0,               Jesica R.%Jacobs%NULL%0,               Nimalie D.%Stone%NULL%1,               Sujan C.%Reddy%NULL%0,               John A.%Jernigan%NULL%0,               Margaret A.%Honein%NULL%0,               Thomas A.%Clark%NULL%0,               Jeffrey S.%Duchin%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Nathan M.%Stall%nathan.stall@sinaihealth.ca%1,               Carolyn%Farquharson%NULL%2,               Carolyn%Farquharson%NULL%0,               Chris%Fan‐Lun%NULL%1,               Lesley%Wiesenfeld%NULL%1,               Carla A.%Loftus%NULL%1,               Dylan%Kain%NULL%1,               Jennie%Johnstone%NULL%1,               Liz%McCreight%NULL%1,               Russell D.%Goldman%NULL%1,               Ramona%Mahtani%NULL%1]</t>
+  </si>
+  <si>
+    <t>[ Nathan M.%Stall%null%1,                Aaron%Jones%null%1,                Kevin A.%Brown%null%1,                Paula A.%Rochon%null%1,                Andrew P.%Costa%null%1,               Nathan M.%Stall%null%1,               Aaron%Jones%null%1,               Kevin A.%Brown%null%1,               Paula A.%Rochon%null%1,               Andrew P.%Costa%null%1]</t>
+  </si>
+  <si>
+    <t>[Hubert%Blain%NULL%1,               Yves%Rolland%NULL%1,               Edouard%Tuaillon%NULL%1,               Nadia%Giacosa%NULL%1,               Mylène%Albrand%NULL%1,               Audrey%Jaussent%NULL%1,               Athanase%Benetos%NULL%1,               Stéphanie%Miot%NULL%1,               Jean%Bousquet%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Guillaume%Sacco%NULL%1,               Gonzague%Foucault%NULL%1,               Olivier%Briere%NULL%1,               Cédric%Annweiler%NULL%1]</t>
+  </si>
+  <si>
+    <t>[R.%Guery%NULL%1,               C.%Delaye%NULL%1,               N.%Brule%NULL%1,               V.%Nael%NULL%1,               L.%Castain%NULL%1,               F.%Raffi%NULL%1,               L.%De Decker%NULL%1]</t>
+  </si>
+  <si>
+    <t>[A.%Klein%anke.klein@uke.de%1,               C.%Edler%NULL%1,               A.%Fitzek%NULL%1,               D.%Fröb%NULL%1,               A.%Heinemann%NULL%1,               K.%Meißner%NULL%1,               H.%Mushumba%NULL%1,               K.%Püschel%NULL%1,               A. S.%Schröder%NULL%1,               J. P.%Sperhake%NULL%1,               F.%Ishorst-Witte%NULL%1,               M.%Aepfelbacher%NULL%1,               F.%Heinrich%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Buntinx%Frank%coreGivesNoEmail%1,             Claes%Peter%coreGivesNoEmail%1,             Gulikers%Marjo%coreGivesNoEmail%1,             Jan%De Lepeleire%coreGivesNoEmail%1,             Van%der Elst Michael%coreGivesNoEmail%1,             Van%Elslande Jan%coreGivesNoEmail%1,             Van%Ranst Marc%coreGivesNoEmail%1,             Verbakel%Jan%coreGivesNoEmail%1,             Vernneersch%Pieter%coreGivesNoEmail%1]</t>
+  </si>
+  <si>
+    <t>[Liangcong%Hu%xref no email%1,         Wanyuan%Zhen%xref no email%1,         Xudong%Xie%xref no email%2,         Ze%Lin%xref no email%2,         Tiantian%Wang%xref no email%1,         Jing%Liu%xref no email%5,         Hang%Xue%xref no email%2,         Adriana C.%Panayi%xref no email%2,         Ke%Xu%xref no email%1,         Zexi%Ling%xref no email%1,         Xugui%Li%xref no email%1,         Bobin%Mi%xref no email%1,         Wu%Zhou%xref no email%2,         Guohui%Liu%xref no email%2]</t>
+  </si>
+  <si>
+    <t>[Sean P%Kennelly%Sean.Kennelly@tuh.ie%1,               Adam H%Dyer%dyera@tcd.ie%1,               Claire%Noonan%claire.noonan@tuh.ie%2,               Claire%Noonan%claire.noonan@tuh.ie%0,               Ruth%Martin%ruth.martin1@hse.ie%1,               Siobhan M%Kennelly%siobhan.kennelly1@hse.ie%1,               Alan%Martin%alanmartin@beaumont.ie%1,               Desmond%O’Neill%NULL%1,               Aoife%Fallon%aoife.fallon1@hotmail.com%1]</t>
+  </si>
+  <si>
+    <t>[Antonio%Nouvenne%NULL%1,               Andrea%Ticinesi%NULL%1,               Alberto%Parise%NULL%1,               Beatrice%Prati%NULL%1,               Marcello%Esposito%NULL%1,               Valentina%Cocchi%NULL%1,               Emanuele%Crisafulli%NULL%1,               Annalisa%Volpi%NULL%1,               Sandra%Rossi%NULL%1,               Elena Giovanna%Bignami%NULL%1,               Marco%Baciarello%NULL%1,               Ettore%Brianti%NULL%1,               Massimo%Fabi%NULL%1,               Tiziana%Meschi%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Nicola%Veronese%NULL%1,               Luca Gino%Sbrogiò%NULL%1,               Roberto%Valle%NULL%1,               Laura%Marin%NULL%1,               Elena%Boscolo Fiore%NULL%1,               Andrea%Tiozzo%NULL%1]</t>
+  </si>
+  <si>
+    <t>[ J. H.%van den Besselaar%null%1,                R. S.% Sikkema%null%1,                F. M. H. P. A.% Koene%null%1,                L. W.% van Buul%null%1,                B. B.% Oude Munnink%null%1,                I.% Frenay%null%1,                R.% te Witt%null%1,                M. P. G.% Koopmans%null%1,                C. M. P. M.% Hertogh%null%1,                B. M. % Buurman%null%1]</t>
+  </si>
+  <si>
+    <t>[Laura W.%van Buul%NULL%1,               Judith H.%van den Besselaar%NULL%2,               Judith H.%van den Besselaar%NULL%0,               Fleur M. H. P. H.%Koene%NULL%1,               Bianca M.%Buurman%NULL%1,               Cees M. P. M.%Hertogh%NULL%1,               Martin%Smalbrugge%NULL%1,               Jeanine J. S.%Rutten%NULL%1,               Elke M.%den Boogert%NULL%1,               Michel D.%Wissing%NULL%1,               Ariene%Rietveld%NULL%1,               Mariska W. W.%van Elsakker%NULL%1,               Marga M. G.%Nonneman%NULL%1,               Florien%van Eeden%NULL%1,               Saskia%van de Merwe%NULL%1,               Sophie L.%Niemansburg%NULL%1,               Ewout%Fanoy%NULL%1,               Hinke S.%Bootsma%NULL%1,               Nicoline%van der Hagen%NULL%1,               Mariska%Petrignani%NULL%1,               Jessica Edwards%van Muijen%NULL%1,               Karolien E. M.%Biesheuvel%NULL%1]</t>
+  </si>
+  <si>
+    <t>[B\u00e5rd%Reiakvam Kittang%coreGivesNoEmail%1,             Karina%Koller L\u00f8land%coreGivesNoEmail%1,             Kjell%Kr\u00fcger%coreGivesNoEmail%1,             Kristian%Jansen%coreGivesNoEmail%1,             Sabine%Piepenstock Solheim%coreGivesNoEmail%1,             Sebastian%von Hofacker%coreGivesNoEmail%1]</t>
+  </si>
+  <si>
+    <t>[Shin Young%Park%NULL%1,               Gawon%Choi%NULL%2,               Gawon%Choi%NULL%0,               Hyeyoung%Lee%NULL%2,               Hyeyoung%Lee%NULL%0,               Na-young%Kim%NULL%2,               Na-young%Kim%NULL%0,               Seon-young%Lee%NULL%2,               Seon-young%Lee%NULL%0,               Kyungnam%Kim%NULL%2,               Kyungnam%Kim%NULL%0,               Soyoung%Shin%NULL%2,               Soyoung%Shin%NULL%0,               Eunsu%Jang%NULL%2,               Eunsu%Jang%NULL%0,               YoungSin%Moon%NULL%2,               YoungSin%Moon%NULL%0,               KwangHwan%Oh%NULL%2,               KwangHwan%Oh%NULL%0,               JaeRin%Choi%NULL%2,               JaeRin%Choi%NULL%0,               Sangeun%Lee%NULL%2,               Sangeun%Lee%NULL%0,               Young-Man%Kim%NULL%2,               Young-Man%Kim%NULL%0,               Jieun%Kim%NULL%2,               Jieun%Kim%NULL%0,               Seonju%Yi%NULL%2,               Seonju%Yi%NULL%0,               Jin%Gwack%NULL%2,               Jin%Gwack%NULL%0,               Ok%Park%NULL%2,               Ok%Park%NULL%0,               Young Joon%Park%NULL%2,               Young Joon%Park%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Rok%Song%NULL%1,               Hee-Sook%Kim%NULL%2,               Hee-Sook%Kim%NULL%0,               Seok-Ju%Yoo%NULL%2,               Seok-Ju%Yoo%NULL%0,               Kwan%Lee%NULL%2,               Kwan%Lee%NULL%0,               Ji-Hyuk%Park%NULL%2,               Ji-Hyuk%Park%NULL%0,               Joon Ho%Jang%NULL%2,               Joon Ho%Jang%NULL%0,               Gyoung-Sook%Ahn%NULL%2,               Gyoung-Sook%Ahn%NULL%0,               Jun-Nyun%Kim%NULL%2,               Jun-Nyun%Kim%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Blanca%Borras-Bermejo%NULL%1,               Xavier%Martínez-Gómez%NULL%1,               María Gutierrez%San Miguel%NULL%1,               Juliana%Esperalba%NULL%1,               Andrés%Antón%NULL%1,               Elisabet%Martin%NULL%1,               Marta%Selvi%NULL%1,               María José%Abadías%NULL%1,               Antonio%Román%NULL%1,               Tomàs%Pumarola%NULL%1,               Magda%Campins%NULL%1,               Benito%Almirante%NULL%1]</t>
+  </si>
+  <si>
+    <t>[M.%Bernabeu-Wittel%NULL%1,               J.E.%Ternero-Vega%NULL%1,               P.%Díaz-Jiménez%NULL%1,               C.%Conde-Guzmán%NULL%1,               M.D.%Nieto-Martín%NULL%1,               L.%Moreno-Gaviño%NULL%1,               J.%Delgado-Cuesta%NULL%1,               M.%Rincón-Gómez%NULL%1,               L.%Giménez-Miranda%NULL%1,               M.D.%Navarro-Amuedo%NULL%1,               M.M.%Muñoz-García%NULL%1,               S.%Calzón-Fernández%NULL%1,               M.%Ollero-Baturone%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Shamez N%Ladhani%shamez.ladhani@phe.gov.uk%1,               J.Yimmy%Chow%NULL%1,               Roshni%Janarthanan%NULL%1,               Jonathan%Fok%NULL%1,               Emma%Crawley-Boevey%NULL%1,               Amoolya%Vusirikala%NULL%1,               Elena%Fernandez%NULL%1,               Marina Sanchez%Perez%NULL%1,               Suzanne%Tang%NULL%1,               Kate%Dun-Campbell%NULL%1,               Edward Wynne-%Evans%NULL%1,               Anita%Bell%NULL%1,               Bharat%Patel%NULL%1,               Zahin%Amin-Chowdhury%NULL%1,               Felicity%Aiano%NULL%1,               Karthik%Paranthaman%NULL%1,               Thomas%Ma%NULL%1,               Maria%Saavedra-Campos%NULL%1,               Richard%Myers%NULL%1,               Joanna%Ellis%NULL%2,               Angie%Lackenby%NULL%1,               Robin%Gopal%NULL%1,               Monika%Patel%NULL%1,               Colin%Brown%NULL%1,               Meera%Chand%NULL%1,               Kevin%Brown%NULL%1,               Mary E%Ramsay%NULL%1,               Susan%Hopkins%NULL%2,               Nandini%Shetty%NULL%1,               Maria%Zambon%NULL%2]</t>
+  </si>
+  <si>
+    <t>[N.S.N.%Graham%NULL%1,               C.%Junghans%NULL%1,               R.%Downes%NULL%1,               C.%Sendall%NULL%1,               H.%Lai%NULL%1,               A.%McKirdy%NULL%1,               P.%Elliott%NULL%1,               R.%Howard%NULL%1,               D.%Wingfield%NULL%1,               M.%Priestman%NULL%1,               M.%Ciechonska%NULL%1,               L.%Cameron%NULL%1,               M.%Storch%NULL%1,               M.A.%Crone%NULL%1,               P.S.%Freemont%NULL%1,               P.%Randell%NULL%1,               R.%McLaren%NULL%1,               N.%Lang%NULL%1,               S.%Ladhani%NULL%1,               F.%Sanderson%NULL%1,               D.J.%Sharp%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Agnes%Marossy%agnesmarossy@nhs.net%1,               Stefan%Rakowicz%NULL%1,               Angela%Bhan%NULL%1,               Sarah%Noon%NULL%1,               Amanda%Rees%NULL%1,               Manjinder%Virk%NULL%1,               Ayazali%Nazafi%NULL%1,               Evie%Hay%NULL%1,               Louise%de Thomasson%NULL%1,               Christina%Windle%NULL%1,               Mark%Zuckerman%Mark.Zuckerman@nhs.net%1]</t>
+  </si>
+  <si>
+    <t>[Laura%Shallcross%NULL%1,               Danielle%Burke%NULL%1,               Owen%Abbott%NULL%1,               Alasdair%Donaldson%NULL%1,               Gemma%Hallatt%NULL%1,               Andrew%Hayward%NULL%1,               Susan%Hopkins%NULL%0,               Maria%Krutikov%NULL%1,               Katie%Sharp%NULL%1,               Leone%Wardman%NULL%1,               Sapphira%Thorne%NULL%1]</t>
+  </si>
+  <si>
+    <t>[ E.%Smith%null%1,                C. F.% Aldus%null%1,                J.% Brainard%null%1,                S.% Dunham%null%1,                P. R.% Hunter%null%1,                N.% Steel%null%1,                P. % Everden%null%1]</t>
+  </si>
+  <si>
+    <t>[Mahesh C%Patel%mp3@uic.edu%1,               Lelia H%Chaisson%NULL%1,               Scott%Borgetti%NULL%1,               Deborah%Burdsall%NULL%1,               Rashmi K%Chugh%NULL%1,               Christopher R%Hoff%NULL%1,               Elizabeth B%Murphy%NULL%1,               Emily A%Murskyj%NULL%1,               Shannon%Wilson%NULL%1,               Joe%Ramos%NULL%1,               Lynn%Akker%NULL%1,               Debra%Bryars%NULL%1,               Evonda%Thomas-Smith%NULL%1,               Susan C%Bleasdale%NULL%1,               Ngozi O%Ezike%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Helena%Temkin‐Greener%helena_temkin-greener@urmc.rochester.edu%1,               Wenhan%Guo%NULL%2,               Wenhan%Guo%NULL%0,               Yunjiao%Mao%NULL%1,               Xueya%Cai%NULL%1,               Yue%Li%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Ana A.%Weil%anaweil@uw.edu%1,               Kira L.%Newman%NULL%2,               Kira L.%Newman%NULL%0,               Thuan D.%Ong%NULL%1,               Giana H.%Davidson%NULL%1,               Jennifer%Logue%NULL%1,               Elisabeth%Brandstetter%NULL%1,               Ariana%Magedson%NULL%1,               Dylan%McDonald%NULL%1,               Denise J.%McCulloch%NULL%1,               Santiago%Neme%NULL%1,               James%Lewis%NULL%0,               Jeff S.%Duchin%NULL%1,               Weizhi%Zhong%NULL%1,               Lea M.%Starita%NULL%1,               Trevor%Bedford%NULL%1,               Alison C.%Roxby%NULL%1,               Helen Y.%Chu%helenchu@uw.edu%2]</t>
+  </si>
+  <si>
+    <t>[Guillermo V.%Sanchez%NULL%1,               Caitlin%Biedron%NULL%1,               Lauren R.%Fink%NULL%1,               Kelly M.%Hatfield%NULL%1,               Jordan Micah F.%Polistico%NULL%1,               Monica P.%Meyer%NULL%1,               Rebecca S.%Noe%NULL%1,               Casey E.%Copen%NULL%1,               Amanda K.%Lyons%NULL%1,               Gonzalo%Gonzalez%NULL%1,               Keith%Kiama%NULL%1,               Mark%Lebednick%NULL%1,               Bonnie K.%Czander%NULL%1,               Amen%Agbonze%NULL%1,               Aimee R.%Surma%NULL%1,               Avnish%Sandhu%NULL%1,               Valerie H.%Mika%NULL%1,               Tyler%Prentiss%NULL%1,               John%Zervos%NULL%1,               Donia A.%Dalal%NULL%1,               Amber M.%Vasquez%NULL%1,               Sujan C.%Reddy%NULL%0,               John%Jernigan%NULL%1,               Paul E.%Kilgore%NULL%1,               Marcus J.%Zervos%NULL%1,               Teena%Chopra%NULL%1,               Carla P.%Bezold%NULL%1,               Najibah K.%Rehman%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Janice K%Louie%Janice.louie@sfdph.org%1,               Hyman M%Scott%NULL%1,               Amie%DuBois%NULL%1,               Natalya%Sturtz%NULL%1,               Wendy%Lu%NULL%1,               Juliet%Stoltey%NULL%1,               Godfred%Masinde%NULL%1,               Stephanie%Cohen%NULL%1,               Darpun%Sachdev%NULL%1,               Susan%Philip%NULL%1,               Naveena%Bobba%NULL%1,               Tomas%Aragon%NULL%1,               NULL%NULL%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Scott A%Goldberg%sagoldberg@bwh.harvard.edu%1,               Jochen%Lennerz%NULL%1,               Michael%Klompas%NULL%1,               Eden%Mark%NULL%1,               Virginia M%Pierce%NULL%1,               Ryan W%Thompson%NULL%1,               Charles T%Pu%NULL%1,               Lauren L%Ritterhouse%NULL%1,               Anand%Dighe%NULL%1,               Eric S%Rosenberg%NULL%1,               David C%Grabowski%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Amy V.%Dora%NULL%1,               Alexander%Winnett%NULL%1,               Lauren P.%Jatt%NULL%1,               Kusha%Davar%NULL%1,               Mika%Watanabe%NULL%1,               Linda%Sohn%NULL%1,               Hannah S.%Kern%NULL%1,               Christopher J.%Graber%NULL%1,               Matthew B.%Goetz%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Benjamin F.%Bigelow%NULL%1,               Olive%Tang%NULL%1,               Gregory R.%Toci%NULL%1,               Norberth%Stracker%NULL%1,               Fatima%Sheikh%NULL%1,               Kara M.%Jacobs Slifka%NULL%1,               Shannon A.%Novosad%NULL%1,               John A.%Jernigan%NULL%0,               Sujan C.%Reddy%NULL%0,               Morgan J.%Katz%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Matt%Feaster%NULL%1,               Ying-Ying%Goh%NULL%1]</t>
+  </si>
+  <si>
+    <t>[William R.%Mills%NULL%1,               Janet M.%Buccola%NULL%1,               Susan%Sender%NULL%1,               Joseph%Lichtefeld%NULL%1,               Nicholas%Romano%NULL%1,               Karen%Reynolds%NULL%1,               Melissa%Price%NULL%1,               Jennifer%Phipps%NULL%1,               Leigh%White%NULL%1,               Shauen%Howard%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Drew A.%Harris%xref no email%1,         Laurie%Archbald-Pannone%xref no email%1,         Jasveen%Kaur%xref no email%1,         David%Cattell-Gordon%xref no email%1,         Karen S.%Rheuban%xref no email%1,         Rachel L.%Ombres%xref no email%1,         Kimberly%Albero%xref no email%1,         Rebecca%Steele%xref no email%1,         Taison D.%Bell%xref no email%1,         Justin B.%Mutter%xref no email%1]</t>
+  </si>
+  <si>
+    <t>[Carl D.%Shrader%xref no email%1,         Shauna%Assadzandi%xref no email%1,         Courtney S.%Pilkerton%xref no email%1,         Amie M.%Ashcraft%xref no email%1]</t>
+  </si>
+  <si>
+    <t>[Daniel J%Escobar%Daniel.escobar@pennmedicine.upenn.edu%1,                Maria%Lanzi%NULL%1,                Pouné%Saberi%NULL%1,                Ruby%Love%NULL%1,                Darren R%Linkin%NULL%1,                John J%Kelly%NULL%1,                Darshana%Jhala%NULL%1,                Valerianna%Amorosa%NULL%1,                Mary%Hofmann%NULL%1,                Jeffrey B%Doyon%NULL%1]</t>
+  </si>
+  <si>
+    <t>[James L.%Rudolph%NULL%1,                Christopher W.%Halladay%NULL%1,                Malisa%Barber%NULL%1,                Kevin W.%McConeghy%NULL%1,                Vince%Mor%NULL%1,                Aman%Nanda%NULL%1,                Stefan%Gravenstein%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Paula%Eckardt%NULL%1,                Rachel%Guran%NULL%1,                Jon%Hennemyre%NULL%1,                Roshan%Arikupurathu%NULL%1,                Julie%Poveda%NULL%1,                Nancimae%Miller%NULL%1,                Randy%Katz%NULL%1,                Judith%Frum%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Carson%Telford%NULL%1,                Udodirim%Onwubiko%NULL%1,                David%Holland%NULL%1,                Kim%Turner%NULL%1,                Juliana%Prieto%NULL%1,                Sasha%Smith%NULL%1,                Jane%Yoon%NULL%1,                Wecheeta%Brown%NULL%1,                Allison%Chamberlain%NULL%1,                Neel%Gandhi%NULL%1,                Shamimul%Khan%NULL%1,                Steve%Williams%NULL%1,                Fazle%Khan%NULL%1,                Sarita%Shah%NULL%1,                 C. T.%Telford%null%1,                 U.% Onwubiko%null%1,                 D.% Holland%null%1,                 K.% Turner%null%1,                 J.% Prieto%null%1,                 S.% Smith%null%1,                 J.% Yoon%null%1,                 W.% Brown%null%1,                 A.% Chamberlain%null%1,                 N.% Gandhi%null%1,                 S.% Khan%null%1,                 S.% Williams%null%1,                 F.% Khan%null%1,                 S. % Shah%null%1,                C. T.%Telford%null%1,                U.% Onwubiko%null%1,                D.% Holland%null%1,                K.% Turner%null%1,                J.% Prieto%null%1,                S.% Smith%null%1,                J.% Yoon%null%1,                W.% Brown%null%1,                A.% Chamberlain%null%1,                N.% Gandhi%null%1,                S.% Khan%null%1,                S.% Williams%null%1,                F.% Khan%null%1,                S. % Shah%null%1]</t>
+  </si>
+  <si>
+    <t>[Sandra M.%Shi%NULL%1,                Innokentiy%Bakaev%NULL%1,                Helen%Chen%NULL%1,                Thomas G.%Travison%NULL%1,                Sarah D.%Berry%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Temet M.%McMichael%NULL%0,                Dustin W.%Currie%NULL%0,                Shauna%Clark%NULL%0,                Sargis%Pogosjans%NULL%0,                Meagan%Kay%NULL%0,                Noah G.%Schwartz%NULL%0,                James%Lewis%NULL%0,                Atar%Baer%NULL%0,                Vance%Kawakami%NULL%0,                Margaret D.%Lukoff%NULL%0,                Jessica%Ferro%NULL%0,                Claire%Brostrom-Smith%NULL%0,                Thomas D.%Rea%NULL%1,                Michael R.%Sayre%NULL%1,                Francis X.%Riedo%NULL%0,                Denny%Russell%NULL%0,                Brian%Hiatt%NULL%0,                Patricia%Montgomery%NULL%0,                Agam K.%Rao%NULL%0,                Eric J.%Chow%NULL%0,                Farrell%Tobolowsky%NULL%0,                Michael J.%Hughes%NULL%1,                Ana C.%Bardossy%NULL%0,                Lisa P.%Oakley%NULL%0,                Jesica R.%Jacobs%NULL%0,                Nimalie D.%Stone%NULL%1,                Sujan C.%Reddy%NULL%0,                John A.%Jernigan%NULL%0,                Margaret A.%Honein%NULL%0,                Thomas A.%Clark%NULL%0,                Jeffrey S.%Duchin%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Nathan M.%Stall%nathan.stall@sinaihealth.ca%1,                Carolyn%Farquharson%NULL%2,                Carolyn%Farquharson%NULL%0,                Chris%Fan‐Lun%NULL%1,                Lesley%Wiesenfeld%NULL%1,                Carla A.%Loftus%NULL%1,                Dylan%Kain%NULL%1,                Jennie%Johnstone%NULL%1,                Liz%McCreight%NULL%1,                Russell D.%Goldman%NULL%1,                Ramona%Mahtani%NULL%1]</t>
+  </si>
+  <si>
+    <t>[ Nathan M.%Stall%null%1,                 Aaron%Jones%null%1,                 Kevin A.%Brown%null%1,                 Paula A.%Rochon%null%1,                 Andrew P.%Costa%null%1,                Nathan M.%Stall%null%1,                Aaron%Jones%null%1,                Kevin A.%Brown%null%1,                Paula A.%Rochon%null%1,                Andrew P.%Costa%null%1]</t>
+  </si>
+  <si>
+    <t>[Hubert%Blain%NULL%1,                Yves%Rolland%NULL%1,                Edouard%Tuaillon%NULL%1,                Nadia%Giacosa%NULL%1,                Mylène%Albrand%NULL%1,                Audrey%Jaussent%NULL%1,                Athanase%Benetos%NULL%1,                Stéphanie%Miot%NULL%1,                Jean%Bousquet%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Guillaume%Sacco%NULL%1,                Gonzague%Foucault%NULL%1,                Olivier%Briere%NULL%1,                Cédric%Annweiler%NULL%1]</t>
+  </si>
+  <si>
+    <t>[R.%Guery%NULL%1,                C.%Delaye%NULL%1,                N.%Brule%NULL%1,                V.%Nael%NULL%1,                L.%Castain%NULL%1,                F.%Raffi%NULL%1,                L.%De Decker%NULL%1]</t>
+  </si>
+  <si>
+    <t>[A.%Klein%anke.klein@uke.de%1,                C.%Edler%NULL%1,                A.%Fitzek%NULL%1,                D.%Fröb%NULL%1,                A.%Heinemann%NULL%1,                K.%Meißner%NULL%1,                H.%Mushumba%NULL%1,                K.%Püschel%NULL%1,                A. S.%Schröder%NULL%1,                J. P.%Sperhake%NULL%1,                F.%Ishorst-Witte%NULL%1,                M.%Aepfelbacher%NULL%1,                F.%Heinrich%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Buntinx%Frank%coreGivesNoEmail%1,              Claes%Peter%coreGivesNoEmail%1,              Gulikers%Marjo%coreGivesNoEmail%1,              Jan%De Lepeleire%coreGivesNoEmail%1,              Van%der Elst Michael%coreGivesNoEmail%1,              Van%Elslande Jan%coreGivesNoEmail%1,              Van%Ranst Marc%coreGivesNoEmail%1,              Verbakel%Jan%coreGivesNoEmail%1,              Vernneersch%Pieter%coreGivesNoEmail%1]</t>
+  </si>
+  <si>
+    <t>[Liangcong%Hu%xref no email%1,          Wanyuan%Zhen%xref no email%1,          Xudong%Xie%xref no email%2,          Ze%Lin%xref no email%2,          Tiantian%Wang%xref no email%1,          Jing%Liu%xref no email%5,          Hang%Xue%xref no email%2,          Adriana C.%Panayi%xref no email%2,          Ke%Xu%xref no email%1,          Zexi%Ling%xref no email%1,          Xugui%Li%xref no email%1,          Bobin%Mi%xref no email%1,          Wu%Zhou%xref no email%2,          Guohui%Liu%xref no email%2]</t>
+  </si>
+  <si>
+    <t>[Sean P%Kennelly%Sean.Kennelly@tuh.ie%1,                Adam H%Dyer%dyera@tcd.ie%1,                Claire%Noonan%claire.noonan@tuh.ie%2,                Claire%Noonan%claire.noonan@tuh.ie%0,                Ruth%Martin%ruth.martin1@hse.ie%1,                Siobhan M%Kennelly%siobhan.kennelly1@hse.ie%1,                Alan%Martin%alanmartin@beaumont.ie%1,                Desmond%O’Neill%NULL%1,                Aoife%Fallon%aoife.fallon1@hotmail.com%1]</t>
+  </si>
+  <si>
+    <t>[Antonio%Nouvenne%NULL%1,                Andrea%Ticinesi%NULL%1,                Alberto%Parise%NULL%1,                Beatrice%Prati%NULL%1,                Marcello%Esposito%NULL%1,                Valentina%Cocchi%NULL%1,                Emanuele%Crisafulli%NULL%1,                Annalisa%Volpi%NULL%1,                Sandra%Rossi%NULL%1,                Elena Giovanna%Bignami%NULL%1,                Marco%Baciarello%NULL%1,                Ettore%Brianti%NULL%1,                Massimo%Fabi%NULL%1,                Tiziana%Meschi%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Nicola%Veronese%NULL%1,                Luca Gino%Sbrogiò%NULL%1,                Roberto%Valle%NULL%1,                Laura%Marin%NULL%1,                Elena%Boscolo Fiore%NULL%1,                Andrea%Tiozzo%NULL%1]</t>
+  </si>
+  <si>
+    <t>[ J. H.%van den Besselaar%null%1,                 R. S.% Sikkema%null%1,                 F. M. H. P. A.% Koene%null%1,                 L. W.% van Buul%null%1,                 B. B.% Oude Munnink%null%1,                 I.% Frenay%null%1,                 R.% te Witt%null%1,                 M. P. G.% Koopmans%null%1,                 C. M. P. M.% Hertogh%null%1,                 B. M. % Buurman%null%1]</t>
+  </si>
+  <si>
+    <t>[Laura W.%van Buul%NULL%1,                Judith H.%van den Besselaar%NULL%2,                Judith H.%van den Besselaar%NULL%0,                Fleur M. H. P. H.%Koene%NULL%1,                Bianca M.%Buurman%NULL%1,                Cees M. P. M.%Hertogh%NULL%1,                Martin%Smalbrugge%NULL%1,                Jeanine J. S.%Rutten%NULL%1,                Elke M.%den Boogert%NULL%1,                Michel D.%Wissing%NULL%1,                Ariene%Rietveld%NULL%1,                Mariska W. W.%van Elsakker%NULL%1,                Marga M. G.%Nonneman%NULL%1,                Florien%van Eeden%NULL%1,                Saskia%van de Merwe%NULL%1,                Sophie L.%Niemansburg%NULL%1,                Ewout%Fanoy%NULL%1,                Hinke S.%Bootsma%NULL%1,                Nicoline%van der Hagen%NULL%1,                Mariska%Petrignani%NULL%1,                Jessica Edwards%van Muijen%NULL%1,                Karolien E. M.%Biesheuvel%NULL%1]</t>
+  </si>
+  <si>
+    <t>[B\u00e5rd%Reiakvam Kittang%coreGivesNoEmail%1,              Karina%Koller L\u00f8land%coreGivesNoEmail%1,              Kjell%Kr\u00fcger%coreGivesNoEmail%1,              Kristian%Jansen%coreGivesNoEmail%1,              Sabine%Piepenstock Solheim%coreGivesNoEmail%1,              Sebastian%von Hofacker%coreGivesNoEmail%1]</t>
+  </si>
+  <si>
+    <t>[Shin Young%Park%NULL%1,                Gawon%Choi%NULL%2,                Gawon%Choi%NULL%0,                Hyeyoung%Lee%NULL%2,                Hyeyoung%Lee%NULL%0,                Na-young%Kim%NULL%2,                Na-young%Kim%NULL%0,                Seon-young%Lee%NULL%2,                Seon-young%Lee%NULL%0,                Kyungnam%Kim%NULL%2,                Kyungnam%Kim%NULL%0,                Soyoung%Shin%NULL%2,                Soyoung%Shin%NULL%0,                Eunsu%Jang%NULL%2,                Eunsu%Jang%NULL%0,                YoungSin%Moon%NULL%2,                YoungSin%Moon%NULL%0,                KwangHwan%Oh%NULL%2,                KwangHwan%Oh%NULL%0,                JaeRin%Choi%NULL%2,                JaeRin%Choi%NULL%0,                Sangeun%Lee%NULL%2,                Sangeun%Lee%NULL%0,                Young-Man%Kim%NULL%2,                Young-Man%Kim%NULL%0,                Jieun%Kim%NULL%2,                Jieun%Kim%NULL%0,                Seonju%Yi%NULL%2,                Seonju%Yi%NULL%0,                Jin%Gwack%NULL%2,                Jin%Gwack%NULL%0,                Ok%Park%NULL%2,                Ok%Park%NULL%0,                Young Joon%Park%NULL%2,                Young Joon%Park%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Rok%Song%NULL%1,                Hee-Sook%Kim%NULL%2,                Hee-Sook%Kim%NULL%0,                Seok-Ju%Yoo%NULL%2,                Seok-Ju%Yoo%NULL%0,                Kwan%Lee%NULL%2,                Kwan%Lee%NULL%0,                Ji-Hyuk%Park%NULL%2,                Ji-Hyuk%Park%NULL%0,                Joon Ho%Jang%NULL%2,                Joon Ho%Jang%NULL%0,                Gyoung-Sook%Ahn%NULL%2,                Gyoung-Sook%Ahn%NULL%0,                Jun-Nyun%Kim%NULL%2,                Jun-Nyun%Kim%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Blanca%Borras-Bermejo%NULL%1,                Xavier%Martínez-Gómez%NULL%1,                María Gutierrez%San Miguel%NULL%1,                Juliana%Esperalba%NULL%1,                Andrés%Antón%NULL%1,                Elisabet%Martin%NULL%1,                Marta%Selvi%NULL%1,                María José%Abadías%NULL%1,                Antonio%Román%NULL%1,                Tomàs%Pumarola%NULL%1,                Magda%Campins%NULL%1,                Benito%Almirante%NULL%1]</t>
+  </si>
+  <si>
+    <t>[M.%Bernabeu-Wittel%NULL%1,                J.E.%Ternero-Vega%NULL%1,                P.%Díaz-Jiménez%NULL%1,                C.%Conde-Guzmán%NULL%1,                M.D.%Nieto-Martín%NULL%1,                L.%Moreno-Gaviño%NULL%1,                J.%Delgado-Cuesta%NULL%1,                M.%Rincón-Gómez%NULL%1,                L.%Giménez-Miranda%NULL%1,                M.D.%Navarro-Amuedo%NULL%1,                M.M.%Muñoz-García%NULL%1,                S.%Calzón-Fernández%NULL%1,                M.%Ollero-Baturone%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Shamez N%Ladhani%shamez.ladhani@phe.gov.uk%1,                J.Yimmy%Chow%NULL%1,                Roshni%Janarthanan%NULL%1,                Jonathan%Fok%NULL%1,                Emma%Crawley-Boevey%NULL%1,                Amoolya%Vusirikala%NULL%1,                Elena%Fernandez%NULL%1,                Marina Sanchez%Perez%NULL%1,                Suzanne%Tang%NULL%1,                Kate%Dun-Campbell%NULL%1,                Edward Wynne-%Evans%NULL%1,                Anita%Bell%NULL%1,                Bharat%Patel%NULL%1,                Zahin%Amin-Chowdhury%NULL%1,                Felicity%Aiano%NULL%1,                Karthik%Paranthaman%NULL%1,                Thomas%Ma%NULL%1,                Maria%Saavedra-Campos%NULL%1,                Richard%Myers%NULL%1,                Joanna%Ellis%NULL%2,                Angie%Lackenby%NULL%1,                Robin%Gopal%NULL%1,                Monika%Patel%NULL%1,                Colin%Brown%NULL%1,                Meera%Chand%NULL%1,                Kevin%Brown%NULL%1,                Mary E%Ramsay%NULL%1,                Susan%Hopkins%NULL%2,                Nandini%Shetty%NULL%1,                Maria%Zambon%NULL%2]</t>
+  </si>
+  <si>
+    <t>[N.S.N.%Graham%NULL%1,                C.%Junghans%NULL%1,                R.%Downes%NULL%1,                C.%Sendall%NULL%1,                H.%Lai%NULL%1,                A.%McKirdy%NULL%1,                P.%Elliott%NULL%1,                R.%Howard%NULL%1,                D.%Wingfield%NULL%1,                M.%Priestman%NULL%1,                M.%Ciechonska%NULL%1,                L.%Cameron%NULL%1,                M.%Storch%NULL%1,                M.A.%Crone%NULL%1,                P.S.%Freemont%NULL%1,                P.%Randell%NULL%1,                R.%McLaren%NULL%1,                N.%Lang%NULL%1,                S.%Ladhani%NULL%1,                F.%Sanderson%NULL%1,                D.J.%Sharp%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Agnes%Marossy%agnesmarossy@nhs.net%1,                Stefan%Rakowicz%NULL%1,                Angela%Bhan%NULL%1,                Sarah%Noon%NULL%1,                Amanda%Rees%NULL%1,                Manjinder%Virk%NULL%1,                Ayazali%Nazafi%NULL%1,                Evie%Hay%NULL%1,                Louise%de Thomasson%NULL%1,                Christina%Windle%NULL%1,                Mark%Zuckerman%Mark.Zuckerman@nhs.net%1]</t>
+  </si>
+  <si>
+    <t>[Laura%Shallcross%NULL%1,                Danielle%Burke%NULL%1,                Owen%Abbott%NULL%1,                Alasdair%Donaldson%NULL%1,                Gemma%Hallatt%NULL%1,                Andrew%Hayward%NULL%1,                Susan%Hopkins%NULL%0,                Maria%Krutikov%NULL%1,                Katie%Sharp%NULL%1,                Leone%Wardman%NULL%1,                Sapphira%Thorne%NULL%1]</t>
+  </si>
+  <si>
+    <t>[ E.%Smith%null%1,                 C. F.% Aldus%null%1,                 J.% Brainard%null%1,                 S.% Dunham%null%1,                 P. R.% Hunter%null%1,                 N.% Steel%null%1,                 P. % Everden%null%1]</t>
+  </si>
+  <si>
+    <t>[Mahesh C%Patel%mp3@uic.edu%1,                Lelia H%Chaisson%NULL%1,                Scott%Borgetti%NULL%1,                Deborah%Burdsall%NULL%1,                Rashmi K%Chugh%NULL%1,                Christopher R%Hoff%NULL%1,                Elizabeth B%Murphy%NULL%1,                Emily A%Murskyj%NULL%1,                Shannon%Wilson%NULL%1,                Joe%Ramos%NULL%1,                Lynn%Akker%NULL%1,                Debra%Bryars%NULL%1,                Evonda%Thomas-Smith%NULL%1,                Susan C%Bleasdale%NULL%1,                Ngozi O%Ezike%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Helena%Temkin‐Greener%helena_temkin-greener@urmc.rochester.edu%1,                Wenhan%Guo%NULL%2,                Wenhan%Guo%NULL%0,                Yunjiao%Mao%NULL%1,                Xueya%Cai%NULL%1,                Yue%Li%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Ana A.%Weil%anaweil@uw.edu%1,                Kira L.%Newman%NULL%2,                Kira L.%Newman%NULL%0,                Thuan D.%Ong%NULL%1,                Giana H.%Davidson%NULL%1,                Jennifer%Logue%NULL%1,                Elisabeth%Brandstetter%NULL%1,                Ariana%Magedson%NULL%1,                Dylan%McDonald%NULL%1,                Denise J.%McCulloch%NULL%1,                Santiago%Neme%NULL%1,                James%Lewis%NULL%0,                Jeff S.%Duchin%NULL%1,                Weizhi%Zhong%NULL%1,                Lea M.%Starita%NULL%1,                Trevor%Bedford%NULL%1,                Alison C.%Roxby%NULL%1,                Helen Y.%Chu%helenchu@uw.edu%2]</t>
+  </si>
+  <si>
+    <t>[Guillermo V.%Sanchez%NULL%1,                Caitlin%Biedron%NULL%1,                Lauren R.%Fink%NULL%1,                Kelly M.%Hatfield%NULL%1,                Jordan Micah F.%Polistico%NULL%1,                Monica P.%Meyer%NULL%1,                Rebecca S.%Noe%NULL%1,                Casey E.%Copen%NULL%1,                Amanda K.%Lyons%NULL%1,                Gonzalo%Gonzalez%NULL%1,                Keith%Kiama%NULL%1,                Mark%Lebednick%NULL%1,                Bonnie K.%Czander%NULL%1,                Amen%Agbonze%NULL%1,                Aimee R.%Surma%NULL%1,                Avnish%Sandhu%NULL%1,                Valerie H.%Mika%NULL%1,                Tyler%Prentiss%NULL%1,                John%Zervos%NULL%1,                Donia A.%Dalal%NULL%1,                Amber M.%Vasquez%NULL%1,                Sujan C.%Reddy%NULL%0,                John%Jernigan%NULL%1,                Paul E.%Kilgore%NULL%1,                Marcus J.%Zervos%NULL%1,                Teena%Chopra%NULL%1,                Carla P.%Bezold%NULL%1,                Najibah K.%Rehman%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Janice K%Louie%Janice.louie@sfdph.org%1,                Hyman M%Scott%NULL%1,                Amie%DuBois%NULL%1,                Natalya%Sturtz%NULL%1,                Wendy%Lu%NULL%1,                Juliet%Stoltey%NULL%1,                Godfred%Masinde%NULL%1,                Stephanie%Cohen%NULL%1,                Darpun%Sachdev%NULL%1,                Susan%Philip%NULL%1,                Naveena%Bobba%NULL%1,                Tomas%Aragon%NULL%1,                NULL%NULL%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Scott A%Goldberg%sagoldberg@bwh.harvard.edu%1,                Jochen%Lennerz%NULL%1,                Michael%Klompas%NULL%1,                Eden%Mark%NULL%1,                Virginia M%Pierce%NULL%1,                Ryan W%Thompson%NULL%1,                Charles T%Pu%NULL%1,                Lauren L%Ritterhouse%NULL%1,                Anand%Dighe%NULL%1,                Eric S%Rosenberg%NULL%1,                David C%Grabowski%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Amy V.%Dora%NULL%1,                Alexander%Winnett%NULL%1,                Lauren P.%Jatt%NULL%1,                Kusha%Davar%NULL%1,                Mika%Watanabe%NULL%1,                Linda%Sohn%NULL%1,                Hannah S.%Kern%NULL%1,                Christopher J.%Graber%NULL%1,                Matthew B.%Goetz%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Benjamin F.%Bigelow%NULL%1,                Olive%Tang%NULL%1,                Gregory R.%Toci%NULL%1,                Norberth%Stracker%NULL%1,                Fatima%Sheikh%NULL%1,                Kara M.%Jacobs Slifka%NULL%1,                Shannon A.%Novosad%NULL%1,                John A.%Jernigan%NULL%0,                Sujan C.%Reddy%NULL%0,                Morgan J.%Katz%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Matt%Feaster%NULL%1,                Ying-Ying%Goh%NULL%1]</t>
+  </si>
+  <si>
+    <t>[William R.%Mills%NULL%1,                Janet M.%Buccola%NULL%1,                Susan%Sender%NULL%1,                Joseph%Lichtefeld%NULL%1,                Nicholas%Romano%NULL%1,                Karen%Reynolds%NULL%1,                Melissa%Price%NULL%1,                Jennifer%Phipps%NULL%1,                Leigh%White%NULL%1,                Shauen%Howard%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Drew A.%Harris%xref no email%1,          Laurie%Archbald-Pannone%xref no email%1,          Jasveen%Kaur%xref no email%1,          David%Cattell-Gordon%xref no email%1,          Karen S.%Rheuban%xref no email%1,          Rachel L.%Ombres%xref no email%1,          Kimberly%Albero%xref no email%1,          Rebecca%Steele%xref no email%1,          Taison D.%Bell%xref no email%1,          Justin B.%Mutter%xref no email%1]</t>
+  </si>
+  <si>
+    <t>[Carl D.%Shrader%xref no email%1,          Shauna%Assadzandi%xref no email%1,          Courtney S.%Pilkerton%xref no email%1,          Amie M.%Ashcraft%xref no email%1]</t>
   </si>
 </sst>
 </file>
@@ -1707,7 +1953,7 @@
         <v>59</v>
       </c>
       <c r="E2" t="s">
-        <v>285</v>
+        <v>367</v>
       </c>
       <c r="F2" t="s">
         <v>60</v>
@@ -1736,7 +1982,7 @@
         <v>64</v>
       </c>
       <c r="E3" t="s">
-        <v>286</v>
+        <v>368</v>
       </c>
       <c r="F3" t="s">
         <v>65</v>
@@ -1765,7 +2011,7 @@
         <v>67</v>
       </c>
       <c r="E4" t="s">
-        <v>287</v>
+        <v>369</v>
       </c>
       <c r="F4" t="s">
         <v>68</v>
@@ -1823,7 +2069,7 @@
         <v>70</v>
       </c>
       <c r="E6" t="s">
-        <v>288</v>
+        <v>370</v>
       </c>
       <c r="F6" t="s">
         <v>6</v>
@@ -1852,7 +2098,7 @@
         <v>73</v>
       </c>
       <c r="E7" t="s">
-        <v>289</v>
+        <v>371</v>
       </c>
       <c r="F7" t="s">
         <v>74</v>
@@ -1881,7 +2127,7 @@
         <v>76</v>
       </c>
       <c r="E8" t="s">
-        <v>290</v>
+        <v>372</v>
       </c>
       <c r="F8" t="s">
         <v>77</v>
@@ -1939,7 +2185,7 @@
         <v>79</v>
       </c>
       <c r="E10" t="s">
-        <v>291</v>
+        <v>373</v>
       </c>
       <c r="F10" t="s">
         <v>80</v>
@@ -1968,7 +2214,7 @@
         <v>83</v>
       </c>
       <c r="E11" t="s">
-        <v>292</v>
+        <v>374</v>
       </c>
       <c r="F11" t="s">
         <v>84</v>
@@ -1997,7 +2243,7 @@
         <v>88</v>
       </c>
       <c r="E12" t="s">
-        <v>293</v>
+        <v>375</v>
       </c>
       <c r="F12" t="s">
         <v>89</v>
@@ -2055,7 +2301,7 @@
         <v>91</v>
       </c>
       <c r="E14" t="s">
-        <v>294</v>
+        <v>376</v>
       </c>
       <c r="F14" t="s">
         <v>92</v>
@@ -2084,7 +2330,7 @@
         <v>95</v>
       </c>
       <c r="E15" t="s">
-        <v>295</v>
+        <v>377</v>
       </c>
       <c r="F15" t="s">
         <v>96</v>
@@ -2113,7 +2359,7 @@
         <v>99</v>
       </c>
       <c r="E16" t="s">
-        <v>296</v>
+        <v>378</v>
       </c>
       <c r="F16" t="s">
         <v>100</v>
@@ -2142,7 +2388,7 @@
         <v>190</v>
       </c>
       <c r="E17" t="s">
-        <v>297</v>
+        <v>379</v>
       </c>
       <c r="F17" t="s">
         <v>16</v>
@@ -2200,7 +2446,7 @@
         <v>51</v>
       </c>
       <c r="E19" t="s">
-        <v>298</v>
+        <v>380</v>
       </c>
       <c r="F19" t="s">
         <v>18</v>
@@ -2229,7 +2475,7 @@
         <v>105</v>
       </c>
       <c r="E20" t="s">
-        <v>299</v>
+        <v>381</v>
       </c>
       <c r="F20" t="s">
         <v>106</v>
@@ -2258,7 +2504,7 @@
         <v>109</v>
       </c>
       <c r="E21" t="s">
-        <v>300</v>
+        <v>382</v>
       </c>
       <c r="F21" t="s">
         <v>110</v>
@@ -2287,7 +2533,7 @@
         <v>112</v>
       </c>
       <c r="E22" t="s">
-        <v>301</v>
+        <v>383</v>
       </c>
       <c r="F22" t="s">
         <v>113</v>
@@ -2345,7 +2591,7 @@
         <v>115</v>
       </c>
       <c r="E24" t="s">
-        <v>302</v>
+        <v>384</v>
       </c>
       <c r="F24" t="s">
         <v>23</v>
@@ -2374,7 +2620,7 @@
         <v>118</v>
       </c>
       <c r="E25" t="s">
-        <v>303</v>
+        <v>385</v>
       </c>
       <c r="F25" t="s">
         <v>119</v>
@@ -2403,7 +2649,7 @@
         <v>51</v>
       </c>
       <c r="E26" t="s">
-        <v>304</v>
+        <v>386</v>
       </c>
       <c r="F26" t="s">
         <v>25</v>
@@ -2432,7 +2678,7 @@
         <v>122</v>
       </c>
       <c r="E27" t="s">
-        <v>305</v>
+        <v>387</v>
       </c>
       <c r="F27" t="s">
         <v>123</v>
@@ -2461,7 +2707,7 @@
         <v>126</v>
       </c>
       <c r="E28" t="s">
-        <v>306</v>
+        <v>388</v>
       </c>
       <c r="F28" t="s">
         <v>127</v>
@@ -2490,7 +2736,7 @@
         <v>130</v>
       </c>
       <c r="E29" t="s">
-        <v>307</v>
+        <v>389</v>
       </c>
       <c r="F29" t="s">
         <v>131</v>
@@ -2519,7 +2765,7 @@
         <v>95</v>
       </c>
       <c r="E30" t="s">
-        <v>308</v>
+        <v>390</v>
       </c>
       <c r="F30" t="s">
         <v>133</v>
@@ -2548,7 +2794,7 @@
         <v>136</v>
       </c>
       <c r="E31" t="s">
-        <v>309</v>
+        <v>391</v>
       </c>
       <c r="F31" t="s">
         <v>137</v>
@@ -2577,7 +2823,7 @@
         <v>140</v>
       </c>
       <c r="E32" t="s">
-        <v>310</v>
+        <v>392</v>
       </c>
       <c r="F32" t="s">
         <v>141</v>
@@ -2606,7 +2852,7 @@
         <v>144</v>
       </c>
       <c r="E33" t="s">
-        <v>311</v>
+        <v>393</v>
       </c>
       <c r="F33" t="s">
         <v>145</v>
@@ -2635,7 +2881,7 @@
         <v>147</v>
       </c>
       <c r="E34" t="s">
-        <v>312</v>
+        <v>394</v>
       </c>
       <c r="F34" t="s">
         <v>148</v>
@@ -2664,7 +2910,7 @@
         <v>150</v>
       </c>
       <c r="E35" t="s">
-        <v>313</v>
+        <v>395</v>
       </c>
       <c r="F35" t="s">
         <v>34</v>
@@ -2693,7 +2939,7 @@
         <v>153</v>
       </c>
       <c r="E36" t="s">
-        <v>314</v>
+        <v>396</v>
       </c>
       <c r="F36" t="s">
         <v>154</v>
@@ -2722,7 +2968,7 @@
         <v>157</v>
       </c>
       <c r="E37" t="s">
-        <v>315</v>
+        <v>397</v>
       </c>
       <c r="F37" t="s">
         <v>158</v>
@@ -2751,7 +2997,7 @@
         <v>201</v>
       </c>
       <c r="E38" t="s">
-        <v>316</v>
+        <v>398</v>
       </c>
       <c r="F38" t="s">
         <v>161</v>
@@ -2780,7 +3026,7 @@
         <v>95</v>
       </c>
       <c r="E39" t="s">
-        <v>317</v>
+        <v>399</v>
       </c>
       <c r="F39" t="s">
         <v>164</v>
@@ -2809,7 +3055,7 @@
         <v>166</v>
       </c>
       <c r="E40" t="s">
-        <v>318</v>
+        <v>400</v>
       </c>
       <c r="F40" t="s">
         <v>167</v>
@@ -2838,7 +3084,7 @@
         <v>169</v>
       </c>
       <c r="E41" t="s">
-        <v>319</v>
+        <v>401</v>
       </c>
       <c r="F41" t="s">
         <v>170</v>
@@ -2867,7 +3113,7 @@
         <v>95</v>
       </c>
       <c r="E42" t="s">
-        <v>320</v>
+        <v>402</v>
       </c>
       <c r="F42" t="s">
         <v>172</v>
@@ -2896,7 +3142,7 @@
         <v>95</v>
       </c>
       <c r="E43" t="s">
-        <v>321</v>
+        <v>403</v>
       </c>
       <c r="F43" t="s">
         <v>174</v>
@@ -2925,7 +3171,7 @@
         <v>176</v>
       </c>
       <c r="E44" t="s">
-        <v>322</v>
+        <v>404</v>
       </c>
       <c r="F44" t="s">
         <v>177</v>
@@ -2954,7 +3200,7 @@
         <v>179</v>
       </c>
       <c r="E45" t="s">
-        <v>323</v>
+        <v>405</v>
       </c>
       <c r="F45" t="s">
         <v>180</v>
@@ -2983,7 +3229,7 @@
         <v>51</v>
       </c>
       <c r="E46" t="s">
-        <v>324</v>
+        <v>406</v>
       </c>
       <c r="F46" t="s">
         <v>45</v>
@@ -3012,7 +3258,7 @@
         <v>199</v>
       </c>
       <c r="E47" t="s">
-        <v>325</v>
+        <v>407</v>
       </c>
       <c r="F47" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
Cleaned (hopefully) the last bit of data, removing bad data and replacing it
</commit_message>
<xml_diff>
--- a/Covid_19_Dataset_and_References/References/10.xlsx
+++ b/Covid_19_Dataset_and_References/References/10.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1694" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2023" uniqueCount="449">
   <si>
     <t>Doi</t>
   </si>
@@ -1612,6 +1612,129 @@
   </si>
   <si>
     <t>[Carl D.%Shrader%xref no email%1,          Shauna%Assadzandi%xref no email%1,          Courtney S.%Pilkerton%xref no email%1,          Amie M.%Ashcraft%xref no email%1]</t>
+  </si>
+  <si>
+    <t>[Daniel J%Escobar%Daniel.escobar@pennmedicine.upenn.edu%1,                 Maria%Lanzi%NULL%1,                 Pouné%Saberi%NULL%1,                 Ruby%Love%NULL%1,                 Darren R%Linkin%NULL%1,                 John J%Kelly%NULL%1,                 Darshana%Jhala%NULL%1,                 Valerianna%Amorosa%NULL%1,                 Mary%Hofmann%NULL%1,                 Jeffrey B%Doyon%NULL%1]</t>
+  </si>
+  <si>
+    <t>[James L.%Rudolph%NULL%1,                 Christopher W.%Halladay%NULL%1,                 Malisa%Barber%NULL%1,                 Kevin W.%McConeghy%NULL%1,                 Vince%Mor%NULL%1,                 Aman%Nanda%NULL%1,                 Stefan%Gravenstein%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Paula%Eckardt%NULL%1,                 Rachel%Guran%NULL%1,                 Jon%Hennemyre%NULL%1,                 Roshan%Arikupurathu%NULL%1,                 Julie%Poveda%NULL%1,                 Nancimae%Miller%NULL%1,                 Randy%Katz%NULL%1,                 Judith%Frum%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Carson%Telford%NULL%1,                 Udodirim%Onwubiko%NULL%1,                 David%Holland%NULL%1,                 Kim%Turner%NULL%1,                 Juliana%Prieto%NULL%1,                 Sasha%Smith%NULL%1,                 Jane%Yoon%NULL%1,                 Wecheeta%Brown%NULL%1,                 Allison%Chamberlain%NULL%1,                 Neel%Gandhi%NULL%1,                 Shamimul%Khan%NULL%1,                 Steve%Williams%NULL%1,                 Fazle%Khan%NULL%1,                 Sarita%Shah%NULL%1,                  C. T.%Telford%null%1,                  U.% Onwubiko%null%1,                  D.% Holland%null%1,                  K.% Turner%null%1,                  J.% Prieto%null%1,                  S.% Smith%null%1,                  J.% Yoon%null%1,                  W.% Brown%null%1,                  A.% Chamberlain%null%1,                  N.% Gandhi%null%1,                  S.% Khan%null%1,                  S.% Williams%null%1,                  F.% Khan%null%1,                  S. % Shah%null%1,                 C. T.%Telford%null%1,                 U.% Onwubiko%null%1,                 D.% Holland%null%1,                 K.% Turner%null%1,                 J.% Prieto%null%1,                 S.% Smith%null%1,                 J.% Yoon%null%1,                 W.% Brown%null%1,                 A.% Chamberlain%null%1,                 N.% Gandhi%null%1,                 S.% Khan%null%1,                 S.% Williams%null%1,                 F.% Khan%null%1,                 S. % Shah%null%1]</t>
+  </si>
+  <si>
+    <t>[Sandra M.%Shi%NULL%1,                 Innokentiy%Bakaev%NULL%1,                 Helen%Chen%NULL%1,                 Thomas G.%Travison%NULL%1,                 Sarah D.%Berry%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Temet M.%McMichael%NULL%0,                 Dustin W.%Currie%NULL%0,                 Shauna%Clark%NULL%0,                 Sargis%Pogosjans%NULL%0,                 Meagan%Kay%NULL%0,                 Noah G.%Schwartz%NULL%0,                 James%Lewis%NULL%0,                 Atar%Baer%NULL%0,                 Vance%Kawakami%NULL%0,                 Margaret D.%Lukoff%NULL%0,                 Jessica%Ferro%NULL%0,                 Claire%Brostrom-Smith%NULL%0,                 Thomas D.%Rea%NULL%1,                 Michael R.%Sayre%NULL%1,                 Francis X.%Riedo%NULL%0,                 Denny%Russell%NULL%0,                 Brian%Hiatt%NULL%0,                 Patricia%Montgomery%NULL%0,                 Agam K.%Rao%NULL%0,                 Eric J.%Chow%NULL%0,                 Farrell%Tobolowsky%NULL%0,                 Michael J.%Hughes%NULL%1,                 Ana C.%Bardossy%NULL%0,                 Lisa P.%Oakley%NULL%0,                 Jesica R.%Jacobs%NULL%0,                 Nimalie D.%Stone%NULL%1,                 Sujan C.%Reddy%NULL%0,                 John A.%Jernigan%NULL%0,                 Margaret A.%Honein%NULL%0,                 Thomas A.%Clark%NULL%0,                 Jeffrey S.%Duchin%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Nathan M.%Stall%nathan.stall@sinaihealth.ca%1,                 Carolyn%Farquharson%NULL%2,                 Carolyn%Farquharson%NULL%0,                 Chris%Fan‐Lun%NULL%1,                 Lesley%Wiesenfeld%NULL%1,                 Carla A.%Loftus%NULL%1,                 Dylan%Kain%NULL%1,                 Jennie%Johnstone%NULL%1,                 Liz%McCreight%NULL%1,                 Russell D.%Goldman%NULL%1,                 Ramona%Mahtani%NULL%1]</t>
+  </si>
+  <si>
+    <t>[ Nathan M.%Stall%null%1,                  Aaron%Jones%null%1,                  Kevin A.%Brown%null%1,                  Paula A.%Rochon%null%1,                  Andrew P.%Costa%null%1,                 Nathan M.%Stall%null%1,                 Aaron%Jones%null%1,                 Kevin A.%Brown%null%1,                 Paula A.%Rochon%null%1,                 Andrew P.%Costa%null%1]</t>
+  </si>
+  <si>
+    <t>[Hubert%Blain%NULL%1,                 Yves%Rolland%NULL%1,                 Edouard%Tuaillon%NULL%1,                 Nadia%Giacosa%NULL%1,                 Mylène%Albrand%NULL%1,                 Audrey%Jaussent%NULL%1,                 Athanase%Benetos%NULL%1,                 Stéphanie%Miot%NULL%1,                 Jean%Bousquet%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Guillaume%Sacco%NULL%1,                 Gonzague%Foucault%NULL%1,                 Olivier%Briere%NULL%1,                 Cédric%Annweiler%NULL%1]</t>
+  </si>
+  <si>
+    <t>[R.%Guery%NULL%1,                 C.%Delaye%NULL%1,                 N.%Brule%NULL%1,                 V.%Nael%NULL%1,                 L.%Castain%NULL%1,                 F.%Raffi%NULL%1,                 L.%De Decker%NULL%1]</t>
+  </si>
+  <si>
+    <t>[A.%Klein%anke.klein@uke.de%1,                 C.%Edler%NULL%1,                 A.%Fitzek%NULL%1,                 D.%Fröb%NULL%1,                 A.%Heinemann%NULL%1,                 K.%Meißner%NULL%1,                 H.%Mushumba%NULL%1,                 K.%Püschel%NULL%1,                 A. S.%Schröder%NULL%1,                 J. P.%Sperhake%NULL%1,                 F.%Ishorst-Witte%NULL%1,                 M.%Aepfelbacher%NULL%1,                 F.%Heinrich%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Buntinx%Frank%coreGivesNoEmail%1,               Claes%Peter%coreGivesNoEmail%1,               Gulikers%Marjo%coreGivesNoEmail%1,               Jan%De Lepeleire%coreGivesNoEmail%1,               Van%der Elst Michael%coreGivesNoEmail%1,               Van%Elslande Jan%coreGivesNoEmail%1,               Van%Ranst Marc%coreGivesNoEmail%1,               Verbakel%Jan%coreGivesNoEmail%1,               Vernneersch%Pieter%coreGivesNoEmail%1]</t>
+  </si>
+  <si>
+    <t>[Liangcong%Hu%xref no email%1,           Wanyuan%Zhen%xref no email%1,           Xudong%Xie%xref no email%2,           Ze%Lin%xref no email%2,           Tiantian%Wang%xref no email%1,           Jing%Liu%xref no email%6,           Hang%Xue%xref no email%2,           Adriana C.%Panayi%xref no email%2,           Ke%Xu%xref no email%1,           Zexi%Ling%xref no email%1,           Xugui%Li%xref no email%1,           Bobin%Mi%xref no email%1,           Wu%Zhou%xref no email%2,           Guohui%Liu%xref no email%2]</t>
+  </si>
+  <si>
+    <t>[Sean P%Kennelly%Sean.Kennelly@tuh.ie%1,                 Adam H%Dyer%dyera@tcd.ie%1,                 Claire%Noonan%claire.noonan@tuh.ie%2,                 Claire%Noonan%claire.noonan@tuh.ie%0,                 Ruth%Martin%ruth.martin1@hse.ie%1,                 Siobhan M%Kennelly%siobhan.kennelly1@hse.ie%1,                 Alan%Martin%alanmartin@beaumont.ie%1,                 Desmond%O’Neill%NULL%1,                 Aoife%Fallon%aoife.fallon1@hotmail.com%1]</t>
+  </si>
+  <si>
+    <t>[Antonio%Nouvenne%NULL%1,                 Andrea%Ticinesi%NULL%1,                 Alberto%Parise%NULL%1,                 Beatrice%Prati%NULL%1,                 Marcello%Esposito%NULL%1,                 Valentina%Cocchi%NULL%1,                 Emanuele%Crisafulli%NULL%1,                 Annalisa%Volpi%NULL%1,                 Sandra%Rossi%NULL%1,                 Elena Giovanna%Bignami%NULL%1,                 Marco%Baciarello%NULL%1,                 Ettore%Brianti%NULL%1,                 Massimo%Fabi%NULL%1,                 Tiziana%Meschi%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Nicola%Veronese%NULL%1,                 Luca Gino%Sbrogiò%NULL%1,                 Roberto%Valle%NULL%1,                 Laura%Marin%NULL%1,                 Elena%Boscolo Fiore%NULL%1,                 Andrea%Tiozzo%NULL%1]</t>
+  </si>
+  <si>
+    <t>[ J. H.%van den Besselaar%null%1,                  R. S.% Sikkema%null%1,                  F. M. H. P. A.% Koene%null%1,                  L. W.% van Buul%null%1,                  B. B.% Oude Munnink%null%1,                  I.% Frenay%null%1,                  R.% te Witt%null%1,                  M. P. G.% Koopmans%null%1,                  C. M. P. M.% Hertogh%null%1,                  B. M. % Buurman%null%1]</t>
+  </si>
+  <si>
+    <t>[Laura W.%van Buul%NULL%1,                 Judith H.%van den Besselaar%NULL%2,                 Judith H.%van den Besselaar%NULL%0,                 Fleur M. H. P. H.%Koene%NULL%1,                 Bianca M.%Buurman%NULL%1,                 Cees M. P. M.%Hertogh%NULL%1,                 Martin%Smalbrugge%NULL%1,                 Jeanine J. S.%Rutten%NULL%1,                 Elke M.%den Boogert%NULL%1,                 Michel D.%Wissing%NULL%1,                 Ariene%Rietveld%NULL%1,                 Mariska W. W.%van Elsakker%NULL%1,                 Marga M. G.%Nonneman%NULL%1,                 Florien%van Eeden%NULL%1,                 Saskia%van de Merwe%NULL%1,                 Sophie L.%Niemansburg%NULL%1,                 Ewout%Fanoy%NULL%1,                 Hinke S.%Bootsma%NULL%1,                 Nicoline%van der Hagen%NULL%1,                 Mariska%Petrignani%NULL%1,                 Jessica Edwards%van Muijen%NULL%1,                 Karolien E. M.%Biesheuvel%NULL%1]</t>
+  </si>
+  <si>
+    <t>[B\u00e5rd%Reiakvam Kittang%coreGivesNoEmail%1,               Karina%Koller L\u00f8land%coreGivesNoEmail%1,               Kjell%Kr\u00fcger%coreGivesNoEmail%1,               Kristian%Jansen%coreGivesNoEmail%1,               Sabine%Piepenstock Solheim%coreGivesNoEmail%1,               Sebastian%von Hofacker%coreGivesNoEmail%1]</t>
+  </si>
+  <si>
+    <t>[Shin Young%Park%NULL%1,                 Gawon%Choi%NULL%2,                 Gawon%Choi%NULL%0,                 Hyeyoung%Lee%NULL%2,                 Hyeyoung%Lee%NULL%0,                 Na-young%Kim%NULL%2,                 Na-young%Kim%NULL%0,                 Seon-young%Lee%NULL%2,                 Seon-young%Lee%NULL%0,                 Kyungnam%Kim%NULL%2,                 Kyungnam%Kim%NULL%0,                 Soyoung%Shin%NULL%2,                 Soyoung%Shin%NULL%0,                 Eunsu%Jang%NULL%2,                 Eunsu%Jang%NULL%0,                 YoungSin%Moon%NULL%2,                 YoungSin%Moon%NULL%0,                 KwangHwan%Oh%NULL%2,                 KwangHwan%Oh%NULL%0,                 JaeRin%Choi%NULL%2,                 JaeRin%Choi%NULL%0,                 Sangeun%Lee%NULL%2,                 Sangeun%Lee%NULL%0,                 Young-Man%Kim%NULL%2,                 Young-Man%Kim%NULL%0,                 Jieun%Kim%NULL%2,                 Jieun%Kim%NULL%0,                 Seonju%Yi%NULL%2,                 Seonju%Yi%NULL%0,                 Jin%Gwack%NULL%2,                 Jin%Gwack%NULL%0,                 Ok%Park%NULL%2,                 Ok%Park%NULL%0,                 Young Joon%Park%NULL%2,                 Young Joon%Park%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Rok%Song%NULL%1,                 Hee-Sook%Kim%NULL%2,                 Hee-Sook%Kim%NULL%0,                 Seok-Ju%Yoo%NULL%2,                 Seok-Ju%Yoo%NULL%0,                 Kwan%Lee%NULL%2,                 Kwan%Lee%NULL%0,                 Ji-Hyuk%Park%NULL%2,                 Ji-Hyuk%Park%NULL%0,                 Joon Ho%Jang%NULL%2,                 Joon Ho%Jang%NULL%0,                 Gyoung-Sook%Ahn%NULL%2,                 Gyoung-Sook%Ahn%NULL%0,                 Jun-Nyun%Kim%NULL%2,                 Jun-Nyun%Kim%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Blanca%Borras-Bermejo%NULL%1,                 Xavier%Martínez-Gómez%NULL%1,                 María Gutierrez%San Miguel%NULL%1,                 Juliana%Esperalba%NULL%1,                 Andrés%Antón%NULL%1,                 Elisabet%Martin%NULL%1,                 Marta%Selvi%NULL%1,                 María José%Abadías%NULL%1,                 Antonio%Román%NULL%1,                 Tomàs%Pumarola%NULL%1,                 Magda%Campins%NULL%1,                 Benito%Almirante%NULL%1]</t>
+  </si>
+  <si>
+    <t>[M.%Bernabeu-Wittel%NULL%1,                 J.E.%Ternero-Vega%NULL%1,                 P.%Díaz-Jiménez%NULL%1,                 C.%Conde-Guzmán%NULL%1,                 M.D.%Nieto-Martín%NULL%1,                 L.%Moreno-Gaviño%NULL%1,                 J.%Delgado-Cuesta%NULL%1,                 M.%Rincón-Gómez%NULL%1,                 L.%Giménez-Miranda%NULL%1,                 M.D.%Navarro-Amuedo%NULL%1,                 M.M.%Muñoz-García%NULL%1,                 S.%Calzón-Fernández%NULL%1,                 M.%Ollero-Baturone%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Shamez N%Ladhani%shamez.ladhani@phe.gov.uk%1,                 J.Yimmy%Chow%NULL%1,                 Roshni%Janarthanan%NULL%1,                 Jonathan%Fok%NULL%1,                 Emma%Crawley-Boevey%NULL%1,                 Amoolya%Vusirikala%NULL%1,                 Elena%Fernandez%NULL%1,                 Marina Sanchez%Perez%NULL%1,                 Suzanne%Tang%NULL%1,                 Kate%Dun-Campbell%NULL%1,                 Edward Wynne-%Evans%NULL%1,                 Anita%Bell%NULL%1,                 Bharat%Patel%NULL%1,                 Zahin%Amin-Chowdhury%NULL%1,                 Felicity%Aiano%NULL%1,                 Karthik%Paranthaman%NULL%1,                 Thomas%Ma%NULL%1,                 Maria%Saavedra-Campos%NULL%1,                 Richard%Myers%NULL%1,                 Joanna%Ellis%NULL%2,                 Angie%Lackenby%NULL%1,                 Robin%Gopal%NULL%1,                 Monika%Patel%NULL%1,                 Colin%Brown%NULL%1,                 Meera%Chand%NULL%1,                 Kevin%Brown%NULL%1,                 Mary E%Ramsay%NULL%1,                 Susan%Hopkins%NULL%2,                 Nandini%Shetty%NULL%1,                 Maria%Zambon%NULL%2]</t>
+  </si>
+  <si>
+    <t>[N.S.N.%Graham%NULL%1,                 C.%Junghans%NULL%1,                 R.%Downes%NULL%1,                 C.%Sendall%NULL%1,                 H.%Lai%NULL%1,                 A.%McKirdy%NULL%1,                 P.%Elliott%NULL%1,                 R.%Howard%NULL%1,                 D.%Wingfield%NULL%1,                 M.%Priestman%NULL%1,                 M.%Ciechonska%NULL%1,                 L.%Cameron%NULL%1,                 M.%Storch%NULL%1,                 M.A.%Crone%NULL%1,                 P.S.%Freemont%NULL%1,                 P.%Randell%NULL%1,                 R.%McLaren%NULL%1,                 N.%Lang%NULL%1,                 S.%Ladhani%NULL%1,                 F.%Sanderson%NULL%1,                 D.J.%Sharp%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Agnes%Marossy%agnesmarossy@nhs.net%1,                 Stefan%Rakowicz%NULL%1,                 Angela%Bhan%NULL%1,                 Sarah%Noon%NULL%1,                 Amanda%Rees%NULL%1,                 Manjinder%Virk%NULL%1,                 Ayazali%Nazafi%NULL%1,                 Evie%Hay%NULL%1,                 Louise%de Thomasson%NULL%1,                 Christina%Windle%NULL%1,                 Mark%Zuckerman%Mark.Zuckerman@nhs.net%1]</t>
+  </si>
+  <si>
+    <t>[Laura%Shallcross%NULL%1,                 Danielle%Burke%NULL%1,                 Owen%Abbott%NULL%1,                 Alasdair%Donaldson%NULL%1,                 Gemma%Hallatt%NULL%1,                 Andrew%Hayward%NULL%1,                 Susan%Hopkins%NULL%0,                 Maria%Krutikov%NULL%1,                 Katie%Sharp%NULL%1,                 Leone%Wardman%NULL%1,                 Sapphira%Thorne%NULL%1]</t>
+  </si>
+  <si>
+    <t>[ E.%Smith%null%1,                  C. F.% Aldus%null%1,                  J.% Brainard%null%1,                  S.% Dunham%null%1,                  P. R.% Hunter%null%1,                  N.% Steel%null%1,                  P. % Everden%null%1]</t>
+  </si>
+  <si>
+    <t>[Mahesh C%Patel%mp3@uic.edu%1,                 Lelia H%Chaisson%NULL%1,                 Scott%Borgetti%NULL%1,                 Deborah%Burdsall%NULL%1,                 Rashmi K%Chugh%NULL%1,                 Christopher R%Hoff%NULL%1,                 Elizabeth B%Murphy%NULL%1,                 Emily A%Murskyj%NULL%1,                 Shannon%Wilson%NULL%1,                 Joe%Ramos%NULL%1,                 Lynn%Akker%NULL%1,                 Debra%Bryars%NULL%1,                 Evonda%Thomas-Smith%NULL%1,                 Susan C%Bleasdale%NULL%1,                 Ngozi O%Ezike%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Helena%Temkin‐Greener%helena_temkin-greener@urmc.rochester.edu%1,                 Wenhan%Guo%NULL%2,                 Wenhan%Guo%NULL%0,                 Yunjiao%Mao%NULL%1,                 Xueya%Cai%NULL%1,                 Yue%Li%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Ana A.%Weil%anaweil@uw.edu%1,                 Kira L.%Newman%NULL%2,                 Kira L.%Newman%NULL%0,                 Thuan D.%Ong%NULL%1,                 Giana H.%Davidson%NULL%1,                 Jennifer%Logue%NULL%1,                 Elisabeth%Brandstetter%NULL%1,                 Ariana%Magedson%NULL%1,                 Dylan%McDonald%NULL%1,                 Denise J.%McCulloch%NULL%1,                 Santiago%Neme%NULL%1,                 James%Lewis%NULL%0,                 Jeff S.%Duchin%NULL%1,                 Weizhi%Zhong%NULL%1,                 Lea M.%Starita%NULL%1,                 Trevor%Bedford%NULL%1,                 Alison C.%Roxby%NULL%1,                 Helen Y.%Chu%helenchu@uw.edu%2]</t>
+  </si>
+  <si>
+    <t>[Guillermo V.%Sanchez%NULL%1,                 Caitlin%Biedron%NULL%1,                 Lauren R.%Fink%NULL%1,                 Kelly M.%Hatfield%NULL%1,                 Jordan Micah F.%Polistico%NULL%1,                 Monica P.%Meyer%NULL%1,                 Rebecca S.%Noe%NULL%1,                 Casey E.%Copen%NULL%1,                 Amanda K.%Lyons%NULL%1,                 Gonzalo%Gonzalez%NULL%1,                 Keith%Kiama%NULL%1,                 Mark%Lebednick%NULL%1,                 Bonnie K.%Czander%NULL%1,                 Amen%Agbonze%NULL%1,                 Aimee R.%Surma%NULL%1,                 Avnish%Sandhu%NULL%1,                 Valerie H.%Mika%NULL%1,                 Tyler%Prentiss%NULL%1,                 John%Zervos%NULL%1,                 Donia A.%Dalal%NULL%1,                 Amber M.%Vasquez%NULL%1,                 Sujan C.%Reddy%NULL%0,                 John%Jernigan%NULL%1,                 Paul E.%Kilgore%NULL%1,                 Marcus J.%Zervos%NULL%1,                 Teena%Chopra%NULL%1,                 Carla P.%Bezold%NULL%1,                 Najibah K.%Rehman%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Janice K%Louie%Janice.louie@sfdph.org%1,                 Hyman M%Scott%NULL%1,                 Amie%DuBois%NULL%1,                 Natalya%Sturtz%NULL%1,                 Wendy%Lu%NULL%1,                 Juliet%Stoltey%NULL%1,                 Godfred%Masinde%NULL%1,                 Stephanie%Cohen%NULL%1,                 Darpun%Sachdev%NULL%1,                 Susan%Philip%NULL%1,                 Naveena%Bobba%NULL%1,                 Tomas%Aragon%NULL%1,                 NULL%NULL%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Scott A%Goldberg%sagoldberg@bwh.harvard.edu%1,                 Jochen%Lennerz%NULL%1,                 Michael%Klompas%NULL%1,                 Eden%Mark%NULL%1,                 Virginia M%Pierce%NULL%1,                 Ryan W%Thompson%NULL%1,                 Charles T%Pu%NULL%1,                 Lauren L%Ritterhouse%NULL%1,                 Anand%Dighe%NULL%1,                 Eric S%Rosenberg%NULL%1,                 David C%Grabowski%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Amy V.%Dora%NULL%1,                 Alexander%Winnett%NULL%1,                 Lauren P.%Jatt%NULL%1,                 Kusha%Davar%NULL%1,                 Mika%Watanabe%NULL%1,                 Linda%Sohn%NULL%1,                 Hannah S.%Kern%NULL%1,                 Christopher J.%Graber%NULL%1,                 Matthew B.%Goetz%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Benjamin F.%Bigelow%NULL%1,                 Olive%Tang%NULL%1,                 Gregory R.%Toci%NULL%1,                 Norberth%Stracker%NULL%1,                 Fatima%Sheikh%NULL%1,                 Kara M.%Jacobs Slifka%NULL%1,                 Shannon A.%Novosad%NULL%1,                 John A.%Jernigan%NULL%0,                 Sujan C.%Reddy%NULL%0,                 Morgan J.%Katz%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Matt%Feaster%NULL%1,                 Ying-Ying%Goh%NULL%1]</t>
+  </si>
+  <si>
+    <t>[William R.%Mills%NULL%1,                 Janet M.%Buccola%NULL%1,                 Susan%Sender%NULL%1,                 Joseph%Lichtefeld%NULL%1,                 Nicholas%Romano%NULL%1,                 Karen%Reynolds%NULL%1,                 Melissa%Price%NULL%1,                 Jennifer%Phipps%NULL%1,                 Leigh%White%NULL%1,                 Shauen%Howard%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Drew A.%Harris%xref no email%1,           Laurie%Archbald-Pannone%xref no email%1,           Jasveen%Kaur%xref no email%1,           David%Cattell-Gordon%xref no email%1,           Karen S.%Rheuban%xref no email%1,           Rachel L.%Ombres%xref no email%1,           Kimberly%Albero%xref no email%1,           Rebecca%Steele%xref no email%1,           Taison D.%Bell%xref no email%1,           Justin B.%Mutter%xref no email%1]</t>
+  </si>
+  <si>
+    <t>[Carl D.%Shrader%xref no email%1,           Shauna%Assadzandi%xref no email%1,           Courtney S.%Pilkerton%xref no email%1,           Amie M.%Ashcraft%xref no email%1]</t>
   </si>
 </sst>
 </file>
@@ -1953,7 +2076,7 @@
         <v>59</v>
       </c>
       <c r="E2" t="s">
-        <v>367</v>
+        <v>408</v>
       </c>
       <c r="F2" t="s">
         <v>60</v>
@@ -1982,7 +2105,7 @@
         <v>64</v>
       </c>
       <c r="E3" t="s">
-        <v>368</v>
+        <v>409</v>
       </c>
       <c r="F3" t="s">
         <v>65</v>
@@ -2011,7 +2134,7 @@
         <v>67</v>
       </c>
       <c r="E4" t="s">
-        <v>369</v>
+        <v>410</v>
       </c>
       <c r="F4" t="s">
         <v>68</v>
@@ -2069,7 +2192,7 @@
         <v>70</v>
       </c>
       <c r="E6" t="s">
-        <v>370</v>
+        <v>411</v>
       </c>
       <c r="F6" t="s">
         <v>6</v>
@@ -2098,7 +2221,7 @@
         <v>73</v>
       </c>
       <c r="E7" t="s">
-        <v>371</v>
+        <v>412</v>
       </c>
       <c r="F7" t="s">
         <v>74</v>
@@ -2127,7 +2250,7 @@
         <v>76</v>
       </c>
       <c r="E8" t="s">
-        <v>372</v>
+        <v>413</v>
       </c>
       <c r="F8" t="s">
         <v>77</v>
@@ -2185,7 +2308,7 @@
         <v>79</v>
       </c>
       <c r="E10" t="s">
-        <v>373</v>
+        <v>414</v>
       </c>
       <c r="F10" t="s">
         <v>80</v>
@@ -2214,7 +2337,7 @@
         <v>83</v>
       </c>
       <c r="E11" t="s">
-        <v>374</v>
+        <v>415</v>
       </c>
       <c r="F11" t="s">
         <v>84</v>
@@ -2243,7 +2366,7 @@
         <v>88</v>
       </c>
       <c r="E12" t="s">
-        <v>375</v>
+        <v>416</v>
       </c>
       <c r="F12" t="s">
         <v>89</v>
@@ -2301,7 +2424,7 @@
         <v>91</v>
       </c>
       <c r="E14" t="s">
-        <v>376</v>
+        <v>417</v>
       </c>
       <c r="F14" t="s">
         <v>92</v>
@@ -2330,7 +2453,7 @@
         <v>95</v>
       </c>
       <c r="E15" t="s">
-        <v>377</v>
+        <v>418</v>
       </c>
       <c r="F15" t="s">
         <v>96</v>
@@ -2359,7 +2482,7 @@
         <v>99</v>
       </c>
       <c r="E16" t="s">
-        <v>378</v>
+        <v>419</v>
       </c>
       <c r="F16" t="s">
         <v>100</v>
@@ -2388,7 +2511,7 @@
         <v>190</v>
       </c>
       <c r="E17" t="s">
-        <v>379</v>
+        <v>420</v>
       </c>
       <c r="F17" t="s">
         <v>16</v>
@@ -2446,7 +2569,7 @@
         <v>51</v>
       </c>
       <c r="E19" t="s">
-        <v>380</v>
+        <v>421</v>
       </c>
       <c r="F19" t="s">
         <v>18</v>
@@ -2475,7 +2598,7 @@
         <v>105</v>
       </c>
       <c r="E20" t="s">
-        <v>381</v>
+        <v>422</v>
       </c>
       <c r="F20" t="s">
         <v>106</v>
@@ -2504,7 +2627,7 @@
         <v>109</v>
       </c>
       <c r="E21" t="s">
-        <v>382</v>
+        <v>423</v>
       </c>
       <c r="F21" t="s">
         <v>110</v>
@@ -2533,7 +2656,7 @@
         <v>112</v>
       </c>
       <c r="E22" t="s">
-        <v>383</v>
+        <v>424</v>
       </c>
       <c r="F22" t="s">
         <v>113</v>
@@ -2591,7 +2714,7 @@
         <v>115</v>
       </c>
       <c r="E24" t="s">
-        <v>384</v>
+        <v>425</v>
       </c>
       <c r="F24" t="s">
         <v>23</v>
@@ -2620,7 +2743,7 @@
         <v>118</v>
       </c>
       <c r="E25" t="s">
-        <v>385</v>
+        <v>426</v>
       </c>
       <c r="F25" t="s">
         <v>119</v>
@@ -2649,7 +2772,7 @@
         <v>51</v>
       </c>
       <c r="E26" t="s">
-        <v>386</v>
+        <v>427</v>
       </c>
       <c r="F26" t="s">
         <v>25</v>
@@ -2678,7 +2801,7 @@
         <v>122</v>
       </c>
       <c r="E27" t="s">
-        <v>387</v>
+        <v>428</v>
       </c>
       <c r="F27" t="s">
         <v>123</v>
@@ -2707,7 +2830,7 @@
         <v>126</v>
       </c>
       <c r="E28" t="s">
-        <v>388</v>
+        <v>429</v>
       </c>
       <c r="F28" t="s">
         <v>127</v>
@@ -2736,7 +2859,7 @@
         <v>130</v>
       </c>
       <c r="E29" t="s">
-        <v>389</v>
+        <v>430</v>
       </c>
       <c r="F29" t="s">
         <v>131</v>
@@ -2765,7 +2888,7 @@
         <v>95</v>
       </c>
       <c r="E30" t="s">
-        <v>390</v>
+        <v>431</v>
       </c>
       <c r="F30" t="s">
         <v>133</v>
@@ -2794,7 +2917,7 @@
         <v>136</v>
       </c>
       <c r="E31" t="s">
-        <v>391</v>
+        <v>432</v>
       </c>
       <c r="F31" t="s">
         <v>137</v>
@@ -2823,7 +2946,7 @@
         <v>140</v>
       </c>
       <c r="E32" t="s">
-        <v>392</v>
+        <v>433</v>
       </c>
       <c r="F32" t="s">
         <v>141</v>
@@ -2852,7 +2975,7 @@
         <v>144</v>
       </c>
       <c r="E33" t="s">
-        <v>393</v>
+        <v>434</v>
       </c>
       <c r="F33" t="s">
         <v>145</v>
@@ -2881,7 +3004,7 @@
         <v>147</v>
       </c>
       <c r="E34" t="s">
-        <v>394</v>
+        <v>435</v>
       </c>
       <c r="F34" t="s">
         <v>148</v>
@@ -2910,7 +3033,7 @@
         <v>150</v>
       </c>
       <c r="E35" t="s">
-        <v>395</v>
+        <v>436</v>
       </c>
       <c r="F35" t="s">
         <v>34</v>
@@ -2939,7 +3062,7 @@
         <v>153</v>
       </c>
       <c r="E36" t="s">
-        <v>396</v>
+        <v>437</v>
       </c>
       <c r="F36" t="s">
         <v>154</v>
@@ -2968,7 +3091,7 @@
         <v>157</v>
       </c>
       <c r="E37" t="s">
-        <v>397</v>
+        <v>438</v>
       </c>
       <c r="F37" t="s">
         <v>158</v>
@@ -2997,7 +3120,7 @@
         <v>201</v>
       </c>
       <c r="E38" t="s">
-        <v>398</v>
+        <v>439</v>
       </c>
       <c r="F38" t="s">
         <v>161</v>
@@ -3026,7 +3149,7 @@
         <v>95</v>
       </c>
       <c r="E39" t="s">
-        <v>399</v>
+        <v>440</v>
       </c>
       <c r="F39" t="s">
         <v>164</v>
@@ -3055,7 +3178,7 @@
         <v>166</v>
       </c>
       <c r="E40" t="s">
-        <v>400</v>
+        <v>441</v>
       </c>
       <c r="F40" t="s">
         <v>167</v>
@@ -3084,7 +3207,7 @@
         <v>169</v>
       </c>
       <c r="E41" t="s">
-        <v>401</v>
+        <v>442</v>
       </c>
       <c r="F41" t="s">
         <v>170</v>
@@ -3113,7 +3236,7 @@
         <v>95</v>
       </c>
       <c r="E42" t="s">
-        <v>402</v>
+        <v>443</v>
       </c>
       <c r="F42" t="s">
         <v>172</v>
@@ -3142,7 +3265,7 @@
         <v>95</v>
       </c>
       <c r="E43" t="s">
-        <v>403</v>
+        <v>444</v>
       </c>
       <c r="F43" t="s">
         <v>174</v>
@@ -3171,7 +3294,7 @@
         <v>176</v>
       </c>
       <c r="E44" t="s">
-        <v>404</v>
+        <v>445</v>
       </c>
       <c r="F44" t="s">
         <v>177</v>
@@ -3200,7 +3323,7 @@
         <v>179</v>
       </c>
       <c r="E45" t="s">
-        <v>405</v>
+        <v>446</v>
       </c>
       <c r="F45" t="s">
         <v>180</v>
@@ -3229,7 +3352,7 @@
         <v>51</v>
       </c>
       <c r="E46" t="s">
-        <v>406</v>
+        <v>447</v>
       </c>
       <c r="F46" t="s">
         <v>45</v>
@@ -3258,7 +3381,7 @@
         <v>199</v>
       </c>
       <c r="E47" t="s">
-        <v>407</v>
+        <v>448</v>
       </c>
       <c r="F47" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
Populated all files with crossref tags, when applicable
</commit_message>
<xml_diff>
--- a/Covid_19_Dataset_and_References/References/10.xlsx
+++ b/Covid_19_Dataset_and_References/References/10.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2023" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2352" uniqueCount="498">
   <si>
     <t>Doi</t>
   </si>
@@ -1735,6 +1735,153 @@
   </si>
   <si>
     <t>[Carl D.%Shrader%xref no email%1,           Shauna%Assadzandi%xref no email%1,           Courtney S.%Pilkerton%xref no email%1,           Amie M.%Ashcraft%xref no email%1]</t>
+  </si>
+  <si>
+    <t>[Daniel J%Escobar%Daniel.escobar@pennmedicine.upenn.edu%1,                  Maria%Lanzi%NULL%1,                  Pouné%Saberi%NULL%1,                  Ruby%Love%NULL%1,                  Darren R%Linkin%NULL%1,                  John J%Kelly%NULL%1,                  Darshana%Jhala%NULL%1,                  Valerianna%Amorosa%NULL%1,                  Mary%Hofmann%NULL%1,                  Jeffrey B%Doyon%NULL%1]</t>
+  </si>
+  <si>
+    <t>_PMC_CROSSREF</t>
+  </si>
+  <si>
+    <t>[James L.%Rudolph%NULL%1,                  Christopher W.%Halladay%NULL%1,                  Malisa%Barber%NULL%1,                  Kevin W.%McConeghy%NULL%1,                  Vince%Mor%NULL%1,                  Aman%Nanda%NULL%1,                  Stefan%Gravenstein%NULL%1]</t>
+  </si>
+  <si>
+    <t>_PMC_elsevier_CROSSREF</t>
+  </si>
+  <si>
+    <t>[Paula%Eckardt%NULL%1,                  Rachel%Guran%NULL%1,                  Jon%Hennemyre%NULL%1,                  Roshan%Arikupurathu%NULL%1,                  Julie%Poveda%NULL%1,                  Nancimae%Miller%NULL%1,                  Randy%Katz%NULL%1,                  Judith%Frum%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Carson%Telford%NULL%1,                  Udodirim%Onwubiko%NULL%1,                  David%Holland%NULL%1,                  Kim%Turner%NULL%1,                  Juliana%Prieto%NULL%1,                  Sasha%Smith%NULL%1,                  Jane%Yoon%NULL%1,                  Wecheeta%Brown%NULL%1,                  Allison%Chamberlain%NULL%1,                  Neel%Gandhi%NULL%1,                  Shamimul%Khan%NULL%1,                  Steve%Williams%NULL%1,                  Fazle%Khan%NULL%1,                  Sarita%Shah%NULL%1,                   C. T.%Telford%null%1,                   U.% Onwubiko%null%1,                   D.% Holland%null%1,                   K.% Turner%null%1,                   J.% Prieto%null%1,                   S.% Smith%null%1,                   J.% Yoon%null%1,                   W.% Brown%null%1,                   A.% Chamberlain%null%1,                   N.% Gandhi%null%1,                   S.% Khan%null%1,                   S.% Williams%null%1,                   F.% Khan%null%1,                   S. % Shah%null%1,                  C. T.%Telford%null%1,                  U.% Onwubiko%null%1,                  D.% Holland%null%1,                  K.% Turner%null%1,                  J.% Prieto%null%1,                  S.% Smith%null%1,                  J.% Yoon%null%1,                  W.% Brown%null%1,                  A.% Chamberlain%null%1,                  N.% Gandhi%null%1,                  S.% Khan%null%1,                  S.% Williams%null%1,                  F.% Khan%null%1,                  S. % Shah%null%1]</t>
+  </si>
+  <si>
+    <t>[Sandra M.%Shi%NULL%1,                  Innokentiy%Bakaev%NULL%1,                  Helen%Chen%NULL%1,                  Thomas G.%Travison%NULL%1,                  Sarah D.%Berry%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Temet M.%McMichael%NULL%0,                  Dustin W.%Currie%NULL%0,                  Shauna%Clark%NULL%0,                  Sargis%Pogosjans%NULL%0,                  Meagan%Kay%NULL%0,                  Noah G.%Schwartz%NULL%0,                  James%Lewis%NULL%0,                  Atar%Baer%NULL%0,                  Vance%Kawakami%NULL%0,                  Margaret D.%Lukoff%NULL%0,                  Jessica%Ferro%NULL%0,                  Claire%Brostrom-Smith%NULL%0,                  Thomas D.%Rea%NULL%1,                  Michael R.%Sayre%NULL%1,                  Francis X.%Riedo%NULL%0,                  Denny%Russell%NULL%0,                  Brian%Hiatt%NULL%0,                  Patricia%Montgomery%NULL%0,                  Agam K.%Rao%NULL%0,                  Eric J.%Chow%NULL%0,                  Farrell%Tobolowsky%NULL%0,                  Michael J.%Hughes%NULL%1,                  Ana C.%Bardossy%NULL%0,                  Lisa P.%Oakley%NULL%0,                  Jesica R.%Jacobs%NULL%0,                  Nimalie D.%Stone%NULL%1,                  Sujan C.%Reddy%NULL%0,                  John A.%Jernigan%NULL%0,                  Margaret A.%Honein%NULL%0,                  Thomas A.%Clark%NULL%0,                  Jeffrey S.%Duchin%NULL%0]</t>
+  </si>
+  <si>
+    <t>_CROSSREF</t>
+  </si>
+  <si>
+    <t>[Nathan M.%Stall%nathan.stall@sinaihealth.ca%1,                  Carolyn%Farquharson%NULL%2,                  Carolyn%Farquharson%NULL%0,                  Chris%Fan‐Lun%NULL%1,                  Lesley%Wiesenfeld%NULL%1,                  Carla A.%Loftus%NULL%1,                  Dylan%Kain%NULL%1,                  Jennie%Johnstone%NULL%1,                  Liz%McCreight%NULL%1,                  Russell D.%Goldman%NULL%1,                  Ramona%Mahtani%NULL%1]</t>
+  </si>
+  <si>
+    <t>[ Nathan M.%Stall%null%1,                   Aaron%Jones%null%1,                   Kevin A.%Brown%null%1,                   Paula A.%Rochon%null%1,                   Andrew P.%Costa%null%1,                  Nathan M.%Stall%null%1,                  Aaron%Jones%null%1,                  Kevin A.%Brown%null%1,                  Paula A.%Rochon%null%1,                  Andrew P.%Costa%null%1]</t>
+  </si>
+  <si>
+    <t>[Hubert%Blain%NULL%1,                  Yves%Rolland%NULL%1,                  Edouard%Tuaillon%NULL%1,                  Nadia%Giacosa%NULL%1,                  Mylène%Albrand%NULL%1,                  Audrey%Jaussent%NULL%1,                  Athanase%Benetos%NULL%1,                  Stéphanie%Miot%NULL%1,                  Jean%Bousquet%NULL%1]</t>
+  </si>
+  <si>
+    <t>"Coronavirus Disease 2019 Outcomes in French Nursing Homes That Implemented Staff Confinement With Residents"</t>
+  </si>
+  <si>
+    <t>[Jo\u00ebl%Belmin%xref no email%1, Nathavy%Um-Din%xref no email%1, Cristiano%Donadio%xref no email%1, Maurizio%Magri%xref no email%1, Quoc Duy%Nghiem%xref no email%1, Bruno%Oquendo%xref no email%1, Sylvie%Pariel%xref no email%1, Carmelo%Lafuente-Lafuente%xref no email%1]</t>
+  </si>
+  <si>
+    <t>2023-05-11</t>
+  </si>
+  <si>
+    <t>[Guillaume%Sacco%NULL%1,                  Gonzague%Foucault%NULL%1,                  Olivier%Briere%NULL%1,                  Cédric%Annweiler%NULL%1]</t>
+  </si>
+  <si>
+    <t>[R.%Guery%NULL%1,                  C.%Delaye%NULL%1,                  N.%Brule%NULL%1,                  V.%Nael%NULL%1,                  L.%Castain%NULL%1,                  F.%Raffi%NULL%1,                  L.%De Decker%NULL%1]</t>
+  </si>
+  <si>
+    <t>[A.%Klein%anke.klein@uke.de%1,                  C.%Edler%NULL%1,                  A.%Fitzek%NULL%1,                  D.%Fröb%NULL%1,                  A.%Heinemann%NULL%1,                  K.%Meißner%NULL%1,                  H.%Mushumba%NULL%1,                  K.%Püschel%NULL%1,                  A. S.%Schröder%NULL%1,                  J. P.%Sperhake%NULL%1,                  F.%Ishorst-Witte%NULL%1,                  M.%Aepfelbacher%NULL%1,                  F.%Heinrich%NULL%1]</t>
+  </si>
+  <si>
+    <t>_PMC_Springer_CROSSREF</t>
+  </si>
+  <si>
+    <t>[Buntinx%Frank%coreGivesNoEmail%1,                Claes%Peter%coreGivesNoEmail%1,                Gulikers%Marjo%coreGivesNoEmail%1,                Jan%De Lepeleire%coreGivesNoEmail%1,                Van%der Elst Michael%coreGivesNoEmail%1,                Van%Elslande Jan%coreGivesNoEmail%1,                Van%Ranst Marc%coreGivesNoEmail%1,                Verbakel%Jan%coreGivesNoEmail%1,                Vernneersch%Pieter%coreGivesNoEmail%1]</t>
+  </si>
+  <si>
+    <t>[Liangcong%Hu%xref no email%1,            Wanyuan%Zhen%xref no email%1,            Xudong%Xie%xref no email%2,            Ze%Lin%xref no email%2,            Tiantian%Wang%xref no email%1,            Jing%Liu%xref no email%5,            Hang%Xue%xref no email%2,            Adriana C.%Panayi%xref no email%2,            Ke%Xu%xref no email%1,            Zexi%Ling%xref no email%1,            Xugui%Li%xref no email%1,            Bobin%Mi%xref no email%1,            Wu%Zhou%xref no email%2,            Guohui%Liu%xref no email%2]</t>
+  </si>
+  <si>
+    <t>[Sean P%Kennelly%Sean.Kennelly@tuh.ie%1,                  Adam H%Dyer%dyera@tcd.ie%1,                  Claire%Noonan%claire.noonan@tuh.ie%2,                  Claire%Noonan%claire.noonan@tuh.ie%0,                  Ruth%Martin%ruth.martin1@hse.ie%1,                  Siobhan M%Kennelly%siobhan.kennelly1@hse.ie%1,                  Alan%Martin%alanmartin@beaumont.ie%1,                  Desmond%O’Neill%NULL%1,                  Aoife%Fallon%aoife.fallon1@hotmail.com%1]</t>
+  </si>
+  <si>
+    <t>[Antonio%Nouvenne%NULL%1,                  Andrea%Ticinesi%NULL%1,                  Alberto%Parise%NULL%1,                  Beatrice%Prati%NULL%1,                  Marcello%Esposito%NULL%1,                  Valentina%Cocchi%NULL%1,                  Emanuele%Crisafulli%NULL%1,                  Annalisa%Volpi%NULL%1,                  Sandra%Rossi%NULL%1,                  Elena Giovanna%Bignami%NULL%1,                  Marco%Baciarello%NULL%1,                  Ettore%Brianti%NULL%1,                  Massimo%Fabi%NULL%1,                  Tiziana%Meschi%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Nicola%Veronese%NULL%1,                  Luca Gino%Sbrogiò%NULL%1,                  Roberto%Valle%NULL%1,                  Laura%Marin%NULL%1,                  Elena%Boscolo Fiore%NULL%1,                  Andrea%Tiozzo%NULL%1]</t>
+  </si>
+  <si>
+    <t>[ J. H.%van den Besselaar%null%1,                   R. S.% Sikkema%null%1,                   F. M. H. P. A.% Koene%null%1,                   L. W.% van Buul%null%1,                   B. B.% Oude Munnink%null%1,                   I.% Frenay%null%1,                   R.% te Witt%null%1,                   M. P. G.% Koopmans%null%1,                   C. M. P. M.% Hertogh%null%1,                   B. M. % Buurman%null%1]</t>
+  </si>
+  <si>
+    <t>_MedBiorxiv_CROSSREF</t>
+  </si>
+  <si>
+    <t>[Laura W.%van Buul%NULL%1,                  Judith H.%van den Besselaar%NULL%2,                  Judith H.%van den Besselaar%NULL%0,                  Fleur M. H. P. H.%Koene%NULL%1,                  Bianca M.%Buurman%NULL%1,                  Cees M. P. M.%Hertogh%NULL%1,                  Martin%Smalbrugge%NULL%1,                  Jeanine J. S.%Rutten%NULL%1,                  Elke M.%den Boogert%NULL%1,                  Michel D.%Wissing%NULL%1,                  Ariene%Rietveld%NULL%1,                  Mariska W. W.%van Elsakker%NULL%1,                  Marga M. G.%Nonneman%NULL%1,                  Florien%van Eeden%NULL%1,                  Saskia%van de Merwe%NULL%1,                  Sophie L.%Niemansburg%NULL%1,                  Ewout%Fanoy%NULL%1,                  Hinke S.%Bootsma%NULL%1,                  Nicoline%van der Hagen%NULL%1,                  Mariska%Petrignani%NULL%1,                  Jessica Edwards%van Muijen%NULL%1,                  Karolien E. M.%Biesheuvel%NULL%1]</t>
+  </si>
+  <si>
+    <t>[B\u00e5rd%Reiakvam Kittang%coreGivesNoEmail%1,                Karina%Koller L\u00f8land%coreGivesNoEmail%1,                Kjell%Kr\u00fcger%coreGivesNoEmail%1,                Kristian%Jansen%coreGivesNoEmail%1,                Sabine%Piepenstock Solheim%coreGivesNoEmail%1,                Sebastian%von Hofacker%coreGivesNoEmail%1]</t>
+  </si>
+  <si>
+    <t>[Shin Young%Park%NULL%1,                  Gawon%Choi%NULL%2,                  Gawon%Choi%NULL%0,                  Hyeyoung%Lee%NULL%2,                  Hyeyoung%Lee%NULL%0,                  Na-young%Kim%NULL%2,                  Na-young%Kim%NULL%0,                  Seon-young%Lee%NULL%2,                  Seon-young%Lee%NULL%0,                  Kyungnam%Kim%NULL%2,                  Kyungnam%Kim%NULL%0,                  Soyoung%Shin%NULL%2,                  Soyoung%Shin%NULL%0,                  Eunsu%Jang%NULL%2,                  Eunsu%Jang%NULL%0,                  YoungSin%Moon%NULL%2,                  YoungSin%Moon%NULL%0,                  KwangHwan%Oh%NULL%2,                  KwangHwan%Oh%NULL%0,                  JaeRin%Choi%NULL%2,                  JaeRin%Choi%NULL%0,                  Sangeun%Lee%NULL%2,                  Sangeun%Lee%NULL%0,                  Young-Man%Kim%NULL%2,                  Young-Man%Kim%NULL%0,                  Jieun%Kim%NULL%2,                  Jieun%Kim%NULL%0,                  Seonju%Yi%NULL%2,                  Seonju%Yi%NULL%0,                  Jin%Gwack%NULL%2,                  Jin%Gwack%NULL%0,                  Ok%Park%NULL%2,                  Ok%Park%NULL%0,                  Young Joon%Park%NULL%2,                  Young Joon%Park%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Rok%Song%NULL%1,                  Hee-Sook%Kim%NULL%2,                  Hee-Sook%Kim%NULL%0,                  Seok-Ju%Yoo%NULL%2,                  Seok-Ju%Yoo%NULL%0,                  Kwan%Lee%NULL%2,                  Kwan%Lee%NULL%0,                  Ji-Hyuk%Park%NULL%2,                  Ji-Hyuk%Park%NULL%0,                  Joon Ho%Jang%NULL%2,                  Joon Ho%Jang%NULL%0,                  Gyoung-Sook%Ahn%NULL%2,                  Gyoung-Sook%Ahn%NULL%0,                  Jun-Nyun%Kim%NULL%2,                  Jun-Nyun%Kim%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Blanca%Borras-Bermejo%NULL%1,                  Xavier%Martínez-Gómez%NULL%1,                  María Gutierrez%San Miguel%NULL%1,                  Juliana%Esperalba%NULL%1,                  Andrés%Antón%NULL%1,                  Elisabet%Martin%NULL%1,                  Marta%Selvi%NULL%1,                  María José%Abadías%NULL%1,                  Antonio%Román%NULL%1,                  Tomàs%Pumarola%NULL%1,                  Magda%Campins%NULL%1,                  Benito%Almirante%NULL%1]</t>
+  </si>
+  <si>
+    <t>[M.%Bernabeu-Wittel%NULL%1,                  J.E.%Ternero-Vega%NULL%1,                  P.%Díaz-Jiménez%NULL%1,                  C.%Conde-Guzmán%NULL%1,                  M.D.%Nieto-Martín%NULL%1,                  L.%Moreno-Gaviño%NULL%1,                  J.%Delgado-Cuesta%NULL%1,                  M.%Rincón-Gómez%NULL%1,                  L.%Giménez-Miranda%NULL%1,                  M.D.%Navarro-Amuedo%NULL%1,                  M.M.%Muñoz-García%NULL%1,                  S.%Calzón-Fernández%NULL%1,                  M.%Ollero-Baturone%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Shamez N%Ladhani%shamez.ladhani@phe.gov.uk%1,                  J.Yimmy%Chow%NULL%1,                  Roshni%Janarthanan%NULL%1,                  Jonathan%Fok%NULL%1,                  Emma%Crawley-Boevey%NULL%1,                  Amoolya%Vusirikala%NULL%1,                  Elena%Fernandez%NULL%1,                  Marina Sanchez%Perez%NULL%1,                  Suzanne%Tang%NULL%1,                  Kate%Dun-Campbell%NULL%1,                  Edward Wynne-%Evans%NULL%1,                  Anita%Bell%NULL%1,                  Bharat%Patel%NULL%1,                  Zahin%Amin-Chowdhury%NULL%1,                  Felicity%Aiano%NULL%1,                  Karthik%Paranthaman%NULL%1,                  Thomas%Ma%NULL%1,                  Maria%Saavedra-Campos%NULL%1,                  Richard%Myers%NULL%1,                  Joanna%Ellis%NULL%2,                  Angie%Lackenby%NULL%1,                  Robin%Gopal%NULL%1,                  Monika%Patel%NULL%1,                  Colin%Brown%NULL%1,                  Meera%Chand%NULL%1,                  Kevin%Brown%NULL%1,                  Mary E%Ramsay%NULL%1,                  Susan%Hopkins%NULL%2,                  Nandini%Shetty%NULL%1,                  Maria%Zambon%NULL%2]</t>
+  </si>
+  <si>
+    <t>[N.S.N.%Graham%NULL%1,                  C.%Junghans%NULL%1,                  R.%Downes%NULL%1,                  C.%Sendall%NULL%1,                  H.%Lai%NULL%1,                  A.%McKirdy%NULL%1,                  P.%Elliott%NULL%1,                  R.%Howard%NULL%1,                  D.%Wingfield%NULL%1,                  M.%Priestman%NULL%1,                  M.%Ciechonska%NULL%1,                  L.%Cameron%NULL%1,                  M.%Storch%NULL%1,                  M.A.%Crone%NULL%1,                  P.S.%Freemont%NULL%1,                  P.%Randell%NULL%1,                  R.%McLaren%NULL%1,                  N.%Lang%NULL%1,                  S.%Ladhani%NULL%1,                  F.%Sanderson%NULL%1,                  D.J.%Sharp%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Agnes%Marossy%agnesmarossy@nhs.net%1,                  Stefan%Rakowicz%NULL%1,                  Angela%Bhan%NULL%1,                  Sarah%Noon%NULL%1,                  Amanda%Rees%NULL%1,                  Manjinder%Virk%NULL%1,                  Ayazali%Nazafi%NULL%1,                  Evie%Hay%NULL%1,                  Louise%de Thomasson%NULL%1,                  Christina%Windle%NULL%1,                  Mark%Zuckerman%Mark.Zuckerman@nhs.net%1]</t>
+  </si>
+  <si>
+    <t>[Laura%Shallcross%NULL%1,                  Danielle%Burke%NULL%1,                  Owen%Abbott%NULL%1,                  Alasdair%Donaldson%NULL%1,                  Gemma%Hallatt%NULL%1,                  Andrew%Hayward%NULL%1,                  Susan%Hopkins%NULL%0,                  Maria%Krutikov%NULL%1,                  Katie%Sharp%NULL%1,                  Leone%Wardman%NULL%1,                  Sapphira%Thorne%NULL%1]</t>
+  </si>
+  <si>
+    <t>[ E.%Smith%null%1,                   C. F.% Aldus%null%1,                   J.% Brainard%null%1,                   S.% Dunham%null%1,                   P. R.% Hunter%null%1,                   N.% Steel%null%1,                   P. % Everden%null%1]</t>
+  </si>
+  <si>
+    <t>[Mahesh C%Patel%mp3@uic.edu%1,                  Lelia H%Chaisson%NULL%1,                  Scott%Borgetti%NULL%1,                  Deborah%Burdsall%NULL%1,                  Rashmi K%Chugh%NULL%1,                  Christopher R%Hoff%NULL%1,                  Elizabeth B%Murphy%NULL%1,                  Emily A%Murskyj%NULL%1,                  Shannon%Wilson%NULL%1,                  Joe%Ramos%NULL%1,                  Lynn%Akker%NULL%1,                  Debra%Bryars%NULL%1,                  Evonda%Thomas-Smith%NULL%1,                  Susan C%Bleasdale%NULL%1,                  Ngozi O%Ezike%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Helena%Temkin‐Greener%helena_temkin-greener@urmc.rochester.edu%1,                  Wenhan%Guo%NULL%2,                  Wenhan%Guo%NULL%0,                  Yunjiao%Mao%NULL%1,                  Xueya%Cai%NULL%1,                  Yue%Li%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Ana A.%Weil%anaweil@uw.edu%1,                  Kira L.%Newman%NULL%2,                  Kira L.%Newman%NULL%0,                  Thuan D.%Ong%NULL%1,                  Giana H.%Davidson%NULL%1,                  Jennifer%Logue%NULL%1,                  Elisabeth%Brandstetter%NULL%1,                  Ariana%Magedson%NULL%1,                  Dylan%McDonald%NULL%1,                  Denise J.%McCulloch%NULL%1,                  Santiago%Neme%NULL%1,                  James%Lewis%NULL%0,                  Jeff S.%Duchin%NULL%1,                  Weizhi%Zhong%NULL%1,                  Lea M.%Starita%NULL%1,                  Trevor%Bedford%NULL%1,                  Alison C.%Roxby%NULL%1,                  Helen Y.%Chu%helenchu@uw.edu%2]</t>
+  </si>
+  <si>
+    <t>[Guillermo V.%Sanchez%NULL%1,                  Caitlin%Biedron%NULL%1,                  Lauren R.%Fink%NULL%1,                  Kelly M.%Hatfield%NULL%1,                  Jordan Micah F.%Polistico%NULL%1,                  Monica P.%Meyer%NULL%1,                  Rebecca S.%Noe%NULL%1,                  Casey E.%Copen%NULL%1,                  Amanda K.%Lyons%NULL%1,                  Gonzalo%Gonzalez%NULL%1,                  Keith%Kiama%NULL%1,                  Mark%Lebednick%NULL%1,                  Bonnie K.%Czander%NULL%1,                  Amen%Agbonze%NULL%1,                  Aimee R.%Surma%NULL%1,                  Avnish%Sandhu%NULL%1,                  Valerie H.%Mika%NULL%1,                  Tyler%Prentiss%NULL%1,                  John%Zervos%NULL%1,                  Donia A.%Dalal%NULL%1,                  Amber M.%Vasquez%NULL%1,                  Sujan C.%Reddy%NULL%0,                  John%Jernigan%NULL%1,                  Paul E.%Kilgore%NULL%1,                  Marcus J.%Zervos%NULL%1,                  Teena%Chopra%NULL%1,                  Carla P.%Bezold%NULL%1,                  Najibah K.%Rehman%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Janice K%Louie%Janice.louie@sfdph.org%1,                  Hyman M%Scott%NULL%1,                  Amie%DuBois%NULL%1,                  Natalya%Sturtz%NULL%1,                  Wendy%Lu%NULL%1,                  Juliet%Stoltey%NULL%1,                  Godfred%Masinde%NULL%1,                  Stephanie%Cohen%NULL%1,                  Darpun%Sachdev%NULL%1,                  Susan%Philip%NULL%1,                  Naveena%Bobba%NULL%1,                  Tomas%Aragon%NULL%1,                  NULL%NULL%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Scott A%Goldberg%sagoldberg@bwh.harvard.edu%1,                  Jochen%Lennerz%NULL%1,                  Michael%Klompas%NULL%1,                  Eden%Mark%NULL%1,                  Virginia M%Pierce%NULL%1,                  Ryan W%Thompson%NULL%1,                  Charles T%Pu%NULL%1,                  Lauren L%Ritterhouse%NULL%1,                  Anand%Dighe%NULL%1,                  Eric S%Rosenberg%NULL%1,                  David C%Grabowski%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Amy V.%Dora%NULL%1,                  Alexander%Winnett%NULL%1,                  Lauren P.%Jatt%NULL%1,                  Kusha%Davar%NULL%1,                  Mika%Watanabe%NULL%1,                  Linda%Sohn%NULL%1,                  Hannah S.%Kern%NULL%1,                  Christopher J.%Graber%NULL%1,                  Matthew B.%Goetz%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Benjamin F.%Bigelow%NULL%1,                  Olive%Tang%NULL%1,                  Gregory R.%Toci%NULL%1,                  Norberth%Stracker%NULL%1,                  Fatima%Sheikh%NULL%1,                  Kara M.%Jacobs Slifka%NULL%1,                  Shannon A.%Novosad%NULL%1,                  John A.%Jernigan%NULL%0,                  Sujan C.%Reddy%NULL%0,                  Morgan J.%Katz%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Matt%Feaster%NULL%1,                  Ying-Ying%Goh%NULL%1]</t>
+  </si>
+  <si>
+    <t>[William R.%Mills%NULL%1,                  Janet M.%Buccola%NULL%1,                  Susan%Sender%NULL%1,                  Joseph%Lichtefeld%NULL%1,                  Nicholas%Romano%NULL%1,                  Karen%Reynolds%NULL%1,                  Melissa%Price%NULL%1,                  Jennifer%Phipps%NULL%1,                  Leigh%White%NULL%1,                  Shauen%Howard%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Drew A.%Harris%xref no email%1,            Laurie%Archbald-Pannone%xref no email%1,            Jasveen%Kaur%xref no email%1,            David%Cattell-Gordon%xref no email%1,            Karen S.%Rheuban%xref no email%1,            Rachel L.%Ombres%xref no email%1,            Kimberly%Albero%xref no email%1,            Rebecca%Steele%xref no email%1,            Taison D.%Bell%xref no email%1,            Justin B.%Mutter%xref no email%1]</t>
+  </si>
+  <si>
+    <t>[Carl D.%Shrader%xref no email%1,            Shauna%Assadzandi%xref no email%1,            Courtney S.%Pilkerton%xref no email%1,            Amie M.%Ashcraft%xref no email%1]</t>
   </si>
 </sst>
 </file>
@@ -2076,7 +2223,7 @@
         <v>59</v>
       </c>
       <c r="E2" t="s">
-        <v>408</v>
+        <v>449</v>
       </c>
       <c r="F2" t="s">
         <v>60</v>
@@ -2088,7 +2235,7 @@
         <v>62</v>
       </c>
       <c r="I2" t="s">
-        <v>182</v>
+        <v>450</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -2105,7 +2252,7 @@
         <v>64</v>
       </c>
       <c r="E3" t="s">
-        <v>409</v>
+        <v>451</v>
       </c>
       <c r="F3" t="s">
         <v>65</v>
@@ -2117,7 +2264,7 @@
         <v>62</v>
       </c>
       <c r="I3" t="s">
-        <v>183</v>
+        <v>452</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -2134,7 +2281,7 @@
         <v>67</v>
       </c>
       <c r="E4" t="s">
-        <v>410</v>
+        <v>453</v>
       </c>
       <c r="F4" t="s">
         <v>68</v>
@@ -2146,7 +2293,7 @@
         <v>62</v>
       </c>
       <c r="I4" t="s">
-        <v>183</v>
+        <v>452</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -2192,7 +2339,7 @@
         <v>70</v>
       </c>
       <c r="E6" t="s">
-        <v>411</v>
+        <v>454</v>
       </c>
       <c r="F6" t="s">
         <v>6</v>
@@ -2204,7 +2351,7 @@
         <v>71</v>
       </c>
       <c r="I6" t="s">
-        <v>182</v>
+        <v>450</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -2221,7 +2368,7 @@
         <v>73</v>
       </c>
       <c r="E7" t="s">
-        <v>412</v>
+        <v>455</v>
       </c>
       <c r="F7" t="s">
         <v>74</v>
@@ -2233,7 +2380,7 @@
         <v>62</v>
       </c>
       <c r="I7" t="s">
-        <v>183</v>
+        <v>452</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -2250,7 +2397,7 @@
         <v>76</v>
       </c>
       <c r="E8" t="s">
-        <v>413</v>
+        <v>456</v>
       </c>
       <c r="F8" t="s">
         <v>77</v>
@@ -2262,7 +2409,7 @@
         <v>62</v>
       </c>
       <c r="I8" t="s">
-        <v>182</v>
+        <v>450</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -2291,7 +2438,7 @@
         <v>62</v>
       </c>
       <c r="I9" t="s">
-        <v>95</v>
+        <v>457</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -2308,7 +2455,7 @@
         <v>79</v>
       </c>
       <c r="E10" t="s">
-        <v>414</v>
+        <v>458</v>
       </c>
       <c r="F10" t="s">
         <v>80</v>
@@ -2320,7 +2467,7 @@
         <v>81</v>
       </c>
       <c r="I10" t="s">
-        <v>182</v>
+        <v>450</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -2337,7 +2484,7 @@
         <v>83</v>
       </c>
       <c r="E11" t="s">
-        <v>415</v>
+        <v>459</v>
       </c>
       <c r="F11" t="s">
         <v>84</v>
@@ -2349,7 +2496,7 @@
         <v>86</v>
       </c>
       <c r="I11" t="s">
-        <v>95</v>
+        <v>457</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -2366,7 +2513,7 @@
         <v>88</v>
       </c>
       <c r="E12" t="s">
-        <v>416</v>
+        <v>460</v>
       </c>
       <c r="F12" t="s">
         <v>89</v>
@@ -2378,7 +2525,7 @@
         <v>62</v>
       </c>
       <c r="I12" t="s">
-        <v>183</v>
+        <v>452</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -2389,22 +2536,22 @@
         <v>44046</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>461</v>
       </c>
       <c r="D13" t="s">
         <v>51</v>
       </c>
       <c r="E13" t="s">
-        <v>54</v>
+        <v>462</v>
       </c>
       <c r="F13" t="s">
-        <v>55</v>
+        <v>243</v>
       </c>
       <c r="G13" t="s">
-        <v>56</v>
+        <v>194</v>
       </c>
       <c r="H13" t="s">
-        <v>62</v>
+        <v>463</v>
       </c>
       <c r="I13" t="s">
         <v>95</v>
@@ -2424,7 +2571,7 @@
         <v>91</v>
       </c>
       <c r="E14" t="s">
-        <v>417</v>
+        <v>464</v>
       </c>
       <c r="F14" t="s">
         <v>92</v>
@@ -2436,7 +2583,7 @@
         <v>93</v>
       </c>
       <c r="I14" t="s">
-        <v>183</v>
+        <v>452</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -2453,7 +2600,7 @@
         <v>95</v>
       </c>
       <c r="E15" t="s">
-        <v>418</v>
+        <v>465</v>
       </c>
       <c r="F15" t="s">
         <v>96</v>
@@ -2465,7 +2612,7 @@
         <v>97</v>
       </c>
       <c r="I15" t="s">
-        <v>183</v>
+        <v>452</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -2482,7 +2629,7 @@
         <v>99</v>
       </c>
       <c r="E16" t="s">
-        <v>419</v>
+        <v>466</v>
       </c>
       <c r="F16" t="s">
         <v>100</v>
@@ -2494,7 +2641,7 @@
         <v>62</v>
       </c>
       <c r="I16" t="s">
-        <v>185</v>
+        <v>467</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -2511,7 +2658,7 @@
         <v>190</v>
       </c>
       <c r="E17" t="s">
-        <v>420</v>
+        <v>468</v>
       </c>
       <c r="F17" t="s">
         <v>16</v>
@@ -2523,7 +2670,7 @@
         <v>62</v>
       </c>
       <c r="I17" t="s">
-        <v>95</v>
+        <v>457</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -2552,7 +2699,7 @@
         <v>62</v>
       </c>
       <c r="I18" t="s">
-        <v>182</v>
+        <v>450</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -2569,7 +2716,7 @@
         <v>51</v>
       </c>
       <c r="E19" t="s">
-        <v>421</v>
+        <v>469</v>
       </c>
       <c r="F19" t="s">
         <v>18</v>
@@ -2581,7 +2728,7 @@
         <v>195</v>
       </c>
       <c r="I19" t="s">
-        <v>95</v>
+        <v>457</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -2598,7 +2745,7 @@
         <v>105</v>
       </c>
       <c r="E20" t="s">
-        <v>422</v>
+        <v>470</v>
       </c>
       <c r="F20" t="s">
         <v>106</v>
@@ -2610,7 +2757,7 @@
         <v>107</v>
       </c>
       <c r="I20" t="s">
-        <v>182</v>
+        <v>450</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
@@ -2627,7 +2774,7 @@
         <v>109</v>
       </c>
       <c r="E21" t="s">
-        <v>423</v>
+        <v>471</v>
       </c>
       <c r="F21" t="s">
         <v>110</v>
@@ -2639,7 +2786,7 @@
         <v>62</v>
       </c>
       <c r="I21" t="s">
-        <v>183</v>
+        <v>452</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -2656,7 +2803,7 @@
         <v>112</v>
       </c>
       <c r="E22" t="s">
-        <v>424</v>
+        <v>472</v>
       </c>
       <c r="F22" t="s">
         <v>113</v>
@@ -2668,7 +2815,7 @@
         <v>62</v>
       </c>
       <c r="I22" t="s">
-        <v>183</v>
+        <v>452</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -2697,7 +2844,7 @@
         <v>62</v>
       </c>
       <c r="I23" t="s">
-        <v>95</v>
+        <v>457</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
@@ -2714,7 +2861,7 @@
         <v>115</v>
       </c>
       <c r="E24" t="s">
-        <v>425</v>
+        <v>473</v>
       </c>
       <c r="F24" t="s">
         <v>23</v>
@@ -2726,7 +2873,7 @@
         <v>116</v>
       </c>
       <c r="I24" t="s">
-        <v>186</v>
+        <v>474</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
@@ -2743,7 +2890,7 @@
         <v>118</v>
       </c>
       <c r="E25" t="s">
-        <v>426</v>
+        <v>475</v>
       </c>
       <c r="F25" t="s">
         <v>119</v>
@@ -2755,7 +2902,7 @@
         <v>120</v>
       </c>
       <c r="I25" t="s">
-        <v>182</v>
+        <v>450</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
@@ -2772,7 +2919,7 @@
         <v>51</v>
       </c>
       <c r="E26" t="s">
-        <v>427</v>
+        <v>476</v>
       </c>
       <c r="F26" t="s">
         <v>25</v>
@@ -2784,7 +2931,7 @@
         <v>62</v>
       </c>
       <c r="I26" t="s">
-        <v>95</v>
+        <v>457</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
@@ -2801,7 +2948,7 @@
         <v>122</v>
       </c>
       <c r="E27" t="s">
-        <v>428</v>
+        <v>477</v>
       </c>
       <c r="F27" t="s">
         <v>123</v>
@@ -2813,7 +2960,7 @@
         <v>124</v>
       </c>
       <c r="I27" t="s">
-        <v>182</v>
+        <v>450</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
@@ -2830,7 +2977,7 @@
         <v>126</v>
       </c>
       <c r="E28" t="s">
-        <v>429</v>
+        <v>478</v>
       </c>
       <c r="F28" t="s">
         <v>127</v>
@@ -2842,7 +2989,7 @@
         <v>128</v>
       </c>
       <c r="I28" t="s">
-        <v>182</v>
+        <v>450</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
@@ -2859,7 +3006,7 @@
         <v>130</v>
       </c>
       <c r="E29" t="s">
-        <v>430</v>
+        <v>479</v>
       </c>
       <c r="F29" t="s">
         <v>131</v>
@@ -2871,7 +3018,7 @@
         <v>62</v>
       </c>
       <c r="I29" t="s">
-        <v>182</v>
+        <v>450</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
@@ -2888,7 +3035,7 @@
         <v>95</v>
       </c>
       <c r="E30" t="s">
-        <v>431</v>
+        <v>480</v>
       </c>
       <c r="F30" t="s">
         <v>133</v>
@@ -2900,7 +3047,7 @@
         <v>134</v>
       </c>
       <c r="I30" t="s">
-        <v>183</v>
+        <v>452</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
@@ -2917,7 +3064,7 @@
         <v>136</v>
       </c>
       <c r="E31" t="s">
-        <v>432</v>
+        <v>481</v>
       </c>
       <c r="F31" t="s">
         <v>137</v>
@@ -2929,7 +3076,7 @@
         <v>138</v>
       </c>
       <c r="I31" t="s">
-        <v>183</v>
+        <v>452</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -2946,7 +3093,7 @@
         <v>140</v>
       </c>
       <c r="E32" t="s">
-        <v>433</v>
+        <v>482</v>
       </c>
       <c r="F32" t="s">
         <v>141</v>
@@ -2958,7 +3105,7 @@
         <v>142</v>
       </c>
       <c r="I32" t="s">
-        <v>183</v>
+        <v>452</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
@@ -2975,7 +3122,7 @@
         <v>144</v>
       </c>
       <c r="E33" t="s">
-        <v>434</v>
+        <v>483</v>
       </c>
       <c r="F33" t="s">
         <v>145</v>
@@ -2987,7 +3134,7 @@
         <v>62</v>
       </c>
       <c r="I33" t="s">
-        <v>182</v>
+        <v>450</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
@@ -3004,7 +3151,7 @@
         <v>147</v>
       </c>
       <c r="E34" t="s">
-        <v>435</v>
+        <v>484</v>
       </c>
       <c r="F34" t="s">
         <v>148</v>
@@ -3016,7 +3163,7 @@
         <v>62</v>
       </c>
       <c r="I34" t="s">
-        <v>183</v>
+        <v>452</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
@@ -3033,7 +3180,7 @@
         <v>150</v>
       </c>
       <c r="E35" t="s">
-        <v>436</v>
+        <v>485</v>
       </c>
       <c r="F35" t="s">
         <v>34</v>
@@ -3045,7 +3192,7 @@
         <v>151</v>
       </c>
       <c r="I35" t="s">
-        <v>186</v>
+        <v>474</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
@@ -3062,7 +3209,7 @@
         <v>153</v>
       </c>
       <c r="E36" t="s">
-        <v>437</v>
+        <v>486</v>
       </c>
       <c r="F36" t="s">
         <v>154</v>
@@ -3074,7 +3221,7 @@
         <v>155</v>
       </c>
       <c r="I36" t="s">
-        <v>182</v>
+        <v>450</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
@@ -3091,7 +3238,7 @@
         <v>157</v>
       </c>
       <c r="E37" t="s">
-        <v>438</v>
+        <v>487</v>
       </c>
       <c r="F37" t="s">
         <v>158</v>
@@ -3103,7 +3250,7 @@
         <v>159</v>
       </c>
       <c r="I37" t="s">
-        <v>182</v>
+        <v>450</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
@@ -3120,7 +3267,7 @@
         <v>201</v>
       </c>
       <c r="E38" t="s">
-        <v>439</v>
+        <v>488</v>
       </c>
       <c r="F38" t="s">
         <v>161</v>
@@ -3132,7 +3279,7 @@
         <v>162</v>
       </c>
       <c r="I38" t="s">
-        <v>185</v>
+        <v>467</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
@@ -3149,7 +3296,7 @@
         <v>95</v>
       </c>
       <c r="E39" t="s">
-        <v>440</v>
+        <v>489</v>
       </c>
       <c r="F39" t="s">
         <v>164</v>
@@ -3161,7 +3308,7 @@
         <v>62</v>
       </c>
       <c r="I39" t="s">
-        <v>182</v>
+        <v>450</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
@@ -3178,7 +3325,7 @@
         <v>166</v>
       </c>
       <c r="E40" t="s">
-        <v>441</v>
+        <v>490</v>
       </c>
       <c r="F40" t="s">
         <v>167</v>
@@ -3190,7 +3337,7 @@
         <v>62</v>
       </c>
       <c r="I40" t="s">
-        <v>182</v>
+        <v>450</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
@@ -3207,7 +3354,7 @@
         <v>169</v>
       </c>
       <c r="E41" t="s">
-        <v>442</v>
+        <v>491</v>
       </c>
       <c r="F41" t="s">
         <v>170</v>
@@ -3219,7 +3366,7 @@
         <v>62</v>
       </c>
       <c r="I41" t="s">
-        <v>182</v>
+        <v>450</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
@@ -3236,7 +3383,7 @@
         <v>95</v>
       </c>
       <c r="E42" t="s">
-        <v>443</v>
+        <v>492</v>
       </c>
       <c r="F42" t="s">
         <v>172</v>
@@ -3248,7 +3395,7 @@
         <v>62</v>
       </c>
       <c r="I42" t="s">
-        <v>182</v>
+        <v>450</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
@@ -3265,7 +3412,7 @@
         <v>95</v>
       </c>
       <c r="E43" t="s">
-        <v>444</v>
+        <v>493</v>
       </c>
       <c r="F43" t="s">
         <v>174</v>
@@ -3277,7 +3424,7 @@
         <v>62</v>
       </c>
       <c r="I43" t="s">
-        <v>182</v>
+        <v>450</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
@@ -3294,7 +3441,7 @@
         <v>176</v>
       </c>
       <c r="E44" t="s">
-        <v>445</v>
+        <v>494</v>
       </c>
       <c r="F44" t="s">
         <v>177</v>
@@ -3306,7 +3453,7 @@
         <v>62</v>
       </c>
       <c r="I44" t="s">
-        <v>182</v>
+        <v>450</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
@@ -3323,7 +3470,7 @@
         <v>179</v>
       </c>
       <c r="E45" t="s">
-        <v>446</v>
+        <v>495</v>
       </c>
       <c r="F45" t="s">
         <v>180</v>
@@ -3335,7 +3482,7 @@
         <v>62</v>
       </c>
       <c r="I45" t="s">
-        <v>183</v>
+        <v>452</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
@@ -3352,7 +3499,7 @@
         <v>51</v>
       </c>
       <c r="E46" t="s">
-        <v>447</v>
+        <v>496</v>
       </c>
       <c r="F46" t="s">
         <v>45</v>
@@ -3364,7 +3511,7 @@
         <v>197</v>
       </c>
       <c r="I46" t="s">
-        <v>95</v>
+        <v>457</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
@@ -3381,7 +3528,7 @@
         <v>199</v>
       </c>
       <c r="E47" t="s">
-        <v>448</v>
+        <v>497</v>
       </c>
       <c r="F47" t="s">
         <v>46</v>
@@ -3393,7 +3540,7 @@
         <v>200</v>
       </c>
       <c r="I47" t="s">
-        <v>95</v>
+        <v>457</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed a bug where a single reference with a field too large (authors/abstract) would cause the entire SLR to not be updated.
</commit_message>
<xml_diff>
--- a/Covid_19_Dataset_and_References/References/10.xlsx
+++ b/Covid_19_Dataset_and_References/References/10.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2681" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4561" uniqueCount="755">
   <si>
     <t>Doi</t>
   </si>
@@ -2008,6 +2008,651 @@
   </si>
   <si>
     <t>[Carl D.%Shrader%xref no email%1,             Shauna%Assadzandi%xref no email%1,             Courtney S.%Pilkerton%xref no email%1,             Amie M.%Ashcraft%xref no email%1]</t>
+  </si>
+  <si>
+    <t>Misc. Data</t>
+  </si>
+  <si>
+    <t>[Daniel J%Escobar%Daniel.escobar@pennmedicine.upenn.edu%1,                    Maria%Lanzi%NULL%1,                    Pouné%Saberi%NULL%1,                    Ruby%Love%NULL%1,                    Darren R%Linkin%NULL%1,                    John J%Kelly%NULL%1,                    Darshana%Jhala%NULL%1,                    Valerianna%Amorosa%NULL%1,                    Mary%Hofmann%NULL%1,                    Jeffrey B%Doyon%NULL%1]</t>
+  </si>
+  <si>
+    <t>[James L.%Rudolph%NULL%1,                    Christopher W.%Halladay%NULL%1,                    Malisa%Barber%NULL%1,                    Kevin W.%McConeghy%NULL%1,                    Vince%Mor%NULL%1,                    Aman%Nanda%NULL%1,                    Stefan%Gravenstein%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Paula%Eckardt%NULL%1,                    Rachel%Guran%NULL%1,                    Jon%Hennemyre%NULL%1,                    Roshan%Arikupurathu%NULL%1,                    Julie%Poveda%NULL%1,                    Nancimae%Miller%NULL%1,                    Randy%Katz%NULL%1,                    Judith%Frum%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Carson%Telford%NULL%1,                    Udodirim%Onwubiko%NULL%1,                    David%Holland%NULL%1,                    Kim%Turner%NULL%1,                    Juliana%Prieto%NULL%1,                    Sasha%Smith%NULL%1,                    Jane%Yoon%NULL%1,                    Wecheeta%Brown%NULL%1,                    Allison%Chamberlain%NULL%1,                    Neel%Gandhi%NULL%1,                    Shamimul%Khan%NULL%1,                    Steve%Williams%NULL%1,                    Fazle%Khan%NULL%1,                    Sarita%Shah%NULL%1,                     C. T.%Telford%null%1,                     U.% Onwubiko%null%1,                     D.% Holland%null%1,                     K.% Turner%null%1,                     J.% Prieto%null%1,                     S.% Smith%null%1,                     J.% Yoon%null%1,                     W.% Brown%null%1,                     A.% Chamberlain%null%1,                     N.% Gandhi%null%1,                     S.% Khan%null%1,                     S.% Williams%null%1,                     F.% Khan%null%1,                     S. % Shah%null%1,                    C. T.%Telford%null%1,                    U.% Onwubiko%null%1,                    D.% Holland%null%1,                    K.% Turner%null%1,                    J.% Prieto%null%1,                    S.% Smith%null%1,                    J.% Yoon%null%1,                    W.% Brown%null%1,                    A.% Chamberlain%null%1,                    N.% Gandhi%null%1,                    S.% Khan%null%1,                    S.% Williams%null%1,                    F.% Khan%null%1,                    S. % Shah%null%1,   C. T.%Telford%null%1,   U.% Onwubiko%null%1,   D.% Holland%null%1,   K.% Turner%null%1,   J.% Prieto%null%1,   S.% Smith%null%1,   J.% Yoon%null%1,   W.% Brown%null%1,   A.% Chamberlain%null%1,   N.% Gandhi%null%1,   S.% Khan%null%1,   S.% Williams%null%1,   F.% Khan%null%1,   S. % Shah%null%1]</t>
+  </si>
+  <si>
+    <t>[Sandra M.%Shi%NULL%1,                    Innokentiy%Bakaev%NULL%1,                    Helen%Chen%NULL%1,                    Thomas G.%Travison%NULL%1,                    Sarah D.%Berry%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Temet M.%McMichael%NULL%0,                    Dustin W.%Currie%NULL%0,                    Shauna%Clark%NULL%0,                    Sargis%Pogosjans%NULL%0,                    Meagan%Kay%NULL%0,                    Noah G.%Schwartz%NULL%0,                    James%Lewis%NULL%0,                    Atar%Baer%NULL%0,                    Vance%Kawakami%NULL%0,                    Margaret D.%Lukoff%NULL%0,                    Jessica%Ferro%NULL%0,                    Claire%Brostrom-Smith%NULL%0,                    Thomas D.%Rea%NULL%1,                    Michael R.%Sayre%NULL%1,                    Francis X.%Riedo%NULL%0,                    Denny%Russell%NULL%0,                    Brian%Hiatt%NULL%0,                    Patricia%Montgomery%NULL%0,                    Agam K.%Rao%NULL%0,                    Eric J.%Chow%NULL%0,                    Farrell%Tobolowsky%NULL%0,                    Michael J.%Hughes%NULL%1,                    Ana C.%Bardossy%NULL%0,                    Lisa P.%Oakley%NULL%0,                    Jesica R.%Jacobs%NULL%0,                    Nimalie D.%Stone%NULL%1,                    Sujan C.%Reddy%NULL%0,                    John A.%Jernigan%NULL%0,                    Margaret A.%Honein%NULL%0,                    Thomas A.%Clark%NULL%0,                    Jeffrey S.%Duchin%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Nathan M.%Stall%nathan.stall@sinaihealth.ca%1,                    Carolyn%Farquharson%NULL%2,                    Carolyn%Farquharson%NULL%0,                    Chris%Fan‐Lun%NULL%1,                    Lesley%Wiesenfeld%NULL%1,                    Carla A.%Loftus%NULL%1,                    Dylan%Kain%NULL%1,                    Jennie%Johnstone%NULL%1,                    Liz%McCreight%NULL%1,                    Russell D.%Goldman%NULL%1,                    Ramona%Mahtani%NULL%1]</t>
+  </si>
+  <si>
+    <t>[ Nathan M.%Stall%null%1,                     Aaron%Jones%null%1,                     Kevin A.%Brown%null%1,                     Paula A.%Rochon%null%1,                     Andrew P.%Costa%null%1,                    Nathan M.%Stall%null%1,                    Aaron%Jones%null%1,                    Kevin A.%Brown%null%1,                    Paula A.%Rochon%null%1,                    Andrew P.%Costa%null%1]</t>
+  </si>
+  <si>
+    <t>[Hubert%Blain%NULL%1,                    Yves%Rolland%NULL%1,                    Edouard%Tuaillon%NULL%1,                    Nadia%Giacosa%NULL%1,                    Mylène%Albrand%NULL%1,                    Audrey%Jaussent%NULL%1,                    Athanase%Benetos%NULL%1,                    Stéphanie%Miot%NULL%1,                    Jean%Bousquet%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Jo\u00ebl%Belmin%xref no email%0, Nathavy%Um-Din%xref no email%1, Cristiano%Donadio%xref no email%1, Maurizio%Magri%xref no email%1, Quoc Duy%Nghiem%xref no email%1, Bruno%Oquendo%xref no email%1, Sylvie%Pariel%xref no email%1, Carmelo%Lafuente-Lafuente%xref no email%1]</t>
+  </si>
+  <si>
+    <t>PUBLISHER: American Medical Association (AMA)</t>
+  </si>
+  <si>
+    <t>[Guillaume%Sacco%NULL%1,                    Gonzague%Foucault%NULL%1,                    Olivier%Briere%NULL%1,                    Cédric%Annweiler%NULL%1]</t>
+  </si>
+  <si>
+    <t>[R.%Guery%NULL%1,                    C.%Delaye%NULL%1,                    N.%Brule%NULL%1,                    V.%Nael%NULL%1,                    L.%Castain%NULL%1,                    F.%Raffi%NULL%1,                    L.%De Decker%NULL%1]</t>
+  </si>
+  <si>
+    <t>[A.%Klein%anke.klein@uke.de%1,                    C.%Edler%NULL%1,                    A.%Fitzek%NULL%1,                    D.%Fröb%NULL%1,                    A.%Heinemann%NULL%1,                    K.%Meißner%NULL%1,                    H.%Mushumba%NULL%1,                    K.%Püschel%NULL%1,                    A. S.%Schröder%NULL%1,                    J. P.%Sperhake%NULL%1,                    F.%Ishorst-Witte%NULL%1,                    M.%Aepfelbacher%NULL%1,                    F.%Heinrich%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Buntinx%Frank%coreGivesNoEmail%1,                  Claes%Peter%coreGivesNoEmail%1,                  Gulikers%Marjo%coreGivesNoEmail%1,                  Jan%De Lepeleire%coreGivesNoEmail%1,                  Van%der Elst Michael%coreGivesNoEmail%1,                  Van%Elslande Jan%coreGivesNoEmail%1,                  Van%Ranst Marc%coreGivesNoEmail%1,                  Verbakel%Jan%coreGivesNoEmail%1,                  Vernneersch%Pieter%coreGivesNoEmail%1]</t>
+  </si>
+  <si>
+    <t>[Liangcong%Hu%xref no email%0, Wanyuan%Zhen%xref no email%1, Xudong%Xie%xref no email%2, Ze%Lin%xref no email%2, Tiantian%Wang%xref no email%1, Jing%Liu%xref no email%0, Hang%Xue%xref no email%2, Adriana C.%Panayi%xref no email%2, Ke%Xu%xref no email%1, Zexi%Ling%xref no email%1, Xugui%Li%xref no email%1, Bobin%Mi%xref no email%0, Wu%Zhou%xref no email%2, Guohui%Liu%xref no email%2]</t>
+  </si>
+  <si>
+    <t>PUBLISHER: Elsevier BV</t>
+  </si>
+  <si>
+    <t>[Sean P%Kennelly%Sean.Kennelly@tuh.ie%1,                    Adam H%Dyer%dyera@tcd.ie%1,                    Claire%Noonan%claire.noonan@tuh.ie%2,                    Claire%Noonan%claire.noonan@tuh.ie%0,                    Ruth%Martin%ruth.martin1@hse.ie%1,                    Siobhan M%Kennelly%siobhan.kennelly1@hse.ie%1,                    Alan%Martin%alanmartin@beaumont.ie%1,                    Desmond%O’Neill%NULL%1,                    Aoife%Fallon%aoife.fallon1@hotmail.com%1]</t>
+  </si>
+  <si>
+    <t>[Antonio%Nouvenne%NULL%1,                    Andrea%Ticinesi%NULL%1,                    Alberto%Parise%NULL%1,                    Beatrice%Prati%NULL%1,                    Marcello%Esposito%NULL%1,                    Valentina%Cocchi%NULL%1,                    Emanuele%Crisafulli%NULL%1,                    Annalisa%Volpi%NULL%1,                    Sandra%Rossi%NULL%1,                    Elena Giovanna%Bignami%NULL%1,                    Marco%Baciarello%NULL%1,                    Ettore%Brianti%NULL%1,                    Massimo%Fabi%NULL%1,                    Tiziana%Meschi%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Nicola%Veronese%NULL%1,                    Luca Gino%Sbrogiò%NULL%1,                    Roberto%Valle%NULL%1,                    Laura%Marin%NULL%1,                    Elena%Boscolo Fiore%NULL%1,                    Andrea%Tiozzo%NULL%1]</t>
+  </si>
+  <si>
+    <t>[ J. H.%van den Besselaar%null%1,                     R. S.% Sikkema%null%1,                     F. M. H. P. A.% Koene%null%1,                     L. W.% van Buul%null%1,                     B. B.% Oude Munnink%null%1,                     I.% Frenay%null%1,                     R.% te Witt%null%1,                     M. P. G.% Koopmans%null%1,                     C. M. P. M.% Hertogh%null%1,                     B. M. % Buurman%null%1,   J. H.%van den Besselaar%null%1,   R. S.% Sikkema%null%1,   F. M. H. P. A.% Koene%null%1,   L. W.% van Buul%null%1,   B. B.% Oude Munnink%null%1,   I.% Frenay%null%1,   R.% te Witt%null%1,   M. P. G.% Koopmans%null%1,   C. M. P. M.% Hertogh%null%1,   B. M. % Buurman%null%1]</t>
+  </si>
+  <si>
+    <t>[Laura W.%van Buul%NULL%1,                    Judith H.%van den Besselaar%NULL%2,                    Judith H.%van den Besselaar%NULL%0,                    Fleur M. H. P. H.%Koene%NULL%1,                    Bianca M.%Buurman%NULL%1,                    Cees M. P. M.%Hertogh%NULL%1,                    Martin%Smalbrugge%NULL%1,                    Jeanine J. S.%Rutten%NULL%1,                    Elke M.%den Boogert%NULL%1,                    Michel D.%Wissing%NULL%1,                    Ariene%Rietveld%NULL%1,                    Mariska W. W.%van Elsakker%NULL%1,                    Marga M. G.%Nonneman%NULL%1,                    Florien%van Eeden%NULL%1,                    Saskia%van de Merwe%NULL%1,                    Sophie L.%Niemansburg%NULL%1,                    Ewout%Fanoy%NULL%1,                    Hinke S.%Bootsma%NULL%1,                    Nicoline%van der Hagen%NULL%1,                    Mariska%Petrignani%NULL%1,                    Jessica Edwards%van Muijen%NULL%1,                    Karolien E. M.%Biesheuvel%NULL%1]</t>
+  </si>
+  <si>
+    <t>[B\u00e5rd%Reiakvam Kittang%coreGivesNoEmail%1,                  Karina%Koller L\u00f8land%coreGivesNoEmail%1,                  Kjell%Kr\u00fcger%coreGivesNoEmail%1,                  Kristian%Jansen%coreGivesNoEmail%1,                  Sabine%Piepenstock Solheim%coreGivesNoEmail%1,                  Sebastian%von Hofacker%coreGivesNoEmail%1]</t>
+  </si>
+  <si>
+    <t>[Shin Young%Park%NULL%1,                    Gawon%Choi%NULL%2,                    Gawon%Choi%NULL%0,                    Hyeyoung%Lee%NULL%2,                    Hyeyoung%Lee%NULL%0,                    Na-young%Kim%NULL%2,                    Na-young%Kim%NULL%0,                    Seon-young%Lee%NULL%2,                    Seon-young%Lee%NULL%0,                    Kyungnam%Kim%NULL%2,                    Kyungnam%Kim%NULL%0,                    Soyoung%Shin%NULL%2,                    Soyoung%Shin%NULL%0,                    Eunsu%Jang%NULL%2,                    Eunsu%Jang%NULL%0,                    YoungSin%Moon%NULL%2,                    YoungSin%Moon%NULL%0,                    KwangHwan%Oh%NULL%2,                    KwangHwan%Oh%NULL%0,                    JaeRin%Choi%NULL%2,                    JaeRin%Choi%NULL%0,                    Sangeun%Lee%NULL%2,                    Sangeun%Lee%NULL%0,                    Young-Man%Kim%NULL%2,                    Young-Man%Kim%NULL%0,                    Jieun%Kim%NULL%2,                    Jieun%Kim%NULL%0,                    Seonju%Yi%NULL%2,                    Seonju%Yi%NULL%0,                    Jin%Gwack%NULL%2,                    Jin%Gwack%NULL%0,                    Ok%Park%NULL%2,                    Ok%Park%NULL%0,                    Young Joon%Park%NULL%2,                    Young Joon%Park%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Rok%Song%NULL%1,                    Hee-Sook%Kim%NULL%2,                    Hee-Sook%Kim%NULL%0,                    Seok-Ju%Yoo%NULL%2,                    Seok-Ju%Yoo%NULL%0,                    Kwan%Lee%NULL%2,                    Kwan%Lee%NULL%0,                    Ji-Hyuk%Park%NULL%2,                    Ji-Hyuk%Park%NULL%0,                    Joon Ho%Jang%NULL%2,                    Joon Ho%Jang%NULL%0,                    Gyoung-Sook%Ahn%NULL%2,                    Gyoung-Sook%Ahn%NULL%0,                    Jun-Nyun%Kim%NULL%2,                    Jun-Nyun%Kim%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Blanca%Borras-Bermejo%NULL%1,                    Xavier%Martínez-Gómez%NULL%1,                    María Gutierrez%San Miguel%NULL%1,                    Juliana%Esperalba%NULL%1,                    Andrés%Antón%NULL%1,                    Elisabet%Martin%NULL%1,                    Marta%Selvi%NULL%1,                    María José%Abadías%NULL%1,                    Antonio%Román%NULL%1,                    Tomàs%Pumarola%NULL%1,                    Magda%Campins%NULL%1,                    Benito%Almirante%NULL%1]</t>
+  </si>
+  <si>
+    <t>[M.%Bernabeu-Wittel%NULL%1,                    J.E.%Ternero-Vega%NULL%1,                    P.%Díaz-Jiménez%NULL%1,                    C.%Conde-Guzmán%NULL%1,                    M.D.%Nieto-Martín%NULL%1,                    L.%Moreno-Gaviño%NULL%1,                    J.%Delgado-Cuesta%NULL%1,                    M.%Rincón-Gómez%NULL%1,                    L.%Giménez-Miranda%NULL%1,                    M.D.%Navarro-Amuedo%NULL%1,                    M.M.%Muñoz-García%NULL%1,                    S.%Calzón-Fernández%NULL%1,                    M.%Ollero-Baturone%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Shamez N%Ladhani%shamez.ladhani@phe.gov.uk%1,                    J.Yimmy%Chow%NULL%1,                    Roshni%Janarthanan%NULL%1,                    Jonathan%Fok%NULL%1,                    Emma%Crawley-Boevey%NULL%1,                    Amoolya%Vusirikala%NULL%1,                    Elena%Fernandez%NULL%1,                    Marina Sanchez%Perez%NULL%1,                    Suzanne%Tang%NULL%1,                    Kate%Dun-Campbell%NULL%1,                    Edward Wynne-%Evans%NULL%1,                    Anita%Bell%NULL%1,                    Bharat%Patel%NULL%1,                    Zahin%Amin-Chowdhury%NULL%1,                    Felicity%Aiano%NULL%1,                    Karthik%Paranthaman%NULL%1,                    Thomas%Ma%NULL%1,                    Maria%Saavedra-Campos%NULL%1,                    Richard%Myers%NULL%1,                    Joanna%Ellis%NULL%2,                    Angie%Lackenby%NULL%1,                    Robin%Gopal%NULL%1,                    Monika%Patel%NULL%1,                    Colin%Brown%NULL%1,                    Meera%Chand%NULL%1,                    Kevin%Brown%NULL%1,                    Mary E%Ramsay%NULL%1,                    Susan%Hopkins%NULL%2,                    Nandini%Shetty%NULL%1,                    Maria%Zambon%NULL%2]</t>
+  </si>
+  <si>
+    <t>[N.S.N.%Graham%NULL%1,                    C.%Junghans%NULL%1,                    R.%Downes%NULL%1,                    C.%Sendall%NULL%1,                    H.%Lai%NULL%1,                    A.%McKirdy%NULL%1,                    P.%Elliott%NULL%1,                    R.%Howard%NULL%1,                    D.%Wingfield%NULL%1,                    M.%Priestman%NULL%1,                    M.%Ciechonska%NULL%1,                    L.%Cameron%NULL%1,                    M.%Storch%NULL%1,                    M.A.%Crone%NULL%1,                    P.S.%Freemont%NULL%1,                    P.%Randell%NULL%1,                    R.%McLaren%NULL%1,                    N.%Lang%NULL%1,                    S.%Ladhani%NULL%1,                    F.%Sanderson%NULL%1,                    D.J.%Sharp%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Agnes%Marossy%agnesmarossy@nhs.net%1,                    Stefan%Rakowicz%NULL%1,                    Angela%Bhan%NULL%1,                    Sarah%Noon%NULL%1,                    Amanda%Rees%NULL%1,                    Manjinder%Virk%NULL%1,                    Ayazali%Nazafi%NULL%1,                    Evie%Hay%NULL%1,                    Louise%de Thomasson%NULL%1,                    Christina%Windle%NULL%1,                    Mark%Zuckerman%Mark.Zuckerman@nhs.net%1]</t>
+  </si>
+  <si>
+    <t>[Laura%Shallcross%NULL%1,                    Danielle%Burke%NULL%1,                    Owen%Abbott%NULL%1,                    Alasdair%Donaldson%NULL%1,                    Gemma%Hallatt%NULL%1,                    Andrew%Hayward%NULL%1,                    Susan%Hopkins%NULL%0,                    Maria%Krutikov%NULL%1,                    Katie%Sharp%NULL%1,                    Leone%Wardman%NULL%1,                    Sapphira%Thorne%NULL%1]</t>
+  </si>
+  <si>
+    <t>[ E.%Smith%null%1,                     C. F.% Aldus%null%1,                     J.% Brainard%null%1,                     S.% Dunham%null%1,                     P. R.% Hunter%null%1,                     N.% Steel%null%1,                     P. % Everden%null%1,   E.%Smith%null%1,   C. F.% Aldus%null%1,   J.% Brainard%null%1,   S.% Dunham%null%1,   P. R.% Hunter%null%1,   N.% Steel%null%1,   P. % Everden%null%1]</t>
+  </si>
+  <si>
+    <t>[Mahesh C%Patel%mp3@uic.edu%1,                    Lelia H%Chaisson%NULL%1,                    Scott%Borgetti%NULL%1,                    Deborah%Burdsall%NULL%1,                    Rashmi K%Chugh%NULL%1,                    Christopher R%Hoff%NULL%1,                    Elizabeth B%Murphy%NULL%1,                    Emily A%Murskyj%NULL%1,                    Shannon%Wilson%NULL%1,                    Joe%Ramos%NULL%1,                    Lynn%Akker%NULL%1,                    Debra%Bryars%NULL%1,                    Evonda%Thomas-Smith%NULL%1,                    Susan C%Bleasdale%NULL%1,                    Ngozi O%Ezike%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Helena%Temkin‐Greener%helena_temkin-greener@urmc.rochester.edu%1,                    Wenhan%Guo%NULL%2,                    Wenhan%Guo%NULL%0,                    Yunjiao%Mao%NULL%1,                    Xueya%Cai%NULL%1,                    Yue%Li%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Ana A.%Weil%anaweil@uw.edu%1,                    Kira L.%Newman%NULL%2,                    Kira L.%Newman%NULL%0,                    Thuan D.%Ong%NULL%1,                    Giana H.%Davidson%NULL%1,                    Jennifer%Logue%NULL%1,                    Elisabeth%Brandstetter%NULL%1,                    Ariana%Magedson%NULL%1,                    Dylan%McDonald%NULL%1,                    Denise J.%McCulloch%NULL%1,                    Santiago%Neme%NULL%1,                    James%Lewis%NULL%0,                    Jeff S.%Duchin%NULL%1,                    Weizhi%Zhong%NULL%1,                    Lea M.%Starita%NULL%1,                    Trevor%Bedford%NULL%1,                    Alison C.%Roxby%NULL%1,                    Helen Y.%Chu%helenchu@uw.edu%2]</t>
+  </si>
+  <si>
+    <t>[Guillermo V.%Sanchez%NULL%1,                    Caitlin%Biedron%NULL%1,                    Lauren R.%Fink%NULL%1,                    Kelly M.%Hatfield%NULL%1,                    Jordan Micah F.%Polistico%NULL%1,                    Monica P.%Meyer%NULL%1,                    Rebecca S.%Noe%NULL%1,                    Casey E.%Copen%NULL%1,                    Amanda K.%Lyons%NULL%1,                    Gonzalo%Gonzalez%NULL%1,                    Keith%Kiama%NULL%1,                    Mark%Lebednick%NULL%1,                    Bonnie K.%Czander%NULL%1,                    Amen%Agbonze%NULL%1,                    Aimee R.%Surma%NULL%1,                    Avnish%Sandhu%NULL%1,                    Valerie H.%Mika%NULL%1,                    Tyler%Prentiss%NULL%1,                    John%Zervos%NULL%1,                    Donia A.%Dalal%NULL%1,                    Amber M.%Vasquez%NULL%1,                    Sujan C.%Reddy%NULL%0,                    John%Jernigan%NULL%1,                    Paul E.%Kilgore%NULL%1,                    Marcus J.%Zervos%NULL%1,                    Teena%Chopra%NULL%1,                    Carla P.%Bezold%NULL%1,                    Najibah K.%Rehman%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Janice K%Louie%Janice.louie@sfdph.org%1,                    Hyman M%Scott%NULL%1,                    Amie%DuBois%NULL%1,                    Natalya%Sturtz%NULL%1,                    Wendy%Lu%NULL%1,                    Juliet%Stoltey%NULL%1,                    Godfred%Masinde%NULL%1,                    Stephanie%Cohen%NULL%1,                    Darpun%Sachdev%NULL%1,                    Susan%Philip%NULL%1,                    Naveena%Bobba%NULL%1,                    Tomas%Aragon%NULL%1,                    NULL%NULL%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Scott A%Goldberg%sagoldberg@bwh.harvard.edu%1,                    Jochen%Lennerz%NULL%1,                    Michael%Klompas%NULL%1,                    Eden%Mark%NULL%1,                    Virginia M%Pierce%NULL%1,                    Ryan W%Thompson%NULL%1,                    Charles T%Pu%NULL%1,                    Lauren L%Ritterhouse%NULL%1,                    Anand%Dighe%NULL%1,                    Eric S%Rosenberg%NULL%1,                    David C%Grabowski%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Amy V.%Dora%NULL%1,                    Alexander%Winnett%NULL%1,                    Lauren P.%Jatt%NULL%1,                    Kusha%Davar%NULL%1,                    Mika%Watanabe%NULL%1,                    Linda%Sohn%NULL%1,                    Hannah S.%Kern%NULL%1,                    Christopher J.%Graber%NULL%1,                    Matthew B.%Goetz%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Benjamin F.%Bigelow%NULL%1,                    Olive%Tang%NULL%1,                    Gregory R.%Toci%NULL%1,                    Norberth%Stracker%NULL%1,                    Fatima%Sheikh%NULL%1,                    Kara M.%Jacobs Slifka%NULL%1,                    Shannon A.%Novosad%NULL%1,                    John A.%Jernigan%NULL%0,                    Sujan C.%Reddy%NULL%0,                    Morgan J.%Katz%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Matt%Feaster%NULL%1,                    Ying-Ying%Goh%NULL%1]</t>
+  </si>
+  <si>
+    <t>[William R.%Mills%NULL%1,                    Janet M.%Buccola%NULL%1,                    Susan%Sender%NULL%1,                    Joseph%Lichtefeld%NULL%1,                    Nicholas%Romano%NULL%1,                    Karen%Reynolds%NULL%1,                    Melissa%Price%NULL%1,                    Jennifer%Phipps%NULL%1,                    Leigh%White%NULL%1,                    Shauen%Howard%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Drew A.%Harris%xref no email%0, Laurie%Archbald-Pannone%xref no email%1, Jasveen%Kaur%xref no email%1, David%Cattell-Gordon%xref no email%1, Karen S.%Rheuban%xref no email%1, Rachel L.%Ombres%xref no email%1, Kimberly%Albero%xref no email%1, Rebecca%Steele%xref no email%1, Taison D.%Bell%xref no email%1, Justin B.%Mutter%xref no email%1]</t>
+  </si>
+  <si>
+    <t>2023-06-05</t>
+  </si>
+  <si>
+    <t>PUBLISHER: Mary Ann Liebert Inc</t>
+  </si>
+  <si>
+    <t>[Carl D.%Shrader%xref no email%0, Shauna%Assadzandi%xref no email%1, Courtney S.%Pilkerton%xref no email%1, Amie M.%Ashcraft%xref no email%1]</t>
+  </si>
+  <si>
+    <t>PUBLISHER: SAGE Publications</t>
+  </si>
+  <si>
+    <t>[Daniel J%Escobar%Daniel.escobar@pennmedicine.upenn.edu%1,                     Maria%Lanzi%NULL%1,                     Pouné%Saberi%NULL%1,                     Ruby%Love%NULL%1,                     Darren R%Linkin%NULL%1,                     John J%Kelly%NULL%1,                     Darshana%Jhala%NULL%1,                     Valerianna%Amorosa%NULL%1,                     Mary%Hofmann%NULL%1,                     Jeffrey B%Doyon%NULL%1]</t>
+  </si>
+  <si>
+    <t>[James L.%Rudolph%NULL%1,                     Christopher W.%Halladay%NULL%1,                     Malisa%Barber%NULL%1,                     Kevin W.%McConeghy%NULL%1,                     Vince%Mor%NULL%1,                     Aman%Nanda%NULL%1,                     Stefan%Gravenstein%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Paula%Eckardt%NULL%1,                     Rachel%Guran%NULL%1,                     Jon%Hennemyre%NULL%1,                     Roshan%Arikupurathu%NULL%1,                     Julie%Poveda%NULL%1,                     Nancimae%Miller%NULL%1,                     Randy%Katz%NULL%1,                     Judith%Frum%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Carson%Telford%NULL%1,                     Udodirim%Onwubiko%NULL%1,                     David%Holland%NULL%1,                     Kim%Turner%NULL%1,                     Juliana%Prieto%NULL%1,                     Sasha%Smith%NULL%1,                     Jane%Yoon%NULL%1,                     Wecheeta%Brown%NULL%1,                     Allison%Chamberlain%NULL%1,                     Neel%Gandhi%NULL%1,                     Shamimul%Khan%NULL%1,                     Steve%Williams%NULL%1,                     Fazle%Khan%NULL%1,                     Sarita%Shah%NULL%1,                      C. T.%Telford%null%1,                      U.% Onwubiko%null%1,                      D.% Holland%null%1,                      K.% Turner%null%1,                      J.% Prieto%null%1,                      S.% Smith%null%1,                      J.% Yoon%null%1,                      W.% Brown%null%1,                      A.% Chamberlain%null%1,                      N.% Gandhi%null%1,                      S.% Khan%null%1,                      S.% Williams%null%1,                      F.% Khan%null%1,                      S. % Shah%null%1,                     C. T.%Telford%null%1,                     U.% Onwubiko%null%1,                     D.% Holland%null%1,                     K.% Turner%null%1,                     J.% Prieto%null%1,                     S.% Smith%null%1,                     J.% Yoon%null%1,                     W.% Brown%null%1,                     A.% Chamberlain%null%1,                     N.% Gandhi%null%1,                     S.% Khan%null%1,                     S.% Williams%null%1,                     F.% Khan%null%1,                     S. % Shah%null%1,    C. T.%Telford%null%1,    U.% Onwubiko%null%1,    D.% Holland%null%1,    K.% Turner%null%1,    J.% Prieto%null%1,    S.% Smith%null%1,    J.% Yoon%null%1,    W.% Brown%null%1,    A.% Chamberlain%null%1,    N.% Gandhi%null%1,    S.% Khan%null%1,    S.% Williams%null%1,    F.% Khan%null%1,    S. % Shah%null%1]</t>
+  </si>
+  <si>
+    <t>[Sandra M.%Shi%NULL%1,                     Innokentiy%Bakaev%NULL%1,                     Helen%Chen%NULL%1,                     Thomas G.%Travison%NULL%1,                     Sarah D.%Berry%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Temet M.%McMichael%NULL%0,                     Dustin W.%Currie%NULL%0,                     Shauna%Clark%NULL%0,                     Sargis%Pogosjans%NULL%0,                     Meagan%Kay%NULL%0,                     Noah G.%Schwartz%NULL%0,                     James%Lewis%NULL%0,                     Atar%Baer%NULL%0,                     Vance%Kawakami%NULL%0,                     Margaret D.%Lukoff%NULL%0,                     Jessica%Ferro%NULL%0,                     Claire%Brostrom-Smith%NULL%0,                     Thomas D.%Rea%NULL%1,                     Michael R.%Sayre%NULL%1,                     Francis X.%Riedo%NULL%0,                     Denny%Russell%NULL%0,                     Brian%Hiatt%NULL%0,                     Patricia%Montgomery%NULL%0,                     Agam K.%Rao%NULL%0,                     Eric J.%Chow%NULL%0,                     Farrell%Tobolowsky%NULL%0,                     Michael J.%Hughes%NULL%1,                     Ana C.%Bardossy%NULL%0,                     Lisa P.%Oakley%NULL%0,                     Jesica R.%Jacobs%NULL%0,                     Nimalie D.%Stone%NULL%1,                     Sujan C.%Reddy%NULL%0,                     John A.%Jernigan%NULL%0,                     Margaret A.%Honein%NULL%0,                     Thomas A.%Clark%NULL%0,                     Jeffrey S.%Duchin%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Nathan M.%Stall%nathan.stall@sinaihealth.ca%1,                     Carolyn%Farquharson%NULL%2,                     Carolyn%Farquharson%NULL%0,                     Chris%Fan‐Lun%NULL%1,                     Lesley%Wiesenfeld%NULL%1,                     Carla A.%Loftus%NULL%1,                     Dylan%Kain%NULL%1,                     Jennie%Johnstone%NULL%1,                     Liz%McCreight%NULL%1,                     Russell D.%Goldman%NULL%1,                     Ramona%Mahtani%NULL%1]</t>
+  </si>
+  <si>
+    <t>[ Nathan M.%Stall%null%1,                      Aaron%Jones%null%1,                      Kevin A.%Brown%null%1,                      Paula A.%Rochon%null%1,                      Andrew P.%Costa%null%1,                     Nathan M.%Stall%null%1,                     Aaron%Jones%null%1,                     Kevin A.%Brown%null%1,                     Paula A.%Rochon%null%1,                     Andrew P.%Costa%null%1]</t>
+  </si>
+  <si>
+    <t>[Hubert%Blain%NULL%1,                     Yves%Rolland%NULL%1,                     Edouard%Tuaillon%NULL%1,                     Nadia%Giacosa%NULL%1,                     Mylène%Albrand%NULL%1,                     Audrey%Jaussent%NULL%1,                     Athanase%Benetos%NULL%1,                     Stéphanie%Miot%NULL%1,                     Jean%Bousquet%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Guillaume%Sacco%NULL%1,                     Gonzague%Foucault%NULL%1,                     Olivier%Briere%NULL%1,                     Cédric%Annweiler%NULL%1]</t>
+  </si>
+  <si>
+    <t>[R.%Guery%NULL%1,                     C.%Delaye%NULL%1,                     N.%Brule%NULL%1,                     V.%Nael%NULL%1,                     L.%Castain%NULL%1,                     F.%Raffi%NULL%1,                     L.%De Decker%NULL%1]</t>
+  </si>
+  <si>
+    <t>[A.%Klein%anke.klein@uke.de%1,                     C.%Edler%NULL%1,                     A.%Fitzek%NULL%1,                     D.%Fröb%NULL%1,                     A.%Heinemann%NULL%1,                     K.%Meißner%NULL%1,                     H.%Mushumba%NULL%1,                     K.%Püschel%NULL%1,                     A. S.%Schröder%NULL%1,                     J. P.%Sperhake%NULL%1,                     F.%Ishorst-Witte%NULL%1,                     M.%Aepfelbacher%NULL%1,                     F.%Heinrich%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Buntinx%Frank%coreGivesNoEmail%1,                   Claes%Peter%coreGivesNoEmail%1,                   Gulikers%Marjo%coreGivesNoEmail%1,                   Jan%De Lepeleire%coreGivesNoEmail%1,                   Van%der Elst Michael%coreGivesNoEmail%1,                   Van%Elslande Jan%coreGivesNoEmail%1,                   Van%Ranst Marc%coreGivesNoEmail%1,                   Verbakel%Jan%coreGivesNoEmail%1,                   Vernneersch%Pieter%coreGivesNoEmail%1]</t>
+  </si>
+  <si>
+    <t>[Liangcong%Hu%xref no email%1,  Wanyuan%Zhen%xref no email%1,  Xudong%Xie%xref no email%2,  Ze%Lin%xref no email%2,  Tiantian%Wang%xref no email%1,  Jing%Liu%xref no email%5,  Hang%Xue%xref no email%2,  Adriana C.%Panayi%xref no email%2,  Ke%Xu%xref no email%1,  Zexi%Ling%xref no email%1,  Xugui%Li%xref no email%1,  Bobin%Mi%xref no email%1,  Wu%Zhou%xref no email%2,  Guohui%Liu%xref no email%2]</t>
+  </si>
+  <si>
+    <t>[Sean P%Kennelly%Sean.Kennelly@tuh.ie%1,                     Adam H%Dyer%dyera@tcd.ie%1,                     Claire%Noonan%claire.noonan@tuh.ie%2,                     Claire%Noonan%claire.noonan@tuh.ie%0,                     Ruth%Martin%ruth.martin1@hse.ie%1,                     Siobhan M%Kennelly%siobhan.kennelly1@hse.ie%1,                     Alan%Martin%alanmartin@beaumont.ie%1,                     Desmond%O’Neill%NULL%1,                     Aoife%Fallon%aoife.fallon1@hotmail.com%1]</t>
+  </si>
+  <si>
+    <t>[Antonio%Nouvenne%NULL%1,                     Andrea%Ticinesi%NULL%1,                     Alberto%Parise%NULL%1,                     Beatrice%Prati%NULL%1,                     Marcello%Esposito%NULL%1,                     Valentina%Cocchi%NULL%1,                     Emanuele%Crisafulli%NULL%1,                     Annalisa%Volpi%NULL%1,                     Sandra%Rossi%NULL%1,                     Elena Giovanna%Bignami%NULL%1,                     Marco%Baciarello%NULL%1,                     Ettore%Brianti%NULL%1,                     Massimo%Fabi%NULL%1,                     Tiziana%Meschi%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Nicola%Veronese%NULL%1,                     Luca Gino%Sbrogiò%NULL%1,                     Roberto%Valle%NULL%1,                     Laura%Marin%NULL%1,                     Elena%Boscolo Fiore%NULL%1,                     Andrea%Tiozzo%NULL%1]</t>
+  </si>
+  <si>
+    <t>[ J. H.%van den Besselaar%null%1,                      R. S.% Sikkema%null%1,                      F. M. H. P. A.% Koene%null%1,                      L. W.% van Buul%null%1,                      B. B.% Oude Munnink%null%1,                      I.% Frenay%null%1,                      R.% te Witt%null%1,                      M. P. G.% Koopmans%null%1,                      C. M. P. M.% Hertogh%null%1,                      B. M. % Buurman%null%1,    J. H.%van den Besselaar%null%1,    R. S.% Sikkema%null%1,    F. M. H. P. A.% Koene%null%1,    L. W.% van Buul%null%1,    B. B.% Oude Munnink%null%1,    I.% Frenay%null%1,    R.% te Witt%null%1,    M. P. G.% Koopmans%null%1,    C. M. P. M.% Hertogh%null%1,    B. M. % Buurman%null%1]</t>
+  </si>
+  <si>
+    <t>[Laura W.%van Buul%NULL%1,                     Judith H.%van den Besselaar%NULL%2,                     Judith H.%van den Besselaar%NULL%0,                     Fleur M. H. P. H.%Koene%NULL%1,                     Bianca M.%Buurman%NULL%1,                     Cees M. P. M.%Hertogh%NULL%1,                     Martin%Smalbrugge%NULL%1,                     Jeanine J. S.%Rutten%NULL%1,                     Elke M.%den Boogert%NULL%1,                     Michel D.%Wissing%NULL%1,                     Ariene%Rietveld%NULL%1,                     Mariska W. W.%van Elsakker%NULL%1,                     Marga M. G.%Nonneman%NULL%1,                     Florien%van Eeden%NULL%1,                     Saskia%van de Merwe%NULL%1,                     Sophie L.%Niemansburg%NULL%1,                     Ewout%Fanoy%NULL%1,                     Hinke S.%Bootsma%NULL%1,                     Nicoline%van der Hagen%NULL%1,                     Mariska%Petrignani%NULL%1,                     Jessica Edwards%van Muijen%NULL%1,                     Karolien E. M.%Biesheuvel%NULL%1]</t>
+  </si>
+  <si>
+    <t>[B\u00e5rd%Reiakvam Kittang%coreGivesNoEmail%1,                   Karina%Koller L\u00f8land%coreGivesNoEmail%1,                   Kjell%Kr\u00fcger%coreGivesNoEmail%1,                   Kristian%Jansen%coreGivesNoEmail%1,                   Sabine%Piepenstock Solheim%coreGivesNoEmail%1,                   Sebastian%von Hofacker%coreGivesNoEmail%1]</t>
+  </si>
+  <si>
+    <t>[Shin Young%Park%NULL%1,                     Gawon%Choi%NULL%2,                     Gawon%Choi%NULL%0,                     Hyeyoung%Lee%NULL%2,                     Hyeyoung%Lee%NULL%0,                     Na-young%Kim%NULL%2,                     Na-young%Kim%NULL%0,                     Seon-young%Lee%NULL%2,                     Seon-young%Lee%NULL%0,                     Kyungnam%Kim%NULL%2,                     Kyungnam%Kim%NULL%0,                     Soyoung%Shin%NULL%2,                     Soyoung%Shin%NULL%0,                     Eunsu%Jang%NULL%2,                     Eunsu%Jang%NULL%0,                     YoungSin%Moon%NULL%2,                     YoungSin%Moon%NULL%0,                     KwangHwan%Oh%NULL%2,                     KwangHwan%Oh%NULL%0,                     JaeRin%Choi%NULL%2,                     JaeRin%Choi%NULL%0,                     Sangeun%Lee%NULL%2,                     Sangeun%Lee%NULL%0,                     Young-Man%Kim%NULL%2,                     Young-Man%Kim%NULL%0,                     Jieun%Kim%NULL%2,                     Jieun%Kim%NULL%0,                     Seonju%Yi%NULL%2,                     Seonju%Yi%NULL%0,                     Jin%Gwack%NULL%2,                     Jin%Gwack%NULL%0,                     Ok%Park%NULL%2,                     Ok%Park%NULL%0,                     Young Joon%Park%NULL%2,                     Young Joon%Park%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Rok%Song%NULL%1,                     Hee-Sook%Kim%NULL%2,                     Hee-Sook%Kim%NULL%0,                     Seok-Ju%Yoo%NULL%2,                     Seok-Ju%Yoo%NULL%0,                     Kwan%Lee%NULL%2,                     Kwan%Lee%NULL%0,                     Ji-Hyuk%Park%NULL%2,                     Ji-Hyuk%Park%NULL%0,                     Joon Ho%Jang%NULL%2,                     Joon Ho%Jang%NULL%0,                     Gyoung-Sook%Ahn%NULL%2,                     Gyoung-Sook%Ahn%NULL%0,                     Jun-Nyun%Kim%NULL%2,                     Jun-Nyun%Kim%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Blanca%Borras-Bermejo%NULL%1,                     Xavier%Martínez-Gómez%NULL%1,                     María Gutierrez%San Miguel%NULL%1,                     Juliana%Esperalba%NULL%1,                     Andrés%Antón%NULL%1,                     Elisabet%Martin%NULL%1,                     Marta%Selvi%NULL%1,                     María José%Abadías%NULL%1,                     Antonio%Román%NULL%1,                     Tomàs%Pumarola%NULL%1,                     Magda%Campins%NULL%1,                     Benito%Almirante%NULL%1]</t>
+  </si>
+  <si>
+    <t>[M.%Bernabeu-Wittel%NULL%1,                     J.E.%Ternero-Vega%NULL%1,                     P.%Díaz-Jiménez%NULL%1,                     C.%Conde-Guzmán%NULL%1,                     M.D.%Nieto-Martín%NULL%1,                     L.%Moreno-Gaviño%NULL%1,                     J.%Delgado-Cuesta%NULL%1,                     M.%Rincón-Gómez%NULL%1,                     L.%Giménez-Miranda%NULL%1,                     M.D.%Navarro-Amuedo%NULL%1,                     M.M.%Muñoz-García%NULL%1,                     S.%Calzón-Fernández%NULL%1,                     M.%Ollero-Baturone%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Shamez N%Ladhani%shamez.ladhani@phe.gov.uk%1,                     J.Yimmy%Chow%NULL%1,                     Roshni%Janarthanan%NULL%1,                     Jonathan%Fok%NULL%1,                     Emma%Crawley-Boevey%NULL%1,                     Amoolya%Vusirikala%NULL%1,                     Elena%Fernandez%NULL%1,                     Marina Sanchez%Perez%NULL%1,                     Suzanne%Tang%NULL%1,                     Kate%Dun-Campbell%NULL%1,                     Edward Wynne-%Evans%NULL%1,                     Anita%Bell%NULL%1,                     Bharat%Patel%NULL%1,                     Zahin%Amin-Chowdhury%NULL%1,                     Felicity%Aiano%NULL%1,                     Karthik%Paranthaman%NULL%1,                     Thomas%Ma%NULL%1,                     Maria%Saavedra-Campos%NULL%1,                     Richard%Myers%NULL%1,                     Joanna%Ellis%NULL%2,                     Angie%Lackenby%NULL%1,                     Robin%Gopal%NULL%1,                     Monika%Patel%NULL%1,                     Colin%Brown%NULL%1,                     Meera%Chand%NULL%1,                     Kevin%Brown%NULL%1,                     Mary E%Ramsay%NULL%1,                     Susan%Hopkins%NULL%2,                     Nandini%Shetty%NULL%1,                     Maria%Zambon%NULL%2]</t>
+  </si>
+  <si>
+    <t>[N.S.N.%Graham%NULL%1,                     C.%Junghans%NULL%1,                     R.%Downes%NULL%1,                     C.%Sendall%NULL%1,                     H.%Lai%NULL%1,                     A.%McKirdy%NULL%1,                     P.%Elliott%NULL%1,                     R.%Howard%NULL%1,                     D.%Wingfield%NULL%1,                     M.%Priestman%NULL%1,                     M.%Ciechonska%NULL%1,                     L.%Cameron%NULL%1,                     M.%Storch%NULL%1,                     M.A.%Crone%NULL%1,                     P.S.%Freemont%NULL%1,                     P.%Randell%NULL%1,                     R.%McLaren%NULL%1,                     N.%Lang%NULL%1,                     S.%Ladhani%NULL%1,                     F.%Sanderson%NULL%1,                     D.J.%Sharp%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Agnes%Marossy%agnesmarossy@nhs.net%1,                     Stefan%Rakowicz%NULL%1,                     Angela%Bhan%NULL%1,                     Sarah%Noon%NULL%1,                     Amanda%Rees%NULL%1,                     Manjinder%Virk%NULL%1,                     Ayazali%Nazafi%NULL%1,                     Evie%Hay%NULL%1,                     Louise%de Thomasson%NULL%1,                     Christina%Windle%NULL%1,                     Mark%Zuckerman%Mark.Zuckerman@nhs.net%1]</t>
+  </si>
+  <si>
+    <t>[Laura%Shallcross%NULL%1,                     Danielle%Burke%NULL%1,                     Owen%Abbott%NULL%1,                     Alasdair%Donaldson%NULL%1,                     Gemma%Hallatt%NULL%1,                     Andrew%Hayward%NULL%1,                     Susan%Hopkins%NULL%0,                     Maria%Krutikov%NULL%1,                     Katie%Sharp%NULL%1,                     Leone%Wardman%NULL%1,                     Sapphira%Thorne%NULL%1]</t>
+  </si>
+  <si>
+    <t>[ E.%Smith%null%1,                      C. F.% Aldus%null%1,                      J.% Brainard%null%1,                      S.% Dunham%null%1,                      P. R.% Hunter%null%1,                      N.% Steel%null%1,                      P. % Everden%null%1,    E.%Smith%null%1,    C. F.% Aldus%null%1,    J.% Brainard%null%1,    S.% Dunham%null%1,    P. R.% Hunter%null%1,    N.% Steel%null%1,    P. % Everden%null%1]</t>
+  </si>
+  <si>
+    <t>[Mahesh C%Patel%mp3@uic.edu%1,                     Lelia H%Chaisson%NULL%1,                     Scott%Borgetti%NULL%1,                     Deborah%Burdsall%NULL%1,                     Rashmi K%Chugh%NULL%1,                     Christopher R%Hoff%NULL%1,                     Elizabeth B%Murphy%NULL%1,                     Emily A%Murskyj%NULL%1,                     Shannon%Wilson%NULL%1,                     Joe%Ramos%NULL%1,                     Lynn%Akker%NULL%1,                     Debra%Bryars%NULL%1,                     Evonda%Thomas-Smith%NULL%1,                     Susan C%Bleasdale%NULL%1,                     Ngozi O%Ezike%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Helena%Temkin‐Greener%helena_temkin-greener@urmc.rochester.edu%1,                     Wenhan%Guo%NULL%2,                     Wenhan%Guo%NULL%0,                     Yunjiao%Mao%NULL%1,                     Xueya%Cai%NULL%1,                     Yue%Li%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Ana A.%Weil%anaweil@uw.edu%1,                     Kira L.%Newman%NULL%2,                     Kira L.%Newman%NULL%0,                     Thuan D.%Ong%NULL%1,                     Giana H.%Davidson%NULL%1,                     Jennifer%Logue%NULL%1,                     Elisabeth%Brandstetter%NULL%1,                     Ariana%Magedson%NULL%1,                     Dylan%McDonald%NULL%1,                     Denise J.%McCulloch%NULL%1,                     Santiago%Neme%NULL%1,                     James%Lewis%NULL%0,                     Jeff S.%Duchin%NULL%1,                     Weizhi%Zhong%NULL%1,                     Lea M.%Starita%NULL%1,                     Trevor%Bedford%NULL%1,                     Alison C.%Roxby%NULL%1,                     Helen Y.%Chu%helenchu@uw.edu%2]</t>
+  </si>
+  <si>
+    <t>[Guillermo V.%Sanchez%NULL%1,                     Caitlin%Biedron%NULL%1,                     Lauren R.%Fink%NULL%1,                     Kelly M.%Hatfield%NULL%1,                     Jordan Micah F.%Polistico%NULL%1,                     Monica P.%Meyer%NULL%1,                     Rebecca S.%Noe%NULL%1,                     Casey E.%Copen%NULL%1,                     Amanda K.%Lyons%NULL%1,                     Gonzalo%Gonzalez%NULL%1,                     Keith%Kiama%NULL%1,                     Mark%Lebednick%NULL%1,                     Bonnie K.%Czander%NULL%1,                     Amen%Agbonze%NULL%1,                     Aimee R.%Surma%NULL%1,                     Avnish%Sandhu%NULL%1,                     Valerie H.%Mika%NULL%1,                     Tyler%Prentiss%NULL%1,                     John%Zervos%NULL%1,                     Donia A.%Dalal%NULL%1,                     Amber M.%Vasquez%NULL%1,                     Sujan C.%Reddy%NULL%0,                     John%Jernigan%NULL%1,                     Paul E.%Kilgore%NULL%1,                     Marcus J.%Zervos%NULL%1,                     Teena%Chopra%NULL%1,                     Carla P.%Bezold%NULL%1,                     Najibah K.%Rehman%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Janice K%Louie%Janice.louie@sfdph.org%1,                     Hyman M%Scott%NULL%1,                     Amie%DuBois%NULL%1,                     Natalya%Sturtz%NULL%1,                     Wendy%Lu%NULL%1,                     Juliet%Stoltey%NULL%1,                     Godfred%Masinde%NULL%1,                     Stephanie%Cohen%NULL%1,                     Darpun%Sachdev%NULL%1,                     Susan%Philip%NULL%1,                     Naveena%Bobba%NULL%1,                     Tomas%Aragon%NULL%1,                     NULL%NULL%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Scott A%Goldberg%sagoldberg@bwh.harvard.edu%1,                     Jochen%Lennerz%NULL%1,                     Michael%Klompas%NULL%1,                     Eden%Mark%NULL%1,                     Virginia M%Pierce%NULL%1,                     Ryan W%Thompson%NULL%1,                     Charles T%Pu%NULL%1,                     Lauren L%Ritterhouse%NULL%1,                     Anand%Dighe%NULL%1,                     Eric S%Rosenberg%NULL%1,                     David C%Grabowski%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Amy V.%Dora%NULL%1,                     Alexander%Winnett%NULL%1,                     Lauren P.%Jatt%NULL%1,                     Kusha%Davar%NULL%1,                     Mika%Watanabe%NULL%1,                     Linda%Sohn%NULL%1,                     Hannah S.%Kern%NULL%1,                     Christopher J.%Graber%NULL%1,                     Matthew B.%Goetz%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Benjamin F.%Bigelow%NULL%1,                     Olive%Tang%NULL%1,                     Gregory R.%Toci%NULL%1,                     Norberth%Stracker%NULL%1,                     Fatima%Sheikh%NULL%1,                     Kara M.%Jacobs Slifka%NULL%1,                     Shannon A.%Novosad%NULL%1,                     John A.%Jernigan%NULL%0,                     Sujan C.%Reddy%NULL%0,                     Morgan J.%Katz%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Matt%Feaster%NULL%1,                     Ying-Ying%Goh%NULL%1]</t>
+  </si>
+  <si>
+    <t>[William R.%Mills%NULL%1,                     Janet M.%Buccola%NULL%1,                     Susan%Sender%NULL%1,                     Joseph%Lichtefeld%NULL%1,                     Nicholas%Romano%NULL%1,                     Karen%Reynolds%NULL%1,                     Melissa%Price%NULL%1,                     Jennifer%Phipps%NULL%1,                     Leigh%White%NULL%1,                     Shauen%Howard%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Drew A.%Harris%xref no email%1,  Laurie%Archbald-Pannone%xref no email%1,  Jasveen%Kaur%xref no email%1,  David%Cattell-Gordon%xref no email%1,  Karen S.%Rheuban%xref no email%1,  Rachel L.%Ombres%xref no email%1,  Kimberly%Albero%xref no email%1,  Rebecca%Steele%xref no email%1,  Taison D.%Bell%xref no email%1,  Justin B.%Mutter%xref no email%1]</t>
+  </si>
+  <si>
+    <t>[Carl D.%Shrader%xref no email%1,  Shauna%Assadzandi%xref no email%1,  Courtney S.%Pilkerton%xref no email%1,  Amie M.%Ashcraft%xref no email%1]</t>
+  </si>
+  <si>
+    <t>[Daniel J%Escobar%Daniel.escobar@pennmedicine.upenn.edu%1,                      Maria%Lanzi%NULL%1,                      Pouné%Saberi%NULL%1,                      Ruby%Love%NULL%1,                      Darren R%Linkin%NULL%1,                      John J%Kelly%NULL%1,                      Darshana%Jhala%NULL%1,                      Valerianna%Amorosa%NULL%1,                      Mary%Hofmann%NULL%1,                      Jeffrey B%Doyon%NULL%1]</t>
+  </si>
+  <si>
+    <t>[James L.%Rudolph%NULL%1,                      Christopher W.%Halladay%NULL%1,                      Malisa%Barber%NULL%1,                      Kevin W.%McConeghy%NULL%1,                      Vince%Mor%NULL%1,                      Aman%Nanda%NULL%1,                      Stefan%Gravenstein%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Paula%Eckardt%NULL%1,                      Rachel%Guran%NULL%1,                      Jon%Hennemyre%NULL%1,                      Roshan%Arikupurathu%NULL%1,                      Julie%Poveda%NULL%1,                      Nancimae%Miller%NULL%1,                      Randy%Katz%NULL%1,                      Judith%Frum%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Carson%Telford%NULL%1,                      Udodirim%Onwubiko%NULL%1,                      David%Holland%NULL%1,                      Kim%Turner%NULL%1,                      Juliana%Prieto%NULL%1,                      Sasha%Smith%NULL%1,                      Jane%Yoon%NULL%1,                      Wecheeta%Brown%NULL%1,                      Allison%Chamberlain%NULL%1,                      Neel%Gandhi%NULL%1,                      Shamimul%Khan%NULL%1,                      Steve%Williams%NULL%1,                      Fazle%Khan%NULL%1,                      Sarita%Shah%NULL%1,                       C. T.%Telford%null%1,                       U.% Onwubiko%null%1,                       D.% Holland%null%1,                       K.% Turner%null%1,                       J.% Prieto%null%1,                       S.% Smith%null%1,                       J.% Yoon%null%1,                       W.% Brown%null%1,                       A.% Chamberlain%null%1,                       N.% Gandhi%null%1,                       S.% Khan%null%1,                       S.% Williams%null%1,                       F.% Khan%null%1,                       S. % Shah%null%1,                      C. T.%Telford%null%1,                      U.% Onwubiko%null%1,                      D.% Holland%null%1,                      K.% Turner%null%1,                      J.% Prieto%null%1,                      S.% Smith%null%1,                      J.% Yoon%null%1,                      W.% Brown%null%1,                      A.% Chamberlain%null%1,                      N.% Gandhi%null%1,                      S.% Khan%null%1,                      S.% Williams%null%1,                      F.% Khan%null%1,                      S. % Shah%null%1,     C. T.%Telford%null%1,     U.% Onwubiko%null%1,     D.% Holland%null%1,     K.% Turner%null%1,     J.% Prieto%null%1,     S.% Smith%null%1,     J.% Yoon%null%1,     W.% Brown%null%1,     A.% Chamberlain%null%1,     N.% Gandhi%null%1,     S.% Khan%null%1,     S.% Williams%null%1,     F.% Khan%null%1,     S. % Shah%null%1]</t>
+  </si>
+  <si>
+    <t>[Sandra M.%Shi%NULL%1,                      Innokentiy%Bakaev%NULL%1,                      Helen%Chen%NULL%1,                      Thomas G.%Travison%NULL%1,                      Sarah D.%Berry%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Temet M.%McMichael%NULL%0,                      Dustin W.%Currie%NULL%0,                      Shauna%Clark%NULL%0,                      Sargis%Pogosjans%NULL%0,                      Meagan%Kay%NULL%0,                      Noah G.%Schwartz%NULL%0,                      James%Lewis%NULL%0,                      Atar%Baer%NULL%0,                      Vance%Kawakami%NULL%0,                      Margaret D.%Lukoff%NULL%0,                      Jessica%Ferro%NULL%0,                      Claire%Brostrom-Smith%NULL%0,                      Thomas D.%Rea%NULL%1,                      Michael R.%Sayre%NULL%1,                      Francis X.%Riedo%NULL%0,                      Denny%Russell%NULL%0,                      Brian%Hiatt%NULL%0,                      Patricia%Montgomery%NULL%0,                      Agam K.%Rao%NULL%0,                      Eric J.%Chow%NULL%0,                      Farrell%Tobolowsky%NULL%0,                      Michael J.%Hughes%NULL%1,                      Ana C.%Bardossy%NULL%0,                      Lisa P.%Oakley%NULL%0,                      Jesica R.%Jacobs%NULL%0,                      Nimalie D.%Stone%NULL%1,                      Sujan C.%Reddy%NULL%0,                      John A.%Jernigan%NULL%0,                      Margaret A.%Honein%NULL%0,                      Thomas A.%Clark%NULL%0,                      Jeffrey S.%Duchin%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Nathan M.%Stall%nathan.stall@sinaihealth.ca%1,                      Carolyn%Farquharson%NULL%2,                      Carolyn%Farquharson%NULL%0,                      Chris%Fan‐Lun%NULL%1,                      Lesley%Wiesenfeld%NULL%1,                      Carla A.%Loftus%NULL%1,                      Dylan%Kain%NULL%1,                      Jennie%Johnstone%NULL%1,                      Liz%McCreight%NULL%1,                      Russell D.%Goldman%NULL%1,                      Ramona%Mahtani%NULL%1]</t>
+  </si>
+  <si>
+    <t>[ Nathan M.%Stall%null%1,                       Aaron%Jones%null%1,                       Kevin A.%Brown%null%1,                       Paula A.%Rochon%null%1,                       Andrew P.%Costa%null%1,                      Nathan M.%Stall%null%1,                      Aaron%Jones%null%1,                      Kevin A.%Brown%null%1,                      Paula A.%Rochon%null%1,                      Andrew P.%Costa%null%1]</t>
+  </si>
+  <si>
+    <t>[Hubert%Blain%NULL%1,                      Yves%Rolland%NULL%1,                      Edouard%Tuaillon%NULL%1,                      Nadia%Giacosa%NULL%1,                      Mylène%Albrand%NULL%1,                      Audrey%Jaussent%NULL%1,                      Athanase%Benetos%NULL%1,                      Stéphanie%Miot%NULL%1,                      Jean%Bousquet%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Jo\u00ebl%Belmin%xref no email%1,   Nathavy%Um-Din%xref no email%1,   Cristiano%Donadio%xref no email%1,   Maurizio%Magri%xref no email%1,   Quoc Duy%Nghiem%xref no email%1,   Bruno%Oquendo%xref no email%1,   Sylvie%Pariel%xref no email%1,   Carmelo%Lafuente-Lafuente%xref no email%1]</t>
+  </si>
+  <si>
+    <t>[Guillaume%Sacco%NULL%1,                      Gonzague%Foucault%NULL%1,                      Olivier%Briere%NULL%1,                      Cédric%Annweiler%NULL%1]</t>
+  </si>
+  <si>
+    <t>[R.%Guery%NULL%1,                      C.%Delaye%NULL%1,                      N.%Brule%NULL%1,                      V.%Nael%NULL%1,                      L.%Castain%NULL%1,                      F.%Raffi%NULL%1,                      L.%De Decker%NULL%1]</t>
+  </si>
+  <si>
+    <t>[A.%Klein%anke.klein@uke.de%1,                      C.%Edler%NULL%1,                      A.%Fitzek%NULL%1,                      D.%Fröb%NULL%1,                      A.%Heinemann%NULL%1,                      K.%Meißner%NULL%1,                      H.%Mushumba%NULL%1,                      K.%Püschel%NULL%1,                      A. S.%Schröder%NULL%1,                      J. P.%Sperhake%NULL%1,                      F.%Ishorst-Witte%NULL%1,                      M.%Aepfelbacher%NULL%1,                      F.%Heinrich%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Buntinx%Frank%coreGivesNoEmail%1,                    Claes%Peter%coreGivesNoEmail%1,                    Gulikers%Marjo%coreGivesNoEmail%1,                    Jan%De Lepeleire%coreGivesNoEmail%1,                    Van%der Elst Michael%coreGivesNoEmail%1,                    Van%Elslande Jan%coreGivesNoEmail%1,                    Van%Ranst Marc%coreGivesNoEmail%1,                    Verbakel%Jan%coreGivesNoEmail%1,                    Vernneersch%Pieter%coreGivesNoEmail%1]</t>
+  </si>
+  <si>
+    <t>[Liangcong%Hu%xref no email%1,   Wanyuan%Zhen%xref no email%1,   Xudong%Xie%xref no email%2,   Ze%Lin%xref no email%2,   Tiantian%Wang%xref no email%1,   Jing%Liu%xref no email%5,   Hang%Xue%xref no email%2,   Adriana C.%Panayi%xref no email%2,   Ke%Xu%xref no email%1,   Zexi%Ling%xref no email%1,   Xugui%Li%xref no email%1,   Bobin%Mi%xref no email%1,   Wu%Zhou%xref no email%2,   Guohui%Liu%xref no email%2]</t>
+  </si>
+  <si>
+    <t>[Sean P%Kennelly%Sean.Kennelly@tuh.ie%1,                      Adam H%Dyer%dyera@tcd.ie%1,                      Claire%Noonan%claire.noonan@tuh.ie%2,                      Claire%Noonan%claire.noonan@tuh.ie%0,                      Ruth%Martin%ruth.martin1@hse.ie%1,                      Siobhan M%Kennelly%siobhan.kennelly1@hse.ie%1,                      Alan%Martin%alanmartin@beaumont.ie%1,                      Desmond%O’Neill%NULL%1,                      Aoife%Fallon%aoife.fallon1@hotmail.com%1]</t>
+  </si>
+  <si>
+    <t>[Antonio%Nouvenne%NULL%1,                      Andrea%Ticinesi%NULL%1,                      Alberto%Parise%NULL%1,                      Beatrice%Prati%NULL%1,                      Marcello%Esposito%NULL%1,                      Valentina%Cocchi%NULL%1,                      Emanuele%Crisafulli%NULL%1,                      Annalisa%Volpi%NULL%1,                      Sandra%Rossi%NULL%1,                      Elena Giovanna%Bignami%NULL%1,                      Marco%Baciarello%NULL%1,                      Ettore%Brianti%NULL%1,                      Massimo%Fabi%NULL%1,                      Tiziana%Meschi%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Nicola%Veronese%NULL%1,                      Luca Gino%Sbrogiò%NULL%1,                      Roberto%Valle%NULL%1,                      Laura%Marin%NULL%1,                      Elena%Boscolo Fiore%NULL%1,                      Andrea%Tiozzo%NULL%1]</t>
+  </si>
+  <si>
+    <t>[ J. H.%van den Besselaar%null%1,                       R. S.% Sikkema%null%1,                       F. M. H. P. A.% Koene%null%1,                       L. W.% van Buul%null%1,                       B. B.% Oude Munnink%null%1,                       I.% Frenay%null%1,                       R.% te Witt%null%1,                       M. P. G.% Koopmans%null%1,                       C. M. P. M.% Hertogh%null%1,                       B. M. % Buurman%null%1,     J. H.%van den Besselaar%null%1,     R. S.% Sikkema%null%1,     F. M. H. P. A.% Koene%null%1,     L. W.% van Buul%null%1,     B. B.% Oude Munnink%null%1,     I.% Frenay%null%1,     R.% te Witt%null%1,     M. P. G.% Koopmans%null%1,     C. M. P. M.% Hertogh%null%1,     B. M. % Buurman%null%1]</t>
+  </si>
+  <si>
+    <t>[Laura W.%van Buul%NULL%1,                      Judith H.%van den Besselaar%NULL%2,                      Judith H.%van den Besselaar%NULL%0,                      Fleur M. H. P. H.%Koene%NULL%1,                      Bianca M.%Buurman%NULL%1,                      Cees M. P. M.%Hertogh%NULL%1,                      Martin%Smalbrugge%NULL%1,                      Jeanine J. S.%Rutten%NULL%1,                      Elke M.%den Boogert%NULL%1,                      Michel D.%Wissing%NULL%1,                      Ariene%Rietveld%NULL%1,                      Mariska W. W.%van Elsakker%NULL%1,                      Marga M. G.%Nonneman%NULL%1,                      Florien%van Eeden%NULL%1,                      Saskia%van de Merwe%NULL%1,                      Sophie L.%Niemansburg%NULL%1,                      Ewout%Fanoy%NULL%1,                      Hinke S.%Bootsma%NULL%1,                      Nicoline%van der Hagen%NULL%1,                      Mariska%Petrignani%NULL%1,                      Jessica Edwards%van Muijen%NULL%1,                      Karolien E. M.%Biesheuvel%NULL%1]</t>
+  </si>
+  <si>
+    <t>[B\u00e5rd%Reiakvam Kittang%coreGivesNoEmail%1,                    Karina%Koller L\u00f8land%coreGivesNoEmail%1,                    Kjell%Kr\u00fcger%coreGivesNoEmail%1,                    Kristian%Jansen%coreGivesNoEmail%1,                    Sabine%Piepenstock Solheim%coreGivesNoEmail%1,                    Sebastian%von Hofacker%coreGivesNoEmail%1]</t>
+  </si>
+  <si>
+    <t>[Shin Young%Park%NULL%1,                      Gawon%Choi%NULL%2,                      Gawon%Choi%NULL%0,                      Hyeyoung%Lee%NULL%2,                      Hyeyoung%Lee%NULL%0,                      Na-young%Kim%NULL%2,                      Na-young%Kim%NULL%0,                      Seon-young%Lee%NULL%2,                      Seon-young%Lee%NULL%0,                      Kyungnam%Kim%NULL%2,                      Kyungnam%Kim%NULL%0,                      Soyoung%Shin%NULL%2,                      Soyoung%Shin%NULL%0,                      Eunsu%Jang%NULL%2,                      Eunsu%Jang%NULL%0,                      YoungSin%Moon%NULL%2,                      YoungSin%Moon%NULL%0,                      KwangHwan%Oh%NULL%2,                      KwangHwan%Oh%NULL%0,                      JaeRin%Choi%NULL%2,                      JaeRin%Choi%NULL%0,                      Sangeun%Lee%NULL%2,                      Sangeun%Lee%NULL%0,                      Young-Man%Kim%NULL%2,                      Young-Man%Kim%NULL%0,                      Jieun%Kim%NULL%2,                      Jieun%Kim%NULL%0,                      Seonju%Yi%NULL%2,                      Seonju%Yi%NULL%0,                      Jin%Gwack%NULL%2,                      Jin%Gwack%NULL%0,                      Ok%Park%NULL%2,                      Ok%Park%NULL%0,                      Young Joon%Park%NULL%2,                      Young Joon%Park%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Rok%Song%NULL%1,                      Hee-Sook%Kim%NULL%2,                      Hee-Sook%Kim%NULL%0,                      Seok-Ju%Yoo%NULL%2,                      Seok-Ju%Yoo%NULL%0,                      Kwan%Lee%NULL%2,                      Kwan%Lee%NULL%0,                      Ji-Hyuk%Park%NULL%2,                      Ji-Hyuk%Park%NULL%0,                      Joon Ho%Jang%NULL%2,                      Joon Ho%Jang%NULL%0,                      Gyoung-Sook%Ahn%NULL%2,                      Gyoung-Sook%Ahn%NULL%0,                      Jun-Nyun%Kim%NULL%2,                      Jun-Nyun%Kim%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Blanca%Borras-Bermejo%NULL%1,                      Xavier%Martínez-Gómez%NULL%1,                      María Gutierrez%San Miguel%NULL%1,                      Juliana%Esperalba%NULL%1,                      Andrés%Antón%NULL%1,                      Elisabet%Martin%NULL%1,                      Marta%Selvi%NULL%1,                      María José%Abadías%NULL%1,                      Antonio%Román%NULL%1,                      Tomàs%Pumarola%NULL%1,                      Magda%Campins%NULL%1,                      Benito%Almirante%NULL%1]</t>
+  </si>
+  <si>
+    <t>[M.%Bernabeu-Wittel%NULL%1,                      J.E.%Ternero-Vega%NULL%1,                      P.%Díaz-Jiménez%NULL%1,                      C.%Conde-Guzmán%NULL%1,                      M.D.%Nieto-Martín%NULL%1,                      L.%Moreno-Gaviño%NULL%1,                      J.%Delgado-Cuesta%NULL%1,                      M.%Rincón-Gómez%NULL%1,                      L.%Giménez-Miranda%NULL%1,                      M.D.%Navarro-Amuedo%NULL%1,                      M.M.%Muñoz-García%NULL%1,                      S.%Calzón-Fernández%NULL%1,                      M.%Ollero-Baturone%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Shamez N%Ladhani%shamez.ladhani@phe.gov.uk%1,                      J.Yimmy%Chow%NULL%1,                      Roshni%Janarthanan%NULL%1,                      Jonathan%Fok%NULL%1,                      Emma%Crawley-Boevey%NULL%1,                      Amoolya%Vusirikala%NULL%1,                      Elena%Fernandez%NULL%1,                      Marina Sanchez%Perez%NULL%1,                      Suzanne%Tang%NULL%1,                      Kate%Dun-Campbell%NULL%1,                      Edward Wynne-%Evans%NULL%1,                      Anita%Bell%NULL%1,                      Bharat%Patel%NULL%1,                      Zahin%Amin-Chowdhury%NULL%1,                      Felicity%Aiano%NULL%1,                      Karthik%Paranthaman%NULL%1,                      Thomas%Ma%NULL%1,                      Maria%Saavedra-Campos%NULL%1,                      Richard%Myers%NULL%1,                      Joanna%Ellis%NULL%2,                      Angie%Lackenby%NULL%1,                      Robin%Gopal%NULL%1,                      Monika%Patel%NULL%1,                      Colin%Brown%NULL%1,                      Meera%Chand%NULL%1,                      Kevin%Brown%NULL%1,                      Mary E%Ramsay%NULL%1,                      Susan%Hopkins%NULL%2,                      Nandini%Shetty%NULL%1,                      Maria%Zambon%NULL%2]</t>
+  </si>
+  <si>
+    <t>[N.S.N.%Graham%NULL%1,                      C.%Junghans%NULL%1,                      R.%Downes%NULL%1,                      C.%Sendall%NULL%1,                      H.%Lai%NULL%1,                      A.%McKirdy%NULL%1,                      P.%Elliott%NULL%1,                      R.%Howard%NULL%1,                      D.%Wingfield%NULL%1,                      M.%Priestman%NULL%1,                      M.%Ciechonska%NULL%1,                      L.%Cameron%NULL%1,                      M.%Storch%NULL%1,                      M.A.%Crone%NULL%1,                      P.S.%Freemont%NULL%1,                      P.%Randell%NULL%1,                      R.%McLaren%NULL%1,                      N.%Lang%NULL%1,                      S.%Ladhani%NULL%1,                      F.%Sanderson%NULL%1,                      D.J.%Sharp%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Agnes%Marossy%agnesmarossy@nhs.net%1,                      Stefan%Rakowicz%NULL%1,                      Angela%Bhan%NULL%1,                      Sarah%Noon%NULL%1,                      Amanda%Rees%NULL%1,                      Manjinder%Virk%NULL%1,                      Ayazali%Nazafi%NULL%1,                      Evie%Hay%NULL%1,                      Louise%de Thomasson%NULL%1,                      Christina%Windle%NULL%1,                      Mark%Zuckerman%Mark.Zuckerman@nhs.net%1]</t>
+  </si>
+  <si>
+    <t>[Laura%Shallcross%NULL%1,                      Danielle%Burke%NULL%1,                      Owen%Abbott%NULL%1,                      Alasdair%Donaldson%NULL%1,                      Gemma%Hallatt%NULL%1,                      Andrew%Hayward%NULL%1,                      Susan%Hopkins%NULL%0,                      Maria%Krutikov%NULL%1,                      Katie%Sharp%NULL%1,                      Leone%Wardman%NULL%1,                      Sapphira%Thorne%NULL%1]</t>
+  </si>
+  <si>
+    <t>[ E.%Smith%null%1,                       C. F.% Aldus%null%1,                       J.% Brainard%null%1,                       S.% Dunham%null%1,                       P. R.% Hunter%null%1,                       N.% Steel%null%1,                       P. % Everden%null%1,     E.%Smith%null%1,     C. F.% Aldus%null%1,     J.% Brainard%null%1,     S.% Dunham%null%1,     P. R.% Hunter%null%1,     N.% Steel%null%1,     P. % Everden%null%1]</t>
+  </si>
+  <si>
+    <t>[Mahesh C%Patel%mp3@uic.edu%1,                      Lelia H%Chaisson%NULL%1,                      Scott%Borgetti%NULL%1,                      Deborah%Burdsall%NULL%1,                      Rashmi K%Chugh%NULL%1,                      Christopher R%Hoff%NULL%1,                      Elizabeth B%Murphy%NULL%1,                      Emily A%Murskyj%NULL%1,                      Shannon%Wilson%NULL%1,                      Joe%Ramos%NULL%1,                      Lynn%Akker%NULL%1,                      Debra%Bryars%NULL%1,                      Evonda%Thomas-Smith%NULL%1,                      Susan C%Bleasdale%NULL%1,                      Ngozi O%Ezike%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Helena%Temkin‐Greener%helena_temkin-greener@urmc.rochester.edu%1,                      Wenhan%Guo%NULL%2,                      Wenhan%Guo%NULL%0,                      Yunjiao%Mao%NULL%1,                      Xueya%Cai%NULL%1,                      Yue%Li%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Ana A.%Weil%anaweil@uw.edu%1,                      Kira L.%Newman%NULL%2,                      Kira L.%Newman%NULL%0,                      Thuan D.%Ong%NULL%1,                      Giana H.%Davidson%NULL%1,                      Jennifer%Logue%NULL%1,                      Elisabeth%Brandstetter%NULL%1,                      Ariana%Magedson%NULL%1,                      Dylan%McDonald%NULL%1,                      Denise J.%McCulloch%NULL%1,                      Santiago%Neme%NULL%1,                      James%Lewis%NULL%0,                      Jeff S.%Duchin%NULL%1,                      Weizhi%Zhong%NULL%1,                      Lea M.%Starita%NULL%1,                      Trevor%Bedford%NULL%1,                      Alison C.%Roxby%NULL%1,                      Helen Y.%Chu%helenchu@uw.edu%2]</t>
+  </si>
+  <si>
+    <t>[Guillermo V.%Sanchez%NULL%1,                      Caitlin%Biedron%NULL%1,                      Lauren R.%Fink%NULL%1,                      Kelly M.%Hatfield%NULL%1,                      Jordan Micah F.%Polistico%NULL%1,                      Monica P.%Meyer%NULL%1,                      Rebecca S.%Noe%NULL%1,                      Casey E.%Copen%NULL%1,                      Amanda K.%Lyons%NULL%1,                      Gonzalo%Gonzalez%NULL%1,                      Keith%Kiama%NULL%1,                      Mark%Lebednick%NULL%1,                      Bonnie K.%Czander%NULL%1,                      Amen%Agbonze%NULL%1,                      Aimee R.%Surma%NULL%1,                      Avnish%Sandhu%NULL%1,                      Valerie H.%Mika%NULL%1,                      Tyler%Prentiss%NULL%1,                      John%Zervos%NULL%1,                      Donia A.%Dalal%NULL%1,                      Amber M.%Vasquez%NULL%1,                      Sujan C.%Reddy%NULL%0,                      John%Jernigan%NULL%1,                      Paul E.%Kilgore%NULL%1,                      Marcus J.%Zervos%NULL%1,                      Teena%Chopra%NULL%1,                      Carla P.%Bezold%NULL%1,                      Najibah K.%Rehman%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Janice K%Louie%Janice.louie@sfdph.org%1,                      Hyman M%Scott%NULL%1,                      Amie%DuBois%NULL%1,                      Natalya%Sturtz%NULL%1,                      Wendy%Lu%NULL%1,                      Juliet%Stoltey%NULL%1,                      Godfred%Masinde%NULL%1,                      Stephanie%Cohen%NULL%1,                      Darpun%Sachdev%NULL%1,                      Susan%Philip%NULL%1,                      Naveena%Bobba%NULL%1,                      Tomas%Aragon%NULL%1,                      NULL%NULL%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Scott A%Goldberg%sagoldberg@bwh.harvard.edu%1,                      Jochen%Lennerz%NULL%1,                      Michael%Klompas%NULL%1,                      Eden%Mark%NULL%1,                      Virginia M%Pierce%NULL%1,                      Ryan W%Thompson%NULL%1,                      Charles T%Pu%NULL%1,                      Lauren L%Ritterhouse%NULL%1,                      Anand%Dighe%NULL%1,                      Eric S%Rosenberg%NULL%1,                      David C%Grabowski%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Amy V.%Dora%NULL%1,                      Alexander%Winnett%NULL%1,                      Lauren P.%Jatt%NULL%1,                      Kusha%Davar%NULL%1,                      Mika%Watanabe%NULL%1,                      Linda%Sohn%NULL%1,                      Hannah S.%Kern%NULL%1,                      Christopher J.%Graber%NULL%1,                      Matthew B.%Goetz%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Benjamin F.%Bigelow%NULL%1,                      Olive%Tang%NULL%1,                      Gregory R.%Toci%NULL%1,                      Norberth%Stracker%NULL%1,                      Fatima%Sheikh%NULL%1,                      Kara M.%Jacobs Slifka%NULL%1,                      Shannon A.%Novosad%NULL%1,                      John A.%Jernigan%NULL%0,                      Sujan C.%Reddy%NULL%0,                      Morgan J.%Katz%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Matt%Feaster%NULL%1,                      Ying-Ying%Goh%NULL%1]</t>
+  </si>
+  <si>
+    <t>[William R.%Mills%NULL%1,                      Janet M.%Buccola%NULL%1,                      Susan%Sender%NULL%1,                      Joseph%Lichtefeld%NULL%1,                      Nicholas%Romano%NULL%1,                      Karen%Reynolds%NULL%1,                      Melissa%Price%NULL%1,                      Jennifer%Phipps%NULL%1,                      Leigh%White%NULL%1,                      Shauen%Howard%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Drew A.%Harris%xref no email%1,   Laurie%Archbald-Pannone%xref no email%1,   Jasveen%Kaur%xref no email%1,   David%Cattell-Gordon%xref no email%1,   Karen S.%Rheuban%xref no email%1,   Rachel L.%Ombres%xref no email%1,   Kimberly%Albero%xref no email%1,   Rebecca%Steele%xref no email%1,   Taison D.%Bell%xref no email%1,   Justin B.%Mutter%xref no email%1]</t>
+  </si>
+  <si>
+    <t>[Carl D.%Shrader%xref no email%1,   Shauna%Assadzandi%xref no email%1,   Courtney S.%Pilkerton%xref no email%1,   Amie M.%Ashcraft%xref no email%1]</t>
+  </si>
+  <si>
+    <t>[Daniel J%Escobar%Daniel.escobar@pennmedicine.upenn.edu%1,                       Maria%Lanzi%NULL%1,                       Pouné%Saberi%NULL%1,                       Ruby%Love%NULL%1,                       Darren R%Linkin%NULL%1,                       John J%Kelly%NULL%1,                       Darshana%Jhala%NULL%1,                       Valerianna%Amorosa%NULL%1,                       Mary%Hofmann%NULL%1,                       Jeffrey B%Doyon%NULL%1]</t>
+  </si>
+  <si>
+    <t>[James L.%Rudolph%NULL%1,                       Christopher W.%Halladay%NULL%1,                       Malisa%Barber%NULL%1,                       Kevin W.%McConeghy%NULL%1,                       Vince%Mor%NULL%1,                       Aman%Nanda%NULL%1,                       Stefan%Gravenstein%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Paula%Eckardt%NULL%1,                       Rachel%Guran%NULL%1,                       Jon%Hennemyre%NULL%1,                       Roshan%Arikupurathu%NULL%1,                       Julie%Poveda%NULL%1,                       Nancimae%Miller%NULL%1,                       Randy%Katz%NULL%1,                       Judith%Frum%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Carson%Telford%NULL%1,                       Udodirim%Onwubiko%NULL%1,                       David%Holland%NULL%1,                       Kim%Turner%NULL%1,                       Juliana%Prieto%NULL%1,                       Sasha%Smith%NULL%1,                       Jane%Yoon%NULL%1,                       Wecheeta%Brown%NULL%1,                       Allison%Chamberlain%NULL%1,                       Neel%Gandhi%NULL%1,                       Shamimul%Khan%NULL%1,                       Steve%Williams%NULL%1,                       Fazle%Khan%NULL%1,                       Sarita%Shah%NULL%1,                        C. T.%Telford%null%1,                        U.% Onwubiko%null%1,                        D.% Holland%null%1,                        K.% Turner%null%1,                        J.% Prieto%null%1,                        S.% Smith%null%1,                        J.% Yoon%null%1,                        W.% Brown%null%1,                        A.% Chamberlain%null%1,                        N.% Gandhi%null%1,                        S.% Khan%null%1,                        S.% Williams%null%1,                        F.% Khan%null%1,                        S. % Shah%null%1,                       C. T.%Telford%null%1,                       U.% Onwubiko%null%1,                       D.% Holland%null%1,                       K.% Turner%null%1,                       J.% Prieto%null%1,                       S.% Smith%null%1,                       J.% Yoon%null%1,                       W.% Brown%null%1,                       A.% Chamberlain%null%1,                       N.% Gandhi%null%1,                       S.% Khan%null%1,                       S.% Williams%null%1,                       F.% Khan%null%1,                       S. % Shah%null%1,      C. T.%Telford%null%1,      U.% Onwubiko%null%1,      D.% Holland%null%1,      K.% Turner%null%1,      J.% Prieto%null%1,      S.% Smith%null%1,      J.% Yoon%null%1,      W.% Brown%null%1,      A.% Chamberlain%null%1,      N.% Gandhi%null%1,      S.% Khan%null%1,      S.% Williams%null%1,      F.% Khan%null%1,      S. % Shah%null%1]</t>
+  </si>
+  <si>
+    <t>[Sandra M.%Shi%NULL%1,                       Innokentiy%Bakaev%NULL%1,                       Helen%Chen%NULL%1,                       Thomas G.%Travison%NULL%1,                       Sarah D.%Berry%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Temet M.%McMichael%NULL%0,                       Dustin W.%Currie%NULL%0,                       Shauna%Clark%NULL%0,                       Sargis%Pogosjans%NULL%0,                       Meagan%Kay%NULL%0,                       Noah G.%Schwartz%NULL%0,                       James%Lewis%NULL%0,                       Atar%Baer%NULL%0,                       Vance%Kawakami%NULL%0,                       Margaret D.%Lukoff%NULL%0,                       Jessica%Ferro%NULL%0,                       Claire%Brostrom-Smith%NULL%0,                       Thomas D.%Rea%NULL%1,                       Michael R.%Sayre%NULL%1,                       Francis X.%Riedo%NULL%0,                       Denny%Russell%NULL%0,                       Brian%Hiatt%NULL%0,                       Patricia%Montgomery%NULL%0,                       Agam K.%Rao%NULL%0,                       Eric J.%Chow%NULL%0,                       Farrell%Tobolowsky%NULL%0,                       Michael J.%Hughes%NULL%1,                       Ana C.%Bardossy%NULL%0,                       Lisa P.%Oakley%NULL%0,                       Jesica R.%Jacobs%NULL%0,                       Nimalie D.%Stone%NULL%1,                       Sujan C.%Reddy%NULL%0,                       John A.%Jernigan%NULL%0,                       Margaret A.%Honein%NULL%0,                       Thomas A.%Clark%NULL%0,                       Jeffrey S.%Duchin%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Nathan M.%Stall%nathan.stall@sinaihealth.ca%1,                       Carolyn%Farquharson%NULL%2,                       Carolyn%Farquharson%NULL%0,                       Chris%Fan‐Lun%NULL%1,                       Lesley%Wiesenfeld%NULL%1,                       Carla A.%Loftus%NULL%1,                       Dylan%Kain%NULL%1,                       Jennie%Johnstone%NULL%1,                       Liz%McCreight%NULL%1,                       Russell D.%Goldman%NULL%1,                       Ramona%Mahtani%NULL%1]</t>
+  </si>
+  <si>
+    <t>[ Nathan M.%Stall%null%1,                        Aaron%Jones%null%1,                        Kevin A.%Brown%null%1,                        Paula A.%Rochon%null%1,                        Andrew P.%Costa%null%1,                       Nathan M.%Stall%null%1,                       Aaron%Jones%null%1,                       Kevin A.%Brown%null%1,                       Paula A.%Rochon%null%1,                       Andrew P.%Costa%null%1]</t>
+  </si>
+  <si>
+    <t>[Hubert%Blain%NULL%1,                       Yves%Rolland%NULL%1,                       Edouard%Tuaillon%NULL%1,                       Nadia%Giacosa%NULL%1,                       Mylène%Albrand%NULL%1,                       Audrey%Jaussent%NULL%1,                       Athanase%Benetos%NULL%1,                       Stéphanie%Miot%NULL%1,                       Jean%Bousquet%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Jo\u00ebl%Belmin%xref no email%1,    Nathavy%Um-Din%xref no email%1,    Cristiano%Donadio%xref no email%1,    Maurizio%Magri%xref no email%1,    Quoc Duy%Nghiem%xref no email%1,    Bruno%Oquendo%xref no email%1,    Sylvie%Pariel%xref no email%1,    Carmelo%Lafuente-Lafuente%xref no email%1]</t>
+  </si>
+  <si>
+    <t>[Guillaume%Sacco%NULL%1,                       Gonzague%Foucault%NULL%1,                       Olivier%Briere%NULL%1,                       Cédric%Annweiler%NULL%1]</t>
+  </si>
+  <si>
+    <t>[R.%Guery%NULL%1,                       C.%Delaye%NULL%1,                       N.%Brule%NULL%1,                       V.%Nael%NULL%1,                       L.%Castain%NULL%1,                       F.%Raffi%NULL%1,                       L.%De Decker%NULL%1]</t>
+  </si>
+  <si>
+    <t>[A.%Klein%anke.klein@uke.de%1,                       C.%Edler%NULL%1,                       A.%Fitzek%NULL%1,                       D.%Fröb%NULL%1,                       A.%Heinemann%NULL%1,                       K.%Meißner%NULL%1,                       H.%Mushumba%NULL%1,                       K.%Püschel%NULL%1,                       A. S.%Schröder%NULL%1,                       J. P.%Sperhake%NULL%1,                       F.%Ishorst-Witte%NULL%1,                       M.%Aepfelbacher%NULL%1,                       F.%Heinrich%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Buntinx%Frank%coreGivesNoEmail%1,                     Claes%Peter%coreGivesNoEmail%1,                     Gulikers%Marjo%coreGivesNoEmail%1,                     Jan%De Lepeleire%coreGivesNoEmail%1,                     Van%der Elst Michael%coreGivesNoEmail%1,                     Van%Elslande Jan%coreGivesNoEmail%1,                     Van%Ranst Marc%coreGivesNoEmail%1,                     Verbakel%Jan%coreGivesNoEmail%1,                     Vernneersch%Pieter%coreGivesNoEmail%1]</t>
+  </si>
+  <si>
+    <t>[Liangcong%Hu%xref no email%1,    Wanyuan%Zhen%xref no email%1,    Xudong%Xie%xref no email%2,    Ze%Lin%xref no email%2,    Tiantian%Wang%xref no email%1,    Jing%Liu%xref no email%5,    Hang%Xue%xref no email%2,    Adriana C.%Panayi%xref no email%2,    Ke%Xu%xref no email%1,    Zexi%Ling%xref no email%1,    Xugui%Li%xref no email%1,    Bobin%Mi%xref no email%1,    Wu%Zhou%xref no email%2,    Guohui%Liu%xref no email%2]</t>
+  </si>
+  <si>
+    <t>[Sean P%Kennelly%Sean.Kennelly@tuh.ie%1,                       Adam H%Dyer%dyera@tcd.ie%1,                       Claire%Noonan%claire.noonan@tuh.ie%2,                       Claire%Noonan%claire.noonan@tuh.ie%0,                       Ruth%Martin%ruth.martin1@hse.ie%1,                       Siobhan M%Kennelly%siobhan.kennelly1@hse.ie%1,                       Alan%Martin%alanmartin@beaumont.ie%1,                       Desmond%O’Neill%NULL%1,                       Aoife%Fallon%aoife.fallon1@hotmail.com%1]</t>
+  </si>
+  <si>
+    <t>[Antonio%Nouvenne%NULL%1,                       Andrea%Ticinesi%NULL%1,                       Alberto%Parise%NULL%1,                       Beatrice%Prati%NULL%1,                       Marcello%Esposito%NULL%1,                       Valentina%Cocchi%NULL%1,                       Emanuele%Crisafulli%NULL%1,                       Annalisa%Volpi%NULL%1,                       Sandra%Rossi%NULL%1,                       Elena Giovanna%Bignami%NULL%1,                       Marco%Baciarello%NULL%1,                       Ettore%Brianti%NULL%1,                       Massimo%Fabi%NULL%1,                       Tiziana%Meschi%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Nicola%Veronese%NULL%1,                       Luca Gino%Sbrogiò%NULL%1,                       Roberto%Valle%NULL%1,                       Laura%Marin%NULL%1,                       Elena%Boscolo Fiore%NULL%1,                       Andrea%Tiozzo%NULL%1]</t>
+  </si>
+  <si>
+    <t>[ J. H.%van den Besselaar%null%1,                        R. S.% Sikkema%null%1,                        F. M. H. P. A.% Koene%null%1,                        L. W.% van Buul%null%1,                        B. B.% Oude Munnink%null%1,                        I.% Frenay%null%1,                        R.% te Witt%null%1,                        M. P. G.% Koopmans%null%1,                        C. M. P. M.% Hertogh%null%1,                        B. M. % Buurman%null%1,      J. H.%van den Besselaar%null%1,      R. S.% Sikkema%null%1,      F. M. H. P. A.% Koene%null%1,      L. W.% van Buul%null%1,      B. B.% Oude Munnink%null%1,      I.% Frenay%null%1,      R.% te Witt%null%1,      M. P. G.% Koopmans%null%1,      C. M. P. M.% Hertogh%null%1,      B. M. % Buurman%null%1]</t>
+  </si>
+  <si>
+    <t>[Laura W.%van Buul%NULL%1,                       Judith H.%van den Besselaar%NULL%2,                       Judith H.%van den Besselaar%NULL%0,                       Fleur M. H. P. H.%Koene%NULL%1,                       Bianca M.%Buurman%NULL%1,                       Cees M. P. M.%Hertogh%NULL%1,                       Martin%Smalbrugge%NULL%1,                       Jeanine J. S.%Rutten%NULL%1,                       Elke M.%den Boogert%NULL%1,                       Michel D.%Wissing%NULL%1,                       Ariene%Rietveld%NULL%1,                       Mariska W. W.%van Elsakker%NULL%1,                       Marga M. G.%Nonneman%NULL%1,                       Florien%van Eeden%NULL%1,                       Saskia%van de Merwe%NULL%1,                       Sophie L.%Niemansburg%NULL%1,                       Ewout%Fanoy%NULL%1,                       Hinke S.%Bootsma%NULL%1,                       Nicoline%van der Hagen%NULL%1,                       Mariska%Petrignani%NULL%1,                       Jessica Edwards%van Muijen%NULL%1,                       Karolien E. M.%Biesheuvel%NULL%1]</t>
+  </si>
+  <si>
+    <t>[B\u00e5rd%Reiakvam Kittang%coreGivesNoEmail%1,                     Karina%Koller L\u00f8land%coreGivesNoEmail%1,                     Kjell%Kr\u00fcger%coreGivesNoEmail%1,                     Kristian%Jansen%coreGivesNoEmail%1,                     Sabine%Piepenstock Solheim%coreGivesNoEmail%1,                     Sebastian%von Hofacker%coreGivesNoEmail%1]</t>
+  </si>
+  <si>
+    <t>[Shin Young%Park%NULL%1,                       Gawon%Choi%NULL%2,                       Gawon%Choi%NULL%0,                       Hyeyoung%Lee%NULL%2,                       Hyeyoung%Lee%NULL%0,                       Na-young%Kim%NULL%2,                       Na-young%Kim%NULL%0,                       Seon-young%Lee%NULL%2,                       Seon-young%Lee%NULL%0,                       Kyungnam%Kim%NULL%2,                       Kyungnam%Kim%NULL%0,                       Soyoung%Shin%NULL%2,                       Soyoung%Shin%NULL%0,                       Eunsu%Jang%NULL%2,                       Eunsu%Jang%NULL%0,                       YoungSin%Moon%NULL%2,                       YoungSin%Moon%NULL%0,                       KwangHwan%Oh%NULL%2,                       KwangHwan%Oh%NULL%0,                       JaeRin%Choi%NULL%2,                       JaeRin%Choi%NULL%0,                       Sangeun%Lee%NULL%2,                       Sangeun%Lee%NULL%0,                       Young-Man%Kim%NULL%2,                       Young-Man%Kim%NULL%0,                       Jieun%Kim%NULL%2,                       Jieun%Kim%NULL%0,                       Seonju%Yi%NULL%2,                       Seonju%Yi%NULL%0,                       Jin%Gwack%NULL%2,                       Jin%Gwack%NULL%0,                       Ok%Park%NULL%2,                       Ok%Park%NULL%0,                       Young Joon%Park%NULL%2,                       Young Joon%Park%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Rok%Song%NULL%1,                       Hee-Sook%Kim%NULL%2,                       Hee-Sook%Kim%NULL%0,                       Seok-Ju%Yoo%NULL%2,                       Seok-Ju%Yoo%NULL%0,                       Kwan%Lee%NULL%2,                       Kwan%Lee%NULL%0,                       Ji-Hyuk%Park%NULL%2,                       Ji-Hyuk%Park%NULL%0,                       Joon Ho%Jang%NULL%2,                       Joon Ho%Jang%NULL%0,                       Gyoung-Sook%Ahn%NULL%2,                       Gyoung-Sook%Ahn%NULL%0,                       Jun-Nyun%Kim%NULL%2,                       Jun-Nyun%Kim%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Blanca%Borras-Bermejo%NULL%1,                       Xavier%Martínez-Gómez%NULL%1,                       María Gutierrez%San Miguel%NULL%1,                       Juliana%Esperalba%NULL%1,                       Andrés%Antón%NULL%1,                       Elisabet%Martin%NULL%1,                       Marta%Selvi%NULL%1,                       María José%Abadías%NULL%1,                       Antonio%Román%NULL%1,                       Tomàs%Pumarola%NULL%1,                       Magda%Campins%NULL%1,                       Benito%Almirante%NULL%1]</t>
+  </si>
+  <si>
+    <t>[M.%Bernabeu-Wittel%NULL%1,                       J.E.%Ternero-Vega%NULL%1,                       P.%Díaz-Jiménez%NULL%1,                       C.%Conde-Guzmán%NULL%1,                       M.D.%Nieto-Martín%NULL%1,                       L.%Moreno-Gaviño%NULL%1,                       J.%Delgado-Cuesta%NULL%1,                       M.%Rincón-Gómez%NULL%1,                       L.%Giménez-Miranda%NULL%1,                       M.D.%Navarro-Amuedo%NULL%1,                       M.M.%Muñoz-García%NULL%1,                       S.%Calzón-Fernández%NULL%1,                       M.%Ollero-Baturone%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Shamez N%Ladhani%shamez.ladhani@phe.gov.uk%1,                       J.Yimmy%Chow%NULL%1,                       Roshni%Janarthanan%NULL%1,                       Jonathan%Fok%NULL%1,                       Emma%Crawley-Boevey%NULL%1,                       Amoolya%Vusirikala%NULL%1,                       Elena%Fernandez%NULL%1,                       Marina Sanchez%Perez%NULL%1,                       Suzanne%Tang%NULL%1,                       Kate%Dun-Campbell%NULL%1,                       Edward Wynne-%Evans%NULL%1,                       Anita%Bell%NULL%1,                       Bharat%Patel%NULL%1,                       Zahin%Amin-Chowdhury%NULL%1,                       Felicity%Aiano%NULL%1,                       Karthik%Paranthaman%NULL%1,                       Thomas%Ma%NULL%1,                       Maria%Saavedra-Campos%NULL%1,                       Richard%Myers%NULL%1,                       Joanna%Ellis%NULL%2,                       Angie%Lackenby%NULL%1,                       Robin%Gopal%NULL%1,                       Monika%Patel%NULL%1,                       Colin%Brown%NULL%1,                       Meera%Chand%NULL%1,                       Kevin%Brown%NULL%1,                       Mary E%Ramsay%NULL%1,                       Susan%Hopkins%NULL%2,                       Nandini%Shetty%NULL%1,                       Maria%Zambon%NULL%2]</t>
+  </si>
+  <si>
+    <t>[N.S.N.%Graham%NULL%1,                       C.%Junghans%NULL%1,                       R.%Downes%NULL%1,                       C.%Sendall%NULL%1,                       H.%Lai%NULL%1,                       A.%McKirdy%NULL%1,                       P.%Elliott%NULL%1,                       R.%Howard%NULL%1,                       D.%Wingfield%NULL%1,                       M.%Priestman%NULL%1,                       M.%Ciechonska%NULL%1,                       L.%Cameron%NULL%1,                       M.%Storch%NULL%1,                       M.A.%Crone%NULL%1,                       P.S.%Freemont%NULL%1,                       P.%Randell%NULL%1,                       R.%McLaren%NULL%1,                       N.%Lang%NULL%1,                       S.%Ladhani%NULL%1,                       F.%Sanderson%NULL%1,                       D.J.%Sharp%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Agnes%Marossy%agnesmarossy@nhs.net%1,                       Stefan%Rakowicz%NULL%1,                       Angela%Bhan%NULL%1,                       Sarah%Noon%NULL%1,                       Amanda%Rees%NULL%1,                       Manjinder%Virk%NULL%1,                       Ayazali%Nazafi%NULL%1,                       Evie%Hay%NULL%1,                       Louise%de Thomasson%NULL%1,                       Christina%Windle%NULL%1,                       Mark%Zuckerman%Mark.Zuckerman@nhs.net%1]</t>
+  </si>
+  <si>
+    <t>[Laura%Shallcross%NULL%1,                       Danielle%Burke%NULL%1,                       Owen%Abbott%NULL%1,                       Alasdair%Donaldson%NULL%1,                       Gemma%Hallatt%NULL%1,                       Andrew%Hayward%NULL%1,                       Susan%Hopkins%NULL%0,                       Maria%Krutikov%NULL%1,                       Katie%Sharp%NULL%1,                       Leone%Wardman%NULL%1,                       Sapphira%Thorne%NULL%1]</t>
+  </si>
+  <si>
+    <t>[ E.%Smith%null%1,                        C. F.% Aldus%null%1,                        J.% Brainard%null%1,                        S.% Dunham%null%1,                        P. R.% Hunter%null%1,                        N.% Steel%null%1,                        P. % Everden%null%1,      E.%Smith%null%1,      C. F.% Aldus%null%1,      J.% Brainard%null%1,      S.% Dunham%null%1,      P. R.% Hunter%null%1,      N.% Steel%null%1,      P. % Everden%null%1]</t>
+  </si>
+  <si>
+    <t>[Mahesh C%Patel%mp3@uic.edu%1,                       Lelia H%Chaisson%NULL%1,                       Scott%Borgetti%NULL%1,                       Deborah%Burdsall%NULL%1,                       Rashmi K%Chugh%NULL%1,                       Christopher R%Hoff%NULL%1,                       Elizabeth B%Murphy%NULL%1,                       Emily A%Murskyj%NULL%1,                       Shannon%Wilson%NULL%1,                       Joe%Ramos%NULL%1,                       Lynn%Akker%NULL%1,                       Debra%Bryars%NULL%1,                       Evonda%Thomas-Smith%NULL%1,                       Susan C%Bleasdale%NULL%1,                       Ngozi O%Ezike%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Helena%Temkin‐Greener%helena_temkin-greener@urmc.rochester.edu%1,                       Wenhan%Guo%NULL%2,                       Wenhan%Guo%NULL%0,                       Yunjiao%Mao%NULL%1,                       Xueya%Cai%NULL%1,                       Yue%Li%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Ana A.%Weil%anaweil@uw.edu%1,                       Kira L.%Newman%NULL%2,                       Kira L.%Newman%NULL%0,                       Thuan D.%Ong%NULL%1,                       Giana H.%Davidson%NULL%1,                       Jennifer%Logue%NULL%1,                       Elisabeth%Brandstetter%NULL%1,                       Ariana%Magedson%NULL%1,                       Dylan%McDonald%NULL%1,                       Denise J.%McCulloch%NULL%1,                       Santiago%Neme%NULL%1,                       James%Lewis%NULL%0,                       Jeff S.%Duchin%NULL%1,                       Weizhi%Zhong%NULL%1,                       Lea M.%Starita%NULL%1,                       Trevor%Bedford%NULL%1,                       Alison C.%Roxby%NULL%1,                       Helen Y.%Chu%helenchu@uw.edu%2]</t>
+  </si>
+  <si>
+    <t>[Guillermo V.%Sanchez%NULL%1,                       Caitlin%Biedron%NULL%1,                       Lauren R.%Fink%NULL%1,                       Kelly M.%Hatfield%NULL%1,                       Jordan Micah F.%Polistico%NULL%1,                       Monica P.%Meyer%NULL%1,                       Rebecca S.%Noe%NULL%1,                       Casey E.%Copen%NULL%1,                       Amanda K.%Lyons%NULL%1,                       Gonzalo%Gonzalez%NULL%1,                       Keith%Kiama%NULL%1,                       Mark%Lebednick%NULL%1,                       Bonnie K.%Czander%NULL%1,                       Amen%Agbonze%NULL%1,                       Aimee R.%Surma%NULL%1,                       Avnish%Sandhu%NULL%1,                       Valerie H.%Mika%NULL%1,                       Tyler%Prentiss%NULL%1,                       John%Zervos%NULL%1,                       Donia A.%Dalal%NULL%1,                       Amber M.%Vasquez%NULL%1,                       Sujan C.%Reddy%NULL%0,                       John%Jernigan%NULL%1,                       Paul E.%Kilgore%NULL%1,                       Marcus J.%Zervos%NULL%1,                       Teena%Chopra%NULL%1,                       Carla P.%Bezold%NULL%1,                       Najibah K.%Rehman%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Janice K%Louie%Janice.louie@sfdph.org%1,                       Hyman M%Scott%NULL%1,                       Amie%DuBois%NULL%1,                       Natalya%Sturtz%NULL%1,                       Wendy%Lu%NULL%1,                       Juliet%Stoltey%NULL%1,                       Godfred%Masinde%NULL%1,                       Stephanie%Cohen%NULL%1,                       Darpun%Sachdev%NULL%1,                       Susan%Philip%NULL%1,                       Naveena%Bobba%NULL%1,                       Tomas%Aragon%NULL%1,                       NULL%NULL%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Scott A%Goldberg%sagoldberg@bwh.harvard.edu%1,                       Jochen%Lennerz%NULL%1,                       Michael%Klompas%NULL%1,                       Eden%Mark%NULL%1,                       Virginia M%Pierce%NULL%1,                       Ryan W%Thompson%NULL%1,                       Charles T%Pu%NULL%1,                       Lauren L%Ritterhouse%NULL%1,                       Anand%Dighe%NULL%1,                       Eric S%Rosenberg%NULL%1,                       David C%Grabowski%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Amy V.%Dora%NULL%1,                       Alexander%Winnett%NULL%1,                       Lauren P.%Jatt%NULL%1,                       Kusha%Davar%NULL%1,                       Mika%Watanabe%NULL%1,                       Linda%Sohn%NULL%1,                       Hannah S.%Kern%NULL%1,                       Christopher J.%Graber%NULL%1,                       Matthew B.%Goetz%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Benjamin F.%Bigelow%NULL%1,                       Olive%Tang%NULL%1,                       Gregory R.%Toci%NULL%1,                       Norberth%Stracker%NULL%1,                       Fatima%Sheikh%NULL%1,                       Kara M.%Jacobs Slifka%NULL%1,                       Shannon A.%Novosad%NULL%1,                       John A.%Jernigan%NULL%0,                       Sujan C.%Reddy%NULL%0,                       Morgan J.%Katz%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Matt%Feaster%NULL%1,                       Ying-Ying%Goh%NULL%1]</t>
+  </si>
+  <si>
+    <t>[William R.%Mills%NULL%1,                       Janet M.%Buccola%NULL%1,                       Susan%Sender%NULL%1,                       Joseph%Lichtefeld%NULL%1,                       Nicholas%Romano%NULL%1,                       Karen%Reynolds%NULL%1,                       Melissa%Price%NULL%1,                       Jennifer%Phipps%NULL%1,                       Leigh%White%NULL%1,                       Shauen%Howard%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Drew A.%Harris%xref no email%1,    Laurie%Archbald-Pannone%xref no email%1,    Jasveen%Kaur%xref no email%1,    David%Cattell-Gordon%xref no email%1,    Karen S.%Rheuban%xref no email%1,    Rachel L.%Ombres%xref no email%1,    Kimberly%Albero%xref no email%1,    Rebecca%Steele%xref no email%1,    Taison D.%Bell%xref no email%1,    Justin B.%Mutter%xref no email%1]</t>
+  </si>
+  <si>
+    <t>[Carl D.%Shrader%xref no email%1,    Shauna%Assadzandi%xref no email%1,    Courtney S.%Pilkerton%xref no email%1,    Amie M.%Ashcraft%xref no email%1]</t>
+  </si>
+  <si>
+    <t>[Daniel J%Escobar%Daniel.escobar@pennmedicine.upenn.edu%1,                        Maria%Lanzi%NULL%1,                        Pouné%Saberi%NULL%1,                        Ruby%Love%NULL%1,                        Darren R%Linkin%NULL%1,                        John J%Kelly%NULL%1,                        Darshana%Jhala%NULL%1,                        Valerianna%Amorosa%NULL%1,                        Mary%Hofmann%NULL%1,                        Jeffrey B%Doyon%NULL%1]</t>
+  </si>
+  <si>
+    <t>[James L.%Rudolph%NULL%1,                        Christopher W.%Halladay%NULL%1,                        Malisa%Barber%NULL%1,                        Kevin W.%McConeghy%NULL%1,                        Vince%Mor%NULL%1,                        Aman%Nanda%NULL%1,                        Stefan%Gravenstein%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Paula%Eckardt%NULL%1,                        Rachel%Guran%NULL%1,                        Jon%Hennemyre%NULL%1,                        Roshan%Arikupurathu%NULL%1,                        Julie%Poveda%NULL%1,                        Nancimae%Miller%NULL%1,                        Randy%Katz%NULL%1,                        Judith%Frum%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Carson%Telford%NULL%1,                        Udodirim%Onwubiko%NULL%1,                        David%Holland%NULL%1,                        Kim%Turner%NULL%1,                        Juliana%Prieto%NULL%1,                        Sasha%Smith%NULL%1,                        Jane%Yoon%NULL%1,                        Wecheeta%Brown%NULL%1,                        Allison%Chamberlain%NULL%1,                        Neel%Gandhi%NULL%1,                        Shamimul%Khan%NULL%1,                        Steve%Williams%NULL%1,                        Fazle%Khan%NULL%1,                        Sarita%Shah%NULL%1,                         C. T.%Telford%null%1,                         U.% Onwubiko%null%1,                         D.% Holland%null%1,                         K.% Turner%null%1,                         J.% Prieto%null%1,                         S.% Smith%null%1,                         J.% Yoon%null%1,                         W.% Brown%null%1,                         A.% Chamberlain%null%1,                         N.% Gandhi%null%1,                         S.% Khan%null%1,                         S.% Williams%null%1,                         F.% Khan%null%1,                         S. % Shah%null%1,                        C. T.%Telford%null%1,                        U.% Onwubiko%null%1,                        D.% Holland%null%1,                        K.% Turner%null%1,                        J.% Prieto%null%1,                        S.% Smith%null%1,                        J.% Yoon%null%1,                        W.% Brown%null%1,                        A.% Chamberlain%null%1,                        N.% Gandhi%null%1,                        S.% Khan%null%1,                        S.% Williams%null%1,                        F.% Khan%null%1,                        S. % Shah%null%1,       C. T.%Telford%null%1,       U.% Onwubiko%null%1,       D.% Holland%null%1,       K.% Turner%null%1,       J.% Prieto%null%1,       S.% Smith%null%1,       J.% Yoon%null%1,       W.% Brown%null%1,       A.% Chamberlain%null%1,       N.% Gandhi%null%1,       S.% Khan%null%1,       S.% Williams%null%1,       F.% Khan%null%1,       S. % Shah%null%1]</t>
+  </si>
+  <si>
+    <t>[Sandra M.%Shi%NULL%1,                        Innokentiy%Bakaev%NULL%1,                        Helen%Chen%NULL%1,                        Thomas G.%Travison%NULL%1,                        Sarah D.%Berry%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Temet M.%McMichael%NULL%0,                        Dustin W.%Currie%NULL%0,                        Shauna%Clark%NULL%0,                        Sargis%Pogosjans%NULL%0,                        Meagan%Kay%NULL%0,                        Noah G.%Schwartz%NULL%0,                        James%Lewis%NULL%0,                        Atar%Baer%NULL%0,                        Vance%Kawakami%NULL%0,                        Margaret D.%Lukoff%NULL%0,                        Jessica%Ferro%NULL%0,                        Claire%Brostrom-Smith%NULL%0,                        Thomas D.%Rea%NULL%1,                        Michael R.%Sayre%NULL%1,                        Francis X.%Riedo%NULL%0,                        Denny%Russell%NULL%0,                        Brian%Hiatt%NULL%0,                        Patricia%Montgomery%NULL%0,                        Agam K.%Rao%NULL%0,                        Eric J.%Chow%NULL%0,                        Farrell%Tobolowsky%NULL%0,                        Michael J.%Hughes%NULL%1,                        Ana C.%Bardossy%NULL%0,                        Lisa P.%Oakley%NULL%0,                        Jesica R.%Jacobs%NULL%0,                        Nimalie D.%Stone%NULL%1,                        Sujan C.%Reddy%NULL%0,                        John A.%Jernigan%NULL%0,                        Margaret A.%Honein%NULL%0,                        Thomas A.%Clark%NULL%0,                        Jeffrey S.%Duchin%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Nathan M.%Stall%nathan.stall@sinaihealth.ca%1,                        Carolyn%Farquharson%NULL%2,                        Carolyn%Farquharson%NULL%0,                        Chris%Fan‐Lun%NULL%1,                        Lesley%Wiesenfeld%NULL%1,                        Carla A.%Loftus%NULL%1,                        Dylan%Kain%NULL%1,                        Jennie%Johnstone%NULL%1,                        Liz%McCreight%NULL%1,                        Russell D.%Goldman%NULL%1,                        Ramona%Mahtani%NULL%1]</t>
+  </si>
+  <si>
+    <t>[ Nathan M.%Stall%null%1,                         Aaron%Jones%null%1,                         Kevin A.%Brown%null%1,                         Paula A.%Rochon%null%1,                         Andrew P.%Costa%null%1,                        Nathan M.%Stall%null%1,                        Aaron%Jones%null%1,                        Kevin A.%Brown%null%1,                        Paula A.%Rochon%null%1,                        Andrew P.%Costa%null%1]</t>
+  </si>
+  <si>
+    <t>[Hubert%Blain%NULL%1,                        Yves%Rolland%NULL%1,                        Edouard%Tuaillon%NULL%1,                        Nadia%Giacosa%NULL%1,                        Mylène%Albrand%NULL%1,                        Audrey%Jaussent%NULL%1,                        Athanase%Benetos%NULL%1,                        Stéphanie%Miot%NULL%1,                        Jean%Bousquet%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Jo\u00ebl%Belmin%xref no email%1,     Nathavy%Um-Din%xref no email%1,     Cristiano%Donadio%xref no email%1,     Maurizio%Magri%xref no email%1,     Quoc Duy%Nghiem%xref no email%1,     Bruno%Oquendo%xref no email%1,     Sylvie%Pariel%xref no email%1,     Carmelo%Lafuente-Lafuente%xref no email%1]</t>
+  </si>
+  <si>
+    <t>[Guillaume%Sacco%NULL%1,                        Gonzague%Foucault%NULL%1,                        Olivier%Briere%NULL%1,                        Cédric%Annweiler%NULL%1]</t>
+  </si>
+  <si>
+    <t>[R.%Guery%NULL%1,                        C.%Delaye%NULL%1,                        N.%Brule%NULL%1,                        V.%Nael%NULL%1,                        L.%Castain%NULL%1,                        F.%Raffi%NULL%1,                        L.%De Decker%NULL%1]</t>
+  </si>
+  <si>
+    <t>[A.%Klein%anke.klein@uke.de%1,                        C.%Edler%NULL%1,                        A.%Fitzek%NULL%1,                        D.%Fröb%NULL%1,                        A.%Heinemann%NULL%1,                        K.%Meißner%NULL%1,                        H.%Mushumba%NULL%1,                        K.%Püschel%NULL%1,                        A. S.%Schröder%NULL%1,                        J. P.%Sperhake%NULL%1,                        F.%Ishorst-Witte%NULL%1,                        M.%Aepfelbacher%NULL%1,                        F.%Heinrich%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Buntinx%Frank%coreGivesNoEmail%1,                      Claes%Peter%coreGivesNoEmail%1,                      Gulikers%Marjo%coreGivesNoEmail%1,                      Jan%De Lepeleire%coreGivesNoEmail%1,                      Van%der Elst Michael%coreGivesNoEmail%1,                      Van%Elslande Jan%coreGivesNoEmail%1,                      Van%Ranst Marc%coreGivesNoEmail%1,                      Verbakel%Jan%coreGivesNoEmail%1,                      Vernneersch%Pieter%coreGivesNoEmail%1]</t>
+  </si>
+  <si>
+    <t>[Liangcong%Hu%xref no email%1,     Wanyuan%Zhen%xref no email%1,     Xudong%Xie%xref no email%2,     Ze%Lin%xref no email%2,     Tiantian%Wang%xref no email%1,     Jing%Liu%xref no email%5,     Hang%Xue%xref no email%2,     Adriana C.%Panayi%xref no email%2,     Ke%Xu%xref no email%1,     Zexi%Ling%xref no email%1,     Xugui%Li%xref no email%1,     Bobin%Mi%xref no email%1,     Wu%Zhou%xref no email%2,     Guohui%Liu%xref no email%2]</t>
+  </si>
+  <si>
+    <t>[Sean P%Kennelly%Sean.Kennelly@tuh.ie%1,                        Adam H%Dyer%dyera@tcd.ie%1,                        Claire%Noonan%claire.noonan@tuh.ie%2,                        Claire%Noonan%claire.noonan@tuh.ie%0,                        Ruth%Martin%ruth.martin1@hse.ie%1,                        Siobhan M%Kennelly%siobhan.kennelly1@hse.ie%1,                        Alan%Martin%alanmartin@beaumont.ie%1,                        Desmond%O’Neill%NULL%1,                        Aoife%Fallon%aoife.fallon1@hotmail.com%1]</t>
+  </si>
+  <si>
+    <t>[Antonio%Nouvenne%NULL%1,                        Andrea%Ticinesi%NULL%1,                        Alberto%Parise%NULL%1,                        Beatrice%Prati%NULL%1,                        Marcello%Esposito%NULL%1,                        Valentina%Cocchi%NULL%1,                        Emanuele%Crisafulli%NULL%1,                        Annalisa%Volpi%NULL%1,                        Sandra%Rossi%NULL%1,                        Elena Giovanna%Bignami%NULL%1,                        Marco%Baciarello%NULL%1,                        Ettore%Brianti%NULL%1,                        Massimo%Fabi%NULL%1,                        Tiziana%Meschi%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Nicola%Veronese%NULL%1,                        Luca Gino%Sbrogiò%NULL%1,                        Roberto%Valle%NULL%1,                        Laura%Marin%NULL%1,                        Elena%Boscolo Fiore%NULL%1,                        Andrea%Tiozzo%NULL%1]</t>
+  </si>
+  <si>
+    <t>[ J. H.%van den Besselaar%null%1,                         R. S.% Sikkema%null%1,                         F. M. H. P. A.% Koene%null%1,                         L. W.% van Buul%null%1,                         B. B.% Oude Munnink%null%1,                         I.% Frenay%null%1,                         R.% te Witt%null%1,                         M. P. G.% Koopmans%null%1,                         C. M. P. M.% Hertogh%null%1,                         B. M. % Buurman%null%1,       J. H.%van den Besselaar%null%1,       R. S.% Sikkema%null%1,       F. M. H. P. A.% Koene%null%1,       L. W.% van Buul%null%1,       B. B.% Oude Munnink%null%1,       I.% Frenay%null%1,       R.% te Witt%null%1,       M. P. G.% Koopmans%null%1,       C. M. P. M.% Hertogh%null%1,       B. M. % Buurman%null%1]</t>
+  </si>
+  <si>
+    <t>[Laura W.%van Buul%NULL%1,                        Judith H.%van den Besselaar%NULL%2,                        Judith H.%van den Besselaar%NULL%0,                        Fleur M. H. P. H.%Koene%NULL%1,                        Bianca M.%Buurman%NULL%1,                        Cees M. P. M.%Hertogh%NULL%1,                        Martin%Smalbrugge%NULL%1,                        Jeanine J. S.%Rutten%NULL%1,                        Elke M.%den Boogert%NULL%1,                        Michel D.%Wissing%NULL%1,                        Ariene%Rietveld%NULL%1,                        Mariska W. W.%van Elsakker%NULL%1,                        Marga M. G.%Nonneman%NULL%1,                        Florien%van Eeden%NULL%1,                        Saskia%van de Merwe%NULL%1,                        Sophie L.%Niemansburg%NULL%1,                        Ewout%Fanoy%NULL%1,                        Hinke S.%Bootsma%NULL%1,                        Nicoline%van der Hagen%NULL%1,                        Mariska%Petrignani%NULL%1,                        Jessica Edwards%van Muijen%NULL%1,                        Karolien E. M.%Biesheuvel%NULL%1]</t>
+  </si>
+  <si>
+    <t>[B\u00e5rd%Reiakvam Kittang%coreGivesNoEmail%1,                      Karina%Koller L\u00f8land%coreGivesNoEmail%1,                      Kjell%Kr\u00fcger%coreGivesNoEmail%1,                      Kristian%Jansen%coreGivesNoEmail%1,                      Sabine%Piepenstock Solheim%coreGivesNoEmail%1,                      Sebastian%von Hofacker%coreGivesNoEmail%1]</t>
+  </si>
+  <si>
+    <t>[Shin Young%Park%NULL%1,                        Gawon%Choi%NULL%2,                        Gawon%Choi%NULL%0,                        Hyeyoung%Lee%NULL%2,                        Hyeyoung%Lee%NULL%0,                        Na-young%Kim%NULL%2,                        Na-young%Kim%NULL%0,                        Seon-young%Lee%NULL%2,                        Seon-young%Lee%NULL%0,                        Kyungnam%Kim%NULL%2,                        Kyungnam%Kim%NULL%0,                        Soyoung%Shin%NULL%2,                        Soyoung%Shin%NULL%0,                        Eunsu%Jang%NULL%2,                        Eunsu%Jang%NULL%0,                        YoungSin%Moon%NULL%2,                        YoungSin%Moon%NULL%0,                        KwangHwan%Oh%NULL%2,                        KwangHwan%Oh%NULL%0,                        JaeRin%Choi%NULL%2,                        JaeRin%Choi%NULL%0,                        Sangeun%Lee%NULL%2,                        Sangeun%Lee%NULL%0,                        Young-Man%Kim%NULL%2,                        Young-Man%Kim%NULL%0,                        Jieun%Kim%NULL%2,                        Jieun%Kim%NULL%0,                        Seonju%Yi%NULL%2,                        Seonju%Yi%NULL%0,                        Jin%Gwack%NULL%2,                        Jin%Gwack%NULL%0,                        Ok%Park%NULL%2,                        Ok%Park%NULL%0,                        Young Joon%Park%NULL%2,                        Young Joon%Park%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Rok%Song%NULL%1,                        Hee-Sook%Kim%NULL%2,                        Hee-Sook%Kim%NULL%0,                        Seok-Ju%Yoo%NULL%2,                        Seok-Ju%Yoo%NULL%0,                        Kwan%Lee%NULL%2,                        Kwan%Lee%NULL%0,                        Ji-Hyuk%Park%NULL%2,                        Ji-Hyuk%Park%NULL%0,                        Joon Ho%Jang%NULL%2,                        Joon Ho%Jang%NULL%0,                        Gyoung-Sook%Ahn%NULL%2,                        Gyoung-Sook%Ahn%NULL%0,                        Jun-Nyun%Kim%NULL%2,                        Jun-Nyun%Kim%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Blanca%Borras-Bermejo%NULL%1,                        Xavier%Martínez-Gómez%NULL%1,                        María Gutierrez%San Miguel%NULL%1,                        Juliana%Esperalba%NULL%1,                        Andrés%Antón%NULL%1,                        Elisabet%Martin%NULL%1,                        Marta%Selvi%NULL%1,                        María José%Abadías%NULL%1,                        Antonio%Román%NULL%1,                        Tomàs%Pumarola%NULL%1,                        Magda%Campins%NULL%1,                        Benito%Almirante%NULL%1]</t>
+  </si>
+  <si>
+    <t>[M.%Bernabeu-Wittel%NULL%1,                        J.E.%Ternero-Vega%NULL%1,                        P.%Díaz-Jiménez%NULL%1,                        C.%Conde-Guzmán%NULL%1,                        M.D.%Nieto-Martín%NULL%1,                        L.%Moreno-Gaviño%NULL%1,                        J.%Delgado-Cuesta%NULL%1,                        M.%Rincón-Gómez%NULL%1,                        L.%Giménez-Miranda%NULL%1,                        M.D.%Navarro-Amuedo%NULL%1,                        M.M.%Muñoz-García%NULL%1,                        S.%Calzón-Fernández%NULL%1,                        M.%Ollero-Baturone%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Shamez N%Ladhani%shamez.ladhani@phe.gov.uk%1,                        J.Yimmy%Chow%NULL%1,                        Roshni%Janarthanan%NULL%1,                        Jonathan%Fok%NULL%1,                        Emma%Crawley-Boevey%NULL%1,                        Amoolya%Vusirikala%NULL%1,                        Elena%Fernandez%NULL%1,                        Marina Sanchez%Perez%NULL%1,                        Suzanne%Tang%NULL%1,                        Kate%Dun-Campbell%NULL%1,                        Edward Wynne-%Evans%NULL%1,                        Anita%Bell%NULL%1,                        Bharat%Patel%NULL%1,                        Zahin%Amin-Chowdhury%NULL%1,                        Felicity%Aiano%NULL%1,                        Karthik%Paranthaman%NULL%1,                        Thomas%Ma%NULL%1,                        Maria%Saavedra-Campos%NULL%1,                        Richard%Myers%NULL%1,                        Joanna%Ellis%NULL%2,                        Angie%Lackenby%NULL%1,                        Robin%Gopal%NULL%1,                        Monika%Patel%NULL%1,                        Colin%Brown%NULL%1,                        Meera%Chand%NULL%1,                        Kevin%Brown%NULL%1,                        Mary E%Ramsay%NULL%1,                        Susan%Hopkins%NULL%2,                        Nandini%Shetty%NULL%1,                        Maria%Zambon%NULL%2]</t>
+  </si>
+  <si>
+    <t>[N.S.N.%Graham%NULL%1,                        C.%Junghans%NULL%1,                        R.%Downes%NULL%1,                        C.%Sendall%NULL%1,                        H.%Lai%NULL%1,                        A.%McKirdy%NULL%1,                        P.%Elliott%NULL%1,                        R.%Howard%NULL%1,                        D.%Wingfield%NULL%1,                        M.%Priestman%NULL%1,                        M.%Ciechonska%NULL%1,                        L.%Cameron%NULL%1,                        M.%Storch%NULL%1,                        M.A.%Crone%NULL%1,                        P.S.%Freemont%NULL%1,                        P.%Randell%NULL%1,                        R.%McLaren%NULL%1,                        N.%Lang%NULL%1,                        S.%Ladhani%NULL%1,                        F.%Sanderson%NULL%1,                        D.J.%Sharp%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Agnes%Marossy%agnesmarossy@nhs.net%1,                        Stefan%Rakowicz%NULL%1,                        Angela%Bhan%NULL%1,                        Sarah%Noon%NULL%1,                        Amanda%Rees%NULL%1,                        Manjinder%Virk%NULL%1,                        Ayazali%Nazafi%NULL%1,                        Evie%Hay%NULL%1,                        Louise%de Thomasson%NULL%1,                        Christina%Windle%NULL%1,                        Mark%Zuckerman%Mark.Zuckerman@nhs.net%1]</t>
+  </si>
+  <si>
+    <t>[Laura%Shallcross%NULL%1,                        Danielle%Burke%NULL%1,                        Owen%Abbott%NULL%1,                        Alasdair%Donaldson%NULL%1,                        Gemma%Hallatt%NULL%1,                        Andrew%Hayward%NULL%1,                        Susan%Hopkins%NULL%0,                        Maria%Krutikov%NULL%1,                        Katie%Sharp%NULL%1,                        Leone%Wardman%NULL%1,                        Sapphira%Thorne%NULL%1]</t>
+  </si>
+  <si>
+    <t>[ E.%Smith%null%1,                         C. F.% Aldus%null%1,                         J.% Brainard%null%1,                         S.% Dunham%null%1,                         P. R.% Hunter%null%1,                         N.% Steel%null%1,                         P. % Everden%null%1,       E.%Smith%null%1,       C. F.% Aldus%null%1,       J.% Brainard%null%1,       S.% Dunham%null%1,       P. R.% Hunter%null%1,       N.% Steel%null%1,       P. % Everden%null%1]</t>
+  </si>
+  <si>
+    <t>[Mahesh C%Patel%mp3@uic.edu%1,                        Lelia H%Chaisson%NULL%1,                        Scott%Borgetti%NULL%1,                        Deborah%Burdsall%NULL%1,                        Rashmi K%Chugh%NULL%1,                        Christopher R%Hoff%NULL%1,                        Elizabeth B%Murphy%NULL%1,                        Emily A%Murskyj%NULL%1,                        Shannon%Wilson%NULL%1,                        Joe%Ramos%NULL%1,                        Lynn%Akker%NULL%1,                        Debra%Bryars%NULL%1,                        Evonda%Thomas-Smith%NULL%1,                        Susan C%Bleasdale%NULL%1,                        Ngozi O%Ezike%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Helena%Temkin‐Greener%helena_temkin-greener@urmc.rochester.edu%1,                        Wenhan%Guo%NULL%2,                        Wenhan%Guo%NULL%0,                        Yunjiao%Mao%NULL%1,                        Xueya%Cai%NULL%1,                        Yue%Li%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Ana A.%Weil%anaweil@uw.edu%1,                        Kira L.%Newman%NULL%2,                        Kira L.%Newman%NULL%0,                        Thuan D.%Ong%NULL%1,                        Giana H.%Davidson%NULL%1,                        Jennifer%Logue%NULL%1,                        Elisabeth%Brandstetter%NULL%1,                        Ariana%Magedson%NULL%1,                        Dylan%McDonald%NULL%1,                        Denise J.%McCulloch%NULL%1,                        Santiago%Neme%NULL%1,                        James%Lewis%NULL%0,                        Jeff S.%Duchin%NULL%1,                        Weizhi%Zhong%NULL%1,                        Lea M.%Starita%NULL%1,                        Trevor%Bedford%NULL%1,                        Alison C.%Roxby%NULL%1,                        Helen Y.%Chu%helenchu@uw.edu%2]</t>
+  </si>
+  <si>
+    <t>[Guillermo V.%Sanchez%NULL%1,                        Caitlin%Biedron%NULL%1,                        Lauren R.%Fink%NULL%1,                        Kelly M.%Hatfield%NULL%1,                        Jordan Micah F.%Polistico%NULL%1,                        Monica P.%Meyer%NULL%1,                        Rebecca S.%Noe%NULL%1,                        Casey E.%Copen%NULL%1,                        Amanda K.%Lyons%NULL%1,                        Gonzalo%Gonzalez%NULL%1,                        Keith%Kiama%NULL%1,                        Mark%Lebednick%NULL%1,                        Bonnie K.%Czander%NULL%1,                        Amen%Agbonze%NULL%1,                        Aimee R.%Surma%NULL%1,                        Avnish%Sandhu%NULL%1,                        Valerie H.%Mika%NULL%1,                        Tyler%Prentiss%NULL%1,                        John%Zervos%NULL%1,                        Donia A.%Dalal%NULL%1,                        Amber M.%Vasquez%NULL%1,                        Sujan C.%Reddy%NULL%0,                        John%Jernigan%NULL%1,                        Paul E.%Kilgore%NULL%1,                        Marcus J.%Zervos%NULL%1,                        Teena%Chopra%NULL%1,                        Carla P.%Bezold%NULL%1,                        Najibah K.%Rehman%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Janice K%Louie%Janice.louie@sfdph.org%1,                        Hyman M%Scott%NULL%1,                        Amie%DuBois%NULL%1,                        Natalya%Sturtz%NULL%1,                        Wendy%Lu%NULL%1,                        Juliet%Stoltey%NULL%1,                        Godfred%Masinde%NULL%1,                        Stephanie%Cohen%NULL%1,                        Darpun%Sachdev%NULL%1,                        Susan%Philip%NULL%1,                        Naveena%Bobba%NULL%1,                        Tomas%Aragon%NULL%1,                        NULL%NULL%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Scott A%Goldberg%sagoldberg@bwh.harvard.edu%1,                        Jochen%Lennerz%NULL%1,                        Michael%Klompas%NULL%1,                        Eden%Mark%NULL%1,                        Virginia M%Pierce%NULL%1,                        Ryan W%Thompson%NULL%1,                        Charles T%Pu%NULL%1,                        Lauren L%Ritterhouse%NULL%1,                        Anand%Dighe%NULL%1,                        Eric S%Rosenberg%NULL%1,                        David C%Grabowski%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Amy V.%Dora%NULL%1,                        Alexander%Winnett%NULL%1,                        Lauren P.%Jatt%NULL%1,                        Kusha%Davar%NULL%1,                        Mika%Watanabe%NULL%1,                        Linda%Sohn%NULL%1,                        Hannah S.%Kern%NULL%1,                        Christopher J.%Graber%NULL%1,                        Matthew B.%Goetz%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Benjamin F.%Bigelow%NULL%1,                        Olive%Tang%NULL%1,                        Gregory R.%Toci%NULL%1,                        Norberth%Stracker%NULL%1,                        Fatima%Sheikh%NULL%1,                        Kara M.%Jacobs Slifka%NULL%1,                        Shannon A.%Novosad%NULL%1,                        John A.%Jernigan%NULL%0,                        Sujan C.%Reddy%NULL%0,                        Morgan J.%Katz%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Matt%Feaster%NULL%1,                        Ying-Ying%Goh%NULL%1]</t>
+  </si>
+  <si>
+    <t>[William R.%Mills%NULL%1,                        Janet M.%Buccola%NULL%1,                        Susan%Sender%NULL%1,                        Joseph%Lichtefeld%NULL%1,                        Nicholas%Romano%NULL%1,                        Karen%Reynolds%NULL%1,                        Melissa%Price%NULL%1,                        Jennifer%Phipps%NULL%1,                        Leigh%White%NULL%1,                        Shauen%Howard%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Drew A.%Harris%xref no email%1,     Laurie%Archbald-Pannone%xref no email%1,     Jasveen%Kaur%xref no email%1,     David%Cattell-Gordon%xref no email%1,     Karen S.%Rheuban%xref no email%1,     Rachel L.%Ombres%xref no email%1,     Kimberly%Albero%xref no email%1,     Rebecca%Steele%xref no email%1,     Taison D.%Bell%xref no email%1,     Justin B.%Mutter%xref no email%1]</t>
+  </si>
+  <si>
+    <t>[Carl D.%Shrader%xref no email%1,     Shauna%Assadzandi%xref no email%1,     Courtney S.%Pilkerton%xref no email%1,     Amie M.%Ashcraft%xref no email%1]</t>
   </si>
 </sst>
 </file>
@@ -2334,6 +2979,9 @@
       <c r="I1" t="s">
         <v>181</v>
       </c>
+      <c r="J1" t="s">
+        <v>540</v>
+      </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -2349,7 +2997,7 @@
         <v>59</v>
       </c>
       <c r="E2" t="s">
-        <v>498</v>
+        <v>713</v>
       </c>
       <c r="F2" t="s">
         <v>60</v>
@@ -2362,6 +3010,9 @@
       </c>
       <c r="I2" t="s">
         <v>450</v>
+      </c>
+      <c r="J2" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -2378,7 +3029,7 @@
         <v>64</v>
       </c>
       <c r="E3" t="s">
-        <v>499</v>
+        <v>714</v>
       </c>
       <c r="F3" t="s">
         <v>65</v>
@@ -2391,6 +3042,9 @@
       </c>
       <c r="I3" t="s">
         <v>452</v>
+      </c>
+      <c r="J3" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -2407,7 +3061,7 @@
         <v>67</v>
       </c>
       <c r="E4" t="s">
-        <v>500</v>
+        <v>715</v>
       </c>
       <c r="F4" t="s">
         <v>68</v>
@@ -2420,6 +3074,9 @@
       </c>
       <c r="I4" t="s">
         <v>452</v>
+      </c>
+      <c r="J4" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -2450,6 +3107,9 @@
       <c r="I5" t="s">
         <v>95</v>
       </c>
+      <c r="J5" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -2465,7 +3125,7 @@
         <v>70</v>
       </c>
       <c r="E6" t="s">
-        <v>501</v>
+        <v>716</v>
       </c>
       <c r="F6" t="s">
         <v>6</v>
@@ -2478,6 +3138,9 @@
       </c>
       <c r="I6" t="s">
         <v>450</v>
+      </c>
+      <c r="J6" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -2494,7 +3157,7 @@
         <v>73</v>
       </c>
       <c r="E7" t="s">
-        <v>502</v>
+        <v>717</v>
       </c>
       <c r="F7" t="s">
         <v>74</v>
@@ -2507,6 +3170,9 @@
       </c>
       <c r="I7" t="s">
         <v>452</v>
+      </c>
+      <c r="J7" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -2523,7 +3189,7 @@
         <v>76</v>
       </c>
       <c r="E8" t="s">
-        <v>503</v>
+        <v>718</v>
       </c>
       <c r="F8" t="s">
         <v>77</v>
@@ -2536,6 +3202,9 @@
       </c>
       <c r="I8" t="s">
         <v>450</v>
+      </c>
+      <c r="J8" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -2566,6 +3235,9 @@
       <c r="I9" t="s">
         <v>457</v>
       </c>
+      <c r="J9" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
@@ -2581,7 +3253,7 @@
         <v>79</v>
       </c>
       <c r="E10" t="s">
-        <v>504</v>
+        <v>719</v>
       </c>
       <c r="F10" t="s">
         <v>80</v>
@@ -2594,6 +3266,9 @@
       </c>
       <c r="I10" t="s">
         <v>450</v>
+      </c>
+      <c r="J10" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -2610,7 +3285,7 @@
         <v>83</v>
       </c>
       <c r="E11" t="s">
-        <v>505</v>
+        <v>720</v>
       </c>
       <c r="F11" t="s">
         <v>84</v>
@@ -2623,6 +3298,9 @@
       </c>
       <c r="I11" t="s">
         <v>457</v>
+      </c>
+      <c r="J11" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -2639,7 +3317,7 @@
         <v>88</v>
       </c>
       <c r="E12" t="s">
-        <v>506</v>
+        <v>721</v>
       </c>
       <c r="F12" t="s">
         <v>89</v>
@@ -2652,6 +3330,9 @@
       </c>
       <c r="I12" t="s">
         <v>452</v>
+      </c>
+      <c r="J12" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -2668,7 +3349,7 @@
         <v>51</v>
       </c>
       <c r="E13" t="s">
-        <v>507</v>
+        <v>722</v>
       </c>
       <c r="F13" t="s">
         <v>243</v>
@@ -2681,6 +3362,9 @@
       </c>
       <c r="I13" t="s">
         <v>95</v>
+      </c>
+      <c r="J13" t="s">
+        <v>551</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -2697,7 +3381,7 @@
         <v>91</v>
       </c>
       <c r="E14" t="s">
-        <v>508</v>
+        <v>723</v>
       </c>
       <c r="F14" t="s">
         <v>92</v>
@@ -2710,6 +3394,9 @@
       </c>
       <c r="I14" t="s">
         <v>452</v>
+      </c>
+      <c r="J14" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -2726,7 +3413,7 @@
         <v>95</v>
       </c>
       <c r="E15" t="s">
-        <v>509</v>
+        <v>724</v>
       </c>
       <c r="F15" t="s">
         <v>96</v>
@@ -2739,6 +3426,9 @@
       </c>
       <c r="I15" t="s">
         <v>452</v>
+      </c>
+      <c r="J15" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -2755,7 +3445,7 @@
         <v>99</v>
       </c>
       <c r="E16" t="s">
-        <v>510</v>
+        <v>725</v>
       </c>
       <c r="F16" t="s">
         <v>100</v>
@@ -2768,6 +3458,9 @@
       </c>
       <c r="I16" t="s">
         <v>467</v>
+      </c>
+      <c r="J16" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -2784,7 +3477,7 @@
         <v>190</v>
       </c>
       <c r="E17" t="s">
-        <v>511</v>
+        <v>726</v>
       </c>
       <c r="F17" t="s">
         <v>16</v>
@@ -2797,6 +3490,9 @@
       </c>
       <c r="I17" t="s">
         <v>457</v>
+      </c>
+      <c r="J17" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -2827,6 +3523,9 @@
       <c r="I18" t="s">
         <v>450</v>
       </c>
+      <c r="J18" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
@@ -2842,7 +3541,7 @@
         <v>51</v>
       </c>
       <c r="E19" t="s">
-        <v>512</v>
+        <v>727</v>
       </c>
       <c r="F19" t="s">
         <v>18</v>
@@ -2854,7 +3553,10 @@
         <v>195</v>
       </c>
       <c r="I19" t="s">
-        <v>457</v>
+        <v>95</v>
+      </c>
+      <c r="J19" t="s">
+        <v>557</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -2871,7 +3573,7 @@
         <v>105</v>
       </c>
       <c r="E20" t="s">
-        <v>513</v>
+        <v>728</v>
       </c>
       <c r="F20" t="s">
         <v>106</v>
@@ -2884,6 +3586,9 @@
       </c>
       <c r="I20" t="s">
         <v>450</v>
+      </c>
+      <c r="J20" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
@@ -2900,7 +3605,7 @@
         <v>109</v>
       </c>
       <c r="E21" t="s">
-        <v>514</v>
+        <v>729</v>
       </c>
       <c r="F21" t="s">
         <v>110</v>
@@ -2913,6 +3618,9 @@
       </c>
       <c r="I21" t="s">
         <v>452</v>
+      </c>
+      <c r="J21" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -2929,7 +3637,7 @@
         <v>112</v>
       </c>
       <c r="E22" t="s">
-        <v>515</v>
+        <v>730</v>
       </c>
       <c r="F22" t="s">
         <v>113</v>
@@ -2942,6 +3650,9 @@
       </c>
       <c r="I22" t="s">
         <v>452</v>
+      </c>
+      <c r="J22" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -2972,6 +3683,9 @@
       <c r="I23" t="s">
         <v>457</v>
       </c>
+      <c r="J23" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
@@ -2987,7 +3701,7 @@
         <v>115</v>
       </c>
       <c r="E24" t="s">
-        <v>516</v>
+        <v>731</v>
       </c>
       <c r="F24" t="s">
         <v>23</v>
@@ -3000,6 +3714,9 @@
       </c>
       <c r="I24" t="s">
         <v>474</v>
+      </c>
+      <c r="J24" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
@@ -3016,7 +3733,7 @@
         <v>118</v>
       </c>
       <c r="E25" t="s">
-        <v>517</v>
+        <v>732</v>
       </c>
       <c r="F25" t="s">
         <v>119</v>
@@ -3029,6 +3746,9 @@
       </c>
       <c r="I25" t="s">
         <v>450</v>
+      </c>
+      <c r="J25" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
@@ -3045,7 +3765,7 @@
         <v>51</v>
       </c>
       <c r="E26" t="s">
-        <v>518</v>
+        <v>733</v>
       </c>
       <c r="F26" t="s">
         <v>25</v>
@@ -3058,6 +3778,9 @@
       </c>
       <c r="I26" t="s">
         <v>457</v>
+      </c>
+      <c r="J26" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
@@ -3074,7 +3797,7 @@
         <v>122</v>
       </c>
       <c r="E27" t="s">
-        <v>519</v>
+        <v>734</v>
       </c>
       <c r="F27" t="s">
         <v>123</v>
@@ -3087,6 +3810,9 @@
       </c>
       <c r="I27" t="s">
         <v>450</v>
+      </c>
+      <c r="J27" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
@@ -3103,7 +3829,7 @@
         <v>126</v>
       </c>
       <c r="E28" t="s">
-        <v>520</v>
+        <v>735</v>
       </c>
       <c r="F28" t="s">
         <v>127</v>
@@ -3116,6 +3842,9 @@
       </c>
       <c r="I28" t="s">
         <v>450</v>
+      </c>
+      <c r="J28" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
@@ -3132,7 +3861,7 @@
         <v>130</v>
       </c>
       <c r="E29" t="s">
-        <v>521</v>
+        <v>736</v>
       </c>
       <c r="F29" t="s">
         <v>131</v>
@@ -3145,6 +3874,9 @@
       </c>
       <c r="I29" t="s">
         <v>450</v>
+      </c>
+      <c r="J29" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
@@ -3161,7 +3893,7 @@
         <v>95</v>
       </c>
       <c r="E30" t="s">
-        <v>522</v>
+        <v>737</v>
       </c>
       <c r="F30" t="s">
         <v>133</v>
@@ -3174,6 +3906,9 @@
       </c>
       <c r="I30" t="s">
         <v>452</v>
+      </c>
+      <c r="J30" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
@@ -3190,7 +3925,7 @@
         <v>136</v>
       </c>
       <c r="E31" t="s">
-        <v>523</v>
+        <v>738</v>
       </c>
       <c r="F31" t="s">
         <v>137</v>
@@ -3203,6 +3938,9 @@
       </c>
       <c r="I31" t="s">
         <v>452</v>
+      </c>
+      <c r="J31" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -3219,7 +3957,7 @@
         <v>140</v>
       </c>
       <c r="E32" t="s">
-        <v>524</v>
+        <v>739</v>
       </c>
       <c r="F32" t="s">
         <v>141</v>
@@ -3232,6 +3970,9 @@
       </c>
       <c r="I32" t="s">
         <v>452</v>
+      </c>
+      <c r="J32" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
@@ -3248,7 +3989,7 @@
         <v>144</v>
       </c>
       <c r="E33" t="s">
-        <v>525</v>
+        <v>740</v>
       </c>
       <c r="F33" t="s">
         <v>145</v>
@@ -3261,6 +4002,9 @@
       </c>
       <c r="I33" t="s">
         <v>450</v>
+      </c>
+      <c r="J33" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
@@ -3277,7 +4021,7 @@
         <v>147</v>
       </c>
       <c r="E34" t="s">
-        <v>526</v>
+        <v>741</v>
       </c>
       <c r="F34" t="s">
         <v>148</v>
@@ -3290,6 +4034,9 @@
       </c>
       <c r="I34" t="s">
         <v>452</v>
+      </c>
+      <c r="J34" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
@@ -3306,7 +4053,7 @@
         <v>150</v>
       </c>
       <c r="E35" t="s">
-        <v>527</v>
+        <v>742</v>
       </c>
       <c r="F35" t="s">
         <v>34</v>
@@ -3319,6 +4066,9 @@
       </c>
       <c r="I35" t="s">
         <v>474</v>
+      </c>
+      <c r="J35" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
@@ -3335,7 +4085,7 @@
         <v>153</v>
       </c>
       <c r="E36" t="s">
-        <v>528</v>
+        <v>743</v>
       </c>
       <c r="F36" t="s">
         <v>154</v>
@@ -3348,6 +4098,9 @@
       </c>
       <c r="I36" t="s">
         <v>450</v>
+      </c>
+      <c r="J36" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
@@ -3364,7 +4117,7 @@
         <v>157</v>
       </c>
       <c r="E37" t="s">
-        <v>529</v>
+        <v>744</v>
       </c>
       <c r="F37" t="s">
         <v>158</v>
@@ -3377,6 +4130,9 @@
       </c>
       <c r="I37" t="s">
         <v>450</v>
+      </c>
+      <c r="J37" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
@@ -3393,7 +4149,7 @@
         <v>201</v>
       </c>
       <c r="E38" t="s">
-        <v>530</v>
+        <v>745</v>
       </c>
       <c r="F38" t="s">
         <v>161</v>
@@ -3406,6 +4162,9 @@
       </c>
       <c r="I38" t="s">
         <v>467</v>
+      </c>
+      <c r="J38" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
@@ -3422,7 +4181,7 @@
         <v>95</v>
       </c>
       <c r="E39" t="s">
-        <v>531</v>
+        <v>746</v>
       </c>
       <c r="F39" t="s">
         <v>164</v>
@@ -3435,6 +4194,9 @@
       </c>
       <c r="I39" t="s">
         <v>450</v>
+      </c>
+      <c r="J39" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
@@ -3451,7 +4213,7 @@
         <v>166</v>
       </c>
       <c r="E40" t="s">
-        <v>532</v>
+        <v>747</v>
       </c>
       <c r="F40" t="s">
         <v>167</v>
@@ -3464,6 +4226,9 @@
       </c>
       <c r="I40" t="s">
         <v>450</v>
+      </c>
+      <c r="J40" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
@@ -3480,7 +4245,7 @@
         <v>169</v>
       </c>
       <c r="E41" t="s">
-        <v>533</v>
+        <v>748</v>
       </c>
       <c r="F41" t="s">
         <v>170</v>
@@ -3493,6 +4258,9 @@
       </c>
       <c r="I41" t="s">
         <v>450</v>
+      </c>
+      <c r="J41" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
@@ -3509,7 +4277,7 @@
         <v>95</v>
       </c>
       <c r="E42" t="s">
-        <v>534</v>
+        <v>749</v>
       </c>
       <c r="F42" t="s">
         <v>172</v>
@@ -3522,6 +4290,9 @@
       </c>
       <c r="I42" t="s">
         <v>450</v>
+      </c>
+      <c r="J42" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
@@ -3538,7 +4309,7 @@
         <v>95</v>
       </c>
       <c r="E43" t="s">
-        <v>535</v>
+        <v>750</v>
       </c>
       <c r="F43" t="s">
         <v>174</v>
@@ -3551,6 +4322,9 @@
       </c>
       <c r="I43" t="s">
         <v>450</v>
+      </c>
+      <c r="J43" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
@@ -3567,7 +4341,7 @@
         <v>176</v>
       </c>
       <c r="E44" t="s">
-        <v>536</v>
+        <v>751</v>
       </c>
       <c r="F44" t="s">
         <v>177</v>
@@ -3580,6 +4354,9 @@
       </c>
       <c r="I44" t="s">
         <v>450</v>
+      </c>
+      <c r="J44" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
@@ -3596,7 +4373,7 @@
         <v>179</v>
       </c>
       <c r="E45" t="s">
-        <v>537</v>
+        <v>752</v>
       </c>
       <c r="F45" t="s">
         <v>180</v>
@@ -3609,6 +4386,9 @@
       </c>
       <c r="I45" t="s">
         <v>452</v>
+      </c>
+      <c r="J45" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
@@ -3625,7 +4405,7 @@
         <v>51</v>
       </c>
       <c r="E46" t="s">
-        <v>538</v>
+        <v>753</v>
       </c>
       <c r="F46" t="s">
         <v>45</v>
@@ -3634,10 +4414,13 @@
         <v>194</v>
       </c>
       <c r="H46" t="s">
-        <v>197</v>
+        <v>584</v>
       </c>
       <c r="I46" t="s">
-        <v>457</v>
+        <v>95</v>
+      </c>
+      <c r="J46" t="s">
+        <v>585</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
@@ -3654,7 +4437,7 @@
         <v>199</v>
       </c>
       <c r="E47" t="s">
-        <v>539</v>
+        <v>754</v>
       </c>
       <c r="F47" t="s">
         <v>46</v>
@@ -3666,7 +4449,10 @@
         <v>200</v>
       </c>
       <c r="I47" t="s">
-        <v>457</v>
+        <v>95</v>
+      </c>
+      <c r="J47" t="s">
+        <v>587</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the ability to read from an elastic search json query output: stored in a specific file.  Now have 99.25% of the references
</commit_message>
<xml_diff>
--- a/Covid_19_Dataset_and_References/References/10.xlsx
+++ b/Covid_19_Dataset_and_References/References/10.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4561" uniqueCount="755">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5313" uniqueCount="833">
   <si>
     <t>Doi</t>
   </si>
@@ -2653,6 +2653,240 @@
   </si>
   <si>
     <t>[Carl D.%Shrader%xref no email%1,     Shauna%Assadzandi%xref no email%1,     Courtney S.%Pilkerton%xref no email%1,     Amie M.%Ashcraft%xref no email%1]</t>
+  </si>
+  <si>
+    <t>[Daniel J%Escobar%Daniel.escobar@pennmedicine.upenn.edu%1,                         Maria%Lanzi%NULL%1,                         Pouné%Saberi%NULL%1,                         Ruby%Love%NULL%1,                         Darren R%Linkin%NULL%1,                         John J%Kelly%NULL%1,                         Darshana%Jhala%NULL%1,                         Valerianna%Amorosa%NULL%1,                         Mary%Hofmann%NULL%1,                         Jeffrey B%Doyon%NULL%1]</t>
+  </si>
+  <si>
+    <t>[James L.%Rudolph%NULL%1,                         Christopher W.%Halladay%NULL%1,                         Malisa%Barber%NULL%1,                         Kevin W.%McConeghy%NULL%1,                         Vince%Mor%NULL%1,                         Aman%Nanda%NULL%1,                         Stefan%Gravenstein%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Paula%Eckardt%NULL%1,                         Rachel%Guran%NULL%1,                         Jon%Hennemyre%NULL%1,                         Roshan%Arikupurathu%NULL%1,                         Julie%Poveda%NULL%1,                         Nancimae%Miller%NULL%1,                         Randy%Katz%NULL%1,                         Judith%Frum%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Carson%Telford%NULL%1,                         Udodirim%Onwubiko%NULL%1,                         David%Holland%NULL%1,                         Kim%Turner%NULL%1,                         Juliana%Prieto%NULL%1,                         Sasha%Smith%NULL%1,                         Jane%Yoon%NULL%1,                         Wecheeta%Brown%NULL%1,                         Allison%Chamberlain%NULL%1,                         Neel%Gandhi%NULL%1,                         Shamimul%Khan%NULL%1,                         Steve%Williams%NULL%1,                         Fazle%Khan%NULL%1,                         Sarita%Shah%NULL%1,                          C. T.%Telford%null%1,                          U.% Onwubiko%null%1,                          D.% Holland%null%1,                          K.% Turner%null%1,                          J.% Prieto%null%1,                          S.% Smith%null%1,                          J.% Yoon%null%1,                          W.% Brown%null%1,                          A.% Chamberlain%null%1,                          N.% Gandhi%null%1,                          S.% Khan%null%1,                          S.% Williams%null%1,                          F.% Khan%null%1,                          S. % Shah%null%1,                         C. T.%Telford%null%1,                         U.% Onwubiko%null%1,                         D.% Holland%null%1,                         K.% Turner%null%1,                         J.% Prieto%null%1,                         S.% Smith%null%1,                         J.% Yoon%null%1,                         W.% Brown%null%1,                         A.% Chamberlain%null%1,                         N.% Gandhi%null%1,                         S.% Khan%null%1,                         S.% Williams%null%1,                         F.% Khan%null%1,                         S. % Shah%null%1,        C. T.%Telford%null%1,        U.% Onwubiko%null%1,        D.% Holland%null%1,        K.% Turner%null%1,        J.% Prieto%null%1,        S.% Smith%null%1,        J.% Yoon%null%1,        W.% Brown%null%1,        A.% Chamberlain%null%1,        N.% Gandhi%null%1,        S.% Khan%null%1,        S.% Williams%null%1,        F.% Khan%null%1,        S. % Shah%null%1]</t>
+  </si>
+  <si>
+    <t>[Sandra M.%Shi%NULL%1,                         Innokentiy%Bakaev%NULL%1,                         Helen%Chen%NULL%1,                         Thomas G.%Travison%NULL%1,                         Sarah D.%Berry%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Temet M.%McMichael%NULL%0,                         Dustin W.%Currie%NULL%0,                         Shauna%Clark%NULL%0,                         Sargis%Pogosjans%NULL%0,                         Meagan%Kay%NULL%0,                         Noah G.%Schwartz%NULL%0,                         James%Lewis%NULL%0,                         Atar%Baer%NULL%0,                         Vance%Kawakami%NULL%0,                         Margaret D.%Lukoff%NULL%0,                         Jessica%Ferro%NULL%0,                         Claire%Brostrom-Smith%NULL%0,                         Thomas D.%Rea%NULL%1,                         Michael R.%Sayre%NULL%1,                         Francis X.%Riedo%NULL%0,                         Denny%Russell%NULL%0,                         Brian%Hiatt%NULL%0,                         Patricia%Montgomery%NULL%0,                         Agam K.%Rao%NULL%0,                         Eric J.%Chow%NULL%0,                         Farrell%Tobolowsky%NULL%0,                         Michael J.%Hughes%NULL%1,                         Ana C.%Bardossy%NULL%0,                         Lisa P.%Oakley%NULL%0,                         Jesica R.%Jacobs%NULL%0,                         Nimalie D.%Stone%NULL%1,                         Sujan C.%Reddy%NULL%0,                         John A.%Jernigan%NULL%0,                         Margaret A.%Honein%NULL%0,                         Thomas A.%Clark%NULL%0,                         Jeffrey S.%Duchin%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Nathan M.%Stall%nathan.stall@sinaihealth.ca%1,                         Carolyn%Farquharson%NULL%2,                         Carolyn%Farquharson%NULL%0,                         Chris%Fan‐Lun%NULL%1,                         Lesley%Wiesenfeld%NULL%1,                         Carla A.%Loftus%NULL%1,                         Dylan%Kain%NULL%1,                         Jennie%Johnstone%NULL%1,                         Liz%McCreight%NULL%1,                         Russell D.%Goldman%NULL%1,                         Ramona%Mahtani%NULL%1]</t>
+  </si>
+  <si>
+    <t>[ Nathan M.%Stall%null%1,                          Aaron%Jones%null%1,                          Kevin A.%Brown%null%1,                          Paula A.%Rochon%null%1,                          Andrew P.%Costa%null%1,                         Nathan M.%Stall%null%1,                         Aaron%Jones%null%1,                         Kevin A.%Brown%null%1,                         Paula A.%Rochon%null%1,                         Andrew P.%Costa%null%1]</t>
+  </si>
+  <si>
+    <t>[Hubert%Blain%NULL%1,                         Yves%Rolland%NULL%1,                         Edouard%Tuaillon%NULL%1,                         Nadia%Giacosa%NULL%1,                         Mylène%Albrand%NULL%1,                         Audrey%Jaussent%NULL%1,                         Athanase%Benetos%NULL%1,                         Stéphanie%Miot%NULL%1,                         Jean%Bousquet%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Jo\u00ebl%Belmin%xref no email%1,      Nathavy%Um-Din%xref no email%1,      Cristiano%Donadio%xref no email%1,      Maurizio%Magri%xref no email%1,      Quoc Duy%Nghiem%xref no email%1,      Bruno%Oquendo%xref no email%1,      Sylvie%Pariel%xref no email%1,      Carmelo%Lafuente-Lafuente%xref no email%1]</t>
+  </si>
+  <si>
+    <t>[Guillaume%Sacco%NULL%1,                         Gonzague%Foucault%NULL%1,                         Olivier%Briere%NULL%1,                         Cédric%Annweiler%NULL%1]</t>
+  </si>
+  <si>
+    <t>[R.%Guery%NULL%1,                         C.%Delaye%NULL%1,                         N.%Brule%NULL%1,                         V.%Nael%NULL%1,                         L.%Castain%NULL%1,                         F.%Raffi%NULL%1,                         L.%De Decker%NULL%1]</t>
+  </si>
+  <si>
+    <t>[A.%Klein%anke.klein@uke.de%1,                         C.%Edler%NULL%1,                         A.%Fitzek%NULL%1,                         D.%Fröb%NULL%1,                         A.%Heinemann%NULL%1,                         K.%Meißner%NULL%1,                         H.%Mushumba%NULL%1,                         K.%Püschel%NULL%1,                         A. S.%Schröder%NULL%1,                         J. P.%Sperhake%NULL%1,                         F.%Ishorst-Witte%NULL%1,                         M.%Aepfelbacher%NULL%1,                         F.%Heinrich%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Buntinx%Frank%coreGivesNoEmail%1,                       Claes%Peter%coreGivesNoEmail%1,                       Gulikers%Marjo%coreGivesNoEmail%1,                       Jan%De Lepeleire%coreGivesNoEmail%1,                       Van%der Elst Michael%coreGivesNoEmail%1,                       Van%Elslande Jan%coreGivesNoEmail%1,                       Van%Ranst Marc%coreGivesNoEmail%1,                       Verbakel%Jan%coreGivesNoEmail%1,                       Vernneersch%Pieter%coreGivesNoEmail%1]</t>
+  </si>
+  <si>
+    <t>[Sean P%Kennelly%Sean.Kennelly@tuh.ie%1,                         Adam H%Dyer%dyera@tcd.ie%1,                         Claire%Noonan%claire.noonan@tuh.ie%2,                         Claire%Noonan%claire.noonan@tuh.ie%0,                         Ruth%Martin%ruth.martin1@hse.ie%1,                         Siobhan M%Kennelly%siobhan.kennelly1@hse.ie%1,                         Alan%Martin%alanmartin@beaumont.ie%1,                         Desmond%O’Neill%NULL%1,                         Aoife%Fallon%aoife.fallon1@hotmail.com%1]</t>
+  </si>
+  <si>
+    <t>[Antonio%Nouvenne%NULL%1,                         Andrea%Ticinesi%NULL%1,                         Alberto%Parise%NULL%1,                         Beatrice%Prati%NULL%1,                         Marcello%Esposito%NULL%1,                         Valentina%Cocchi%NULL%1,                         Emanuele%Crisafulli%NULL%1,                         Annalisa%Volpi%NULL%1,                         Sandra%Rossi%NULL%1,                         Elena Giovanna%Bignami%NULL%1,                         Marco%Baciarello%NULL%1,                         Ettore%Brianti%NULL%1,                         Massimo%Fabi%NULL%1,                         Tiziana%Meschi%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Nicola%Veronese%NULL%1,                         Luca Gino%Sbrogiò%NULL%1,                         Roberto%Valle%NULL%1,                         Laura%Marin%NULL%1,                         Elena%Boscolo Fiore%NULL%1,                         Andrea%Tiozzo%NULL%1]</t>
+  </si>
+  <si>
+    <t>[ J. H.%van den Besselaar%null%1,                          R. S.% Sikkema%null%1,                          F. M. H. P. A.% Koene%null%1,                          L. W.% van Buul%null%1,                          B. B.% Oude Munnink%null%1,                          I.% Frenay%null%1,                          R.% te Witt%null%1,                          M. P. G.% Koopmans%null%1,                          C. M. P. M.% Hertogh%null%1,                          B. M. % Buurman%null%1,        J. H.%van den Besselaar%null%1,        R. S.% Sikkema%null%1,        F. M. H. P. A.% Koene%null%1,        L. W.% van Buul%null%1,        B. B.% Oude Munnink%null%1,        I.% Frenay%null%1,        R.% te Witt%null%1,        M. P. G.% Koopmans%null%1,        C. M. P. M.% Hertogh%null%1,        B. M. % Buurman%null%1]</t>
+  </si>
+  <si>
+    <t>[Laura W.%van Buul%NULL%1,                         Judith H.%van den Besselaar%NULL%2,                         Judith H.%van den Besselaar%NULL%0,                         Fleur M. H. P. H.%Koene%NULL%1,                         Bianca M.%Buurman%NULL%1,                         Cees M. P. M.%Hertogh%NULL%1,                         Martin%Smalbrugge%NULL%1,                         Jeanine J. S.%Rutten%NULL%1,                         Elke M.%den Boogert%NULL%1,                         Michel D.%Wissing%NULL%1,                         Ariene%Rietveld%NULL%1,                         Mariska W. W.%van Elsakker%NULL%1,                         Marga M. G.%Nonneman%NULL%1,                         Florien%van Eeden%NULL%1,                         Saskia%van de Merwe%NULL%1,                         Sophie L.%Niemansburg%NULL%1,                         Ewout%Fanoy%NULL%1,                         Hinke S.%Bootsma%NULL%1,                         Nicoline%van der Hagen%NULL%1,                         Mariska%Petrignani%NULL%1,                         Jessica Edwards%van Muijen%NULL%1,                         Karolien E. M.%Biesheuvel%NULL%1]</t>
+  </si>
+  <si>
+    <t>[B\u00e5rd%Reiakvam Kittang%coreGivesNoEmail%1,                       Karina%Koller L\u00f8land%coreGivesNoEmail%1,                       Kjell%Kr\u00fcger%coreGivesNoEmail%1,                       Kristian%Jansen%coreGivesNoEmail%1,                       Sabine%Piepenstock Solheim%coreGivesNoEmail%1,                       Sebastian%von Hofacker%coreGivesNoEmail%1]</t>
+  </si>
+  <si>
+    <t>[Shin Young%Park%NULL%1,                         Gawon%Choi%NULL%2,                         Gawon%Choi%NULL%0,                         Hyeyoung%Lee%NULL%2,                         Hyeyoung%Lee%NULL%0,                         Na-young%Kim%NULL%2,                         Na-young%Kim%NULL%0,                         Seon-young%Lee%NULL%2,                         Seon-young%Lee%NULL%0,                         Kyungnam%Kim%NULL%2,                         Kyungnam%Kim%NULL%0,                         Soyoung%Shin%NULL%2,                         Soyoung%Shin%NULL%0,                         Eunsu%Jang%NULL%2,                         Eunsu%Jang%NULL%0,                         YoungSin%Moon%NULL%2,                         YoungSin%Moon%NULL%0,                         KwangHwan%Oh%NULL%2,                         KwangHwan%Oh%NULL%0,                         JaeRin%Choi%NULL%2,                         JaeRin%Choi%NULL%0,                         Sangeun%Lee%NULL%2,                         Sangeun%Lee%NULL%0,                         Young-Man%Kim%NULL%2,                         Young-Man%Kim%NULL%0,                         Jieun%Kim%NULL%2,                         Jieun%Kim%NULL%0,                         Seonju%Yi%NULL%2,                         Seonju%Yi%NULL%0,                         Jin%Gwack%NULL%2,                         Jin%Gwack%NULL%0,                         Ok%Park%NULL%2,                         Ok%Park%NULL%0,                         Young Joon%Park%NULL%2,                         Young Joon%Park%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Rok%Song%NULL%1,                         Hee-Sook%Kim%NULL%2,                         Hee-Sook%Kim%NULL%0,                         Seok-Ju%Yoo%NULL%2,                         Seok-Ju%Yoo%NULL%0,                         Kwan%Lee%NULL%2,                         Kwan%Lee%NULL%0,                         Ji-Hyuk%Park%NULL%2,                         Ji-Hyuk%Park%NULL%0,                         Joon Ho%Jang%NULL%2,                         Joon Ho%Jang%NULL%0,                         Gyoung-Sook%Ahn%NULL%2,                         Gyoung-Sook%Ahn%NULL%0,                         Jun-Nyun%Kim%NULL%2,                         Jun-Nyun%Kim%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Blanca%Borras-Bermejo%NULL%1,                         Xavier%Martínez-Gómez%NULL%1,                         María Gutierrez%San Miguel%NULL%1,                         Juliana%Esperalba%NULL%1,                         Andrés%Antón%NULL%1,                         Elisabet%Martin%NULL%1,                         Marta%Selvi%NULL%1,                         María José%Abadías%NULL%1,                         Antonio%Román%NULL%1,                         Tomàs%Pumarola%NULL%1,                         Magda%Campins%NULL%1,                         Benito%Almirante%NULL%1]</t>
+  </si>
+  <si>
+    <t>[M.%Bernabeu-Wittel%NULL%1,                         J.E.%Ternero-Vega%NULL%1,                         P.%Díaz-Jiménez%NULL%1,                         C.%Conde-Guzmán%NULL%1,                         M.D.%Nieto-Martín%NULL%1,                         L.%Moreno-Gaviño%NULL%1,                         J.%Delgado-Cuesta%NULL%1,                         M.%Rincón-Gómez%NULL%1,                         L.%Giménez-Miranda%NULL%1,                         M.D.%Navarro-Amuedo%NULL%1,                         M.M.%Muñoz-García%NULL%1,                         S.%Calzón-Fernández%NULL%1,                         M.%Ollero-Baturone%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Shamez N%Ladhani%shamez.ladhani@phe.gov.uk%1,                         J.Yimmy%Chow%NULL%1,                         Roshni%Janarthanan%NULL%1,                         Jonathan%Fok%NULL%1,                         Emma%Crawley-Boevey%NULL%1,                         Amoolya%Vusirikala%NULL%1,                         Elena%Fernandez%NULL%1,                         Marina Sanchez%Perez%NULL%1,                         Suzanne%Tang%NULL%1,                         Kate%Dun-Campbell%NULL%1,                         Edward Wynne-%Evans%NULL%1,                         Anita%Bell%NULL%1,                         Bharat%Patel%NULL%1,                         Zahin%Amin-Chowdhury%NULL%1,                         Felicity%Aiano%NULL%1,                         Karthik%Paranthaman%NULL%1,                         Thomas%Ma%NULL%1,                         Maria%Saavedra-Campos%NULL%1,                         Richard%Myers%NULL%1,                         Joanna%Ellis%NULL%2,                         Angie%Lackenby%NULL%1,                         Robin%Gopal%NULL%1,                         Monika%Patel%NULL%1,                         Colin%Brown%NULL%1,                         Meera%Chand%NULL%1,                         Kevin%Brown%NULL%1,                         Mary E%Ramsay%NULL%1,                         Susan%Hopkins%NULL%2,                         Nandini%Shetty%NULL%1,                         Maria%Zambon%NULL%2]</t>
+  </si>
+  <si>
+    <t>[N.S.N.%Graham%NULL%1,                         C.%Junghans%NULL%1,                         R.%Downes%NULL%1,                         C.%Sendall%NULL%1,                         H.%Lai%NULL%1,                         A.%McKirdy%NULL%1,                         P.%Elliott%NULL%1,                         R.%Howard%NULL%1,                         D.%Wingfield%NULL%1,                         M.%Priestman%NULL%1,                         M.%Ciechonska%NULL%1,                         L.%Cameron%NULL%1,                         M.%Storch%NULL%1,                         M.A.%Crone%NULL%1,                         P.S.%Freemont%NULL%1,                         P.%Randell%NULL%1,                         R.%McLaren%NULL%1,                         N.%Lang%NULL%1,                         S.%Ladhani%NULL%1,                         F.%Sanderson%NULL%1,                         D.J.%Sharp%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Agnes%Marossy%agnesmarossy@nhs.net%1,                         Stefan%Rakowicz%NULL%1,                         Angela%Bhan%NULL%1,                         Sarah%Noon%NULL%1,                         Amanda%Rees%NULL%1,                         Manjinder%Virk%NULL%1,                         Ayazali%Nazafi%NULL%1,                         Evie%Hay%NULL%1,                         Louise%de Thomasson%NULL%1,                         Christina%Windle%NULL%1,                         Mark%Zuckerman%Mark.Zuckerman@nhs.net%1]</t>
+  </si>
+  <si>
+    <t>[Laura%Shallcross%NULL%1,                         Danielle%Burke%NULL%1,                         Owen%Abbott%NULL%1,                         Alasdair%Donaldson%NULL%1,                         Gemma%Hallatt%NULL%1,                         Andrew%Hayward%NULL%1,                         Susan%Hopkins%NULL%0,                         Maria%Krutikov%NULL%1,                         Katie%Sharp%NULL%1,                         Leone%Wardman%NULL%1,                         Sapphira%Thorne%NULL%1]</t>
+  </si>
+  <si>
+    <t>[ E.%Smith%null%1,                          C. F.% Aldus%null%1,                          J.% Brainard%null%1,                          S.% Dunham%null%1,                          P. R.% Hunter%null%1,                          N.% Steel%null%1,                          P. % Everden%null%1,        E.%Smith%null%1,        C. F.% Aldus%null%1,        J.% Brainard%null%1,        S.% Dunham%null%1,        P. R.% Hunter%null%1,        N.% Steel%null%1,        P. % Everden%null%1]</t>
+  </si>
+  <si>
+    <t>[Mahesh C%Patel%mp3@uic.edu%1,                         Lelia H%Chaisson%NULL%1,                         Scott%Borgetti%NULL%1,                         Deborah%Burdsall%NULL%1,                         Rashmi K%Chugh%NULL%1,                         Christopher R%Hoff%NULL%1,                         Elizabeth B%Murphy%NULL%1,                         Emily A%Murskyj%NULL%1,                         Shannon%Wilson%NULL%1,                         Joe%Ramos%NULL%1,                         Lynn%Akker%NULL%1,                         Debra%Bryars%NULL%1,                         Evonda%Thomas-Smith%NULL%1,                         Susan C%Bleasdale%NULL%1,                         Ngozi O%Ezike%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Helena%Temkin‐Greener%helena_temkin-greener@urmc.rochester.edu%1,                         Wenhan%Guo%NULL%2,                         Wenhan%Guo%NULL%0,                         Yunjiao%Mao%NULL%1,                         Xueya%Cai%NULL%1,                         Yue%Li%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Ana A.%Weil%anaweil@uw.edu%1,                         Kira L.%Newman%NULL%2,                         Kira L.%Newman%NULL%0,                         Thuan D.%Ong%NULL%1,                         Giana H.%Davidson%NULL%1,                         Jennifer%Logue%NULL%1,                         Elisabeth%Brandstetter%NULL%1,                         Ariana%Magedson%NULL%1,                         Dylan%McDonald%NULL%1,                         Denise J.%McCulloch%NULL%1,                         Santiago%Neme%NULL%1,                         James%Lewis%NULL%0,                         Jeff S.%Duchin%NULL%1,                         Weizhi%Zhong%NULL%1,                         Lea M.%Starita%NULL%1,                         Trevor%Bedford%NULL%1,                         Alison C.%Roxby%NULL%1,                         Helen Y.%Chu%helenchu@uw.edu%2]</t>
+  </si>
+  <si>
+    <t>[Guillermo V.%Sanchez%NULL%1,                         Caitlin%Biedron%NULL%1,                         Lauren R.%Fink%NULL%1,                         Kelly M.%Hatfield%NULL%1,                         Jordan Micah F.%Polistico%NULL%1,                         Monica P.%Meyer%NULL%1,                         Rebecca S.%Noe%NULL%1,                         Casey E.%Copen%NULL%1,                         Amanda K.%Lyons%NULL%1,                         Gonzalo%Gonzalez%NULL%1,                         Keith%Kiama%NULL%1,                         Mark%Lebednick%NULL%1,                         Bonnie K.%Czander%NULL%1,                         Amen%Agbonze%NULL%1,                         Aimee R.%Surma%NULL%1,                         Avnish%Sandhu%NULL%1,                         Valerie H.%Mika%NULL%1,                         Tyler%Prentiss%NULL%1,                         John%Zervos%NULL%1,                         Donia A.%Dalal%NULL%1,                         Amber M.%Vasquez%NULL%1,                         Sujan C.%Reddy%NULL%0,                         John%Jernigan%NULL%1,                         Paul E.%Kilgore%NULL%1,                         Marcus J.%Zervos%NULL%1,                         Teena%Chopra%NULL%1,                         Carla P.%Bezold%NULL%1,                         Najibah K.%Rehman%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Janice K%Louie%Janice.louie@sfdph.org%1,                         Hyman M%Scott%NULL%1,                         Amie%DuBois%NULL%1,                         Natalya%Sturtz%NULL%1,                         Wendy%Lu%NULL%1,                         Juliet%Stoltey%NULL%1,                         Godfred%Masinde%NULL%1,                         Stephanie%Cohen%NULL%1,                         Darpun%Sachdev%NULL%1,                         Susan%Philip%NULL%1,                         Naveena%Bobba%NULL%1,                         Tomas%Aragon%NULL%1,                         NULL%NULL%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Scott A%Goldberg%sagoldberg@bwh.harvard.edu%1,                         Jochen%Lennerz%NULL%1,                         Michael%Klompas%NULL%1,                         Eden%Mark%NULL%1,                         Virginia M%Pierce%NULL%1,                         Ryan W%Thompson%NULL%1,                         Charles T%Pu%NULL%1,                         Lauren L%Ritterhouse%NULL%1,                         Anand%Dighe%NULL%1,                         Eric S%Rosenberg%NULL%1,                         David C%Grabowski%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Amy V.%Dora%NULL%1,                         Alexander%Winnett%NULL%1,                         Lauren P.%Jatt%NULL%1,                         Kusha%Davar%NULL%1,                         Mika%Watanabe%NULL%1,                         Linda%Sohn%NULL%1,                         Hannah S.%Kern%NULL%1,                         Christopher J.%Graber%NULL%1,                         Matthew B.%Goetz%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Benjamin F.%Bigelow%NULL%1,                         Olive%Tang%NULL%1,                         Gregory R.%Toci%NULL%1,                         Norberth%Stracker%NULL%1,                         Fatima%Sheikh%NULL%1,                         Kara M.%Jacobs Slifka%NULL%1,                         Shannon A.%Novosad%NULL%1,                         John A.%Jernigan%NULL%0,                         Sujan C.%Reddy%NULL%0,                         Morgan J.%Katz%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Matt%Feaster%NULL%1,                         Ying-Ying%Goh%NULL%1]</t>
+  </si>
+  <si>
+    <t>[William R.%Mills%NULL%1,                         Janet M.%Buccola%NULL%1,                         Susan%Sender%NULL%1,                         Joseph%Lichtefeld%NULL%1,                         Nicholas%Romano%NULL%1,                         Karen%Reynolds%NULL%1,                         Melissa%Price%NULL%1,                         Jennifer%Phipps%NULL%1,                         Leigh%White%NULL%1,                         Shauen%Howard%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Daniel J%Escobar%Daniel.escobar@pennmedicine.upenn.edu%1,                          Maria%Lanzi%NULL%1,                          Pouné%Saberi%NULL%1,                          Ruby%Love%NULL%1,                          Darren R%Linkin%NULL%1,                          John J%Kelly%NULL%1,                          Darshana%Jhala%NULL%1,                          Valerianna%Amorosa%NULL%1,                          Mary%Hofmann%NULL%1,                          Jeffrey B%Doyon%NULL%1]</t>
+  </si>
+  <si>
+    <t>[James L.%Rudolph%NULL%1,                          Christopher W.%Halladay%NULL%1,                          Malisa%Barber%NULL%1,                          Kevin W.%McConeghy%NULL%1,                          Vince%Mor%NULL%1,                          Aman%Nanda%NULL%1,                          Stefan%Gravenstein%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Paula%Eckardt%NULL%1,                          Rachel%Guran%NULL%1,                          Jon%Hennemyre%NULL%1,                          Roshan%Arikupurathu%NULL%1,                          Julie%Poveda%NULL%1,                          Nancimae%Miller%NULL%1,                          Randy%Katz%NULL%1,                          Judith%Frum%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Carson%Telford%NULL%1,                          Udodirim%Onwubiko%NULL%1,                          David%Holland%NULL%1,                          Kim%Turner%NULL%1,                          Juliana%Prieto%NULL%1,                          Sasha%Smith%NULL%1,                          Jane%Yoon%NULL%1,                          Wecheeta%Brown%NULL%1,                          Allison%Chamberlain%NULL%1,                          Neel%Gandhi%NULL%1,                          Shamimul%Khan%NULL%1,                          Steve%Williams%NULL%1,                          Fazle%Khan%NULL%1,                          Sarita%Shah%NULL%1,                           C. T.%Telford%null%1,                           U.% Onwubiko%null%1,                           D.% Holland%null%1,                           K.% Turner%null%1,                           J.% Prieto%null%1,                           S.% Smith%null%1,                           J.% Yoon%null%1,                           W.% Brown%null%1,                           A.% Chamberlain%null%1,                           N.% Gandhi%null%1,                           S.% Khan%null%1,                           S.% Williams%null%1,                           F.% Khan%null%1,                           S. % Shah%null%1,                          C. T.%Telford%null%1,                          U.% Onwubiko%null%1,                          D.% Holland%null%1,                          K.% Turner%null%1,                          J.% Prieto%null%1,                          S.% Smith%null%1,                          J.% Yoon%null%1,                          W.% Brown%null%1,                          A.% Chamberlain%null%1,                          N.% Gandhi%null%1,                          S.% Khan%null%1,                          S.% Williams%null%1,                          F.% Khan%null%1,                          S. % Shah%null%1,         C. T.%Telford%null%1,         U.% Onwubiko%null%1,         D.% Holland%null%1,         K.% Turner%null%1,         J.% Prieto%null%1,         S.% Smith%null%1,         J.% Yoon%null%1,         W.% Brown%null%1,         A.% Chamberlain%null%1,         N.% Gandhi%null%1,         S.% Khan%null%1,         S.% Williams%null%1,         F.% Khan%null%1,         S. % Shah%null%1]</t>
+  </si>
+  <si>
+    <t>[Sandra M.%Shi%NULL%1,                          Innokentiy%Bakaev%NULL%1,                          Helen%Chen%NULL%1,                          Thomas G.%Travison%NULL%1,                          Sarah D.%Berry%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Temet M.%McMichael%NULL%0,                          Dustin W.%Currie%NULL%0,                          Shauna%Clark%NULL%0,                          Sargis%Pogosjans%NULL%0,                          Meagan%Kay%NULL%0,                          Noah G.%Schwartz%NULL%0,                          James%Lewis%NULL%0,                          Atar%Baer%NULL%0,                          Vance%Kawakami%NULL%0,                          Margaret D.%Lukoff%NULL%0,                          Jessica%Ferro%NULL%0,                          Claire%Brostrom-Smith%NULL%0,                          Thomas D.%Rea%NULL%1,                          Michael R.%Sayre%NULL%1,                          Francis X.%Riedo%NULL%0,                          Denny%Russell%NULL%0,                          Brian%Hiatt%NULL%0,                          Patricia%Montgomery%NULL%0,                          Agam K.%Rao%NULL%0,                          Eric J.%Chow%NULL%0,                          Farrell%Tobolowsky%NULL%0,                          Michael J.%Hughes%NULL%1,                          Ana C.%Bardossy%NULL%0,                          Lisa P.%Oakley%NULL%0,                          Jesica R.%Jacobs%NULL%0,                          Nimalie D.%Stone%NULL%1,                          Sujan C.%Reddy%NULL%0,                          John A.%Jernigan%NULL%0,                          Margaret A.%Honein%NULL%0,                          Thomas A.%Clark%NULL%0,                          Jeffrey S.%Duchin%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Nathan M.%Stall%nathan.stall@sinaihealth.ca%1,                          Carolyn%Farquharson%NULL%2,                          Carolyn%Farquharson%NULL%0,                          Chris%Fan‐Lun%NULL%1,                          Lesley%Wiesenfeld%NULL%1,                          Carla A.%Loftus%NULL%1,                          Dylan%Kain%NULL%1,                          Jennie%Johnstone%NULL%1,                          Liz%McCreight%NULL%1,                          Russell D.%Goldman%NULL%1,                          Ramona%Mahtani%NULL%1]</t>
+  </si>
+  <si>
+    <t>[ Nathan M.%Stall%null%1,                           Aaron%Jones%null%1,                           Kevin A.%Brown%null%1,                           Paula A.%Rochon%null%1,                           Andrew P.%Costa%null%1,                          Nathan M.%Stall%null%1,                          Aaron%Jones%null%1,                          Kevin A.%Brown%null%1,                          Paula A.%Rochon%null%1,                          Andrew P.%Costa%null%1]</t>
+  </si>
+  <si>
+    <t>[Hubert%Blain%NULL%1,                          Yves%Rolland%NULL%1,                          Edouard%Tuaillon%NULL%1,                          Nadia%Giacosa%NULL%1,                          Mylène%Albrand%NULL%1,                          Audrey%Jaussent%NULL%1,                          Athanase%Benetos%NULL%1,                          Stéphanie%Miot%NULL%1,                          Jean%Bousquet%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Jo\u00ebl%Belmin%xref no email%1,       Nathavy%Um-Din%xref no email%1,       Cristiano%Donadio%xref no email%1,       Maurizio%Magri%xref no email%1,       Quoc Duy%Nghiem%xref no email%1,       Bruno%Oquendo%xref no email%1,       Sylvie%Pariel%xref no email%1,       Carmelo%Lafuente-Lafuente%xref no email%1]</t>
+  </si>
+  <si>
+    <t>[Guillaume%Sacco%NULL%1,                          Gonzague%Foucault%NULL%1,                          Olivier%Briere%NULL%1,                          Cédric%Annweiler%NULL%1]</t>
+  </si>
+  <si>
+    <t>[R.%Guery%NULL%1,                          C.%Delaye%NULL%1,                          N.%Brule%NULL%1,                          V.%Nael%NULL%1,                          L.%Castain%NULL%1,                          F.%Raffi%NULL%1,                          L.%De Decker%NULL%1]</t>
+  </si>
+  <si>
+    <t>[A.%Klein%anke.klein@uke.de%1,                          C.%Edler%NULL%1,                          A.%Fitzek%NULL%1,                          D.%Fröb%NULL%1,                          A.%Heinemann%NULL%1,                          K.%Meißner%NULL%1,                          H.%Mushumba%NULL%1,                          K.%Püschel%NULL%1,                          A. S.%Schröder%NULL%1,                          J. P.%Sperhake%NULL%1,                          F.%Ishorst-Witte%NULL%1,                          M.%Aepfelbacher%NULL%1,                          F.%Heinrich%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Buntinx%Frank%coreGivesNoEmail%1,                        Claes%Peter%coreGivesNoEmail%1,                        Gulikers%Marjo%coreGivesNoEmail%1,                        Jan%De Lepeleire%coreGivesNoEmail%1,                        Van%der Elst Michael%coreGivesNoEmail%1,                        Van%Elslande Jan%coreGivesNoEmail%1,                        Van%Ranst Marc%coreGivesNoEmail%1,                        Verbakel%Jan%coreGivesNoEmail%1,                        Vernneersch%Pieter%coreGivesNoEmail%1]</t>
+  </si>
+  <si>
+    <t>[Sean P%Kennelly%Sean.Kennelly@tuh.ie%1,                          Adam H%Dyer%dyera@tcd.ie%1,                          Claire%Noonan%claire.noonan@tuh.ie%2,                          Claire%Noonan%claire.noonan@tuh.ie%0,                          Ruth%Martin%ruth.martin1@hse.ie%1,                          Siobhan M%Kennelly%siobhan.kennelly1@hse.ie%1,                          Alan%Martin%alanmartin@beaumont.ie%1,                          Desmond%O’Neill%NULL%1,                          Aoife%Fallon%aoife.fallon1@hotmail.com%1]</t>
+  </si>
+  <si>
+    <t>[Antonio%Nouvenne%NULL%1,                          Andrea%Ticinesi%NULL%1,                          Alberto%Parise%NULL%1,                          Beatrice%Prati%NULL%1,                          Marcello%Esposito%NULL%1,                          Valentina%Cocchi%NULL%1,                          Emanuele%Crisafulli%NULL%1,                          Annalisa%Volpi%NULL%1,                          Sandra%Rossi%NULL%1,                          Elena Giovanna%Bignami%NULL%1,                          Marco%Baciarello%NULL%1,                          Ettore%Brianti%NULL%1,                          Massimo%Fabi%NULL%1,                          Tiziana%Meschi%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Nicola%Veronese%NULL%1,                          Luca Gino%Sbrogiò%NULL%1,                          Roberto%Valle%NULL%1,                          Laura%Marin%NULL%1,                          Elena%Boscolo Fiore%NULL%1,                          Andrea%Tiozzo%NULL%1]</t>
+  </si>
+  <si>
+    <t>[ J. H.%van den Besselaar%null%1,                           R. S.% Sikkema%null%1,                           F. M. H. P. A.% Koene%null%1,                           L. W.% van Buul%null%1,                           B. B.% Oude Munnink%null%1,                           I.% Frenay%null%1,                           R.% te Witt%null%1,                           M. P. G.% Koopmans%null%1,                           C. M. P. M.% Hertogh%null%1,                           B. M. % Buurman%null%1,         J. H.%van den Besselaar%null%1,         R. S.% Sikkema%null%1,         F. M. H. P. A.% Koene%null%1,         L. W.% van Buul%null%1,         B. B.% Oude Munnink%null%1,         I.% Frenay%null%1,         R.% te Witt%null%1,         M. P. G.% Koopmans%null%1,         C. M. P. M.% Hertogh%null%1,         B. M. % Buurman%null%1]</t>
+  </si>
+  <si>
+    <t>[Laura W.%van Buul%NULL%1,                          Judith H.%van den Besselaar%NULL%2,                          Judith H.%van den Besselaar%NULL%0,                          Fleur M. H. P. H.%Koene%NULL%1,                          Bianca M.%Buurman%NULL%1,                          Cees M. P. M.%Hertogh%NULL%1,                          Martin%Smalbrugge%NULL%1,                          Jeanine J. S.%Rutten%NULL%1,                          Elke M.%den Boogert%NULL%1,                          Michel D.%Wissing%NULL%1,                          Ariene%Rietveld%NULL%1,                          Mariska W. W.%van Elsakker%NULL%1,                          Marga M. G.%Nonneman%NULL%1,                          Florien%van Eeden%NULL%1,                          Saskia%van de Merwe%NULL%1,                          Sophie L.%Niemansburg%NULL%1,                          Ewout%Fanoy%NULL%1,                          Hinke S.%Bootsma%NULL%1,                          Nicoline%van der Hagen%NULL%1,                          Mariska%Petrignani%NULL%1,                          Jessica Edwards%van Muijen%NULL%1,                          Karolien E. M.%Biesheuvel%NULL%1]</t>
+  </si>
+  <si>
+    <t>[B\u00e5rd%Reiakvam Kittang%coreGivesNoEmail%1,                        Karina%Koller L\u00f8land%coreGivesNoEmail%1,                        Kjell%Kr\u00fcger%coreGivesNoEmail%1,                        Kristian%Jansen%coreGivesNoEmail%1,                        Sabine%Piepenstock Solheim%coreGivesNoEmail%1,                        Sebastian%von Hofacker%coreGivesNoEmail%1]</t>
+  </si>
+  <si>
+    <t>[Shin Young%Park%NULL%1,                          Gawon%Choi%NULL%2,                          Gawon%Choi%NULL%0,                          Hyeyoung%Lee%NULL%2,                          Hyeyoung%Lee%NULL%0,                          Na-young%Kim%NULL%2,                          Na-young%Kim%NULL%0,                          Seon-young%Lee%NULL%2,                          Seon-young%Lee%NULL%0,                          Kyungnam%Kim%NULL%2,                          Kyungnam%Kim%NULL%0,                          Soyoung%Shin%NULL%2,                          Soyoung%Shin%NULL%0,                          Eunsu%Jang%NULL%2,                          Eunsu%Jang%NULL%0,                          YoungSin%Moon%NULL%2,                          YoungSin%Moon%NULL%0,                          KwangHwan%Oh%NULL%2,                          KwangHwan%Oh%NULL%0,                          JaeRin%Choi%NULL%2,                          JaeRin%Choi%NULL%0,                          Sangeun%Lee%NULL%2,                          Sangeun%Lee%NULL%0,                          Young-Man%Kim%NULL%2,                          Young-Man%Kim%NULL%0,                          Jieun%Kim%NULL%2,                          Jieun%Kim%NULL%0,                          Seonju%Yi%NULL%2,                          Seonju%Yi%NULL%0,                          Jin%Gwack%NULL%2,                          Jin%Gwack%NULL%0,                          Ok%Park%NULL%2,                          Ok%Park%NULL%0,                          Young Joon%Park%NULL%2,                          Young Joon%Park%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Rok%Song%NULL%1,                          Hee-Sook%Kim%NULL%2,                          Hee-Sook%Kim%NULL%0,                          Seok-Ju%Yoo%NULL%2,                          Seok-Ju%Yoo%NULL%0,                          Kwan%Lee%NULL%2,                          Kwan%Lee%NULL%0,                          Ji-Hyuk%Park%NULL%2,                          Ji-Hyuk%Park%NULL%0,                          Joon Ho%Jang%NULL%2,                          Joon Ho%Jang%NULL%0,                          Gyoung-Sook%Ahn%NULL%2,                          Gyoung-Sook%Ahn%NULL%0,                          Jun-Nyun%Kim%NULL%2,                          Jun-Nyun%Kim%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Blanca%Borras-Bermejo%NULL%1,                          Xavier%Martínez-Gómez%NULL%1,                          María Gutierrez%San Miguel%NULL%1,                          Juliana%Esperalba%NULL%1,                          Andrés%Antón%NULL%1,                          Elisabet%Martin%NULL%1,                          Marta%Selvi%NULL%1,                          María José%Abadías%NULL%1,                          Antonio%Román%NULL%1,                          Tomàs%Pumarola%NULL%1,                          Magda%Campins%NULL%1,                          Benito%Almirante%NULL%1]</t>
+  </si>
+  <si>
+    <t>[M.%Bernabeu-Wittel%NULL%1,                          J.E.%Ternero-Vega%NULL%1,                          P.%Díaz-Jiménez%NULL%1,                          C.%Conde-Guzmán%NULL%1,                          M.D.%Nieto-Martín%NULL%1,                          L.%Moreno-Gaviño%NULL%1,                          J.%Delgado-Cuesta%NULL%1,                          M.%Rincón-Gómez%NULL%1,                          L.%Giménez-Miranda%NULL%1,                          M.D.%Navarro-Amuedo%NULL%1,                          M.M.%Muñoz-García%NULL%1,                          S.%Calzón-Fernández%NULL%1,                          M.%Ollero-Baturone%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Shamez N%Ladhani%shamez.ladhani@phe.gov.uk%1,                          J.Yimmy%Chow%NULL%1,                          Roshni%Janarthanan%NULL%1,                          Jonathan%Fok%NULL%1,                          Emma%Crawley-Boevey%NULL%1,                          Amoolya%Vusirikala%NULL%1,                          Elena%Fernandez%NULL%1,                          Marina Sanchez%Perez%NULL%1,                          Suzanne%Tang%NULL%1,                          Kate%Dun-Campbell%NULL%1,                          Edward Wynne-%Evans%NULL%1,                          Anita%Bell%NULL%1,                          Bharat%Patel%NULL%1,                          Zahin%Amin-Chowdhury%NULL%1,                          Felicity%Aiano%NULL%1,                          Karthik%Paranthaman%NULL%1,                          Thomas%Ma%NULL%1,                          Maria%Saavedra-Campos%NULL%1,                          Richard%Myers%NULL%1,                          Joanna%Ellis%NULL%2,                          Angie%Lackenby%NULL%1,                          Robin%Gopal%NULL%1,                          Monika%Patel%NULL%1,                          Colin%Brown%NULL%1,                          Meera%Chand%NULL%1,                          Kevin%Brown%NULL%1,                          Mary E%Ramsay%NULL%1,                          Susan%Hopkins%NULL%2,                          Nandini%Shetty%NULL%1,                          Maria%Zambon%NULL%2]</t>
+  </si>
+  <si>
+    <t>[N.S.N.%Graham%NULL%1,                          C.%Junghans%NULL%1,                          R.%Downes%NULL%1,                          C.%Sendall%NULL%1,                          H.%Lai%NULL%1,                          A.%McKirdy%NULL%1,                          P.%Elliott%NULL%1,                          R.%Howard%NULL%1,                          D.%Wingfield%NULL%1,                          M.%Priestman%NULL%1,                          M.%Ciechonska%NULL%1,                          L.%Cameron%NULL%1,                          M.%Storch%NULL%1,                          M.A.%Crone%NULL%1,                          P.S.%Freemont%NULL%1,                          P.%Randell%NULL%1,                          R.%McLaren%NULL%1,                          N.%Lang%NULL%1,                          S.%Ladhani%NULL%1,                          F.%Sanderson%NULL%1,                          D.J.%Sharp%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Agnes%Marossy%agnesmarossy@nhs.net%1,                          Stefan%Rakowicz%NULL%1,                          Angela%Bhan%NULL%1,                          Sarah%Noon%NULL%1,                          Amanda%Rees%NULL%1,                          Manjinder%Virk%NULL%1,                          Ayazali%Nazafi%NULL%1,                          Evie%Hay%NULL%1,                          Louise%de Thomasson%NULL%1,                          Christina%Windle%NULL%1,                          Mark%Zuckerman%Mark.Zuckerman@nhs.net%1]</t>
+  </si>
+  <si>
+    <t>[Laura%Shallcross%NULL%1,                          Danielle%Burke%NULL%1,                          Owen%Abbott%NULL%1,                          Alasdair%Donaldson%NULL%1,                          Gemma%Hallatt%NULL%1,                          Andrew%Hayward%NULL%1,                          Susan%Hopkins%NULL%0,                          Maria%Krutikov%NULL%1,                          Katie%Sharp%NULL%1,                          Leone%Wardman%NULL%1,                          Sapphira%Thorne%NULL%1]</t>
+  </si>
+  <si>
+    <t>[ E.%Smith%null%1,                           C. F.% Aldus%null%1,                           J.% Brainard%null%1,                           S.% Dunham%null%1,                           P. R.% Hunter%null%1,                           N.% Steel%null%1,                           P. % Everden%null%1,         E.%Smith%null%1,         C. F.% Aldus%null%1,         J.% Brainard%null%1,         S.% Dunham%null%1,         P. R.% Hunter%null%1,         N.% Steel%null%1,         P. % Everden%null%1]</t>
+  </si>
+  <si>
+    <t>[Mahesh C%Patel%mp3@uic.edu%1,                          Lelia H%Chaisson%NULL%1,                          Scott%Borgetti%NULL%1,                          Deborah%Burdsall%NULL%1,                          Rashmi K%Chugh%NULL%1,                          Christopher R%Hoff%NULL%1,                          Elizabeth B%Murphy%NULL%1,                          Emily A%Murskyj%NULL%1,                          Shannon%Wilson%NULL%1,                          Joe%Ramos%NULL%1,                          Lynn%Akker%NULL%1,                          Debra%Bryars%NULL%1,                          Evonda%Thomas-Smith%NULL%1,                          Susan C%Bleasdale%NULL%1,                          Ngozi O%Ezike%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Helena%Temkin‐Greener%helena_temkin-greener@urmc.rochester.edu%1,                          Wenhan%Guo%NULL%2,                          Wenhan%Guo%NULL%0,                          Yunjiao%Mao%NULL%1,                          Xueya%Cai%NULL%1,                          Yue%Li%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Ana A.%Weil%anaweil@uw.edu%1,                          Kira L.%Newman%NULL%2,                          Kira L.%Newman%NULL%0,                          Thuan D.%Ong%NULL%1,                          Giana H.%Davidson%NULL%1,                          Jennifer%Logue%NULL%1,                          Elisabeth%Brandstetter%NULL%1,                          Ariana%Magedson%NULL%1,                          Dylan%McDonald%NULL%1,                          Denise J.%McCulloch%NULL%1,                          Santiago%Neme%NULL%1,                          James%Lewis%NULL%0,                          Jeff S.%Duchin%NULL%1,                          Weizhi%Zhong%NULL%1,                          Lea M.%Starita%NULL%1,                          Trevor%Bedford%NULL%1,                          Alison C.%Roxby%NULL%1,                          Helen Y.%Chu%helenchu@uw.edu%2]</t>
+  </si>
+  <si>
+    <t>[Guillermo V.%Sanchez%NULL%1,                          Caitlin%Biedron%NULL%1,                          Lauren R.%Fink%NULL%1,                          Kelly M.%Hatfield%NULL%1,                          Jordan Micah F.%Polistico%NULL%1,                          Monica P.%Meyer%NULL%1,                          Rebecca S.%Noe%NULL%1,                          Casey E.%Copen%NULL%1,                          Amanda K.%Lyons%NULL%1,                          Gonzalo%Gonzalez%NULL%1,                          Keith%Kiama%NULL%1,                          Mark%Lebednick%NULL%1,                          Bonnie K.%Czander%NULL%1,                          Amen%Agbonze%NULL%1,                          Aimee R.%Surma%NULL%1,                          Avnish%Sandhu%NULL%1,                          Valerie H.%Mika%NULL%1,                          Tyler%Prentiss%NULL%1,                          John%Zervos%NULL%1,                          Donia A.%Dalal%NULL%1,                          Amber M.%Vasquez%NULL%1,                          Sujan C.%Reddy%NULL%0,                          John%Jernigan%NULL%1,                          Paul E.%Kilgore%NULL%1,                          Marcus J.%Zervos%NULL%1,                          Teena%Chopra%NULL%1,                          Carla P.%Bezold%NULL%1,                          Najibah K.%Rehman%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Janice K%Louie%Janice.louie@sfdph.org%1,                          Hyman M%Scott%NULL%1,                          Amie%DuBois%NULL%1,                          Natalya%Sturtz%NULL%1,                          Wendy%Lu%NULL%1,                          Juliet%Stoltey%NULL%1,                          Godfred%Masinde%NULL%1,                          Stephanie%Cohen%NULL%1,                          Darpun%Sachdev%NULL%1,                          Susan%Philip%NULL%1,                          Naveena%Bobba%NULL%1,                          Tomas%Aragon%NULL%1,                          NULL%NULL%NULL%0]</t>
+  </si>
+  <si>
+    <t>[Scott A%Goldberg%sagoldberg@bwh.harvard.edu%1,                          Jochen%Lennerz%NULL%1,                          Michael%Klompas%NULL%1,                          Eden%Mark%NULL%1,                          Virginia M%Pierce%NULL%1,                          Ryan W%Thompson%NULL%1,                          Charles T%Pu%NULL%1,                          Lauren L%Ritterhouse%NULL%1,                          Anand%Dighe%NULL%1,                          Eric S%Rosenberg%NULL%1,                          David C%Grabowski%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Amy V.%Dora%NULL%1,                          Alexander%Winnett%NULL%1,                          Lauren P.%Jatt%NULL%1,                          Kusha%Davar%NULL%1,                          Mika%Watanabe%NULL%1,                          Linda%Sohn%NULL%1,                          Hannah S.%Kern%NULL%1,                          Christopher J.%Graber%NULL%1,                          Matthew B.%Goetz%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Benjamin F.%Bigelow%NULL%1,                          Olive%Tang%NULL%1,                          Gregory R.%Toci%NULL%1,                          Norberth%Stracker%NULL%1,                          Fatima%Sheikh%NULL%1,                          Kara M.%Jacobs Slifka%NULL%1,                          Shannon A.%Novosad%NULL%1,                          John A.%Jernigan%NULL%0,                          Sujan C.%Reddy%NULL%0,                          Morgan J.%Katz%NULL%1]</t>
+  </si>
+  <si>
+    <t>[Matt%Feaster%NULL%1,                          Ying-Ying%Goh%NULL%1]</t>
+  </si>
+  <si>
+    <t>[William R.%Mills%NULL%1,                          Janet M.%Buccola%NULL%1,                          Susan%Sender%NULL%1,                          Joseph%Lichtefeld%NULL%1,                          Nicholas%Romano%NULL%1,                          Karen%Reynolds%NULL%1,                          Melissa%Price%NULL%1,                          Jennifer%Phipps%NULL%1,                          Leigh%White%NULL%1,                          Shauen%Howard%NULL%1]</t>
   </si>
 </sst>
 </file>
@@ -2997,7 +3231,7 @@
         <v>59</v>
       </c>
       <c r="E2" t="s">
-        <v>713</v>
+        <v>794</v>
       </c>
       <c r="F2" t="s">
         <v>60</v>
@@ -3029,7 +3263,7 @@
         <v>64</v>
       </c>
       <c r="E3" t="s">
-        <v>714</v>
+        <v>795</v>
       </c>
       <c r="F3" t="s">
         <v>65</v>
@@ -3061,7 +3295,7 @@
         <v>67</v>
       </c>
       <c r="E4" t="s">
-        <v>715</v>
+        <v>796</v>
       </c>
       <c r="F4" t="s">
         <v>68</v>
@@ -3125,7 +3359,7 @@
         <v>70</v>
       </c>
       <c r="E6" t="s">
-        <v>716</v>
+        <v>797</v>
       </c>
       <c r="F6" t="s">
         <v>6</v>
@@ -3157,7 +3391,7 @@
         <v>73</v>
       </c>
       <c r="E7" t="s">
-        <v>717</v>
+        <v>798</v>
       </c>
       <c r="F7" t="s">
         <v>74</v>
@@ -3189,7 +3423,7 @@
         <v>76</v>
       </c>
       <c r="E8" t="s">
-        <v>718</v>
+        <v>799</v>
       </c>
       <c r="F8" t="s">
         <v>77</v>
@@ -3253,7 +3487,7 @@
         <v>79</v>
       </c>
       <c r="E10" t="s">
-        <v>719</v>
+        <v>800</v>
       </c>
       <c r="F10" t="s">
         <v>80</v>
@@ -3285,7 +3519,7 @@
         <v>83</v>
       </c>
       <c r="E11" t="s">
-        <v>720</v>
+        <v>801</v>
       </c>
       <c r="F11" t="s">
         <v>84</v>
@@ -3317,7 +3551,7 @@
         <v>88</v>
       </c>
       <c r="E12" t="s">
-        <v>721</v>
+        <v>802</v>
       </c>
       <c r="F12" t="s">
         <v>89</v>
@@ -3349,7 +3583,7 @@
         <v>51</v>
       </c>
       <c r="E13" t="s">
-        <v>722</v>
+        <v>803</v>
       </c>
       <c r="F13" t="s">
         <v>243</v>
@@ -3381,7 +3615,7 @@
         <v>91</v>
       </c>
       <c r="E14" t="s">
-        <v>723</v>
+        <v>804</v>
       </c>
       <c r="F14" t="s">
         <v>92</v>
@@ -3413,7 +3647,7 @@
         <v>95</v>
       </c>
       <c r="E15" t="s">
-        <v>724</v>
+        <v>805</v>
       </c>
       <c r="F15" t="s">
         <v>96</v>
@@ -3445,7 +3679,7 @@
         <v>99</v>
       </c>
       <c r="E16" t="s">
-        <v>725</v>
+        <v>806</v>
       </c>
       <c r="F16" t="s">
         <v>100</v>
@@ -3477,7 +3711,7 @@
         <v>190</v>
       </c>
       <c r="E17" t="s">
-        <v>726</v>
+        <v>807</v>
       </c>
       <c r="F17" t="s">
         <v>16</v>
@@ -3541,7 +3775,7 @@
         <v>51</v>
       </c>
       <c r="E19" t="s">
-        <v>727</v>
+        <v>257</v>
       </c>
       <c r="F19" t="s">
         <v>18</v>
@@ -3573,7 +3807,7 @@
         <v>105</v>
       </c>
       <c r="E20" t="s">
-        <v>728</v>
+        <v>808</v>
       </c>
       <c r="F20" t="s">
         <v>106</v>
@@ -3605,7 +3839,7 @@
         <v>109</v>
       </c>
       <c r="E21" t="s">
-        <v>729</v>
+        <v>809</v>
       </c>
       <c r="F21" t="s">
         <v>110</v>
@@ -3637,7 +3871,7 @@
         <v>112</v>
       </c>
       <c r="E22" t="s">
-        <v>730</v>
+        <v>810</v>
       </c>
       <c r="F22" t="s">
         <v>113</v>
@@ -3701,7 +3935,7 @@
         <v>115</v>
       </c>
       <c r="E24" t="s">
-        <v>731</v>
+        <v>811</v>
       </c>
       <c r="F24" t="s">
         <v>23</v>
@@ -3733,7 +3967,7 @@
         <v>118</v>
       </c>
       <c r="E25" t="s">
-        <v>732</v>
+        <v>812</v>
       </c>
       <c r="F25" t="s">
         <v>119</v>
@@ -3765,7 +3999,7 @@
         <v>51</v>
       </c>
       <c r="E26" t="s">
-        <v>733</v>
+        <v>813</v>
       </c>
       <c r="F26" t="s">
         <v>25</v>
@@ -3797,7 +4031,7 @@
         <v>122</v>
       </c>
       <c r="E27" t="s">
-        <v>734</v>
+        <v>814</v>
       </c>
       <c r="F27" t="s">
         <v>123</v>
@@ -3829,7 +4063,7 @@
         <v>126</v>
       </c>
       <c r="E28" t="s">
-        <v>735</v>
+        <v>815</v>
       </c>
       <c r="F28" t="s">
         <v>127</v>
@@ -3861,7 +4095,7 @@
         <v>130</v>
       </c>
       <c r="E29" t="s">
-        <v>736</v>
+        <v>816</v>
       </c>
       <c r="F29" t="s">
         <v>131</v>
@@ -3893,7 +4127,7 @@
         <v>95</v>
       </c>
       <c r="E30" t="s">
-        <v>737</v>
+        <v>817</v>
       </c>
       <c r="F30" t="s">
         <v>133</v>
@@ -3925,7 +4159,7 @@
         <v>136</v>
       </c>
       <c r="E31" t="s">
-        <v>738</v>
+        <v>818</v>
       </c>
       <c r="F31" t="s">
         <v>137</v>
@@ -3957,7 +4191,7 @@
         <v>140</v>
       </c>
       <c r="E32" t="s">
-        <v>739</v>
+        <v>819</v>
       </c>
       <c r="F32" t="s">
         <v>141</v>
@@ -3989,7 +4223,7 @@
         <v>144</v>
       </c>
       <c r="E33" t="s">
-        <v>740</v>
+        <v>820</v>
       </c>
       <c r="F33" t="s">
         <v>145</v>
@@ -4021,7 +4255,7 @@
         <v>147</v>
       </c>
       <c r="E34" t="s">
-        <v>741</v>
+        <v>821</v>
       </c>
       <c r="F34" t="s">
         <v>148</v>
@@ -4053,7 +4287,7 @@
         <v>150</v>
       </c>
       <c r="E35" t="s">
-        <v>742</v>
+        <v>822</v>
       </c>
       <c r="F35" t="s">
         <v>34</v>
@@ -4085,7 +4319,7 @@
         <v>153</v>
       </c>
       <c r="E36" t="s">
-        <v>743</v>
+        <v>823</v>
       </c>
       <c r="F36" t="s">
         <v>154</v>
@@ -4117,7 +4351,7 @@
         <v>157</v>
       </c>
       <c r="E37" t="s">
-        <v>744</v>
+        <v>824</v>
       </c>
       <c r="F37" t="s">
         <v>158</v>
@@ -4149,7 +4383,7 @@
         <v>201</v>
       </c>
       <c r="E38" t="s">
-        <v>745</v>
+        <v>825</v>
       </c>
       <c r="F38" t="s">
         <v>161</v>
@@ -4181,7 +4415,7 @@
         <v>95</v>
       </c>
       <c r="E39" t="s">
-        <v>746</v>
+        <v>826</v>
       </c>
       <c r="F39" t="s">
         <v>164</v>
@@ -4213,7 +4447,7 @@
         <v>166</v>
       </c>
       <c r="E40" t="s">
-        <v>747</v>
+        <v>827</v>
       </c>
       <c r="F40" t="s">
         <v>167</v>
@@ -4245,7 +4479,7 @@
         <v>169</v>
       </c>
       <c r="E41" t="s">
-        <v>748</v>
+        <v>828</v>
       </c>
       <c r="F41" t="s">
         <v>170</v>
@@ -4277,7 +4511,7 @@
         <v>95</v>
       </c>
       <c r="E42" t="s">
-        <v>749</v>
+        <v>829</v>
       </c>
       <c r="F42" t="s">
         <v>172</v>
@@ -4309,7 +4543,7 @@
         <v>95</v>
       </c>
       <c r="E43" t="s">
-        <v>750</v>
+        <v>830</v>
       </c>
       <c r="F43" t="s">
         <v>174</v>
@@ -4341,7 +4575,7 @@
         <v>176</v>
       </c>
       <c r="E44" t="s">
-        <v>751</v>
+        <v>831</v>
       </c>
       <c r="F44" t="s">
         <v>177</v>
@@ -4373,7 +4607,7 @@
         <v>179</v>
       </c>
       <c r="E45" t="s">
-        <v>752</v>
+        <v>832</v>
       </c>
       <c r="F45" t="s">
         <v>180</v>
@@ -4405,7 +4639,7 @@
         <v>51</v>
       </c>
       <c r="E46" t="s">
-        <v>753</v>
+        <v>283</v>
       </c>
       <c r="F46" t="s">
         <v>45</v>
@@ -4437,7 +4671,7 @@
         <v>199</v>
       </c>
       <c r="E47" t="s">
-        <v>754</v>
+        <v>284</v>
       </c>
       <c r="F47" t="s">
         <v>46</v>

</xml_diff>